<commit_message>
Added tools to spreadsheets and TSV
</commit_message>
<xml_diff>
--- a/config/Polycraft Polymers.xlsx
+++ b/config/Polycraft Polymers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13710" yWindow="0" windowWidth="27240" windowHeight="14310" tabRatio="826" activeTab="8"/>
+    <workbookView xWindow="13710" yWindow="0" windowWidth="27240" windowHeight="14310" tabRatio="826" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Pellets" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2250" uniqueCount="2189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2096" uniqueCount="2036">
   <si>
     <t>GC</t>
   </si>
@@ -5595,84 +5595,6 @@
     <t>23</t>
   </si>
   <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>2a</t>
-  </si>
-  <si>
-    <t>2b</t>
-  </si>
-  <si>
-    <t>2c</t>
-  </si>
-  <si>
-    <t>2d</t>
-  </si>
-  <si>
-    <t>2e</t>
-  </si>
-  <si>
-    <t>2f</t>
-  </si>
-  <si>
-    <t>2g</t>
-  </si>
-  <si>
-    <t>2h</t>
-  </si>
-  <si>
-    <t>2i</t>
-  </si>
-  <si>
-    <t>2j</t>
-  </si>
-  <si>
-    <t>2k</t>
-  </si>
-  <si>
-    <t>2l</t>
-  </si>
-  <si>
-    <t>2m</t>
-  </si>
-  <si>
-    <t>2n</t>
-  </si>
-  <si>
-    <t>2o</t>
-  </si>
-  <si>
-    <t>2p</t>
-  </si>
-  <si>
-    <t>2q</t>
-  </si>
-  <si>
-    <t>2r</t>
-  </si>
-  <si>
-    <t>2s</t>
-  </si>
-  <si>
-    <t>2t</t>
-  </si>
-  <si>
     <t>insole</t>
   </si>
   <si>
@@ -5988,84 +5910,6 @@
     <t>Efficiency (Int)</t>
   </si>
   <si>
-    <t>17a</t>
-  </si>
-  <si>
-    <t>179</t>
-  </si>
-  <si>
-    <t>178</t>
-  </si>
-  <si>
-    <t>177</t>
-  </si>
-  <si>
-    <t>176</t>
-  </si>
-  <si>
-    <t>175</t>
-  </si>
-  <si>
-    <t>174</t>
-  </si>
-  <si>
-    <t>173</t>
-  </si>
-  <si>
-    <t>172</t>
-  </si>
-  <si>
-    <t>171</t>
-  </si>
-  <si>
-    <t>170</t>
-  </si>
-  <si>
-    <t>16Z</t>
-  </si>
-  <si>
-    <t>16Y</t>
-  </si>
-  <si>
-    <t>16X</t>
-  </si>
-  <si>
-    <t>16W</t>
-  </si>
-  <si>
-    <t>16V</t>
-  </si>
-  <si>
-    <t>16U</t>
-  </si>
-  <si>
-    <t>16T</t>
-  </si>
-  <si>
-    <t>16S</t>
-  </si>
-  <si>
-    <t>16R</t>
-  </si>
-  <si>
-    <t>16Q</t>
-  </si>
-  <si>
-    <t>16P</t>
-  </si>
-  <si>
-    <t>16O</t>
-  </si>
-  <si>
-    <t>16N</t>
-  </si>
-  <si>
-    <t>16M</t>
-  </si>
-  <si>
-    <t>16L</t>
-  </si>
-  <si>
     <t>16K</t>
   </si>
   <si>
@@ -6108,84 +5952,6 @@
     <t>16x</t>
   </si>
   <si>
-    <t>17O</t>
-  </si>
-  <si>
-    <t>17N</t>
-  </si>
-  <si>
-    <t>17M</t>
-  </si>
-  <si>
-    <t>17L</t>
-  </si>
-  <si>
-    <t>17K</t>
-  </si>
-  <si>
-    <t>17J</t>
-  </si>
-  <si>
-    <t>17I</t>
-  </si>
-  <si>
-    <t>17H</t>
-  </si>
-  <si>
-    <t>17G</t>
-  </si>
-  <si>
-    <t>17F</t>
-  </si>
-  <si>
-    <t>17E</t>
-  </si>
-  <si>
-    <t>17D</t>
-  </si>
-  <si>
-    <t>17C</t>
-  </si>
-  <si>
-    <t>17B</t>
-  </si>
-  <si>
-    <t>17A</t>
-  </si>
-  <si>
-    <t>17z</t>
-  </si>
-  <si>
-    <t>17y</t>
-  </si>
-  <si>
-    <t>17x</t>
-  </si>
-  <si>
-    <t>17w</t>
-  </si>
-  <si>
-    <t>17v</t>
-  </si>
-  <si>
-    <t>17u</t>
-  </si>
-  <si>
-    <t>17t</t>
-  </si>
-  <si>
-    <t>17s</t>
-  </si>
-  <si>
-    <t>17r</t>
-  </si>
-  <si>
-    <t>17q</t>
-  </si>
-  <si>
-    <t>17p</t>
-  </si>
-  <si>
     <t>17o</t>
   </si>
   <si>
@@ -6228,84 +5994,6 @@
     <t>17b</t>
   </si>
   <si>
-    <t>18s</t>
-  </si>
-  <si>
-    <t>18r</t>
-  </si>
-  <si>
-    <t>18q</t>
-  </si>
-  <si>
-    <t>18p</t>
-  </si>
-  <si>
-    <t>18o</t>
-  </si>
-  <si>
-    <t>18n</t>
-  </si>
-  <si>
-    <t>18m</t>
-  </si>
-  <si>
-    <t>18l</t>
-  </si>
-  <si>
-    <t>18k</t>
-  </si>
-  <si>
-    <t>18j</t>
-  </si>
-  <si>
-    <t>18i</t>
-  </si>
-  <si>
-    <t>18h</t>
-  </si>
-  <si>
-    <t>18g</t>
-  </si>
-  <si>
-    <t>18f</t>
-  </si>
-  <si>
-    <t>18e</t>
-  </si>
-  <si>
-    <t>18d</t>
-  </si>
-  <si>
-    <t>18c</t>
-  </si>
-  <si>
-    <t>18b</t>
-  </si>
-  <si>
-    <t>18a</t>
-  </si>
-  <si>
-    <t>189</t>
-  </si>
-  <si>
-    <t>188</t>
-  </si>
-  <si>
-    <t>187</t>
-  </si>
-  <si>
-    <t>186</t>
-  </si>
-  <si>
-    <t>185</t>
-  </si>
-  <si>
-    <t>184</t>
-  </si>
-  <si>
-    <t>183</t>
-  </si>
-  <si>
     <t>182</t>
   </si>
   <si>
@@ -6348,84 +6036,6 @@
     <t>17P</t>
   </si>
   <si>
-    <t>196</t>
-  </si>
-  <si>
-    <t>195</t>
-  </si>
-  <si>
-    <t>194</t>
-  </si>
-  <si>
-    <t>193</t>
-  </si>
-  <si>
-    <t>192</t>
-  </si>
-  <si>
-    <t>191</t>
-  </si>
-  <si>
-    <t>190</t>
-  </si>
-  <si>
-    <t>18Z</t>
-  </si>
-  <si>
-    <t>18Y</t>
-  </si>
-  <si>
-    <t>18X</t>
-  </si>
-  <si>
-    <t>18W</t>
-  </si>
-  <si>
-    <t>18V</t>
-  </si>
-  <si>
-    <t>18U</t>
-  </si>
-  <si>
-    <t>18T</t>
-  </si>
-  <si>
-    <t>18S</t>
-  </si>
-  <si>
-    <t>18R</t>
-  </si>
-  <si>
-    <t>18Q</t>
-  </si>
-  <si>
-    <t>18P</t>
-  </si>
-  <si>
-    <t>18O</t>
-  </si>
-  <si>
-    <t>18N</t>
-  </si>
-  <si>
-    <t>18M</t>
-  </si>
-  <si>
-    <t>18L</t>
-  </si>
-  <si>
-    <t>18K</t>
-  </si>
-  <si>
-    <t>18J</t>
-  </si>
-  <si>
-    <t>18I</t>
-  </si>
-  <si>
-    <t>18H</t>
-  </si>
-  <si>
     <t>18G</t>
   </si>
   <si>
@@ -6468,84 +6078,6 @@
     <t>18t</t>
   </si>
   <si>
-    <t>19K</t>
-  </si>
-  <si>
-    <t>19J</t>
-  </si>
-  <si>
-    <t>19I</t>
-  </si>
-  <si>
-    <t>19H</t>
-  </si>
-  <si>
-    <t>19G</t>
-  </si>
-  <si>
-    <t>19F</t>
-  </si>
-  <si>
-    <t>19E</t>
-  </si>
-  <si>
-    <t>19D</t>
-  </si>
-  <si>
-    <t>19C</t>
-  </si>
-  <si>
-    <t>19B</t>
-  </si>
-  <si>
-    <t>19A</t>
-  </si>
-  <si>
-    <t>19z</t>
-  </si>
-  <si>
-    <t>19y</t>
-  </si>
-  <si>
-    <t>19x</t>
-  </si>
-  <si>
-    <t>19w</t>
-  </si>
-  <si>
-    <t>19v</t>
-  </si>
-  <si>
-    <t>19u</t>
-  </si>
-  <si>
-    <t>19t</t>
-  </si>
-  <si>
-    <t>19s</t>
-  </si>
-  <si>
-    <t>19r</t>
-  </si>
-  <si>
-    <t>19q</t>
-  </si>
-  <si>
-    <t>19p</t>
-  </si>
-  <si>
-    <t>19o</t>
-  </si>
-  <si>
-    <t>19n</t>
-  </si>
-  <si>
-    <t>19m</t>
-  </si>
-  <si>
-    <t>19l</t>
-  </si>
-  <si>
     <t>19k</t>
   </si>
   <si>
@@ -6613,6 +6145,15 @@
   </si>
   <si>
     <t>2.0.2</t>
+  </si>
+  <si>
+    <t>Harvest Level</t>
+  </si>
+  <si>
+    <t>MaxUses</t>
+  </si>
+  <si>
+    <t>DmgVsEntity</t>
   </si>
 </sst>
 </file>
@@ -6717,7 +6258,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6792,6 +6333,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14896,16 +14438,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B115" s="16" t="s">
-        <v>1882</v>
+        <v>1856</v>
       </c>
       <c r="C115" s="16" t="s">
-        <v>1881</v>
+        <v>1855</v>
       </c>
       <c r="D115" s="16" t="s">
-        <v>1880</v>
+        <v>1854</v>
       </c>
       <c r="E115" s="16" t="s">
-        <v>1879</v>
+        <v>1853</v>
       </c>
       <c r="F115" s="1" t="str">
         <f>IF($N115, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
@@ -15607,10 +15149,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15622,62 +15164,69 @@
     <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.5703125" customWidth="1"/>
     <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" customWidth="1"/>
+    <col min="11" max="12" width="25.28515625" customWidth="1"/>
     <col min="13" max="13" width="15.7109375" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="str">
         <f>[1]Enums!$A$1</f>
         <v>Version</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>1969</v>
+        <v>1943</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>1970</v>
+        <v>1944</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>1971</v>
+        <v>1945</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>1972</v>
+        <v>1946</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>1973</v>
+        <v>1947</v>
       </c>
       <c r="G1" s="32" t="s">
-        <v>1974</v>
+        <v>1948</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>1978</v>
+        <v>1952</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>1977</v>
+        <v>1951</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>1975</v>
-      </c>
-      <c r="K1" s="36" t="s">
-        <v>1941</v>
-      </c>
-      <c r="L1" s="36" t="s">
-        <v>1964</v>
+        <v>1949</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>2033</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>2034</v>
       </c>
       <c r="M1" s="28" t="s">
-        <v>1979</v>
-      </c>
-      <c r="N1" s="28" t="s">
-        <v>2184</v>
-      </c>
-      <c r="O1" s="28" t="s">
-        <v>2185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1953</v>
+      </c>
+      <c r="N1" s="36" t="s">
+        <v>2035</v>
+      </c>
+      <c r="O1" s="36" t="s">
+        <v>1938</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>2028</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
@@ -15686,19 +15235,19 @@
         <v>1835</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>2019</v>
+        <v>1967</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>2059</v>
+        <v>1981</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>2099</v>
+        <v>1995</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>2139</v>
+        <v>2009</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>2179</v>
+        <v>2023</v>
       </c>
       <c r="H2" s="43" t="str">
         <f>'Molded Items'!$C$151</f>
@@ -15712,11 +15261,29 @@
         <f>[1]Enums!$A$130&amp;" "&amp;VLOOKUP(I2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Steel</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K2" s="45">
+        <v>3</v>
+      </c>
+      <c r="L2" s="45">
+        <v>2048</v>
+      </c>
+      <c r="M2" s="44">
+        <v>8</v>
+      </c>
+      <c r="N2" s="44">
+        <v>3</v>
+      </c>
+      <c r="O2" s="44">
+        <v>10</v>
+      </c>
+      <c r="P2" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="Q2" s="44">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
@@ -15725,19 +15292,19 @@
         <v>1836</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>2018</v>
+        <v>1966</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>2058</v>
+        <v>1980</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>2098</v>
+        <v>1994</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>2138</v>
+        <v>2008</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>2178</v>
+        <v>2022</v>
       </c>
       <c r="H3" s="43" t="str">
         <f>'Molded Items'!$C$151</f>
@@ -15751,11 +15318,29 @@
         <f>[1]Enums!$A$130&amp;" "&amp;VLOOKUP(I3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Stainless Steel</v>
       </c>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="44"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K3" s="45">
+        <v>3</v>
+      </c>
+      <c r="L3" s="45">
+        <v>2048</v>
+      </c>
+      <c r="M3" s="44">
+        <v>8</v>
+      </c>
+      <c r="N3" s="46">
+        <v>3</v>
+      </c>
+      <c r="O3" s="46">
+        <v>10</v>
+      </c>
+      <c r="P3" s="46">
+        <v>2.5</v>
+      </c>
+      <c r="Q3" s="46">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
@@ -15764,19 +15349,19 @@
         <v>1837</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>2017</v>
+        <v>1965</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>2057</v>
+        <v>1979</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>2097</v>
+        <v>1993</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>2137</v>
+        <v>2007</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>2177</v>
+        <v>2021</v>
       </c>
       <c r="H4" s="43" t="str">
         <f>'Molded Items'!$C$151</f>
@@ -15790,11 +15375,29 @@
         <f>[1]Enums!$A$130&amp;" "&amp;VLOOKUP(I4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Brass</v>
       </c>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="44"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K4" s="45">
+        <v>3</v>
+      </c>
+      <c r="L4" s="45">
+        <v>2048</v>
+      </c>
+      <c r="M4" s="44">
+        <v>8</v>
+      </c>
+      <c r="N4" s="44">
+        <v>3</v>
+      </c>
+      <c r="O4" s="44">
+        <v>10</v>
+      </c>
+      <c r="P4" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="Q4" s="44">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
@@ -15803,19 +15406,19 @@
         <v>1838</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>2016</v>
+        <v>1964</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>2056</v>
+        <v>1978</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>2096</v>
+        <v>1992</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>2136</v>
+        <v>2006</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>2176</v>
+        <v>2020</v>
       </c>
       <c r="H5" s="43" t="str">
         <f>'Molded Items'!$C$151</f>
@@ -15829,11 +15432,29 @@
         <f>[1]Enums!$A$130&amp;" "&amp;VLOOKUP(I5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Bronze</v>
       </c>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="44"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K5" s="45">
+        <v>3</v>
+      </c>
+      <c r="L5" s="45">
+        <v>2048</v>
+      </c>
+      <c r="M5" s="44">
+        <v>8</v>
+      </c>
+      <c r="N5" s="46">
+        <v>3</v>
+      </c>
+      <c r="O5" s="46">
+        <v>10</v>
+      </c>
+      <c r="P5" s="46">
+        <v>2.5</v>
+      </c>
+      <c r="Q5" s="46">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
@@ -15842,19 +15463,19 @@
         <v>1839</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>2015</v>
+        <v>1963</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>2055</v>
+        <v>1977</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>2095</v>
+        <v>1991</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>2135</v>
+        <v>2005</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>2175</v>
+        <v>2019</v>
       </c>
       <c r="H6" s="43" t="str">
         <f>'Molded Items'!$C$151</f>
@@ -15868,11 +15489,29 @@
         <f>[1]Enums!$A$130&amp;" "&amp;VLOOKUP(I6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Tungsten Carbide</v>
       </c>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K6" s="45">
+        <v>3</v>
+      </c>
+      <c r="L6" s="45">
+        <v>2048</v>
+      </c>
+      <c r="M6" s="44">
+        <v>8</v>
+      </c>
+      <c r="N6" s="46">
+        <v>3</v>
+      </c>
+      <c r="O6" s="44">
+        <v>10</v>
+      </c>
+      <c r="P6" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="Q6" s="44">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
@@ -15881,19 +15520,19 @@
         <v>1840</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>2014</v>
+        <v>1962</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>2054</v>
+        <v>1976</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>2094</v>
+        <v>1990</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>2134</v>
+        <v>2004</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>2174</v>
+        <v>2018</v>
       </c>
       <c r="H7" s="43" t="str">
         <f>'Molded Items'!$C$151</f>
@@ -15907,11 +15546,29 @@
         <f>[1]Enums!$A$130&amp;" "&amp;VLOOKUP(I7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Nichrome</v>
       </c>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="44"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K7" s="45">
+        <v>3</v>
+      </c>
+      <c r="L7" s="45">
+        <v>2048</v>
+      </c>
+      <c r="M7" s="44">
+        <v>8</v>
+      </c>
+      <c r="N7" s="46">
+        <v>3</v>
+      </c>
+      <c r="O7" s="46">
+        <v>10</v>
+      </c>
+      <c r="P7" s="46">
+        <v>2.5</v>
+      </c>
+      <c r="Q7" s="46">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
@@ -15920,19 +15577,19 @@
         <v>1841</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>2013</v>
+        <v>1961</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>2053</v>
+        <v>1975</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>2093</v>
+        <v>1989</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>2133</v>
+        <v>2003</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>2173</v>
+        <v>2017</v>
       </c>
       <c r="H8" s="43" t="str">
         <f>'Molded Items'!$C$151</f>
@@ -15946,11 +15603,29 @@
         <f>[1]Enums!$A$130&amp;" "&amp;VLOOKUP(I8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Antimony-Lead</v>
       </c>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="44"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K8" s="45">
+        <v>3</v>
+      </c>
+      <c r="L8" s="45">
+        <v>2048</v>
+      </c>
+      <c r="M8" s="44">
+        <v>8</v>
+      </c>
+      <c r="N8" s="46">
+        <v>3</v>
+      </c>
+      <c r="O8" s="44">
+        <v>10</v>
+      </c>
+      <c r="P8" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="Q8" s="44">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
@@ -15959,19 +15634,19 @@
         <v>1842</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>2012</v>
+        <v>1960</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>2052</v>
+        <v>1974</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>2092</v>
+        <v>1988</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>2132</v>
+        <v>2002</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>2172</v>
+        <v>2016</v>
       </c>
       <c r="H9" s="44" t="str">
         <f>'Molded Items'!$C$150</f>
@@ -15985,11 +15660,29 @@
         <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(I9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Steel</v>
       </c>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="44"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K9" s="45">
+        <v>3</v>
+      </c>
+      <c r="L9" s="45">
+        <v>2048</v>
+      </c>
+      <c r="M9" s="44">
+        <v>8</v>
+      </c>
+      <c r="N9" s="46">
+        <v>3</v>
+      </c>
+      <c r="O9" s="46">
+        <v>10</v>
+      </c>
+      <c r="P9" s="46">
+        <v>2.5</v>
+      </c>
+      <c r="Q9" s="46">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
@@ -15998,19 +15691,19 @@
         <v>1843</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>2011</v>
+        <v>1959</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>2051</v>
+        <v>1973</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>2091</v>
+        <v>1987</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>2131</v>
+        <v>2001</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>2171</v>
+        <v>2015</v>
       </c>
       <c r="H10" s="44" t="str">
         <f>'Molded Items'!$C$150</f>
@@ -16024,11 +15717,29 @@
         <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(I10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Stainless Steel</v>
       </c>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K10" s="45">
+        <v>3</v>
+      </c>
+      <c r="L10" s="45">
+        <v>2048</v>
+      </c>
+      <c r="M10" s="44">
+        <v>8</v>
+      </c>
+      <c r="N10" s="46">
+        <v>3</v>
+      </c>
+      <c r="O10" s="44">
+        <v>10</v>
+      </c>
+      <c r="P10" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="Q10" s="44">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
@@ -16037,19 +15748,19 @@
         <v>1844</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>2010</v>
+        <v>1958</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>2050</v>
+        <v>1972</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>2090</v>
+        <v>1986</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>2130</v>
+        <v>2000</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>2170</v>
+        <v>2014</v>
       </c>
       <c r="H11" s="44" t="str">
         <f>'Molded Items'!$C$150</f>
@@ -16063,11 +15774,29 @@
         <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(I11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Brass</v>
       </c>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="44"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K11" s="45">
+        <v>3</v>
+      </c>
+      <c r="L11" s="45">
+        <v>2048</v>
+      </c>
+      <c r="M11" s="44">
+        <v>8</v>
+      </c>
+      <c r="N11" s="46">
+        <v>3</v>
+      </c>
+      <c r="O11" s="46">
+        <v>10</v>
+      </c>
+      <c r="P11" s="46">
+        <v>2.5</v>
+      </c>
+      <c r="Q11" s="46">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
@@ -16076,19 +15805,19 @@
         <v>1845</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>2009</v>
+        <v>1957</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>2049</v>
+        <v>1971</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>2089</v>
+        <v>1985</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>2129</v>
+        <v>1999</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>2169</v>
+        <v>2013</v>
       </c>
       <c r="H12" s="44" t="str">
         <f>'Molded Items'!$C$150</f>
@@ -16102,11 +15831,29 @@
         <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(I12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Bronze</v>
       </c>
-      <c r="K12" s="44"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K12" s="45">
+        <v>3</v>
+      </c>
+      <c r="L12" s="45">
+        <v>2048</v>
+      </c>
+      <c r="M12" s="44">
+        <v>8</v>
+      </c>
+      <c r="N12" s="46">
+        <v>3</v>
+      </c>
+      <c r="O12" s="44">
+        <v>10</v>
+      </c>
+      <c r="P12" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="Q12" s="44">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
@@ -16115,19 +15862,19 @@
         <v>1846</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>2008</v>
+        <v>1956</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>2048</v>
+        <v>1970</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>2088</v>
+        <v>1984</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>2128</v>
+        <v>1998</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>2168</v>
+        <v>2012</v>
       </c>
       <c r="H13" s="44" t="str">
         <f>'Molded Items'!$C$150</f>
@@ -16141,11 +15888,29 @@
         <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(I13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Tungsten Carbide</v>
       </c>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="44"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K13" s="45">
+        <v>3</v>
+      </c>
+      <c r="L13" s="45">
+        <v>2048</v>
+      </c>
+      <c r="M13" s="44">
+        <v>8</v>
+      </c>
+      <c r="N13" s="46">
+        <v>3</v>
+      </c>
+      <c r="O13" s="46">
+        <v>10</v>
+      </c>
+      <c r="P13" s="46">
+        <v>2.5</v>
+      </c>
+      <c r="Q13" s="46">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
@@ -16154,19 +15919,19 @@
         <v>1847</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>2007</v>
+        <v>1955</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>2047</v>
+        <v>1969</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>2087</v>
+        <v>1983</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>2127</v>
+        <v>1997</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>2167</v>
+        <v>2011</v>
       </c>
       <c r="H14" s="44" t="str">
         <f>'Molded Items'!$C$150</f>
@@ -16180,11 +15945,29 @@
         <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(I14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Nichrome</v>
       </c>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K14" s="45">
+        <v>3</v>
+      </c>
+      <c r="L14" s="45">
+        <v>2048</v>
+      </c>
+      <c r="M14" s="44">
+        <v>8</v>
+      </c>
+      <c r="N14" s="46">
+        <v>3</v>
+      </c>
+      <c r="O14" s="44">
+        <v>10</v>
+      </c>
+      <c r="P14" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="Q14" s="44">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
@@ -16193,19 +15976,19 @@
         <v>1848</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>2006</v>
+        <v>1954</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>2046</v>
+        <v>1968</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>2086</v>
+        <v>1982</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>2126</v>
+        <v>1996</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>2166</v>
+        <v>2010</v>
       </c>
       <c r="H15" s="44" t="str">
         <f>'Molded Items'!$C$150</f>
@@ -16219,702 +16002,304 @@
         <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(I15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Antimony-Lead</v>
       </c>
-      <c r="K15" s="44"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="44"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K15" s="45">
+        <v>3</v>
+      </c>
+      <c r="L15" s="45">
+        <v>2048</v>
+      </c>
+      <c r="M15" s="44">
+        <v>8</v>
+      </c>
+      <c r="N15" s="46">
+        <v>3</v>
+      </c>
+      <c r="O15" s="46">
+        <v>10</v>
+      </c>
+      <c r="P15" s="46">
+        <v>2.5</v>
+      </c>
+      <c r="Q15" s="46">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="23"/>
-      <c r="B16" s="16" t="s">
-        <v>1849</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>2005</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>2045</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>2085</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>2125</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>2165</v>
-      </c>
       <c r="H16" s="44"/>
       <c r="I16" s="44"/>
       <c r="J16" s="44"/>
       <c r="K16" s="44"/>
       <c r="L16" s="44"/>
       <c r="M16" s="44"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16" s="44"/>
+      <c r="O16" s="44"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="23"/>
-      <c r="B17" s="16" t="s">
-        <v>1850</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>2004</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>2044</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>2084</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>2124</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>2164</v>
-      </c>
       <c r="H17" s="44"/>
       <c r="I17" s="44"/>
       <c r="J17" s="44"/>
       <c r="K17" s="44"/>
-      <c r="L17" s="43"/>
+      <c r="L17" s="44"/>
       <c r="M17" s="44"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17" s="44"/>
+      <c r="O17" s="43"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="23"/>
-      <c r="B18" s="16" t="s">
-        <v>1851</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>2003</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>2043</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>2083</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>2123</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>2163</v>
-      </c>
       <c r="H18" s="43"/>
       <c r="I18" s="44"/>
       <c r="J18" s="44"/>
       <c r="K18" s="44"/>
       <c r="L18" s="44"/>
       <c r="M18" s="44"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18" s="44"/>
+      <c r="O18" s="44"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="23"/>
-      <c r="B19" s="16" t="s">
-        <v>1852</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>2002</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>2042</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>2082</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>2122</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>2162</v>
-      </c>
       <c r="H19" s="43"/>
       <c r="I19" s="44"/>
       <c r="J19" s="44"/>
       <c r="K19" s="44"/>
       <c r="L19" s="44"/>
       <c r="M19" s="44"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19" s="44"/>
+      <c r="O19" s="44"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="23"/>
-      <c r="B20" s="16" t="s">
-        <v>1853</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>2001</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>2041</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>2081</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>2121</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>2161</v>
-      </c>
       <c r="H20" s="43"/>
       <c r="I20" s="44"/>
       <c r="J20" s="44"/>
       <c r="K20" s="44"/>
       <c r="L20" s="44"/>
       <c r="M20" s="44"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20" s="44"/>
+      <c r="O20" s="44"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="23"/>
-      <c r="B21" s="16" t="s">
-        <v>1854</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>2000</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>2040</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>2080</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>2120</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>2160</v>
-      </c>
       <c r="H21" s="43"/>
       <c r="I21" s="44"/>
       <c r="J21" s="44"/>
       <c r="K21" s="44"/>
       <c r="L21" s="44"/>
       <c r="M21" s="44"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21" s="44"/>
+      <c r="O21" s="44"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="23"/>
-      <c r="B22" s="16" t="s">
-        <v>1855</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>1999</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>2039</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>2079</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>2119</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>2159</v>
-      </c>
       <c r="I22" s="44"/>
       <c r="J22" s="44"/>
       <c r="K22" s="44"/>
       <c r="L22" s="44"/>
       <c r="M22" s="44"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="23"/>
-      <c r="B23" s="16" t="s">
-        <v>1856</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>1998</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>2038</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>2078</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>2118</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>2158</v>
-      </c>
       <c r="I23" s="44"/>
       <c r="J23" s="44"/>
       <c r="K23" s="44"/>
       <c r="L23" s="44"/>
       <c r="M23" s="44"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23" s="44"/>
+      <c r="O23" s="44"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="23"/>
-      <c r="B24" s="16" t="s">
-        <v>1857</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>1997</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>2037</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>2077</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>2117</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>2157</v>
-      </c>
       <c r="I24" s="44"/>
       <c r="J24" s="44"/>
       <c r="K24" s="44"/>
       <c r="L24" s="44"/>
       <c r="M24" s="44"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="23"/>
-      <c r="B25" s="16" t="s">
-        <v>1858</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>1996</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>2036</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>2076</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>2116</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>2156</v>
-      </c>
       <c r="I25" s="44"/>
       <c r="J25" s="44"/>
       <c r="K25" s="44"/>
       <c r="L25" s="44"/>
       <c r="M25" s="44"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="23"/>
-      <c r="B26" s="16" t="s">
-        <v>1859</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>1995</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>2035</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>2075</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>2115</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>2155</v>
-      </c>
       <c r="I26" s="44"/>
       <c r="J26" s="44"/>
       <c r="K26" s="44"/>
       <c r="L26" s="44"/>
       <c r="M26" s="44"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="23"/>
-      <c r="B27" s="16" t="s">
-        <v>1860</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>1994</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>2034</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>2074</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>2114</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>2154</v>
-      </c>
       <c r="I27" s="44"/>
       <c r="J27" s="44"/>
       <c r="K27" s="44"/>
       <c r="L27" s="44"/>
       <c r="M27" s="44"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="23"/>
-      <c r="B28" s="16" t="s">
-        <v>1861</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>1993</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>2033</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>2073</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>2113</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>2153</v>
-      </c>
       <c r="I28" s="44"/>
       <c r="J28" s="44"/>
       <c r="K28" s="44"/>
       <c r="L28" s="44"/>
       <c r="M28" s="44"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N28" s="44"/>
+      <c r="O28" s="44"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="23"/>
-      <c r="B29" s="16" t="s">
-        <v>1862</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>1992</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>2032</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>2072</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>2112</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>2152</v>
-      </c>
       <c r="I29" s="44"/>
       <c r="J29" s="44"/>
       <c r="K29" s="44"/>
       <c r="L29" s="44"/>
       <c r="M29" s="44"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N29" s="44"/>
+      <c r="O29" s="44"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="23"/>
-      <c r="B30" s="16" t="s">
-        <v>1863</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>1991</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>2031</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>2071</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>2111</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>2151</v>
-      </c>
       <c r="I30" s="44"/>
       <c r="J30" s="44"/>
       <c r="K30" s="44"/>
       <c r="L30" s="44"/>
       <c r="M30" s="44"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N30" s="44"/>
+      <c r="O30" s="44"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="23"/>
-      <c r="B31" s="16" t="s">
-        <v>1864</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>1990</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>2030</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>2070</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>2110</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>2150</v>
-      </c>
       <c r="H31" s="44"/>
       <c r="I31" s="44"/>
       <c r="J31" s="44"/>
       <c r="K31" s="44"/>
       <c r="L31" s="44"/>
       <c r="M31" s="44"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N31" s="44"/>
+      <c r="O31" s="44"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="23"/>
-      <c r="B32" s="16" t="s">
-        <v>1865</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>1989</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>2029</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>2069</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>2109</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>2149</v>
-      </c>
       <c r="H32" s="44"/>
       <c r="I32" s="44"/>
       <c r="J32" s="44"/>
       <c r="K32" s="44"/>
       <c r="L32" s="44"/>
       <c r="M32" s="44"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N32" s="44"/>
+      <c r="O32" s="44"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="23"/>
-      <c r="B33" s="16" t="s">
-        <v>1866</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>1988</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>2028</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>2068</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>2108</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>2148</v>
-      </c>
       <c r="H33" s="44"/>
       <c r="I33" s="44"/>
       <c r="J33" s="44"/>
       <c r="K33" s="44"/>
       <c r="L33" s="44"/>
       <c r="M33" s="44"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N33" s="44"/>
+      <c r="O33" s="44"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="23"/>
-      <c r="B34" s="16" t="s">
-        <v>1867</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>1987</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>2027</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>2067</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>2107</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>2147</v>
-      </c>
       <c r="H34" s="44"/>
       <c r="I34" s="44"/>
       <c r="J34" s="44"/>
       <c r="K34" s="44"/>
       <c r="L34" s="44"/>
       <c r="M34" s="44"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N34" s="44"/>
+      <c r="O34" s="44"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="23"/>
-      <c r="B35" s="16" t="s">
-        <v>1868</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>1986</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>2026</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>2066</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>2106</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>2146</v>
-      </c>
       <c r="H35" s="44"/>
       <c r="I35" s="44"/>
       <c r="J35" s="44"/>
       <c r="K35" s="44"/>
       <c r="L35" s="44"/>
       <c r="M35" s="44"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N35" s="44"/>
+      <c r="O35" s="44"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="23"/>
-      <c r="B36" s="16" t="s">
-        <v>1869</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>1985</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>2025</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>2065</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>2105</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>2145</v>
-      </c>
       <c r="H36" s="44"/>
       <c r="I36" s="44"/>
       <c r="J36" s="44"/>
       <c r="K36" s="44"/>
       <c r="L36" s="44"/>
       <c r="M36" s="44"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N36" s="44"/>
+      <c r="O36" s="44"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="23"/>
-      <c r="B37" s="16" t="s">
-        <v>1870</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>1984</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>2024</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>2064</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>2104</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>2144</v>
-      </c>
       <c r="H37" s="44"/>
       <c r="I37" s="44"/>
       <c r="J37" s="44"/>
       <c r="K37" s="44"/>
       <c r="L37" s="44"/>
       <c r="M37" s="44"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N37" s="44"/>
+      <c r="O37" s="44"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="23"/>
-      <c r="B38" s="16" t="s">
-        <v>1871</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>1983</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>2023</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>2063</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>2103</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>2143</v>
-      </c>
       <c r="H38" s="44"/>
       <c r="I38" s="44"/>
       <c r="J38" s="44"/>
       <c r="K38" s="44"/>
       <c r="L38" s="44"/>
       <c r="M38" s="44"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N38" s="44"/>
+      <c r="O38" s="44"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="23"/>
-      <c r="B39" s="16" t="s">
-        <v>1872</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>1982</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>2022</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>2062</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>2102</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>2142</v>
-      </c>
       <c r="H39" s="44"/>
       <c r="I39" s="44"/>
       <c r="J39" s="44"/>
       <c r="K39" s="44"/>
       <c r="L39" s="44"/>
       <c r="M39" s="44"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N39" s="44"/>
+      <c r="O39" s="44"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="23"/>
-      <c r="B40" s="16" t="s">
-        <v>1873</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>1981</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>2021</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>2061</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>2101</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>2141</v>
-      </c>
       <c r="H40" s="44"/>
       <c r="I40" s="44"/>
       <c r="J40" s="44"/>
       <c r="K40" s="44"/>
       <c r="L40" s="44"/>
       <c r="M40" s="44"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N40" s="44"/>
+      <c r="O40" s="44"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="23"/>
-      <c r="B41" s="16" t="s">
-        <v>1874</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>1980</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>2020</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>2060</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>2100</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>2140</v>
-      </c>
       <c r="H41" s="44"/>
       <c r="I41" s="44"/>
       <c r="J41" s="44"/>
       <c r="K41" s="44"/>
       <c r="L41" s="44"/>
       <c r="M41" s="44"/>
+      <c r="N41" s="44"/>
+      <c r="O41" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18522,7 +17907,7 @@
         <v>595</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>1894</v>
+        <v>1868</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>566</v>
@@ -23029,10 +22414,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B115" s="40" t="s">
-        <v>1884</v>
+        <v>1858</v>
       </c>
       <c r="C115" s="40" t="s">
-        <v>1885</v>
+        <v>1859</v>
       </c>
       <c r="D115" s="1" t="str">
         <f t="shared" si="3"/>
@@ -27614,16 +26999,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B115" s="40" t="s">
-        <v>1886</v>
+        <v>1860</v>
       </c>
       <c r="C115" s="40" t="s">
-        <v>1887</v>
+        <v>1861</v>
       </c>
       <c r="D115" s="40" t="s">
-        <v>1888</v>
+        <v>1862</v>
       </c>
       <c r="E115" s="40" t="s">
-        <v>1889</v>
+        <v>1863</v>
       </c>
       <c r="F115" s="1" t="str">
         <f t="shared" si="3"/>
@@ -31515,10 +30900,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B115" s="40" t="s">
-        <v>1890</v>
+        <v>1864</v>
       </c>
       <c r="C115" s="40" t="s">
-        <v>1891</v>
+        <v>1865</v>
       </c>
       <c r="D115" s="1" t="str">
         <f t="shared" si="3"/>
@@ -35410,10 +34795,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B115" s="40" t="s">
-        <v>1892</v>
+        <v>1866</v>
       </c>
       <c r="C115" s="40" t="s">
-        <v>1893</v>
+        <v>1867</v>
       </c>
       <c r="D115" s="1" t="str">
         <f t="shared" si="3"/>
@@ -36751,7 +36136,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>1878</v>
+        <v>1852</v>
       </c>
       <c r="C27" s="10" t="str">
         <f t="shared" si="0"/>
@@ -36775,7 +36160,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1916</v>
+        <v>1890</v>
       </c>
       <c r="C28" s="10" t="str">
         <f t="shared" si="0"/>
@@ -36799,7 +36184,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>2180</v>
+        <v>2024</v>
       </c>
       <c r="C29" s="10" t="str">
         <f t="shared" si="0"/>
@@ -37056,7 +36441,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>1940</v>
+        <v>1914</v>
       </c>
       <c r="K4" s="24">
         <v>0.25</v>
@@ -37083,7 +36468,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1920</v>
+        <v>1894</v>
       </c>
       <c r="C5" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D5, Molds!C:E, 3, FALSE)&amp;" ("&amp;F5&amp;")"</f>
@@ -37098,7 +36483,7 @@
         <v>Bag (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>1921</v>
+        <v>1895</v>
       </c>
       <c r="G5" s="24">
         <v>12</v>
@@ -37110,7 +36495,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>1922</v>
+        <v>1896</v>
       </c>
       <c r="K5" s="24">
         <v>0.35</v>
@@ -37158,7 +36543,7 @@
         <v>Bag (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>1875</v>
+        <v>1849</v>
       </c>
       <c r="G6" s="24">
         <v>4</v>
@@ -37205,7 +36590,7 @@
         <v>Bag (PolyUrethane Pellets)</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>1876</v>
+        <v>1850</v>
       </c>
       <c r="G7" s="24">
         <v>4</v>
@@ -37249,7 +36634,7 @@
         <v>Bag (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>1877</v>
+        <v>1851</v>
       </c>
       <c r="G8" s="24">
         <v>4</v>
@@ -37293,7 +36678,7 @@
         <v>Bag (PolyIsoPrene Pellets)</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>1897</v>
+        <v>1871</v>
       </c>
       <c r="G9" s="24">
         <v>16</v>
@@ -37333,7 +36718,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>1899</v>
+        <v>1873</v>
       </c>
       <c r="C10" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D10, Molds!C:E, 3, FALSE)&amp;" ("&amp;F10&amp;")"</f>
@@ -37348,7 +36733,7 @@
         <v>Bag (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>1895</v>
+        <v>1869</v>
       </c>
       <c r="G10" s="24">
         <v>16</v>
@@ -37360,7 +36745,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>1925</v>
+        <v>1899</v>
       </c>
       <c r="K10" s="24">
         <v>0.3</v>
@@ -37391,7 +36776,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1923</v>
+        <v>1897</v>
       </c>
       <c r="C11" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D11, Molds!C:E, 3, FALSE)&amp;" ("&amp;F11&amp;")"</f>
@@ -37406,7 +36791,7 @@
         <v>Bag (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>1919</v>
+        <v>1893</v>
       </c>
       <c r="G11" s="24">
         <v>16</v>
@@ -37418,7 +36803,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>1924</v>
+        <v>1898</v>
       </c>
       <c r="K11" s="24">
         <v>0.4</v>
@@ -37455,7 +36840,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>1900</v>
+        <v>1874</v>
       </c>
       <c r="C12" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D12, Molds!C:E, 3, FALSE)&amp;" ("&amp;F12&amp;")"</f>
@@ -37470,7 +36855,7 @@
         <v>Bag (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>1896</v>
+        <v>1870</v>
       </c>
       <c r="G12" s="24">
         <v>16</v>
@@ -37482,7 +36867,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="24" t="s">
-        <v>1925</v>
+        <v>1899</v>
       </c>
       <c r="K12" s="24">
         <v>0.5</v>
@@ -37528,7 +36913,7 @@
         <v>Bag (PolyIsoPrene Pellets)</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>1897</v>
+        <v>1871</v>
       </c>
       <c r="G13" s="24">
         <v>12</v>
@@ -37564,7 +36949,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>1901</v>
+        <v>1875</v>
       </c>
       <c r="C14" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D14, Molds!C:E, 3, FALSE)&amp;" ("&amp;F14&amp;")"</f>
@@ -37579,7 +36964,7 @@
         <v>Bag (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>1895</v>
+        <v>1869</v>
       </c>
       <c r="G14" s="24">
         <v>12</v>
@@ -37591,7 +36976,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>1926</v>
+        <v>1900</v>
       </c>
       <c r="K14" s="24">
         <v>0.01</v>
@@ -37618,7 +37003,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1918</v>
+        <v>1892</v>
       </c>
       <c r="C15" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D15, Molds!C:E, 3, FALSE)&amp;" ("&amp;F15&amp;")"</f>
@@ -37633,7 +37018,7 @@
         <v>Bag (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>1919</v>
+        <v>1893</v>
       </c>
       <c r="G15" s="24">
         <v>12</v>
@@ -37645,7 +37030,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>1935</v>
+        <v>1909</v>
       </c>
       <c r="K15" s="24">
         <v>5.0000000000000001E-3</v>
@@ -37676,7 +37061,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>1902</v>
+        <v>1876</v>
       </c>
       <c r="C16" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D16, Molds!C:E, 3, FALSE)&amp;" ("&amp;F16&amp;")"</f>
@@ -37691,7 +37076,7 @@
         <v>Bag (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>1896</v>
+        <v>1870</v>
       </c>
       <c r="G16" s="24">
         <v>12</v>
@@ -37703,7 +37088,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="24" t="s">
-        <v>1926</v>
+        <v>1900</v>
       </c>
       <c r="K16" s="24">
         <v>1E-3</v>
@@ -37745,7 +37130,7 @@
         <v>Bag (PolyIsoPrene Pellets)</v>
       </c>
       <c r="F17" s="42" t="s">
-        <v>1936</v>
+        <v>1910</v>
       </c>
       <c r="G17" s="24">
         <v>4</v>
@@ -37777,7 +37162,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="C18" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D18, Molds!C:E, 3, FALSE)&amp;" ("&amp;F18&amp;")"</f>
@@ -37792,7 +37177,7 @@
         <v>Bag (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="F18" s="42" t="s">
-        <v>1937</v>
+        <v>1911</v>
       </c>
       <c r="G18" s="24">
         <v>4</v>
@@ -37804,7 +37189,7 @@
         <v>64</v>
       </c>
       <c r="J18" s="24" t="s">
-        <v>1931</v>
+        <v>1905</v>
       </c>
       <c r="K18" s="24" t="str">
         <f>Pellets!$F$19</f>
@@ -37827,7 +37212,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1933</v>
+        <v>1907</v>
       </c>
       <c r="C19" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D19, Molds!C:E, 3, FALSE)&amp;" ("&amp;F19&amp;")"</f>
@@ -37842,7 +37227,7 @@
         <v>Bag (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="F19" s="42" t="s">
-        <v>1938</v>
+        <v>1912</v>
       </c>
       <c r="G19" s="24">
         <v>4</v>
@@ -37854,7 +37239,7 @@
         <v>64</v>
       </c>
       <c r="J19" s="24" t="s">
-        <v>1930</v>
+        <v>1904</v>
       </c>
       <c r="K19" s="24" t="str">
         <f>Pellets!$F$27</f>
@@ -37883,7 +37268,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1934</v>
+        <v>1908</v>
       </c>
       <c r="C20" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D20, Molds!C:E, 3, FALSE)&amp;" ("&amp;F20&amp;")"</f>
@@ -37898,7 +37283,7 @@
         <v>Bag (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="F20" s="42" t="s">
-        <v>1939</v>
+        <v>1913</v>
       </c>
       <c r="G20" s="24">
         <v>4</v>
@@ -37910,7 +37295,7 @@
         <v>64</v>
       </c>
       <c r="J20" s="24" t="s">
-        <v>1931</v>
+        <v>1905</v>
       </c>
       <c r="K20" s="22" t="str">
         <f>Pellets!$F$16</f>
@@ -37961,7 +37346,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="24" t="s">
-        <v>1898</v>
+        <v>1872</v>
       </c>
       <c r="K21" s="24">
         <v>20</v>
@@ -37985,7 +37370,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>1903</v>
+        <v>1877</v>
       </c>
       <c r="C22" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D22, Molds!C:E, 3, FALSE)&amp;" ("&amp;F22&amp;")"</f>
@@ -38013,7 +37398,7 @@
         <v>1</v>
       </c>
       <c r="J22" s="24" t="s">
-        <v>1898</v>
+        <v>1872</v>
       </c>
       <c r="K22" s="24">
         <v>200</v>
@@ -38034,7 +37419,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>1904</v>
+        <v>1878</v>
       </c>
       <c r="C23" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D23, Molds!C:E, 3, FALSE)&amp;" ("&amp;F23&amp;")"</f>
@@ -38062,7 +37447,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="24" t="s">
-        <v>1898</v>
+        <v>1872</v>
       </c>
       <c r="K23" s="24">
         <v>2000</v>
@@ -38198,7 +37583,7 @@
         <v>Bag (PolyIsoPrene Pellets)</v>
       </c>
       <c r="F26" s="42" t="s">
-        <v>1936</v>
+        <v>1910</v>
       </c>
       <c r="G26" s="24">
         <v>16</v>
@@ -38224,7 +37609,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1929</v>
+        <v>1903</v>
       </c>
       <c r="C27" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D27, Molds!C:E, 3, FALSE)&amp;" ("&amp;F27&amp;")"</f>
@@ -38239,7 +37624,7 @@
         <v>Bag (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="F27" s="42" t="s">
-        <v>1937</v>
+        <v>1911</v>
       </c>
       <c r="G27" s="24">
         <v>16</v>
@@ -38251,7 +37636,7 @@
         <v>64</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>1931</v>
+        <v>1905</v>
       </c>
       <c r="K27" s="24" t="str">
         <f>Pellets!$F$19</f>
@@ -38273,7 +37658,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1928</v>
+        <v>1902</v>
       </c>
       <c r="C28" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D28, Molds!C:E, 3, FALSE)&amp;" ("&amp;F28&amp;")"</f>
@@ -38288,7 +37673,7 @@
         <v>Bag (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="F28" s="42" t="s">
-        <v>1938</v>
+        <v>1912</v>
       </c>
       <c r="G28" s="24">
         <v>16</v>
@@ -38300,7 +37685,7 @@
         <v>64</v>
       </c>
       <c r="J28" s="24" t="s">
-        <v>1930</v>
+        <v>1904</v>
       </c>
       <c r="K28" s="24" t="str">
         <f>Pellets!$F$27</f>
@@ -38328,7 +37713,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1927</v>
+        <v>1901</v>
       </c>
       <c r="C29" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D29, Molds!C:E, 3, FALSE)&amp;" ("&amp;F29&amp;")"</f>
@@ -38343,7 +37728,7 @@
         <v>Bag (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="F29" s="42" t="s">
-        <v>1939</v>
+        <v>1913</v>
       </c>
       <c r="G29" s="24">
         <v>16</v>
@@ -38355,7 +37740,7 @@
         <v>64</v>
       </c>
       <c r="J29" s="24" t="s">
-        <v>1931</v>
+        <v>1905</v>
       </c>
       <c r="K29" s="22" t="str">
         <f>Pellets!$F$16</f>
@@ -42403,7 +41788,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B148" s="23" t="s">
-        <v>1883</v>
+        <v>1857</v>
       </c>
       <c r="C148" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D148, Molds!C:E, 3, FALSE)&amp;" ("&amp;F148&amp;")"</f>
@@ -42437,7 +41822,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1917</v>
+        <v>1891</v>
       </c>
       <c r="C149" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D149, Molds!C:E, 3, FALSE)&amp;" ("&amp;F149&amp;")"</f>
@@ -42471,7 +41856,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>2181</v>
+        <v>2025</v>
       </c>
       <c r="C150" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D150, Molds!C:E, 3, FALSE)&amp;" ("&amp;F150&amp;")"</f>
@@ -42505,7 +41890,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>2182</v>
+        <v>2026</v>
       </c>
       <c r="C151" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D151, Molds!C:E, 3, FALSE)&amp;" ("&amp;F151&amp;")"</f>
@@ -42563,8 +41948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -42588,52 +41973,52 @@
         <v>Version</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>1945</v>
+        <v>1919</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>1944</v>
+        <v>1918</v>
       </c>
       <c r="D1" s="32" t="s">
+        <v>1916</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>1917</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>1950</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>1936</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>1935</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>1934</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>1932</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>1933</v>
+      </c>
+      <c r="L1" s="36" t="s">
+        <v>1915</v>
+      </c>
+      <c r="M1" s="36" t="s">
+        <v>1938</v>
+      </c>
+      <c r="N1" s="30" t="s">
         <v>1942</v>
       </c>
-      <c r="E1" s="32" t="s">
-        <v>1943</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>1976</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>1962</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>1961</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>1960</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>1958</v>
-      </c>
-      <c r="K1" s="20" t="s">
-        <v>1959</v>
-      </c>
-      <c r="L1" s="36" t="s">
+      <c r="O1" s="30" t="s">
         <v>1941</v>
       </c>
-      <c r="M1" s="36" t="s">
-        <v>1964</v>
-      </c>
-      <c r="N1" s="30" t="s">
-        <v>1968</v>
-      </c>
-      <c r="O1" s="30" t="s">
-        <v>1967</v>
-      </c>
       <c r="P1" s="30" t="s">
-        <v>1965</v>
+        <v>1939</v>
       </c>
       <c r="Q1" s="30" t="s">
-        <v>1966</v>
+        <v>1940</v>
       </c>
       <c r="R1" s="28"/>
     </row>
@@ -42643,35 +42028,35 @@
         <v>1.1.0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1957</v>
+        <v>1931</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>1953</v>
+        <v>1927</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>1905</v>
+        <v>1879</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1946</v>
+        <v>1920</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>'Molded Items'!$C$100</f>
         <v>Fibers (Natural Rubber)</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>1909</v>
+        <v>1883</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>1963</v>
+        <v>1937</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>1912</v>
+        <v>1886</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>1910</v>
+        <v>1884</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>1911</v>
+        <v>1885</v>
       </c>
       <c r="L2">
         <v>20</v>
@@ -42694,38 +42079,38 @@
     </row>
     <row r="3" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>2186</v>
+        <v>2030</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1956</v>
+        <v>1930</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>1952</v>
+        <v>1926</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>1906</v>
+        <v>1880</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>1947</v>
+        <v>1921</v>
       </c>
       <c r="F3" s="2" t="str">
         <f>'Molded Items'!C131</f>
         <v>Fibers (PVC)</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>1913</v>
+        <v>1887</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>2183</v>
+        <v>2027</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>1912</v>
+        <v>1886</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>1910</v>
+        <v>1884</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>1911</v>
+        <v>1885</v>
       </c>
       <c r="L3">
         <v>20</v>
@@ -42748,38 +42133,38 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
-        <v>2187</v>
+        <v>2031</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1955</v>
+        <v>1929</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>1951</v>
+        <v>1925</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>1907</v>
+        <v>1881</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>1948</v>
+        <v>1922</v>
       </c>
       <c r="F4" s="2" t="str">
         <f>'Molded Items'!C148</f>
         <v>Fibers (Nylon 6)</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>1914</v>
+        <v>1888</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>2183</v>
+        <v>2027</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>1912</v>
+        <v>1886</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>1910</v>
+        <v>1884</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>1911</v>
+        <v>1885</v>
       </c>
       <c r="L4">
         <v>20</v>
@@ -42802,38 +42187,38 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>2188</v>
+        <v>2032</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1954</v>
+        <v>1928</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>1950</v>
+        <v>1924</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>1908</v>
+        <v>1882</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>1949</v>
+        <v>1923</v>
       </c>
       <c r="F5" t="str">
         <f>'Molded Items'!C116</f>
         <v>Fibers (kevlar)</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>1915</v>
+        <v>1889</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>2183</v>
+        <v>2027</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>1912</v>
+        <v>1886</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>1910</v>
+        <v>1884</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>1911</v>
+        <v>1885</v>
       </c>
       <c r="L5">
         <v>40</v>

</xml_diff>

<commit_message>
1.1.1 Texture and Recipe Update
</commit_message>
<xml_diff>
--- a/config/Polycraft Polymers.xlsx
+++ b/config/Polycraft Polymers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16500" yWindow="0" windowWidth="27240" windowHeight="14310" tabRatio="826" activeTab="7"/>
+    <workbookView xWindow="18360" yWindow="0" windowWidth="27240" windowHeight="14310" tabRatio="826"/>
   </bookViews>
   <sheets>
     <sheet name="Pellets" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,6 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -7347,108 +7346,113 @@
             <v>1.1.0</v>
           </cell>
         </row>
-        <row r="21">
-          <cell r="A21" t="str">
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>1.1.1</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
             <v>Bag</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23" t="str">
-            <v>Flask</v>
           </cell>
         </row>
         <row r="24">
           <cell r="A24" t="str">
+            <v>Flask</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25" t="str">
             <v>Sack</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26" t="str">
-            <v>Cartridge</v>
           </cell>
         </row>
         <row r="27">
           <cell r="A27" t="str">
+            <v>Cartridge</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
             <v>Powder Keg</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29" t="str">
-            <v>Canister</v>
           </cell>
         </row>
         <row r="30">
           <cell r="A30" t="str">
+            <v>Canister</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
             <v>Chemical Silo</v>
           </cell>
         </row>
-        <row r="32">
-          <cell r="A32" t="str">
+        <row r="33">
+          <cell r="A33" t="str">
             <v>Chemical Tank</v>
           </cell>
         </row>
-        <row r="69">
-          <cell r="B69" t="str">
+        <row r="70">
+          <cell r="B70" t="str">
             <v>Mold Type</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="B73" t="str">
-            <v>Mold</v>
           </cell>
         </row>
         <row r="74">
           <cell r="B74" t="str">
+            <v>Mold</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="B75" t="str">
             <v>Metal Die</v>
           </cell>
         </row>
-        <row r="92">
-          <cell r="A92" t="str">
+        <row r="93">
+          <cell r="A93" t="str">
             <v>Gripped</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="A95" t="str">
-            <v>Base Material</v>
           </cell>
         </row>
         <row r="96">
           <cell r="A96" t="str">
-            <v>Wooden</v>
+            <v>Base Material</v>
           </cell>
         </row>
         <row r="97">
           <cell r="A97" t="str">
-            <v>Stone</v>
+            <v>Wooden</v>
           </cell>
         </row>
         <row r="98">
           <cell r="A98" t="str">
-            <v>Iron</v>
+            <v>Stone</v>
           </cell>
         </row>
         <row r="99">
           <cell r="A99" t="str">
-            <v>Golden</v>
+            <v>Iron</v>
           </cell>
         </row>
         <row r="100">
           <cell r="A100" t="str">
-            <v>Diamond</v>
+            <v>Golden</v>
           </cell>
         </row>
         <row r="101">
           <cell r="A101" t="str">
+            <v>Diamond</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="A102" t="str">
             <v>Magic</v>
-          </cell>
-        </row>
-        <row r="130">
-          <cell r="A130" t="str">
-            <v>Composite</v>
           </cell>
         </row>
         <row r="131">
           <cell r="A131" t="str">
+            <v>Composite</v>
+          </cell>
+        </row>
+        <row r="132">
+          <cell r="A132" t="str">
             <v>Engineered</v>
           </cell>
         </row>
@@ -8411,7 +8415,7 @@
             <v>PolyM-Phenylene Isophthalamide</v>
           </cell>
           <cell r="C74" t="str">
-            <v>PMIA</v>
+            <v>nomex</v>
           </cell>
           <cell r="D74" t="b">
             <v>1</v>
@@ -9583,8 +9587,8 @@
   </sheetPr>
   <dimension ref="A1:N333"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9626,19 +9630,19 @@
         <v>Game ID XL</v>
       </c>
       <c r="F1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$21&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$22&amp;" ("&amp;J1&amp;")"</f>
         <v>Bag (Pellets)</v>
       </c>
       <c r="G1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$24&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$25&amp;" ("&amp;J1&amp;")"</f>
         <v>Sack (Pellets)</v>
       </c>
       <c r="H1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$27&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$28&amp;" ("&amp;J1&amp;")"</f>
         <v>Powder Keg (Pellets)</v>
       </c>
       <c r="I1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$30&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$31&amp;" ("&amp;J1&amp;")"</f>
         <v>Chemical Silo (Pellets)</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -9674,19 +9678,19 @@
         <v>448</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Flask (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="G2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Cartridge (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="H2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Canister (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Tank (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="J2" s="1" t="str">
@@ -9726,19 +9730,19 @@
         <v>444</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J3" s="1" t="str">
@@ -9775,19 +9779,19 @@
         <v>440</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Flask (Alkyd Resin)</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Cartridge (Alkyd Resin)</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Canister (Alkyd Resin)</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Tank (Alkyd Resin)</v>
       </c>
       <c r="J4" s="1" t="str">
@@ -9827,19 +9831,19 @@
         <v>436</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J5" s="1" t="str">
@@ -9879,19 +9883,19 @@
         <v>432</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J6" s="1" t="str">
@@ -9931,19 +9935,19 @@
         <v>428</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Carbon Fiber Pellets)</v>
       </c>
       <c r="G7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Carbon Fiber Pellets)</v>
       </c>
       <c r="H7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Carbon Fiber Pellets)</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Carbon Fiber Pellets)</v>
       </c>
       <c r="J7" s="1" t="str">
@@ -9980,19 +9984,19 @@
         <v>424</v>
       </c>
       <c r="F8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="G8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="J8" s="1" t="str">
@@ -10032,19 +10036,19 @@
         <v>420</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulosic Pellets)</v>
       </c>
       <c r="G9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulosic Pellets)</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulosic Pellets)</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulosic Pellets)</v>
       </c>
       <c r="J9" s="1" t="str">
@@ -10084,19 +10088,19 @@
         <v>416</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chitin Pellets)</v>
       </c>
       <c r="G10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chitin Pellets)</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chitin Pellets)</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chitin Pellets)</v>
       </c>
       <c r="J10" s="1" t="str">
@@ -10136,19 +10140,19 @@
         <v>412</v>
       </c>
       <c r="F11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J11" s="1" t="str">
@@ -10185,19 +10189,19 @@
         <v>408</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Flask (Epoxy Resin)</v>
       </c>
       <c r="G12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Cartridge (Epoxy Resin)</v>
       </c>
       <c r="H12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Canister (Epoxy Resin)</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Tank (Epoxy Resin)</v>
       </c>
       <c r="J12" s="1" t="str">
@@ -10234,19 +10238,19 @@
         <v>404</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethoxylates Pellets)</v>
       </c>
       <c r="G13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethoxylates Pellets)</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethoxylates Pellets)</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethoxylates Pellets)</v>
       </c>
       <c r="J13" s="1" t="str">
@@ -10286,19 +10290,19 @@
         <v>400</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="G14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="H14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="J14" s="1" t="str">
@@ -10338,19 +10342,19 @@
         <v>396</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="G15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="J15" s="1" t="str">
@@ -10390,19 +10394,19 @@
         <v>392</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="G16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="J16" s="1" t="str">
@@ -10442,19 +10446,19 @@
         <v>388</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="G17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="J17" s="1" t="str">
@@ -10494,19 +10498,19 @@
         <v>384</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J18" s="1" t="str">
@@ -10546,19 +10550,19 @@
         <v>380</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Isobutylene Rubber Pellets)</v>
       </c>
       <c r="G19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Isobutylene Rubber Pellets)</v>
       </c>
       <c r="H19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Isobutylene Rubber Pellets)</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Isobutylene Rubber Pellets)</v>
       </c>
       <c r="J19" s="1" t="str">
@@ -10595,19 +10599,19 @@
         <v>376</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Flask (Lignin)</v>
       </c>
       <c r="G20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Cartridge (Lignin)</v>
       </c>
       <c r="H20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Canister (Lignin)</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Tank (Lignin)</v>
       </c>
       <c r="J20" s="1" t="str">
@@ -10647,19 +10651,19 @@
         <v>372</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J21" s="1" t="str">
@@ -10699,19 +10703,19 @@
         <v>368</v>
       </c>
       <c r="F22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="G22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="H22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="J22" s="1" t="str">
@@ -10751,19 +10755,19 @@
         <v>364</v>
       </c>
       <c r="F23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="G23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="H23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="J23" s="1" t="str">
@@ -10803,19 +10807,19 @@
         <v>360</v>
       </c>
       <c r="F24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="G24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="H24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="J24" s="1" t="str">
@@ -10852,19 +10856,19 @@
         <v>356</v>
       </c>
       <c r="F25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Flask (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="G25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Cartridge (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="H25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Canister (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Tank (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="J25" s="1" t="str">
@@ -10904,19 +10908,19 @@
         <v>352</v>
       </c>
       <c r="F26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Metaldehyde Pellets)</v>
       </c>
       <c r="G26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Metaldehyde Pellets)</v>
       </c>
       <c r="H26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Metaldehyde Pellets)</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Metaldehyde Pellets)</v>
       </c>
       <c r="J26" s="1" t="str">
@@ -10956,19 +10960,19 @@
         <v>348</v>
       </c>
       <c r="F27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J27" s="1" t="str">
@@ -11008,19 +11012,19 @@
         <v>344</v>
       </c>
       <c r="F28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraformaldehyde Pellets)</v>
       </c>
       <c r="G28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraformaldehyde Pellets)</v>
       </c>
       <c r="H28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraformaldehyde Pellets)</v>
       </c>
       <c r="I28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraformaldehyde Pellets)</v>
       </c>
       <c r="J28" s="1" t="str">
@@ -11060,19 +11064,19 @@
         <v>340</v>
       </c>
       <c r="F29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraldehyde Pellets)</v>
       </c>
       <c r="G29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraldehyde Pellets)</v>
       </c>
       <c r="H29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraldehyde Pellets)</v>
       </c>
       <c r="I29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraldehyde Pellets)</v>
       </c>
       <c r="J29" s="1" t="str">
@@ -11109,19 +11113,19 @@
         <v>336</v>
       </c>
       <c r="F30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Flask (Phenolic Resin)</v>
       </c>
       <c r="G30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Cartridge (Phenolic Resin)</v>
       </c>
       <c r="H30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Canister (Phenolic Resin)</v>
       </c>
       <c r="I30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Tank (Phenolic Resin)</v>
       </c>
       <c r="J30" s="1" t="str">
@@ -11161,19 +11165,19 @@
         <v>332</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="G31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="H31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="I31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="J31" s="1" t="str">
@@ -11210,19 +11214,19 @@
         <v>328</v>
       </c>
       <c r="F32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly1-Butene Pellets)</v>
       </c>
       <c r="G32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly1-Butene Pellets)</v>
       </c>
       <c r="H32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly1-Butene Pellets)</v>
       </c>
       <c r="I32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly1-Butene Pellets)</v>
       </c>
       <c r="J32" s="1" t="str">
@@ -11259,19 +11263,19 @@
         <v>324</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2,6-Dimethyl-1,4-Phenylene Ether Pellets)</v>
       </c>
       <c r="G33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2,6-Dimethyl-1,4-Phenylene Ether Pellets)</v>
       </c>
       <c r="H33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2,6-Dimethyl-1,4-Phenylene Ether Pellets)</v>
       </c>
       <c r="I33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2,6-Dimethyl-1,4-Phenylene Ether Pellets)</v>
       </c>
       <c r="J33" s="1" t="str">
@@ -11308,19 +11312,19 @@
         <v>320</v>
       </c>
       <c r="F34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="G34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="H34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="I34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="J34" s="1" t="str">
@@ -11357,19 +11361,19 @@
         <v>316</v>
       </c>
       <c r="F35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="G35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="H35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="I35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="J35" s="1" t="str">
@@ -11406,19 +11410,19 @@
         <v>312</v>
       </c>
       <c r="F36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylic Ester Pellets)</v>
       </c>
       <c r="G36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylic Ester Pellets)</v>
       </c>
       <c r="H36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylic Ester Pellets)</v>
       </c>
       <c r="I36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylic Ester Pellets)</v>
       </c>
       <c r="J36" s="1" t="str">
@@ -11458,19 +11462,19 @@
         <v>308</v>
       </c>
       <c r="F37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="G37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="H37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="I37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="J37" s="1" t="str">
@@ -11510,19 +11514,19 @@
         <v>304</v>
       </c>
       <c r="F38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="G38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="H38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="I38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="J38" s="1" t="str">
@@ -11562,19 +11566,19 @@
         <v>300</v>
       </c>
       <c r="F39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="G39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="H39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="I39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="J39" s="1" t="str">
@@ -11614,19 +11618,19 @@
         <v>296</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="G40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="H40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="I40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="J40" s="1" t="str">
@@ -11666,19 +11670,19 @@
         <v>292</v>
       </c>
       <c r="F41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="G41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="H41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="I41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="J41" s="1" t="str">
@@ -11718,19 +11722,19 @@
         <v>288</v>
       </c>
       <c r="F42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCaprolactone Pellets)</v>
       </c>
       <c r="G42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCaprolactone Pellets)</v>
       </c>
       <c r="H42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCaprolactone Pellets)</v>
       </c>
       <c r="I42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCaprolactone Pellets)</v>
       </c>
       <c r="J42" s="1" t="str">
@@ -11770,19 +11774,19 @@
         <v>284</v>
       </c>
       <c r="F43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCarbonate Pellets)</v>
       </c>
       <c r="G43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCarbonate Pellets)</v>
       </c>
       <c r="H43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCarbonate Pellets)</v>
       </c>
       <c r="I43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCarbonate Pellets)</v>
       </c>
       <c r="J43" s="1" t="str">
@@ -11819,19 +11823,19 @@
         <v>280</v>
       </c>
       <c r="F44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChloroPrene Pellets)</v>
       </c>
       <c r="G44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChloroPrene Pellets)</v>
       </c>
       <c r="H44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChloroPrene Pellets)</v>
       </c>
       <c r="I44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChloroPrene Pellets)</v>
       </c>
       <c r="J44" s="1" t="str">
@@ -11868,19 +11872,19 @@
         <v>276</v>
       </c>
       <c r="F45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="G45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="H45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="I45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="J45" s="1" t="str">
@@ -11920,19 +11924,19 @@
         <v>272</v>
       </c>
       <c r="F46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="G46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="H46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="I46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="J46" s="1" t="str">
@@ -11972,19 +11976,19 @@
         <v>268</v>
       </c>
       <c r="F47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="G47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="H47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="I47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="J47" s="1" t="str">
@@ -12024,19 +12028,19 @@
         <v>264</v>
       </c>
       <c r="F48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEtherImide Pellets)</v>
       </c>
       <c r="G48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEtherImide Pellets)</v>
       </c>
       <c r="H48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEtherImide Pellets)</v>
       </c>
       <c r="I48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEtherImide Pellets)</v>
       </c>
       <c r="J48" s="1" t="str">
@@ -12073,19 +12077,19 @@
         <v>260</v>
       </c>
       <c r="F49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="G49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="H49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="I49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="J49" s="1" t="str">
@@ -12122,19 +12126,19 @@
         <v>256</v>
       </c>
       <c r="F50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="G50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="H50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="I50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="J50" s="1" t="str">
@@ -12174,19 +12178,19 @@
         <v>252</v>
       </c>
       <c r="F51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="G51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="H51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="I51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="J51" s="1" t="str">
@@ -12223,19 +12227,19 @@
         <v>248</v>
       </c>
       <c r="F52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J52" s="1" t="str">
@@ -12275,19 +12279,19 @@
         <v>244</v>
       </c>
       <c r="F53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="G53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="H53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="I53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="J53" s="1" t="str">
@@ -12327,19 +12331,19 @@
         <v>240</v>
       </c>
       <c r="F54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="G54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="H54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="I54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="J54" s="1" t="str">
@@ -12379,19 +12383,19 @@
         <v>236</v>
       </c>
       <c r="F55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="G55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="H55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="I55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="J55" s="1" t="str">
@@ -12431,19 +12435,19 @@
         <v>232</v>
       </c>
       <c r="F56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J56" s="1" t="str">
@@ -12483,19 +12487,19 @@
         <v>228</v>
       </c>
       <c r="F57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="G57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="H57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="I57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="J57" s="1" t="str">
@@ -12535,19 +12539,19 @@
         <v>224</v>
       </c>
       <c r="F58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="G58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="H58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="I58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="J58" s="1" t="str">
@@ -12587,19 +12591,19 @@
         <v>220</v>
       </c>
       <c r="F59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="G59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="H59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="I59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="J59" s="1" t="str">
@@ -12639,19 +12643,19 @@
         <v>216</v>
       </c>
       <c r="F60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="G60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="H60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="I60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="J60" s="1" t="str">
@@ -12691,19 +12695,19 @@
         <v>212</v>
       </c>
       <c r="F61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="G61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="H61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="I61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="J61" s="1" t="str">
@@ -12740,19 +12744,19 @@
         <v>208</v>
       </c>
       <c r="F62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="G62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="H62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="I62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="J62" s="1" t="str">
@@ -12792,19 +12796,19 @@
         <v>204</v>
       </c>
       <c r="F63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyImide Pellets)</v>
       </c>
       <c r="G63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyImide Pellets)</v>
       </c>
       <c r="H63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyImide Pellets)</v>
       </c>
       <c r="I63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyImide Pellets)</v>
       </c>
       <c r="J63" s="1" t="str">
@@ -12841,19 +12845,19 @@
         <v>200</v>
       </c>
       <c r="F64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="G64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="H64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="I64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="J64" s="1" t="str">
@@ -12890,19 +12894,19 @@
         <v>196</v>
       </c>
       <c r="F65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="G65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="H65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="I65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="J65" s="1" t="str">
@@ -12942,19 +12946,19 @@
         <v>192</v>
       </c>
       <c r="F66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButylene Pellets)</v>
       </c>
       <c r="G66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButylene Pellets)</v>
       </c>
       <c r="H66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButylene Pellets)</v>
       </c>
       <c r="I66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButylene Pellets)</v>
       </c>
       <c r="J66" s="1" t="str">
@@ -12994,19 +12998,19 @@
         <v>188</v>
       </c>
       <c r="F67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoPrene Pellets)</v>
       </c>
       <c r="G67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoPrene Pellets)</v>
       </c>
       <c r="H67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoPrene Pellets)</v>
       </c>
       <c r="I67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoPrene Pellets)</v>
       </c>
       <c r="J67" s="1" t="str">
@@ -13046,19 +13050,19 @@
         <v>184</v>
       </c>
       <c r="F68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic Acid Pellets)</v>
       </c>
       <c r="G68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic Acid Pellets)</v>
       </c>
       <c r="H68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic Acid Pellets)</v>
       </c>
       <c r="I68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic Acid Pellets)</v>
       </c>
       <c r="J68" s="1" t="str">
@@ -13095,19 +13099,19 @@
         <v>180</v>
       </c>
       <c r="F69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="G69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="H69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="I69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="J69" s="1" t="str">
@@ -13144,19 +13148,19 @@
         <v>176</v>
       </c>
       <c r="F70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="G70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="H70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="I70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="J70" s="1" t="str">
@@ -13193,19 +13197,19 @@
         <v>172</v>
       </c>
       <c r="F71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="G71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="H71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="I71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="J71" s="1" t="str">
@@ -13242,19 +13246,19 @@
         <v>168</v>
       </c>
       <c r="F72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="G72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="H72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="I72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="J72" s="1" t="str">
@@ -13291,19 +13295,19 @@
         <v>164</v>
       </c>
       <c r="F73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="G73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="H73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="I73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="J73" s="1" t="str">
@@ -13326,7 +13330,10 @@
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A74" s="2"/>
+      <c r="A74" s="2" t="str">
+        <f>[1]Enums!$A$13</f>
+        <v>1.1.1</v>
+      </c>
       <c r="B74" s="3" t="s">
         <v>163</v>
       </c>
@@ -13340,19 +13347,19 @@
         <v>160</v>
       </c>
       <c r="F74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="G74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="H74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="I74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="J74" s="1" t="str">
@@ -13367,7 +13374,7 @@
       </c>
       <c r="M74" s="2" t="str">
         <f>[1]Polymers!$C74</f>
-        <v>PMIA</v>
+        <v>nomex</v>
       </c>
       <c r="N74" s="2" t="b">
         <f>[1]Polymers!$D74</f>
@@ -13389,19 +13396,19 @@
         <v>156</v>
       </c>
       <c r="F75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J75" s="1" t="str">
@@ -13441,19 +13448,19 @@
         <v>152</v>
       </c>
       <c r="F76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyOxymethylene Pellets)</v>
       </c>
       <c r="G76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyOxymethylene Pellets)</v>
       </c>
       <c r="H76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyOxymethylene Pellets)</v>
       </c>
       <c r="I76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyOxymethylene Pellets)</v>
       </c>
       <c r="J76" s="1" t="str">
@@ -13490,19 +13497,19 @@
         <v>148</v>
       </c>
       <c r="F77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J77" s="1" t="str">
@@ -13539,19 +13546,19 @@
         <v>144</v>
       </c>
       <c r="F78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenol Pellets)</v>
       </c>
       <c r="G78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenol Pellets)</v>
       </c>
       <c r="H78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenol Pellets)</v>
       </c>
       <c r="I78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenol Pellets)</v>
       </c>
       <c r="J78" s="1" t="str">
@@ -13588,19 +13595,19 @@
         <v>140</v>
       </c>
       <c r="F79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="G79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="H79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="I79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="J79" s="1" t="str">
@@ -13637,19 +13644,19 @@
         <v>136</v>
       </c>
       <c r="F80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhosphazene Pellets)</v>
       </c>
       <c r="G80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhosphazene Pellets)</v>
       </c>
       <c r="H80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhosphazene Pellets)</v>
       </c>
       <c r="I80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhosphazene Pellets)</v>
       </c>
       <c r="J80" s="1" t="str">
@@ -13686,19 +13693,19 @@
         <v>132</v>
       </c>
       <c r="F81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="G81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="H81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="I81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="J81" s="1" t="str">
@@ -13735,19 +13742,19 @@
         <v>128</v>
       </c>
       <c r="F82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="G82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="H82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="I82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="J82" s="1" t="str">
@@ -13787,19 +13794,19 @@
         <v>124</v>
       </c>
       <c r="F83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="G83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="H83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="I83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="J83" s="1" t="str">
@@ -13839,19 +13846,19 @@
         <v>120</v>
       </c>
       <c r="F84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Pellets)</v>
       </c>
       <c r="G84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Pellets)</v>
       </c>
       <c r="H84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Pellets)</v>
       </c>
       <c r="I84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Pellets)</v>
       </c>
       <c r="J84" s="1" t="str">
@@ -13888,19 +13895,19 @@
         <v>116</v>
       </c>
       <c r="F85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="G85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="H85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="I85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="J85" s="1" t="str">
@@ -13937,19 +13944,19 @@
         <v>112</v>
       </c>
       <c r="F86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="G86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="H86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="I86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="J86" s="1" t="str">
@@ -13989,19 +13996,19 @@
         <v>108</v>
       </c>
       <c r="F87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyStyrene Pellets)</v>
       </c>
       <c r="G87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyStyrene Pellets)</v>
       </c>
       <c r="H87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyStyrene Pellets)</v>
       </c>
       <c r="I87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyStyrene Pellets)</v>
       </c>
       <c r="J87" s="1" t="str">
@@ -14038,19 +14045,19 @@
         <v>104</v>
       </c>
       <c r="F88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J88" s="1" t="str">
@@ -14090,19 +14097,19 @@
         <v>100</v>
       </c>
       <c r="F89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="G89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="H89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="I89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="J89" s="1" t="str">
@@ -14139,19 +14146,19 @@
         <v>96</v>
       </c>
       <c r="F90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="G90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="H90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="I90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="J90" s="1" t="str">
@@ -14188,19 +14195,19 @@
         <v>92</v>
       </c>
       <c r="F91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="G91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="H91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="I91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="J91" s="1" t="str">
@@ -14237,19 +14244,19 @@
         <v>88</v>
       </c>
       <c r="F92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyThiazyl Pellets)</v>
       </c>
       <c r="G92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyThiazyl Pellets)</v>
       </c>
       <c r="H92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyThiazyl Pellets)</v>
       </c>
       <c r="I92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyThiazyl Pellets)</v>
       </c>
       <c r="J92" s="1" t="str">
@@ -14289,19 +14296,19 @@
         <v>84</v>
       </c>
       <c r="F93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="G93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="H93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="I93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="J93" s="1" t="str">
@@ -14341,19 +14348,19 @@
         <v>80</v>
       </c>
       <c r="F94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyUrethane Pellets)</v>
       </c>
       <c r="G94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyUrethane Pellets)</v>
       </c>
       <c r="H94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyUrethane Pellets)</v>
       </c>
       <c r="I94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyUrethane Pellets)</v>
       </c>
       <c r="J94" s="1" t="str">
@@ -14393,19 +14400,19 @@
         <v>76</v>
       </c>
       <c r="F95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="G95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="H95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="I95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="J95" s="1" t="str">
@@ -14445,19 +14452,19 @@
         <v>72</v>
       </c>
       <c r="F96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="G96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="H96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="I96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="J96" s="1" t="str">
@@ -14494,19 +14501,19 @@
         <v>68</v>
       </c>
       <c r="F97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="G97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="H97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="I97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="J97" s="1" t="str">
@@ -14546,19 +14553,19 @@
         <v>64</v>
       </c>
       <c r="F98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="G98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="H98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="I98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="J98" s="1" t="str">
@@ -14598,19 +14605,19 @@
         <v>60</v>
       </c>
       <c r="F99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="G99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="H99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="I99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="J99" s="1" t="str">
@@ -14647,19 +14654,19 @@
         <v>56</v>
       </c>
       <c r="F100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="G100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="H100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="I100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="J100" s="1" t="str">
@@ -14696,19 +14703,19 @@
         <v>52</v>
       </c>
       <c r="F101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="G101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="H101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="I101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="J101" s="1" t="str">
@@ -14745,19 +14752,19 @@
         <v>48</v>
       </c>
       <c r="F102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="G102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="H102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="I102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="J102" s="1" t="str">
@@ -14794,19 +14801,19 @@
         <v>44</v>
       </c>
       <c r="F103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="G103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="H103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="I103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="J103" s="1" t="str">
@@ -14843,19 +14850,19 @@
         <v>40</v>
       </c>
       <c r="F104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="G104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="H104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="I104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="J104" s="1" t="str">
@@ -14892,19 +14899,19 @@
         <v>36</v>
       </c>
       <c r="F105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="G105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="H105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="I105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="J105" s="1" t="str">
@@ -14944,19 +14951,19 @@
         <v>32</v>
       </c>
       <c r="F106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="G106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="H106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="I106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="J106" s="1" t="str">
@@ -14996,19 +15003,19 @@
         <v>28</v>
       </c>
       <c r="F107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J107" s="1" t="str">
@@ -15048,19 +15055,19 @@
         <v>24</v>
       </c>
       <c r="F108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J108" s="1" t="str">
@@ -15097,19 +15104,19 @@
         <v>20</v>
       </c>
       <c r="F109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="G109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="H109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="I109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="J109" s="1" t="str">
@@ -15146,19 +15153,19 @@
         <v>16</v>
       </c>
       <c r="F110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="G110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="H110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="I110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="J110" s="1" t="str">
@@ -15198,19 +15205,19 @@
         <v>12</v>
       </c>
       <c r="F111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="G111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="H111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="I111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="J111" s="1" t="str">
@@ -15247,19 +15254,19 @@
         <v>8</v>
       </c>
       <c r="F112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="G112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="H112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="I112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="J112" s="1" t="str">
@@ -15299,19 +15306,19 @@
         <v>4</v>
       </c>
       <c r="F113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J113" s="1" t="str">
@@ -15351,19 +15358,19 @@
         <v>0</v>
       </c>
       <c r="F114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="G114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="H114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="I114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="J114" s="1" t="str">
@@ -15403,19 +15410,19 @@
         <v>1853</v>
       </c>
       <c r="F115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$21, [1]Enums!$A$23)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$22, [1]Enums!$A$24)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Polycaprolactam Pellets)</v>
       </c>
       <c r="G115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$24, [1]Enums!$A$26)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$25, [1]Enums!$A$27)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Polycaprolactam Pellets)</v>
       </c>
       <c r="H115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$27, [1]Enums!$A$29)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$28, [1]Enums!$A$30)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Polycaprolactam Pellets)</v>
       </c>
       <c r="I115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$30, [1]Enums!$A$32)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$31, [1]Enums!$A$33)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Polycaprolactam Pellets)</v>
       </c>
       <c r="J115" s="1" t="str">
@@ -16196,7 +16203,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I2" s="45" t="str">
-        <f>[1]Enums!$A$130&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Steel</v>
       </c>
       <c r="J2" s="45">
@@ -16244,7 +16251,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I3" s="45" t="str">
-        <f>[1]Enums!$A$130&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Stainless Steel</v>
       </c>
       <c r="J3" s="45">
@@ -16292,7 +16299,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I4" s="45" t="str">
-        <f>[1]Enums!$A$130&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Brass</v>
       </c>
       <c r="J4" s="45">
@@ -16340,7 +16347,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I5" s="45" t="str">
-        <f>[1]Enums!$A$130&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Bronze</v>
       </c>
       <c r="J5" s="45">
@@ -16388,7 +16395,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I6" s="45" t="str">
-        <f>[1]Enums!$A$130&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Tungsten Carbide</v>
       </c>
       <c r="J6" s="45">
@@ -16436,7 +16443,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I7" s="45" t="str">
-        <f>[1]Enums!$A$130&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Nichrome</v>
       </c>
       <c r="J7" s="45">
@@ -16484,7 +16491,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I8" s="45" t="str">
-        <f>[1]Enums!$A$130&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Antimony-Lead</v>
       </c>
       <c r="J8" s="45">
@@ -16532,7 +16539,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I9" s="45" t="str">
-        <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$132&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Steel</v>
       </c>
       <c r="J9" s="45">
@@ -16580,7 +16587,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I10" s="45" t="str">
-        <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$132&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Stainless Steel</v>
       </c>
       <c r="J10" s="45">
@@ -16628,7 +16635,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I11" s="45" t="str">
-        <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$132&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Brass</v>
       </c>
       <c r="J11" s="45">
@@ -16676,7 +16683,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I12" s="45" t="str">
-        <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$132&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Bronze</v>
       </c>
       <c r="J12" s="45">
@@ -16724,7 +16731,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I13" s="45" t="str">
-        <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$132&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Tungsten Carbide</v>
       </c>
       <c r="J13" s="45">
@@ -16772,7 +16779,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I14" s="45" t="str">
-        <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$132&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Nichrome</v>
       </c>
       <c r="J14" s="45">
@@ -16820,7 +16827,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I15" s="45" t="str">
-        <f>[1]Enums!$A$131&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$132&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Antimony-Lead</v>
       </c>
       <c r="J15" s="45">
@@ -16868,7 +16875,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I16" s="45" t="str">
-        <f>[1]Enums!$A$130&amp;" Iron"</f>
+        <f>[1]Enums!$A$131&amp;" Iron"</f>
         <v>Composite Iron</v>
       </c>
       <c r="J16" s="45">
@@ -16916,7 +16923,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I17" s="45" t="str">
-        <f>[1]Enums!$A$131&amp;" Iron"</f>
+        <f>[1]Enums!$A$132&amp;" Iron"</f>
         <v>Engineered Iron</v>
       </c>
       <c r="J17" s="45">
@@ -16964,7 +16971,7 @@
         <v>Diamond</v>
       </c>
       <c r="I18" s="45" t="str">
-        <f>[1]Enums!$A$130&amp;" Diamond"</f>
+        <f>[1]Enums!$A$131&amp;" Diamond"</f>
         <v>Composite Diamond</v>
       </c>
       <c r="J18" s="45">
@@ -17012,7 +17019,7 @@
         <v>Diamond</v>
       </c>
       <c r="I19" s="45" t="str">
-        <f>[1]Enums!$A$131&amp;" Diamond"</f>
+        <f>[1]Enums!$A$132&amp;" Diamond"</f>
         <v>Engineered Diamond</v>
       </c>
       <c r="J19" s="45">
@@ -17313,7 +17320,7 @@
         <v>Molded Item</v>
       </c>
       <c r="F1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$95</f>
+        <f xml:space="preserve"> [1]Enums!$A$96</f>
         <v>Base Material</v>
       </c>
       <c r="G1" s="30" t="s">
@@ -17341,7 +17348,7 @@
         <v>1812</v>
       </c>
       <c r="C2" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D2</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D2</f>
         <v>Gripped Iron Shovel</v>
       </c>
       <c r="D2" s="24" t="str">
@@ -17353,7 +17360,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F2" s="34" t="str">
-        <f>[1]Enums!$A$98</f>
+        <f>[1]Enums!$A$99</f>
         <v>Iron</v>
       </c>
       <c r="G2" s="24">
@@ -17378,7 +17385,7 @@
         <v>1811</v>
       </c>
       <c r="C3" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D3</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D3</f>
         <v>Gripped Iron Pickaxe</v>
       </c>
       <c r="D3" s="21" t="str">
@@ -17390,7 +17397,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F3" s="34" t="str">
-        <f>[1]Enums!$A$98</f>
+        <f>[1]Enums!$A$99</f>
         <v>Iron</v>
       </c>
       <c r="G3" s="24">
@@ -17415,7 +17422,7 @@
         <v>1810</v>
       </c>
       <c r="C4" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D4</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D4</f>
         <v>Gripped Iron Axe</v>
       </c>
       <c r="D4" s="21" t="str">
@@ -17427,7 +17434,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F4" s="34" t="str">
-        <f>[1]Enums!$A$98</f>
+        <f>[1]Enums!$A$99</f>
         <v>Iron</v>
       </c>
       <c r="G4" s="24">
@@ -17452,7 +17459,7 @@
         <v>1809</v>
       </c>
       <c r="C5" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D5</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D5</f>
         <v>Gripped Iron Sword</v>
       </c>
       <c r="D5" s="21" t="str">
@@ -17464,7 +17471,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F5" s="34" t="str">
-        <f>[1]Enums!$A$98</f>
+        <f>[1]Enums!$A$99</f>
         <v>Iron</v>
       </c>
       <c r="G5" s="24">
@@ -17489,7 +17496,7 @@
         <v>1808</v>
       </c>
       <c r="C6" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D6</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D6</f>
         <v>Gripped Wooden Sword</v>
       </c>
       <c r="D6" s="21" t="str">
@@ -17501,7 +17508,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F6" s="34" t="str">
-        <f>[1]Enums!$A$96</f>
+        <f>[1]Enums!$A$97</f>
         <v>Wooden</v>
       </c>
       <c r="G6" s="24">
@@ -17526,7 +17533,7 @@
         <v>1807</v>
       </c>
       <c r="C7" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D7</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D7</f>
         <v>Gripped Wooden Shovel</v>
       </c>
       <c r="D7" s="21" t="str">
@@ -17538,7 +17545,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F7" s="34" t="str">
-        <f>[1]Enums!$A$96</f>
+        <f>[1]Enums!$A$97</f>
         <v>Wooden</v>
       </c>
       <c r="G7" s="24">
@@ -17563,7 +17570,7 @@
         <v>1806</v>
       </c>
       <c r="C8" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D8</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D8</f>
         <v>Gripped Wooden Pickaxe</v>
       </c>
       <c r="D8" s="21" t="str">
@@ -17575,7 +17582,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F8" s="34" t="str">
-        <f>[1]Enums!$A$96</f>
+        <f>[1]Enums!$A$97</f>
         <v>Wooden</v>
       </c>
       <c r="G8" s="24">
@@ -17600,7 +17607,7 @@
         <v>1805</v>
       </c>
       <c r="C9" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D9</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D9</f>
         <v>Gripped Wooden Axe</v>
       </c>
       <c r="D9" s="21" t="str">
@@ -17612,7 +17619,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F9" s="34" t="str">
-        <f>[1]Enums!$A$96</f>
+        <f>[1]Enums!$A$97</f>
         <v>Wooden</v>
       </c>
       <c r="G9" s="24">
@@ -17637,7 +17644,7 @@
         <v>1804</v>
       </c>
       <c r="C10" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D10</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D10</f>
         <v>Gripped Stone Sword</v>
       </c>
       <c r="D10" s="21" t="str">
@@ -17649,7 +17656,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F10" s="34" t="str">
-        <f>[1]Enums!$A$97</f>
+        <f>[1]Enums!$A$98</f>
         <v>Stone</v>
       </c>
       <c r="G10" s="24">
@@ -17674,7 +17681,7 @@
         <v>1803</v>
       </c>
       <c r="C11" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D11</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D11</f>
         <v>Gripped Stone Shovel</v>
       </c>
       <c r="D11" s="21" t="str">
@@ -17686,7 +17693,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F11" s="34" t="str">
-        <f>[1]Enums!$A$97</f>
+        <f>[1]Enums!$A$98</f>
         <v>Stone</v>
       </c>
       <c r="G11" s="24">
@@ -17711,7 +17718,7 @@
         <v>1802</v>
       </c>
       <c r="C12" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D12</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D12</f>
         <v>Gripped Stone Pickaxe</v>
       </c>
       <c r="D12" s="21" t="str">
@@ -17723,7 +17730,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F12" s="34" t="str">
-        <f>[1]Enums!$A$97</f>
+        <f>[1]Enums!$A$98</f>
         <v>Stone</v>
       </c>
       <c r="G12" s="24">
@@ -17748,7 +17755,7 @@
         <v>1801</v>
       </c>
       <c r="C13" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D13</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D13</f>
         <v>Gripped Stone Axe</v>
       </c>
       <c r="D13" s="21" t="str">
@@ -17760,7 +17767,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F13" s="34" t="str">
-        <f>[1]Enums!$A$97</f>
+        <f>[1]Enums!$A$98</f>
         <v>Stone</v>
       </c>
       <c r="G13" s="24">
@@ -17785,7 +17792,7 @@
         <v>1800</v>
       </c>
       <c r="C14" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D14</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D14</f>
         <v>Gripped Diamond Sword</v>
       </c>
       <c r="D14" s="21" t="str">
@@ -17797,7 +17804,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F14" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$101</f>
         <v>Diamond</v>
       </c>
       <c r="G14" s="24">
@@ -17822,7 +17829,7 @@
         <v>1799</v>
       </c>
       <c r="C15" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D15</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D15</f>
         <v>Gripped Diamond Shovel</v>
       </c>
       <c r="D15" s="21" t="str">
@@ -17834,7 +17841,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F15" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$101</f>
         <v>Diamond</v>
       </c>
       <c r="G15" s="24">
@@ -17859,7 +17866,7 @@
         <v>1798</v>
       </c>
       <c r="C16" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D16</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D16</f>
         <v>Gripped Diamond Pickaxe</v>
       </c>
       <c r="D16" s="21" t="str">
@@ -17871,7 +17878,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F16" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$101</f>
         <v>Diamond</v>
       </c>
       <c r="G16" s="24">
@@ -17896,7 +17903,7 @@
         <v>1797</v>
       </c>
       <c r="C17" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D17</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D17</f>
         <v>Gripped Diamond Axe</v>
       </c>
       <c r="D17" s="21" t="str">
@@ -17908,7 +17915,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F17" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$101</f>
         <v>Diamond</v>
       </c>
       <c r="G17" s="24">
@@ -17933,7 +17940,7 @@
         <v>1796</v>
       </c>
       <c r="C18" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D18</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D18</f>
         <v>Gripped Golden Sword</v>
       </c>
       <c r="D18" s="21" t="str">
@@ -17945,7 +17952,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F18" s="34" t="str">
-        <f>[1]Enums!$A$99</f>
+        <f>[1]Enums!$A$100</f>
         <v>Golden</v>
       </c>
       <c r="G18" s="24">
@@ -17970,7 +17977,7 @@
         <v>1795</v>
       </c>
       <c r="C19" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D19</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D19</f>
         <v>Gripped Golden Shovel</v>
       </c>
       <c r="D19" s="21" t="str">
@@ -17982,7 +17989,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F19" s="34" t="str">
-        <f>[1]Enums!$A$99</f>
+        <f>[1]Enums!$A$100</f>
         <v>Golden</v>
       </c>
       <c r="G19" s="24">
@@ -18007,7 +18014,7 @@
         <v>1794</v>
       </c>
       <c r="C20" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D20</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D20</f>
         <v>Gripped Golden Pickaxe</v>
       </c>
       <c r="D20" s="21" t="str">
@@ -18019,7 +18026,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F20" s="34" t="str">
-        <f>[1]Enums!$A$99</f>
+        <f>[1]Enums!$A$100</f>
         <v>Golden</v>
       </c>
       <c r="G20" s="24">
@@ -18044,7 +18051,7 @@
         <v>1793</v>
       </c>
       <c r="C21" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D21</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D21</f>
         <v>Gripped Golden Axe</v>
       </c>
       <c r="D21" s="21" t="str">
@@ -18056,7 +18063,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F21" s="34" t="str">
-        <f>[1]Enums!$A$99</f>
+        <f>[1]Enums!$A$100</f>
         <v>Golden</v>
       </c>
       <c r="G21" s="24">
@@ -18081,7 +18088,7 @@
         <v>1792</v>
       </c>
       <c r="C22" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D22</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D22</f>
         <v>Gripped Wooden Hoe</v>
       </c>
       <c r="D22" s="21" t="str">
@@ -18093,7 +18100,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F22" s="34" t="str">
-        <f>[1]Enums!$A$96</f>
+        <f>[1]Enums!$A$97</f>
         <v>Wooden</v>
       </c>
       <c r="G22" s="24">
@@ -18118,7 +18125,7 @@
         <v>1791</v>
       </c>
       <c r="C23" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D23</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D23</f>
         <v>Gripped Stone Hoe</v>
       </c>
       <c r="D23" s="21" t="str">
@@ -18130,7 +18137,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F23" s="34" t="str">
-        <f>[1]Enums!$A$97</f>
+        <f>[1]Enums!$A$98</f>
         <v>Stone</v>
       </c>
       <c r="G23" s="24">
@@ -18155,7 +18162,7 @@
         <v>1790</v>
       </c>
       <c r="C24" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D24</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D24</f>
         <v>Gripped Iron Hoe</v>
       </c>
       <c r="D24" s="21" t="str">
@@ -18167,7 +18174,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F24" s="34" t="str">
-        <f>[1]Enums!$A$98</f>
+        <f>[1]Enums!$A$99</f>
         <v>Iron</v>
       </c>
       <c r="G24" s="24">
@@ -18192,7 +18199,7 @@
         <v>1789</v>
       </c>
       <c r="C25" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D25</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D25</f>
         <v>Gripped Diamond Hoe</v>
       </c>
       <c r="D25" s="21" t="str">
@@ -18204,7 +18211,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F25" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$101</f>
         <v>Diamond</v>
       </c>
       <c r="G25" s="24">
@@ -18229,7 +18236,7 @@
         <v>1788</v>
       </c>
       <c r="C26" s="22" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;D26</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;D26</f>
         <v>Gripped Golden Hoe</v>
       </c>
       <c r="D26" s="21" t="str">
@@ -18241,7 +18248,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F26" s="34" t="str">
-        <f>[1]Enums!$A$99</f>
+        <f>[1]Enums!$A$100</f>
         <v>Golden</v>
       </c>
       <c r="G26" s="24">
@@ -18303,7 +18310,7 @@
         <v>1832</v>
       </c>
       <c r="D1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$95</f>
+        <f xml:space="preserve"> [1]Enums!$A$96</f>
         <v>Base Material</v>
       </c>
       <c r="E1" s="36" t="s">
@@ -18349,7 +18356,7 @@
         <v>Wooden Pogo Stick</v>
       </c>
       <c r="D2" s="34" t="str">
-        <f>[1]Enums!$A$96</f>
+        <f>[1]Enums!$A$97</f>
         <v>Wooden</v>
       </c>
       <c r="E2" s="37">
@@ -18386,7 +18393,7 @@
         <v>Stone Pogo Stick</v>
       </c>
       <c r="D3" s="34" t="str">
-        <f>[1]Enums!$A$97</f>
+        <f>[1]Enums!$A$98</f>
         <v>Stone</v>
       </c>
       <c r="E3" s="37">
@@ -18422,7 +18429,7 @@
         <v>Iron Pogo Stick</v>
       </c>
       <c r="D4" s="34" t="str">
-        <f>[1]Enums!$A$98</f>
+        <f>[1]Enums!$A$99</f>
         <v>Iron</v>
       </c>
       <c r="E4" s="37">
@@ -18458,7 +18465,7 @@
         <v>Golden Pogo Stick</v>
       </c>
       <c r="D5" s="34" t="str">
-        <f>[1]Enums!$A$99</f>
+        <f>[1]Enums!$A$100</f>
         <v>Golden</v>
       </c>
       <c r="E5" s="37">
@@ -18494,7 +18501,7 @@
         <v>Diamond Pogo Stick</v>
       </c>
       <c r="D6" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$101</f>
         <v>Diamond</v>
       </c>
       <c r="E6" s="37">
@@ -18530,7 +18537,7 @@
         <v>Magic Pogo Stick</v>
       </c>
       <c r="D7" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$102</f>
         <v>Magic</v>
       </c>
       <c r="E7" s="37">
@@ -18562,11 +18569,11 @@
         <v>1821</v>
       </c>
       <c r="C8" s="34" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;I8</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;I8</f>
         <v>Gripped Wooden Pogo Stick</v>
       </c>
       <c r="D8" s="34" t="str">
-        <f>[1]Enums!$A$96</f>
+        <f>[1]Enums!$A$97</f>
         <v>Wooden</v>
       </c>
       <c r="E8" s="37">
@@ -18606,11 +18613,11 @@
         <v>1820</v>
       </c>
       <c r="C9" s="34" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;I9</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;I9</f>
         <v>Gripped Stone Pogo Stick</v>
       </c>
       <c r="D9" s="34" t="str">
-        <f>[1]Enums!$A$97</f>
+        <f>[1]Enums!$A$98</f>
         <v>Stone</v>
       </c>
       <c r="E9" s="37">
@@ -18650,11 +18657,11 @@
         <v>1819</v>
       </c>
       <c r="C10" s="34" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;I10</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;I10</f>
         <v>Gripped Iron Pogo Stick</v>
       </c>
       <c r="D10" s="34" t="str">
-        <f>[1]Enums!$A$98</f>
+        <f>[1]Enums!$A$99</f>
         <v>Iron</v>
       </c>
       <c r="E10" s="37">
@@ -18694,11 +18701,11 @@
         <v>1818</v>
       </c>
       <c r="C11" s="34" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;I11</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;I11</f>
         <v>Gripped Golden Pogo Stick</v>
       </c>
       <c r="D11" s="34" t="str">
-        <f>[1]Enums!$A$99</f>
+        <f>[1]Enums!$A$100</f>
         <v>Golden</v>
       </c>
       <c r="E11" s="37">
@@ -18738,11 +18745,11 @@
         <v>1817</v>
       </c>
       <c r="C12" s="34" t="str">
-        <f>[1]Enums!$A$92&amp;" "&amp;I12</f>
+        <f>[1]Enums!$A$93&amp;" "&amp;I12</f>
         <v>Gripped Diamond Pogo Stick</v>
       </c>
       <c r="D12" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$101</f>
         <v>Diamond</v>
       </c>
       <c r="E12" s="37">
@@ -22265,9 +22272,9 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="2">
+      <c r="A74" s="2" t="str">
         <f>Pellets!A74</f>
-        <v>0</v>
+        <v>1.1.1</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>678</v>
@@ -22277,7 +22284,7 @@
       </c>
       <c r="D74" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Block (PMIA)</v>
+        <v>Block (nomex)</v>
       </c>
       <c r="E74" s="1" t="str">
         <f xml:space="preserve"> Pellets!G74</f>
@@ -22285,7 +22292,7 @@
       </c>
       <c r="F74" s="1" t="str">
         <f>VLOOKUP(E74, Pellets!G:M, 7,FALSE)</f>
-        <v>PMIA</v>
+        <v>nomex</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -26563,9 +26570,9 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74" s="2">
+      <c r="A74" s="2" t="str">
         <f>Pellets!A74</f>
-        <v>0</v>
+        <v>1.1.1</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>988</v>
@@ -26581,15 +26588,15 @@
       </c>
       <c r="F74" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Slab (PMIA)</v>
+        <v>Slab (nomex)</v>
       </c>
       <c r="G74" s="1" t="str">
         <f xml:space="preserve"> 'Blocks (Poly)'!D74</f>
-        <v>Block (PMIA)</v>
+        <v>Block (nomex)</v>
       </c>
       <c r="H74" s="1" t="str">
         <f>VLOOKUP(G74,'Blocks (Poly)'!D:F, 3, FALSE)</f>
-        <v>PMIA</v>
+        <v>nomex</v>
       </c>
       <c r="I74">
         <f>'Blocks (Poly)'!G74/2</f>
@@ -30710,9 +30717,9 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="2">
+      <c r="A74" s="2" t="str">
         <f>Pellets!A74</f>
-        <v>0</v>
+        <v>1.1.1</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>1359</v>
@@ -30722,15 +30729,15 @@
       </c>
       <c r="D74" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Wall (PMIA)</v>
+        <v>Wall (nomex)</v>
       </c>
       <c r="E74" s="1" t="str">
         <f xml:space="preserve"> 'Blocks (Poly)'!D74</f>
-        <v>Block (PMIA)</v>
+        <v>Block (nomex)</v>
       </c>
       <c r="F74" s="1" t="str">
         <f>VLOOKUP(E74,'Blocks (Poly)'!D:F, 3, FALSE)</f>
-        <v>PMIA</v>
+        <v>nomex</v>
       </c>
       <c r="G74">
         <f>'Slabs (Poly)'!I74</f>
@@ -34605,9 +34612,9 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="2">
+      <c r="A74" s="2" t="str">
         <f>Pellets!A74</f>
-        <v>0</v>
+        <v>1.1.1</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>1586</v>
@@ -34617,15 +34624,15 @@
       </c>
       <c r="D74" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Stairs (PMIA)</v>
+        <v>Stairs (nomex)</v>
       </c>
       <c r="E74" s="1" t="str">
         <f xml:space="preserve"> 'Blocks (Poly)'!D74</f>
-        <v>Block (PMIA)</v>
+        <v>Block (nomex)</v>
       </c>
       <c r="F74" s="1" t="str">
         <f>VLOOKUP(E74,'Blocks (Poly)'!D:F, 3, FALSE)</f>
-        <v>PMIA</v>
+        <v>nomex</v>
       </c>
       <c r="G74">
         <f>'Slabs (Poly)'!I74</f>
@@ -36471,7 +36478,7 @@
         <v>590</v>
       </c>
       <c r="D1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$69</f>
+        <f xml:space="preserve"> [1]Enums!$B$70</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="19" t="str">
@@ -36495,7 +36502,7 @@
         <v>Mold (Grip)</v>
       </c>
       <c r="D2" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E2" s="11" t="str">
@@ -36520,7 +36527,7 @@
         <v>Mold (Running Shoes)</v>
       </c>
       <c r="D3" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E3" s="11" t="str">
@@ -36545,7 +36552,7 @@
         <v>Mold (Scuba Fins)</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E4" s="11" t="str">
@@ -36570,7 +36577,7 @@
         <v>Mold (Scuba Mask)</v>
       </c>
       <c r="D5" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E5" s="11" t="str">
@@ -36595,7 +36602,7 @@
         <v>Mold (Gasket)</v>
       </c>
       <c r="D6" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E6" s="11" t="str">
@@ -36620,7 +36627,7 @@
         <v>Mold (Life Preserver)</v>
       </c>
       <c r="D7" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E7" s="11" t="str">
@@ -36645,7 +36652,7 @@
         <v>Metal Die (Fibers)</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$74</f>
+        <f xml:space="preserve"> [1]Enums!$B$75</f>
         <v>Metal Die</v>
       </c>
       <c r="E8" s="11" t="str">
@@ -36670,7 +36677,7 @@
         <v>Metal Die (Tether)</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$74</f>
+        <f xml:space="preserve"> [1]Enums!$B$75</f>
         <v>Metal Die</v>
       </c>
       <c r="E9" s="11" t="str">
@@ -36695,7 +36702,7 @@
         <v>Metal Die (Cord)</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$74</f>
+        <f xml:space="preserve"> [1]Enums!$B$75</f>
         <v>Metal Die</v>
       </c>
       <c r="E10" s="11" t="str">
@@ -36720,7 +36727,7 @@
         <v>Metal Die (Hose)</v>
       </c>
       <c r="D11" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$74</f>
+        <f xml:space="preserve"> [1]Enums!$B$75</f>
         <v>Metal Die</v>
       </c>
       <c r="E11" s="11" t="str">
@@ -36745,7 +36752,7 @@
         <v>Metal Die (Large Pipe)</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$74</f>
+        <f xml:space="preserve"> [1]Enums!$B$75</f>
         <v>Metal Die</v>
       </c>
       <c r="E12" s="11" t="str">
@@ -36770,7 +36777,7 @@
         <v>Mold (Flashlight Shaft)</v>
       </c>
       <c r="D13" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E13" s="11" t="str">
@@ -36794,7 +36801,7 @@
         <v>Mold (Plastic Brick (1 x 1))</v>
       </c>
       <c r="D14" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E14" t="str">
@@ -36818,7 +36825,7 @@
         <v>Mold (Plastic Brick (1 x 2))</v>
       </c>
       <c r="D15" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E15" t="str">
@@ -36842,7 +36849,7 @@
         <v>Mold (Plastic Brick (1 x 3))</v>
       </c>
       <c r="D16" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E16" t="str">
@@ -36866,7 +36873,7 @@
         <v>Mold (Plastic Brick (1 x 4))</v>
       </c>
       <c r="D17" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E17" t="str">
@@ -36890,7 +36897,7 @@
         <v>Mold (Plastic Brick (2 x 2))</v>
       </c>
       <c r="D18" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E18" t="str">
@@ -36914,7 +36921,7 @@
         <v>Mold (Plastic Brick (2 x 3))</v>
       </c>
       <c r="D19" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E19" t="str">
@@ -36938,7 +36945,7 @@
         <v>Mold (Plastic Brick (2 x 4))</v>
       </c>
       <c r="D20" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E20" t="str">
@@ -36962,7 +36969,7 @@
         <v>Mold (Plastic Brick (3 x 3))</v>
       </c>
       <c r="D21" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E21" t="str">
@@ -36986,7 +36993,7 @@
         <v>Mold (Plastic Brick (3 x 4))</v>
       </c>
       <c r="D22" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E22" t="str">
@@ -37010,7 +37017,7 @@
         <v>Mold (Plastic Brick (4 x 4))</v>
       </c>
       <c r="D23" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E23" t="str">
@@ -37034,7 +37041,7 @@
         <v>Mold (Plastic Brick (1 x 8))</v>
       </c>
       <c r="D24" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E24" t="str">
@@ -37058,7 +37065,7 @@
         <v>Mold (Plastic Brick (2 x 8))</v>
       </c>
       <c r="D25" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E25" t="str">
@@ -37082,7 +37089,7 @@
         <v>Mold (Heated Knife Handle)</v>
       </c>
       <c r="D26" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E26" s="11" t="str">
@@ -37106,7 +37113,7 @@
         <v>Mold (Rubber Sole)</v>
       </c>
       <c r="D27" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E27" s="11" t="str">
@@ -37130,7 +37137,7 @@
         <v>Mold (Battery Case)</v>
       </c>
       <c r="D28" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E28" s="11" t="str">
@@ -37154,7 +37161,7 @@
         <v>Mold (Tool Shaft)</v>
       </c>
       <c r="D29" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold</v>
       </c>
       <c r="E29" t="str">
@@ -37177,7 +37184,7 @@
   </sheetPr>
   <dimension ref="A1:U156"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView showZeros="0" topLeftCell="C94" workbookViewId="0">
       <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
@@ -41671,16 +41678,16 @@
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A107" s="23">
+      <c r="A107" s="23" t="str">
         <f>Pellets!A74</f>
-        <v>0</v>
+        <v>1.1.1</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>493</v>
       </c>
       <c r="C107" s="22" t="str">
         <f xml:space="preserve"> VLOOKUP(D107, Molds!C:E, 3, FALSE)&amp;" ("&amp;F107&amp;")"</f>
-        <v>Fibers (PMIA)</v>
+        <v>Fibers (nomex)</v>
       </c>
       <c r="D107" s="24" t="str">
         <f xml:space="preserve"> Molds!$C$8</f>
@@ -41692,7 +41699,7 @@
       </c>
       <c r="F107" s="21" t="str">
         <f>VLOOKUP(E107, Pellets!F:M, 8,FALSE)</f>
-        <v>PMIA</v>
+        <v>nomex</v>
       </c>
       <c r="G107" s="24">
         <v>16</v>

</xml_diff>

<commit_message>
Respect amounts in flow networks and fixed minor bugs
</commit_message>
<xml_diff>
--- a/config/Polycraft Polymers.xlsx
+++ b/config/Polycraft Polymers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21150" yWindow="0" windowWidth="27240" windowHeight="14310" tabRatio="826" activeTab="1"/>
+    <workbookView xWindow="22080" yWindow="0" windowWidth="27240" windowHeight="14310" tabRatio="826" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Pellets" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,6 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -7887,108 +7886,108 @@
             <v>1.1.2</v>
           </cell>
         </row>
-        <row r="23">
-          <cell r="A23" t="str">
+        <row r="25">
+          <cell r="A25" t="str">
             <v>Bag</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24" t="str">
-            <v>Vial</v>
           </cell>
         </row>
         <row r="26">
           <cell r="A26" t="str">
+            <v>Vial</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
             <v>Sack</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27" t="str">
-            <v>Beaker</v>
           </cell>
         </row>
         <row r="29">
           <cell r="A29" t="str">
+            <v>Beaker</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
             <v>Powder Keg</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30" t="str">
-            <v>Drum</v>
           </cell>
         </row>
         <row r="32">
           <cell r="A32" t="str">
+            <v>Drum</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34" t="str">
             <v>Chemical Silo</v>
           </cell>
         </row>
-        <row r="33">
-          <cell r="A33" t="str">
+        <row r="35">
+          <cell r="A35" t="str">
             <v>Chemical Vat</v>
           </cell>
         </row>
-        <row r="71">
-          <cell r="B71" t="str">
+        <row r="73">
+          <cell r="B73" t="str">
             <v>Mold Type</v>
           </cell>
         </row>
-        <row r="75">
-          <cell r="B75" t="str">
+        <row r="77">
+          <cell r="B77" t="str">
             <v>Mold</v>
           </cell>
         </row>
-        <row r="76">
-          <cell r="B76" t="str">
+        <row r="78">
+          <cell r="B78" t="str">
             <v>Metal Die</v>
           </cell>
         </row>
-        <row r="94">
-          <cell r="A94" t="str">
+        <row r="96">
+          <cell r="A96" t="str">
             <v>Gripped</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="A97" t="str">
-            <v>Base Material</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="A98" t="str">
-            <v>Wooden</v>
           </cell>
         </row>
         <row r="99">
           <cell r="A99" t="str">
-            <v>Stone</v>
+            <v>Base Material</v>
           </cell>
         </row>
         <row r="100">
           <cell r="A100" t="str">
-            <v>Iron</v>
+            <v>Wooden</v>
           </cell>
         </row>
         <row r="101">
           <cell r="A101" t="str">
-            <v>Golden</v>
+            <v>Stone</v>
           </cell>
         </row>
         <row r="102">
           <cell r="A102" t="str">
-            <v>Diamond</v>
+            <v>Iron</v>
           </cell>
         </row>
         <row r="103">
           <cell r="A103" t="str">
+            <v>Golden</v>
+          </cell>
+        </row>
+        <row r="104">
+          <cell r="A104" t="str">
+            <v>Diamond</v>
+          </cell>
+        </row>
+        <row r="105">
+          <cell r="A105" t="str">
             <v>Magic</v>
           </cell>
         </row>
-        <row r="132">
-          <cell r="A132" t="str">
+        <row r="134">
+          <cell r="A134" t="str">
             <v>Composite</v>
           </cell>
         </row>
-        <row r="133">
-          <cell r="A133" t="str">
+        <row r="135">
+          <cell r="A135" t="str">
             <v>Engineered</v>
           </cell>
         </row>
@@ -10150,7 +10149,7 @@
   </sheetPr>
   <dimension ref="A1:N333"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
@@ -10193,19 +10192,19 @@
         <v>Game ID XL</v>
       </c>
       <c r="F1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$23&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$25&amp;" ("&amp;J1&amp;")"</f>
         <v>Bag (Pellets)</v>
       </c>
       <c r="G1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$26&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$28&amp;" ("&amp;J1&amp;")"</f>
         <v>Sack (Pellets)</v>
       </c>
       <c r="H1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$29&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$31&amp;" ("&amp;J1&amp;")"</f>
         <v>Powder Keg (Pellets)</v>
       </c>
       <c r="I1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$32&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$34&amp;" ("&amp;J1&amp;")"</f>
         <v>Chemical Silo (Pellets)</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -10241,19 +10240,19 @@
         <v>448</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="G2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="H2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="J2" s="1" t="str">
@@ -10293,19 +10292,19 @@
         <v>444</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J3" s="1" t="str">
@@ -10342,19 +10341,19 @@
         <v>440</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Alkyd Resin)</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Alkyd Resin)</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Alkyd Resin)</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Alkyd Resin)</v>
       </c>
       <c r="J4" s="1" t="str">
@@ -10394,19 +10393,19 @@
         <v>436</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J5" s="1" t="str">
@@ -10446,19 +10445,19 @@
         <v>432</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J6" s="1" t="str">
@@ -10498,19 +10497,19 @@
         <v>428</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$23, [1]Enums!$A$23)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$25, [1]Enums!$A$25)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Carbon Fiber)</v>
       </c>
       <c r="G7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$26, [1]Enums!$A$26)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$28, [1]Enums!$A$28)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Carbon Fiber)</v>
       </c>
       <c r="H7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$29, [1]Enums!$A$29)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$31, [1]Enums!$A$31)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Carbon Fiber)</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$32, [1]Enums!$A$32)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$34, [1]Enums!$A$34)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Carbon Fiber)</v>
       </c>
       <c r="J7" s="1" t="str">
@@ -10547,19 +10546,19 @@
         <v>424</v>
       </c>
       <c r="F8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="G8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="J8" s="1" t="str">
@@ -10599,19 +10598,19 @@
         <v>420</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulosic Pellets)</v>
       </c>
       <c r="G9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulosic Pellets)</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulosic Pellets)</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulosic Pellets)</v>
       </c>
       <c r="J9" s="1" t="str">
@@ -10651,19 +10650,19 @@
         <v>416</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chitin Pellets)</v>
       </c>
       <c r="G10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chitin Pellets)</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chitin Pellets)</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chitin Pellets)</v>
       </c>
       <c r="J10" s="1" t="str">
@@ -10703,19 +10702,19 @@
         <v>412</v>
       </c>
       <c r="F11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J11" s="1" t="str">
@@ -10755,19 +10754,19 @@
         <v>408</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Epoxy Resin)</v>
       </c>
       <c r="G12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Epoxy Resin)</v>
       </c>
       <c r="H12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Epoxy Resin)</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Epoxy Resin)</v>
       </c>
       <c r="J12" s="1" t="str">
@@ -10804,19 +10803,19 @@
         <v>404</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethoxylates Pellets)</v>
       </c>
       <c r="G13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethoxylates Pellets)</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethoxylates Pellets)</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethoxylates Pellets)</v>
       </c>
       <c r="J13" s="1" t="str">
@@ -10856,19 +10855,19 @@
         <v>400</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="G14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="H14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="J14" s="1" t="str">
@@ -10908,19 +10907,19 @@
         <v>396</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="G15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="J15" s="1" t="str">
@@ -10960,19 +10959,19 @@
         <v>392</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="G16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="J16" s="1" t="str">
@@ -11012,19 +11011,19 @@
         <v>388</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="G17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="J17" s="1" t="str">
@@ -11064,19 +11063,19 @@
         <v>384</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J18" s="1" t="str">
@@ -11116,19 +11115,19 @@
         <v>380</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J19" s="1" t="str">
@@ -11165,19 +11164,19 @@
         <v>376</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Lignin)</v>
       </c>
       <c r="G20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Lignin)</v>
       </c>
       <c r="H20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Lignin)</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Lignin)</v>
       </c>
       <c r="J20" s="1" t="str">
@@ -11217,19 +11216,19 @@
         <v>372</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J21" s="1" t="str">
@@ -11269,19 +11268,19 @@
         <v>368</v>
       </c>
       <c r="F22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="G22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="H22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="J22" s="1" t="str">
@@ -11321,19 +11320,19 @@
         <v>364</v>
       </c>
       <c r="F23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="G23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="H23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="J23" s="1" t="str">
@@ -11373,19 +11372,19 @@
         <v>360</v>
       </c>
       <c r="F24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="G24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="H24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="J24" s="1" t="str">
@@ -11422,19 +11421,19 @@
         <v>356</v>
       </c>
       <c r="F25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="G25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="H25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="J25" s="1" t="str">
@@ -11474,19 +11473,19 @@
         <v>352</v>
       </c>
       <c r="F26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Metaldehyde Pellets)</v>
       </c>
       <c r="G26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Metaldehyde Pellets)</v>
       </c>
       <c r="H26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Metaldehyde Pellets)</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Metaldehyde Pellets)</v>
       </c>
       <c r="J26" s="1" t="str">
@@ -11526,19 +11525,19 @@
         <v>348</v>
       </c>
       <c r="F27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J27" s="1" t="str">
@@ -11578,19 +11577,19 @@
         <v>344</v>
       </c>
       <c r="F28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraformaldehyde Pellets)</v>
       </c>
       <c r="G28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraformaldehyde Pellets)</v>
       </c>
       <c r="H28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraformaldehyde Pellets)</v>
       </c>
       <c r="I28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraformaldehyde Pellets)</v>
       </c>
       <c r="J28" s="1" t="str">
@@ -11630,19 +11629,19 @@
         <v>340</v>
       </c>
       <c r="F29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraldehyde Pellets)</v>
       </c>
       <c r="G29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraldehyde Pellets)</v>
       </c>
       <c r="H29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraldehyde Pellets)</v>
       </c>
       <c r="I29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraldehyde Pellets)</v>
       </c>
       <c r="J29" s="1" t="str">
@@ -11682,19 +11681,19 @@
         <v>336</v>
       </c>
       <c r="F30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Phenolic Resin)</v>
       </c>
       <c r="G30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Phenolic Resin)</v>
       </c>
       <c r="H30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Phenolic Resin)</v>
       </c>
       <c r="I30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Phenolic Resin)</v>
       </c>
       <c r="J30" s="1" t="str">
@@ -11734,19 +11733,19 @@
         <v>332</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="G31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="H31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="I31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="J31" s="1" t="str">
@@ -11783,19 +11782,19 @@
         <v>328</v>
       </c>
       <c r="F32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly1-Butene Pellets)</v>
       </c>
       <c r="G32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly1-Butene Pellets)</v>
       </c>
       <c r="H32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly1-Butene Pellets)</v>
       </c>
       <c r="I32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly1-Butene Pellets)</v>
       </c>
       <c r="J32" s="1" t="str">
@@ -11832,19 +11831,19 @@
         <v>324</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2,6-Dimethyl-1,4-Phenylene Ether Pellets)</v>
       </c>
       <c r="G33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2,6-Dimethyl-1,4-Phenylene Ether Pellets)</v>
       </c>
       <c r="H33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2,6-Dimethyl-1,4-Phenylene Ether Pellets)</v>
       </c>
       <c r="I33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2,6-Dimethyl-1,4-Phenylene Ether Pellets)</v>
       </c>
       <c r="J33" s="1" t="str">
@@ -11881,19 +11880,19 @@
         <v>320</v>
       </c>
       <c r="F34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="G34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="H34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="I34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="J34" s="1" t="str">
@@ -11930,19 +11929,19 @@
         <v>316</v>
       </c>
       <c r="F35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="G35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="H35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="I35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="J35" s="1" t="str">
@@ -11982,19 +11981,19 @@
         <v>312</v>
       </c>
       <c r="F36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="G36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="H36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="I36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="J36" s="1" t="str">
@@ -12034,19 +12033,19 @@
         <v>308</v>
       </c>
       <c r="F37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="G37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="H37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="I37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="J37" s="1" t="str">
@@ -12086,19 +12085,19 @@
         <v>304</v>
       </c>
       <c r="F38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="G38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="H38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="I38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="J38" s="1" t="str">
@@ -12138,19 +12137,19 @@
         <v>300</v>
       </c>
       <c r="F39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="G39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="H39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="I39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="J39" s="1" t="str">
@@ -12190,19 +12189,19 @@
         <v>296</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="G40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="H40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="I40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="J40" s="1" t="str">
@@ -12242,19 +12241,19 @@
         <v>292</v>
       </c>
       <c r="F41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="G41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="H41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="I41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="J41" s="1" t="str">
@@ -12294,19 +12293,19 @@
         <v>288</v>
       </c>
       <c r="F42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCaprolactone Pellets)</v>
       </c>
       <c r="G42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCaprolactone Pellets)</v>
       </c>
       <c r="H42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCaprolactone Pellets)</v>
       </c>
       <c r="I42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCaprolactone Pellets)</v>
       </c>
       <c r="J42" s="1" t="str">
@@ -12346,19 +12345,19 @@
         <v>284</v>
       </c>
       <c r="F43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCarbonate Pellets)</v>
       </c>
       <c r="G43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCarbonate Pellets)</v>
       </c>
       <c r="H43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCarbonate Pellets)</v>
       </c>
       <c r="I43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCarbonate Pellets)</v>
       </c>
       <c r="J43" s="1" t="str">
@@ -12395,19 +12394,19 @@
         <v>280</v>
       </c>
       <c r="F44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChloroPrene Pellets)</v>
       </c>
       <c r="G44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChloroPrene Pellets)</v>
       </c>
       <c r="H44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChloroPrene Pellets)</v>
       </c>
       <c r="I44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChloroPrene Pellets)</v>
       </c>
       <c r="J44" s="1" t="str">
@@ -12444,19 +12443,19 @@
         <v>276</v>
       </c>
       <c r="F45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="G45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="H45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="I45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="J45" s="1" t="str">
@@ -12496,19 +12495,19 @@
         <v>272</v>
       </c>
       <c r="F46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="G46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="H46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="I46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="J46" s="1" t="str">
@@ -12548,19 +12547,19 @@
         <v>268</v>
       </c>
       <c r="F47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="G47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="H47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="I47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="J47" s="1" t="str">
@@ -12600,19 +12599,19 @@
         <v>264</v>
       </c>
       <c r="F48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEtherImide Pellets)</v>
       </c>
       <c r="G48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEtherImide Pellets)</v>
       </c>
       <c r="H48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEtherImide Pellets)</v>
       </c>
       <c r="I48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEtherImide Pellets)</v>
       </c>
       <c r="J48" s="1" t="str">
@@ -12649,19 +12648,19 @@
         <v>260</v>
       </c>
       <c r="F49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="G49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="H49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="I49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="J49" s="1" t="str">
@@ -12698,19 +12697,19 @@
         <v>256</v>
       </c>
       <c r="F50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="G50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="H50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="I50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="J50" s="1" t="str">
@@ -12750,19 +12749,19 @@
         <v>252</v>
       </c>
       <c r="F51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="G51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="H51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="I51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="J51" s="1" t="str">
@@ -12799,19 +12798,19 @@
         <v>248</v>
       </c>
       <c r="F52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J52" s="1" t="str">
@@ -12851,19 +12850,19 @@
         <v>244</v>
       </c>
       <c r="F53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="G53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="H53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="I53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="J53" s="1" t="str">
@@ -12903,19 +12902,19 @@
         <v>240</v>
       </c>
       <c r="F54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="G54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="H54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="I54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="J54" s="1" t="str">
@@ -12955,19 +12954,19 @@
         <v>236</v>
       </c>
       <c r="F55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="G55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="H55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="I55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="J55" s="1" t="str">
@@ -13007,19 +13006,19 @@
         <v>232</v>
       </c>
       <c r="F56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J56" s="1" t="str">
@@ -13059,19 +13058,19 @@
         <v>228</v>
       </c>
       <c r="F57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="G57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="H57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="I57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="J57" s="1" t="str">
@@ -13111,19 +13110,19 @@
         <v>224</v>
       </c>
       <c r="F58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="G58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="H58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="I58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="J58" s="1" t="str">
@@ -13163,19 +13162,19 @@
         <v>220</v>
       </c>
       <c r="F59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="G59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="H59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="I59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="J59" s="1" t="str">
@@ -13215,19 +13214,19 @@
         <v>216</v>
       </c>
       <c r="F60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="G60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="H60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="I60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="J60" s="1" t="str">
@@ -13267,19 +13266,19 @@
         <v>212</v>
       </c>
       <c r="F61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="G61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="H61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="I61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="J61" s="1" t="str">
@@ -13316,19 +13315,19 @@
         <v>208</v>
       </c>
       <c r="F62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="G62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="H62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="I62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="J62" s="1" t="str">
@@ -13368,19 +13367,19 @@
         <v>204</v>
       </c>
       <c r="F63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyImide Pellets)</v>
       </c>
       <c r="G63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyImide Pellets)</v>
       </c>
       <c r="H63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyImide Pellets)</v>
       </c>
       <c r="I63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyImide Pellets)</v>
       </c>
       <c r="J63" s="1" t="str">
@@ -13417,19 +13416,19 @@
         <v>200</v>
       </c>
       <c r="F64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="G64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="H64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="I64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="J64" s="1" t="str">
@@ -13466,19 +13465,19 @@
         <v>196</v>
       </c>
       <c r="F65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="G65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="H65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="I65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="J65" s="1" t="str">
@@ -13518,19 +13517,19 @@
         <v>192</v>
       </c>
       <c r="F66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButylene Pellets)</v>
       </c>
       <c r="G66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButylene Pellets)</v>
       </c>
       <c r="H66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButylene Pellets)</v>
       </c>
       <c r="I66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButylene Pellets)</v>
       </c>
       <c r="J66" s="1" t="str">
@@ -13570,19 +13569,19 @@
         <v>188</v>
       </c>
       <c r="F67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoPrene Pellets)</v>
       </c>
       <c r="G67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoPrene Pellets)</v>
       </c>
       <c r="H67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoPrene Pellets)</v>
       </c>
       <c r="I67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoPrene Pellets)</v>
       </c>
       <c r="J67" s="1" t="str">
@@ -13622,19 +13621,19 @@
         <v>184</v>
       </c>
       <c r="F68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic Acid Pellets)</v>
       </c>
       <c r="G68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic Acid Pellets)</v>
       </c>
       <c r="H68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic Acid Pellets)</v>
       </c>
       <c r="I68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic Acid Pellets)</v>
       </c>
       <c r="J68" s="1" t="str">
@@ -13671,19 +13670,19 @@
         <v>180</v>
       </c>
       <c r="F69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="G69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="H69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="I69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="J69" s="1" t="str">
@@ -13720,19 +13719,19 @@
         <v>176</v>
       </c>
       <c r="F70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="G70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="H70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="I70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="J70" s="1" t="str">
@@ -13769,19 +13768,19 @@
         <v>172</v>
       </c>
       <c r="F71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="G71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="H71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="I71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="J71" s="1" t="str">
@@ -13818,19 +13817,19 @@
         <v>168</v>
       </c>
       <c r="F72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="G72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="H72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="I72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="J72" s="1" t="str">
@@ -13867,19 +13866,19 @@
         <v>164</v>
       </c>
       <c r="F73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="G73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="H73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="I73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="J73" s="1" t="str">
@@ -13919,19 +13918,19 @@
         <v>160</v>
       </c>
       <c r="F74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="G74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="H74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="I74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="J74" s="1" t="str">
@@ -13968,19 +13967,19 @@
         <v>156</v>
       </c>
       <c r="F75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J75" s="1" t="str">
@@ -14020,19 +14019,19 @@
         <v>152</v>
       </c>
       <c r="F76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyOxymethylene Pellets)</v>
       </c>
       <c r="G76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyOxymethylene Pellets)</v>
       </c>
       <c r="H76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyOxymethylene Pellets)</v>
       </c>
       <c r="I76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyOxymethylene Pellets)</v>
       </c>
       <c r="J76" s="1" t="str">
@@ -14069,19 +14068,19 @@
         <v>148</v>
       </c>
       <c r="F77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J77" s="1" t="str">
@@ -14118,19 +14117,19 @@
         <v>144</v>
       </c>
       <c r="F78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenol Pellets)</v>
       </c>
       <c r="G78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenol Pellets)</v>
       </c>
       <c r="H78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenol Pellets)</v>
       </c>
       <c r="I78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenol Pellets)</v>
       </c>
       <c r="J78" s="1" t="str">
@@ -14167,19 +14166,19 @@
         <v>140</v>
       </c>
       <c r="F79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="G79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="H79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="I79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="J79" s="1" t="str">
@@ -14216,19 +14215,19 @@
         <v>136</v>
       </c>
       <c r="F80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhosphazene Pellets)</v>
       </c>
       <c r="G80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhosphazene Pellets)</v>
       </c>
       <c r="H80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhosphazene Pellets)</v>
       </c>
       <c r="I80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhosphazene Pellets)</v>
       </c>
       <c r="J80" s="1" t="str">
@@ -14265,19 +14264,19 @@
         <v>132</v>
       </c>
       <c r="F81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="G81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="H81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="I81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="J81" s="1" t="str">
@@ -14314,19 +14313,19 @@
         <v>128</v>
       </c>
       <c r="F82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="G82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="H82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="I82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="J82" s="1" t="str">
@@ -14366,19 +14365,19 @@
         <v>124</v>
       </c>
       <c r="F83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="G83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="H83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="I83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="J83" s="1" t="str">
@@ -14418,19 +14417,19 @@
         <v>120</v>
       </c>
       <c r="F84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Pellets)</v>
       </c>
       <c r="G84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Pellets)</v>
       </c>
       <c r="H84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Pellets)</v>
       </c>
       <c r="I84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Pellets)</v>
       </c>
       <c r="J84" s="1" t="str">
@@ -14467,19 +14466,19 @@
         <v>116</v>
       </c>
       <c r="F85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="G85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="H85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="I85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="J85" s="1" t="str">
@@ -14516,19 +14515,19 @@
         <v>112</v>
       </c>
       <c r="F86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="G86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="H86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="I86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="J86" s="1" t="str">
@@ -14568,19 +14567,19 @@
         <v>108</v>
       </c>
       <c r="F87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyStyrene Pellets)</v>
       </c>
       <c r="G87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyStyrene Pellets)</v>
       </c>
       <c r="H87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyStyrene Pellets)</v>
       </c>
       <c r="I87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyStyrene Pellets)</v>
       </c>
       <c r="J87" s="1" t="str">
@@ -14617,19 +14616,19 @@
         <v>104</v>
       </c>
       <c r="F88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J88" s="1" t="str">
@@ -14669,19 +14668,19 @@
         <v>100</v>
       </c>
       <c r="F89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="G89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="H89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="I89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="J89" s="1" t="str">
@@ -14718,19 +14717,19 @@
         <v>96</v>
       </c>
       <c r="F90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="G90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="H90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="I90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="J90" s="1" t="str">
@@ -14767,19 +14766,19 @@
         <v>92</v>
       </c>
       <c r="F91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="G91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="H91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="I91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="J91" s="1" t="str">
@@ -14816,19 +14815,19 @@
         <v>88</v>
       </c>
       <c r="F92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyThiazyl Pellets)</v>
       </c>
       <c r="G92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyThiazyl Pellets)</v>
       </c>
       <c r="H92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyThiazyl Pellets)</v>
       </c>
       <c r="I92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyThiazyl Pellets)</v>
       </c>
       <c r="J92" s="1" t="str">
@@ -14868,19 +14867,19 @@
         <v>84</v>
       </c>
       <c r="F93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="G93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="H93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="I93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="J93" s="1" t="str">
@@ -14920,19 +14919,19 @@
         <v>80</v>
       </c>
       <c r="F94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyUrethane Pellets)</v>
       </c>
       <c r="G94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyUrethane Pellets)</v>
       </c>
       <c r="H94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyUrethane Pellets)</v>
       </c>
       <c r="I94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyUrethane Pellets)</v>
       </c>
       <c r="J94" s="1" t="str">
@@ -14972,19 +14971,19 @@
         <v>76</v>
       </c>
       <c r="F95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="G95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="H95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="I95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="J95" s="1" t="str">
@@ -15024,19 +15023,19 @@
         <v>72</v>
       </c>
       <c r="F96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="G96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="H96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="I96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="J96" s="1" t="str">
@@ -15073,19 +15072,19 @@
         <v>68</v>
       </c>
       <c r="F97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="G97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="H97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="I97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="J97" s="1" t="str">
@@ -15125,19 +15124,19 @@
         <v>64</v>
       </c>
       <c r="F98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="G98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="H98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="I98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="J98" s="1" t="str">
@@ -15177,19 +15176,19 @@
         <v>60</v>
       </c>
       <c r="F99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="G99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="H99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="I99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="J99" s="1" t="str">
@@ -15226,19 +15225,19 @@
         <v>56</v>
       </c>
       <c r="F100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="G100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="H100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="I100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="J100" s="1" t="str">
@@ -15275,19 +15274,19 @@
         <v>52</v>
       </c>
       <c r="F101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="G101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="H101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="I101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="J101" s="1" t="str">
@@ -15324,19 +15323,19 @@
         <v>48</v>
       </c>
       <c r="F102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="G102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="H102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="I102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="J102" s="1" t="str">
@@ -15373,19 +15372,19 @@
         <v>44</v>
       </c>
       <c r="F103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="G103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="H103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="I103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="J103" s="1" t="str">
@@ -15422,19 +15421,19 @@
         <v>40</v>
       </c>
       <c r="F104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="G104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="H104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="I104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="J104" s="1" t="str">
@@ -15471,19 +15470,19 @@
         <v>36</v>
       </c>
       <c r="F105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="G105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="H105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="I105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="J105" s="1" t="str">
@@ -15523,19 +15522,19 @@
         <v>32</v>
       </c>
       <c r="F106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="G106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="H106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="I106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="J106" s="1" t="str">
@@ -15575,19 +15574,19 @@
         <v>28</v>
       </c>
       <c r="F107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J107" s="1" t="str">
@@ -15627,19 +15626,19 @@
         <v>24</v>
       </c>
       <c r="F108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J108" s="1" t="str">
@@ -15676,19 +15675,19 @@
         <v>20</v>
       </c>
       <c r="F109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="G109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="H109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="I109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="J109" s="1" t="str">
@@ -15725,19 +15724,19 @@
         <v>16</v>
       </c>
       <c r="F110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="G110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="H110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="I110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="J110" s="1" t="str">
@@ -15777,19 +15776,19 @@
         <v>12</v>
       </c>
       <c r="F111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="G111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="H111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="I111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="J111" s="1" t="str">
@@ -15826,19 +15825,19 @@
         <v>8</v>
       </c>
       <c r="F112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="G112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="H112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="I112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="J112" s="1" t="str">
@@ -15878,19 +15877,19 @@
         <v>4</v>
       </c>
       <c r="F113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J113" s="1" t="str">
@@ -15930,19 +15929,19 @@
         <v>0</v>
       </c>
       <c r="F114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="G114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="H114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="I114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="J114" s="1" t="str">
@@ -15982,19 +15981,19 @@
         <v>1853</v>
       </c>
       <c r="F115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Polycaprolactam Pellets)</v>
       </c>
       <c r="G115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Polycaprolactam Pellets)</v>
       </c>
       <c r="H115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Polycaprolactam Pellets)</v>
       </c>
       <c r="I115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Polycaprolactam Pellets)</v>
       </c>
       <c r="J115" s="1" t="str">
@@ -16034,19 +16033,19 @@
         <v>2412</v>
       </c>
       <c r="F116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="G116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="H116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="I116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="J116" s="1" t="str">
@@ -16086,19 +16085,19 @@
         <v>2416</v>
       </c>
       <c r="F117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="G117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="H117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="I117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="J117" s="1" t="str">
@@ -16135,19 +16134,19 @@
         <v>2420</v>
       </c>
       <c r="F118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (0)</v>
       </c>
       <c r="G118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (0)</v>
       </c>
       <c r="H118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (0)</v>
       </c>
       <c r="I118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (0)</v>
       </c>
       <c r="J118" s="1">
@@ -16184,19 +16183,19 @@
         <v>2424</v>
       </c>
       <c r="F119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$23, [1]Enums!$A$24)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (0)</v>
       </c>
       <c r="G119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (0)</v>
       </c>
       <c r="H119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (0)</v>
       </c>
       <c r="I119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (0)</v>
       </c>
       <c r="J119" s="1">
@@ -17176,7 +17175,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I2" s="45" t="str">
-        <f>[1]Enums!$A$132&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$134&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Steel</v>
       </c>
       <c r="J2" s="45">
@@ -17224,7 +17223,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I3" s="45" t="str">
-        <f>[1]Enums!$A$132&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$134&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Stainless Steel</v>
       </c>
       <c r="J3" s="45">
@@ -17272,7 +17271,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I4" s="45" t="str">
-        <f>[1]Enums!$A$132&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$134&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Brass</v>
       </c>
       <c r="J4" s="45">
@@ -17320,7 +17319,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I5" s="45" t="str">
-        <f>[1]Enums!$A$132&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$134&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Bronze</v>
       </c>
       <c r="J5" s="45">
@@ -17368,7 +17367,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I6" s="45" t="str">
-        <f>[1]Enums!$A$132&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$134&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Tungsten Carbide</v>
       </c>
       <c r="J6" s="45">
@@ -17416,7 +17415,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I7" s="45" t="str">
-        <f>[1]Enums!$A$132&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$134&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Nichrome</v>
       </c>
       <c r="J7" s="45">
@@ -17464,7 +17463,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I8" s="45" t="str">
-        <f>[1]Enums!$A$132&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$134&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Antimony-Lead</v>
       </c>
       <c r="J8" s="45">
@@ -17512,7 +17511,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I9" s="45" t="str">
-        <f>[1]Enums!$A$133&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Steel</v>
       </c>
       <c r="J9" s="45">
@@ -17560,7 +17559,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I10" s="45" t="str">
-        <f>[1]Enums!$A$133&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Stainless Steel</v>
       </c>
       <c r="J10" s="45">
@@ -17608,7 +17607,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I11" s="45" t="str">
-        <f>[1]Enums!$A$133&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Brass</v>
       </c>
       <c r="J11" s="45">
@@ -17656,7 +17655,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I12" s="45" t="str">
-        <f>[1]Enums!$A$133&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Bronze</v>
       </c>
       <c r="J12" s="45">
@@ -17704,7 +17703,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I13" s="45" t="str">
-        <f>[1]Enums!$A$133&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Tungsten Carbide</v>
       </c>
       <c r="J13" s="45">
@@ -17752,7 +17751,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I14" s="45" t="str">
-        <f>[1]Enums!$A$133&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Nichrome</v>
       </c>
       <c r="J14" s="45">
@@ -17800,7 +17799,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I15" s="45" t="str">
-        <f>[1]Enums!$A$133&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Antimony-Lead</v>
       </c>
       <c r="J15" s="45">
@@ -17848,7 +17847,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I16" s="45" t="str">
-        <f>[1]Enums!$A$132&amp;" Iron"</f>
+        <f>[1]Enums!$A$134&amp;" Iron"</f>
         <v>Composite Iron</v>
       </c>
       <c r="J16" s="45">
@@ -17896,7 +17895,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I17" s="45" t="str">
-        <f>[1]Enums!$A$133&amp;" Iron"</f>
+        <f>[1]Enums!$A$135&amp;" Iron"</f>
         <v>Engineered Iron</v>
       </c>
       <c r="J17" s="45">
@@ -17944,7 +17943,7 @@
         <v>Diamond</v>
       </c>
       <c r="I18" s="45" t="str">
-        <f>[1]Enums!$A$132&amp;" Diamond"</f>
+        <f>[1]Enums!$A$134&amp;" Diamond"</f>
         <v>Composite Diamond</v>
       </c>
       <c r="J18" s="45">
@@ -17992,7 +17991,7 @@
         <v>Diamond</v>
       </c>
       <c r="I19" s="45" t="str">
-        <f>[1]Enums!$A$133&amp;" Diamond"</f>
+        <f>[1]Enums!$A$135&amp;" Diamond"</f>
         <v>Engineered Diamond</v>
       </c>
       <c r="J19" s="45">
@@ -18293,7 +18292,7 @@
         <v>Molded Item</v>
       </c>
       <c r="F1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$97</f>
+        <f xml:space="preserve"> [1]Enums!$A$99</f>
         <v>Base Material</v>
       </c>
       <c r="G1" s="30" t="s">
@@ -18321,7 +18320,7 @@
         <v>1812</v>
       </c>
       <c r="C2" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D2</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D2</f>
         <v>Gripped Iron Shovel</v>
       </c>
       <c r="D2" s="24" t="str">
@@ -18333,7 +18332,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F2" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$102</f>
         <v>Iron</v>
       </c>
       <c r="G2" s="24">
@@ -18358,7 +18357,7 @@
         <v>1811</v>
       </c>
       <c r="C3" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D3</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D3</f>
         <v>Gripped Iron Pickaxe</v>
       </c>
       <c r="D3" s="21" t="str">
@@ -18370,7 +18369,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F3" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$102</f>
         <v>Iron</v>
       </c>
       <c r="G3" s="24">
@@ -18395,7 +18394,7 @@
         <v>1810</v>
       </c>
       <c r="C4" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D4</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D4</f>
         <v>Gripped Iron Axe</v>
       </c>
       <c r="D4" s="21" t="str">
@@ -18407,7 +18406,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F4" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$102</f>
         <v>Iron</v>
       </c>
       <c r="G4" s="24">
@@ -18432,7 +18431,7 @@
         <v>1809</v>
       </c>
       <c r="C5" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D5</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D5</f>
         <v>Gripped Iron Sword</v>
       </c>
       <c r="D5" s="21" t="str">
@@ -18444,7 +18443,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F5" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$102</f>
         <v>Iron</v>
       </c>
       <c r="G5" s="24">
@@ -18469,7 +18468,7 @@
         <v>1808</v>
       </c>
       <c r="C6" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D6</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D6</f>
         <v>Gripped Wooden Sword</v>
       </c>
       <c r="D6" s="21" t="str">
@@ -18481,7 +18480,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F6" s="34" t="str">
-        <f>[1]Enums!$A$98</f>
+        <f>[1]Enums!$A$100</f>
         <v>Wooden</v>
       </c>
       <c r="G6" s="24">
@@ -18506,7 +18505,7 @@
         <v>1807</v>
       </c>
       <c r="C7" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D7</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D7</f>
         <v>Gripped Wooden Shovel</v>
       </c>
       <c r="D7" s="21" t="str">
@@ -18518,7 +18517,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F7" s="34" t="str">
-        <f>[1]Enums!$A$98</f>
+        <f>[1]Enums!$A$100</f>
         <v>Wooden</v>
       </c>
       <c r="G7" s="24">
@@ -18543,7 +18542,7 @@
         <v>1806</v>
       </c>
       <c r="C8" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D8</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D8</f>
         <v>Gripped Wooden Pickaxe</v>
       </c>
       <c r="D8" s="21" t="str">
@@ -18555,7 +18554,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F8" s="34" t="str">
-        <f>[1]Enums!$A$98</f>
+        <f>[1]Enums!$A$100</f>
         <v>Wooden</v>
       </c>
       <c r="G8" s="24">
@@ -18580,7 +18579,7 @@
         <v>1805</v>
       </c>
       <c r="C9" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D9</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D9</f>
         <v>Gripped Wooden Axe</v>
       </c>
       <c r="D9" s="21" t="str">
@@ -18592,7 +18591,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F9" s="34" t="str">
-        <f>[1]Enums!$A$98</f>
+        <f>[1]Enums!$A$100</f>
         <v>Wooden</v>
       </c>
       <c r="G9" s="24">
@@ -18617,7 +18616,7 @@
         <v>1804</v>
       </c>
       <c r="C10" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D10</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D10</f>
         <v>Gripped Stone Sword</v>
       </c>
       <c r="D10" s="21" t="str">
@@ -18629,7 +18628,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F10" s="34" t="str">
-        <f>[1]Enums!$A$99</f>
+        <f>[1]Enums!$A$101</f>
         <v>Stone</v>
       </c>
       <c r="G10" s="24">
@@ -18654,7 +18653,7 @@
         <v>1803</v>
       </c>
       <c r="C11" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D11</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D11</f>
         <v>Gripped Stone Shovel</v>
       </c>
       <c r="D11" s="21" t="str">
@@ -18666,7 +18665,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F11" s="34" t="str">
-        <f>[1]Enums!$A$99</f>
+        <f>[1]Enums!$A$101</f>
         <v>Stone</v>
       </c>
       <c r="G11" s="24">
@@ -18691,7 +18690,7 @@
         <v>1802</v>
       </c>
       <c r="C12" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D12</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D12</f>
         <v>Gripped Stone Pickaxe</v>
       </c>
       <c r="D12" s="21" t="str">
@@ -18703,7 +18702,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F12" s="34" t="str">
-        <f>[1]Enums!$A$99</f>
+        <f>[1]Enums!$A$101</f>
         <v>Stone</v>
       </c>
       <c r="G12" s="24">
@@ -18728,7 +18727,7 @@
         <v>1801</v>
       </c>
       <c r="C13" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D13</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D13</f>
         <v>Gripped Stone Axe</v>
       </c>
       <c r="D13" s="21" t="str">
@@ -18740,7 +18739,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F13" s="34" t="str">
-        <f>[1]Enums!$A$99</f>
+        <f>[1]Enums!$A$101</f>
         <v>Stone</v>
       </c>
       <c r="G13" s="24">
@@ -18765,7 +18764,7 @@
         <v>1800</v>
       </c>
       <c r="C14" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D14</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D14</f>
         <v>Gripped Diamond Sword</v>
       </c>
       <c r="D14" s="21" t="str">
@@ -18777,7 +18776,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F14" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$104</f>
         <v>Diamond</v>
       </c>
       <c r="G14" s="24">
@@ -18802,7 +18801,7 @@
         <v>1799</v>
       </c>
       <c r="C15" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D15</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D15</f>
         <v>Gripped Diamond Shovel</v>
       </c>
       <c r="D15" s="21" t="str">
@@ -18814,7 +18813,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F15" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$104</f>
         <v>Diamond</v>
       </c>
       <c r="G15" s="24">
@@ -18839,7 +18838,7 @@
         <v>1798</v>
       </c>
       <c r="C16" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D16</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D16</f>
         <v>Gripped Diamond Pickaxe</v>
       </c>
       <c r="D16" s="21" t="str">
@@ -18851,7 +18850,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F16" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$104</f>
         <v>Diamond</v>
       </c>
       <c r="G16" s="24">
@@ -18876,7 +18875,7 @@
         <v>1797</v>
       </c>
       <c r="C17" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D17</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D17</f>
         <v>Gripped Diamond Axe</v>
       </c>
       <c r="D17" s="21" t="str">
@@ -18888,7 +18887,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F17" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$104</f>
         <v>Diamond</v>
       </c>
       <c r="G17" s="24">
@@ -18913,7 +18912,7 @@
         <v>1796</v>
       </c>
       <c r="C18" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D18</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D18</f>
         <v>Gripped Golden Sword</v>
       </c>
       <c r="D18" s="21" t="str">
@@ -18925,7 +18924,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F18" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$103</f>
         <v>Golden</v>
       </c>
       <c r="G18" s="24">
@@ -18950,7 +18949,7 @@
         <v>1795</v>
       </c>
       <c r="C19" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D19</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D19</f>
         <v>Gripped Golden Shovel</v>
       </c>
       <c r="D19" s="21" t="str">
@@ -18962,7 +18961,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F19" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$103</f>
         <v>Golden</v>
       </c>
       <c r="G19" s="24">
@@ -18987,7 +18986,7 @@
         <v>1794</v>
       </c>
       <c r="C20" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D20</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D20</f>
         <v>Gripped Golden Pickaxe</v>
       </c>
       <c r="D20" s="21" t="str">
@@ -18999,7 +18998,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F20" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$103</f>
         <v>Golden</v>
       </c>
       <c r="G20" s="24">
@@ -19024,7 +19023,7 @@
         <v>1793</v>
       </c>
       <c r="C21" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D21</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D21</f>
         <v>Gripped Golden Axe</v>
       </c>
       <c r="D21" s="21" t="str">
@@ -19036,7 +19035,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F21" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$103</f>
         <v>Golden</v>
       </c>
       <c r="G21" s="24">
@@ -19061,7 +19060,7 @@
         <v>1792</v>
       </c>
       <c r="C22" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D22</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D22</f>
         <v>Gripped Wooden Hoe</v>
       </c>
       <c r="D22" s="21" t="str">
@@ -19073,7 +19072,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F22" s="34" t="str">
-        <f>[1]Enums!$A$98</f>
+        <f>[1]Enums!$A$100</f>
         <v>Wooden</v>
       </c>
       <c r="G22" s="24">
@@ -19098,7 +19097,7 @@
         <v>1791</v>
       </c>
       <c r="C23" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D23</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D23</f>
         <v>Gripped Stone Hoe</v>
       </c>
       <c r="D23" s="21" t="str">
@@ -19110,7 +19109,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F23" s="34" t="str">
-        <f>[1]Enums!$A$99</f>
+        <f>[1]Enums!$A$101</f>
         <v>Stone</v>
       </c>
       <c r="G23" s="24">
@@ -19135,7 +19134,7 @@
         <v>1790</v>
       </c>
       <c r="C24" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D24</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D24</f>
         <v>Gripped Iron Hoe</v>
       </c>
       <c r="D24" s="21" t="str">
@@ -19147,7 +19146,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F24" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$102</f>
         <v>Iron</v>
       </c>
       <c r="G24" s="24">
@@ -19172,7 +19171,7 @@
         <v>1789</v>
       </c>
       <c r="C25" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D25</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D25</f>
         <v>Gripped Diamond Hoe</v>
       </c>
       <c r="D25" s="21" t="str">
@@ -19184,7 +19183,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F25" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$104</f>
         <v>Diamond</v>
       </c>
       <c r="G25" s="24">
@@ -19209,7 +19208,7 @@
         <v>1788</v>
       </c>
       <c r="C26" s="22" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;D26</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;D26</f>
         <v>Gripped Golden Hoe</v>
       </c>
       <c r="D26" s="21" t="str">
@@ -19221,7 +19220,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F26" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$103</f>
         <v>Golden</v>
       </c>
       <c r="G26" s="24">
@@ -19283,7 +19282,7 @@
         <v>1832</v>
       </c>
       <c r="D1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$97</f>
+        <f xml:space="preserve"> [1]Enums!$A$99</f>
         <v>Base Material</v>
       </c>
       <c r="E1" s="36" t="s">
@@ -19329,7 +19328,7 @@
         <v>Wooden Pogo Stick</v>
       </c>
       <c r="D2" s="34" t="str">
-        <f>[1]Enums!$A$98</f>
+        <f>[1]Enums!$A$100</f>
         <v>Wooden</v>
       </c>
       <c r="E2" s="37">
@@ -19366,7 +19365,7 @@
         <v>Stone Pogo Stick</v>
       </c>
       <c r="D3" s="34" t="str">
-        <f>[1]Enums!$A$99</f>
+        <f>[1]Enums!$A$101</f>
         <v>Stone</v>
       </c>
       <c r="E3" s="37">
@@ -19402,7 +19401,7 @@
         <v>Iron Pogo Stick</v>
       </c>
       <c r="D4" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$102</f>
         <v>Iron</v>
       </c>
       <c r="E4" s="37">
@@ -19438,7 +19437,7 @@
         <v>Golden Pogo Stick</v>
       </c>
       <c r="D5" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$103</f>
         <v>Golden</v>
       </c>
       <c r="E5" s="37">
@@ -19474,7 +19473,7 @@
         <v>Diamond Pogo Stick</v>
       </c>
       <c r="D6" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$104</f>
         <v>Diamond</v>
       </c>
       <c r="E6" s="37">
@@ -19510,7 +19509,7 @@
         <v>Magic Pogo Stick</v>
       </c>
       <c r="D7" s="34" t="str">
-        <f>[1]Enums!$A$103</f>
+        <f>[1]Enums!$A$105</f>
         <v>Magic</v>
       </c>
       <c r="E7" s="37">
@@ -19542,11 +19541,11 @@
         <v>1821</v>
       </c>
       <c r="C8" s="34" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;I8</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;I8</f>
         <v>Gripped Wooden Pogo Stick</v>
       </c>
       <c r="D8" s="34" t="str">
-        <f>[1]Enums!$A$98</f>
+        <f>[1]Enums!$A$100</f>
         <v>Wooden</v>
       </c>
       <c r="E8" s="37">
@@ -19586,11 +19585,11 @@
         <v>1820</v>
       </c>
       <c r="C9" s="34" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;I9</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;I9</f>
         <v>Gripped Stone Pogo Stick</v>
       </c>
       <c r="D9" s="34" t="str">
-        <f>[1]Enums!$A$99</f>
+        <f>[1]Enums!$A$101</f>
         <v>Stone</v>
       </c>
       <c r="E9" s="37">
@@ -19630,11 +19629,11 @@
         <v>1819</v>
       </c>
       <c r="C10" s="34" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;I10</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;I10</f>
         <v>Gripped Iron Pogo Stick</v>
       </c>
       <c r="D10" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$102</f>
         <v>Iron</v>
       </c>
       <c r="E10" s="37">
@@ -19674,11 +19673,11 @@
         <v>1818</v>
       </c>
       <c r="C11" s="34" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;I11</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;I11</f>
         <v>Gripped Golden Pogo Stick</v>
       </c>
       <c r="D11" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$103</f>
         <v>Golden</v>
       </c>
       <c r="E11" s="37">
@@ -19718,11 +19717,11 @@
         <v>1817</v>
       </c>
       <c r="C12" s="34" t="str">
-        <f>[1]Enums!$A$94&amp;" "&amp;I12</f>
+        <f>[1]Enums!$A$96&amp;" "&amp;I12</f>
         <v>Gripped Diamond Pogo Stick</v>
       </c>
       <c r="D12" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$104</f>
         <v>Diamond</v>
       </c>
       <c r="E12" s="37">
@@ -19821,7 +19820,7 @@
   </sheetPr>
   <dimension ref="A1:N115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
@@ -37804,7 +37803,7 @@
         <v>590</v>
       </c>
       <c r="D1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$71</f>
+        <f xml:space="preserve"> [1]Enums!$B$73</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="19" t="str">
@@ -37828,7 +37827,7 @@
         <v>Mold (Grip)</v>
       </c>
       <c r="D2" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E2" s="11" t="str">
@@ -37853,7 +37852,7 @@
         <v>Mold (Running Shoes)</v>
       </c>
       <c r="D3" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E3" s="11" t="str">
@@ -37878,7 +37877,7 @@
         <v>Mold (Scuba Fins)</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E4" s="11" t="str">
@@ -37903,7 +37902,7 @@
         <v>Mold (Scuba Mask)</v>
       </c>
       <c r="D5" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E5" s="11" t="str">
@@ -37928,7 +37927,7 @@
         <v>Mold (Gasket)</v>
       </c>
       <c r="D6" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E6" s="11" t="str">
@@ -37953,7 +37952,7 @@
         <v>Mold (Life Preserver)</v>
       </c>
       <c r="D7" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E7" s="11" t="str">
@@ -37978,7 +37977,7 @@
         <v>Metal Die (Fibers)</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$76</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Metal Die</v>
       </c>
       <c r="E8" s="11" t="str">
@@ -38003,7 +38002,7 @@
         <v>Metal Die (Tether)</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$76</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Metal Die</v>
       </c>
       <c r="E9" s="11" t="str">
@@ -38028,7 +38027,7 @@
         <v>Metal Die (Cord)</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$76</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Metal Die</v>
       </c>
       <c r="E10" s="11" t="str">
@@ -38053,7 +38052,7 @@
         <v>Metal Die (Hose)</v>
       </c>
       <c r="D11" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$76</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Metal Die</v>
       </c>
       <c r="E11" s="11" t="str">
@@ -38078,7 +38077,7 @@
         <v>Metal Die (Large Pipe)</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$76</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Metal Die</v>
       </c>
       <c r="E12" s="11" t="str">
@@ -38103,7 +38102,7 @@
         <v>Mold (Flashlight Shaft)</v>
       </c>
       <c r="D13" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E13" s="11" t="str">
@@ -38127,7 +38126,7 @@
         <v>Mold (Plastic Brick (1 x 1))</v>
       </c>
       <c r="D14" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E14" t="str">
@@ -38151,7 +38150,7 @@
         <v>Mold (Plastic Brick (1 x 2))</v>
       </c>
       <c r="D15" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E15" t="str">
@@ -38175,7 +38174,7 @@
         <v>Mold (Plastic Brick (1 x 3))</v>
       </c>
       <c r="D16" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E16" t="str">
@@ -38199,7 +38198,7 @@
         <v>Mold (Plastic Brick (1 x 4))</v>
       </c>
       <c r="D17" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E17" t="str">
@@ -38223,7 +38222,7 @@
         <v>Mold (Plastic Brick (2 x 2))</v>
       </c>
       <c r="D18" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E18" t="str">
@@ -38247,7 +38246,7 @@
         <v>Mold (Plastic Brick (2 x 3))</v>
       </c>
       <c r="D19" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E19" t="str">
@@ -38271,7 +38270,7 @@
         <v>Mold (Plastic Brick (2 x 4))</v>
       </c>
       <c r="D20" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E20" t="str">
@@ -38295,7 +38294,7 @@
         <v>Mold (Plastic Brick (3 x 3))</v>
       </c>
       <c r="D21" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E21" t="str">
@@ -38319,7 +38318,7 @@
         <v>Mold (Plastic Brick (3 x 4))</v>
       </c>
       <c r="D22" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E22" t="str">
@@ -38343,7 +38342,7 @@
         <v>Mold (Plastic Brick (4 x 4))</v>
       </c>
       <c r="D23" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E23" t="str">
@@ -38367,7 +38366,7 @@
         <v>Mold (Plastic Brick (1 x 8))</v>
       </c>
       <c r="D24" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E24" t="str">
@@ -38391,7 +38390,7 @@
         <v>Mold (Plastic Brick (2 x 8))</v>
       </c>
       <c r="D25" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E25" t="str">
@@ -38415,7 +38414,7 @@
         <v>Mold (Heated Knife Handle)</v>
       </c>
       <c r="D26" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E26" s="11" t="str">
@@ -38439,7 +38438,7 @@
         <v>Mold (Rubber Sole)</v>
       </c>
       <c r="D27" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E27" s="11" t="str">
@@ -38463,7 +38462,7 @@
         <v>Mold (Battery Case)</v>
       </c>
       <c r="D28" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E28" s="11" t="str">
@@ -38487,7 +38486,7 @@
         <v>Mold (Tool Shaft)</v>
       </c>
       <c r="D29" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E29" t="str">
@@ -38511,7 +38510,7 @@
         <v>Mold (Lighter Body)</v>
       </c>
       <c r="D30" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$75</f>
+        <f xml:space="preserve"> [1]Enums!$B$77</f>
         <v>Mold</v>
       </c>
       <c r="E30" t="str">
@@ -38534,8 +38533,8 @@
   </sheetPr>
   <dimension ref="A1:U156"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="G154" sqref="G154"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added new 3D textures (derrick, ind.oven, mach. mill) and updated armors and small bug fixes
</commit_message>
<xml_diff>
--- a/config/Polycraft Polymers.xlsx
+++ b/config/Polycraft Polymers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22080" yWindow="0" windowWidth="27240" windowHeight="14310" tabRatio="826" activeTab="7"/>
+    <workbookView xWindow="23940" yWindow="0" windowWidth="27240" windowHeight="14310" tabRatio="826" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Pellets" sheetId="1" r:id="rId1"/>
@@ -29889,8 +29889,8 @@
   </sheetPr>
   <dimension ref="A1:G333"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="I124" sqref="I124"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -38533,7 +38533,7 @@
   </sheetPr>
   <dimension ref="A1:U156"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView showZeros="0" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added freeze ray and water cannon
</commit_message>
<xml_diff>
--- a/config/Polycraft Polymers.xlsx
+++ b/config/Polycraft Polymers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="27240" windowHeight="14310" tabRatio="826" activeTab="7"/>
+    <workbookView xWindow="27660" yWindow="0" windowWidth="27240" windowHeight="14310" tabRatio="826"/>
   </bookViews>
   <sheets>
     <sheet name="Pellets" sheetId="1" r:id="rId1"/>
@@ -7886,108 +7886,108 @@
             <v>1.1.2</v>
           </cell>
         </row>
-        <row r="25">
-          <cell r="A25" t="str">
-            <v>Bag</v>
-          </cell>
-        </row>
         <row r="26">
           <cell r="A26" t="str">
+            <v>Bag</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27" t="str">
             <v>Vial</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28" t="str">
-            <v>Sack</v>
           </cell>
         </row>
         <row r="29">
           <cell r="A29" t="str">
+            <v>Sack</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30" t="str">
             <v>Beaker</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31" t="str">
-            <v>Powder Keg</v>
           </cell>
         </row>
         <row r="32">
           <cell r="A32" t="str">
+            <v>Powder Keg</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33" t="str">
             <v>Drum</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34" t="str">
-            <v>Chemical Silo</v>
           </cell>
         </row>
         <row r="35">
           <cell r="A35" t="str">
+            <v>Chemical Silo</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36" t="str">
             <v>Chemical Vat</v>
           </cell>
         </row>
-        <row r="73">
-          <cell r="B73" t="str">
+        <row r="74">
+          <cell r="B74" t="str">
             <v>Mold Type</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="B77" t="str">
-            <v>Mold</v>
           </cell>
         </row>
         <row r="78">
           <cell r="B78" t="str">
+            <v>Mold</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="B79" t="str">
             <v>Metal Die</v>
           </cell>
         </row>
-        <row r="96">
-          <cell r="A96" t="str">
+        <row r="97">
+          <cell r="A97" t="str">
             <v>Gripped</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="A99" t="str">
-            <v>Base Material</v>
           </cell>
         </row>
         <row r="100">
           <cell r="A100" t="str">
-            <v>Wooden</v>
+            <v>Base Material</v>
           </cell>
         </row>
         <row r="101">
           <cell r="A101" t="str">
-            <v>Stone</v>
+            <v>Wooden</v>
           </cell>
         </row>
         <row r="102">
           <cell r="A102" t="str">
-            <v>Iron</v>
+            <v>Stone</v>
           </cell>
         </row>
         <row r="103">
           <cell r="A103" t="str">
-            <v>Golden</v>
+            <v>Iron</v>
           </cell>
         </row>
         <row r="104">
           <cell r="A104" t="str">
-            <v>Diamond</v>
+            <v>Golden</v>
           </cell>
         </row>
         <row r="105">
           <cell r="A105" t="str">
+            <v>Diamond</v>
+          </cell>
+        </row>
+        <row r="106">
+          <cell r="A106" t="str">
             <v>Magic</v>
-          </cell>
-        </row>
-        <row r="134">
-          <cell r="A134" t="str">
-            <v>Composite</v>
           </cell>
         </row>
         <row r="135">
           <cell r="A135" t="str">
+            <v>Composite</v>
+          </cell>
+        </row>
+        <row r="136">
+          <cell r="A136" t="str">
             <v>Engineered</v>
           </cell>
         </row>
@@ -10149,8 +10149,8 @@
   </sheetPr>
   <dimension ref="A1:N333"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10192,19 +10192,19 @@
         <v>Game ID XL</v>
       </c>
       <c r="F1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$25&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$26&amp;" ("&amp;J1&amp;")"</f>
         <v>Bag (Pellets)</v>
       </c>
       <c r="G1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$28&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$29&amp;" ("&amp;J1&amp;")"</f>
         <v>Sack (Pellets)</v>
       </c>
       <c r="H1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$31&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$32&amp;" ("&amp;J1&amp;")"</f>
         <v>Powder Keg (Pellets)</v>
       </c>
       <c r="I1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$34&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$35&amp;" ("&amp;J1&amp;")"</f>
         <v>Chemical Silo (Pellets)</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -10240,19 +10240,19 @@
         <v>448</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="G2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="H2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="J2" s="1" t="str">
@@ -10292,19 +10292,19 @@
         <v>444</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J3" s="1" t="str">
@@ -10341,19 +10341,19 @@
         <v>440</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Alkyd Resin)</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Alkyd Resin)</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Alkyd Resin)</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Alkyd Resin)</v>
       </c>
       <c r="J4" s="1" t="str">
@@ -10393,19 +10393,19 @@
         <v>436</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J5" s="1" t="str">
@@ -10445,19 +10445,19 @@
         <v>432</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J6" s="1" t="str">
@@ -10497,19 +10497,19 @@
         <v>428</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$25, [1]Enums!$A$25)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$26, [1]Enums!$A$26)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Carbon Fiber)</v>
       </c>
       <c r="G7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$28, [1]Enums!$A$28)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$29, [1]Enums!$A$29)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Carbon Fiber)</v>
       </c>
       <c r="H7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$31, [1]Enums!$A$31)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$32, [1]Enums!$A$32)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Carbon Fiber)</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$34, [1]Enums!$A$34)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$35, [1]Enums!$A$35)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Carbon Fiber)</v>
       </c>
       <c r="J7" s="1" t="str">
@@ -10546,19 +10546,19 @@
         <v>424</v>
       </c>
       <c r="F8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="G8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="J8" s="1" t="str">
@@ -10598,19 +10598,19 @@
         <v>420</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulosic Pellets)</v>
       </c>
       <c r="G9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulosic Pellets)</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulosic Pellets)</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulosic Pellets)</v>
       </c>
       <c r="J9" s="1" t="str">
@@ -10650,19 +10650,19 @@
         <v>416</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chitin Pellets)</v>
       </c>
       <c r="G10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chitin Pellets)</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chitin Pellets)</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chitin Pellets)</v>
       </c>
       <c r="J10" s="1" t="str">
@@ -10702,19 +10702,19 @@
         <v>412</v>
       </c>
       <c r="F11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J11" s="1" t="str">
@@ -10754,19 +10754,19 @@
         <v>408</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Epoxy Resin)</v>
       </c>
       <c r="G12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Epoxy Resin)</v>
       </c>
       <c r="H12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Epoxy Resin)</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Epoxy Resin)</v>
       </c>
       <c r="J12" s="1" t="str">
@@ -10803,19 +10803,19 @@
         <v>404</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethoxylates Pellets)</v>
       </c>
       <c r="G13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethoxylates Pellets)</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethoxylates Pellets)</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethoxylates Pellets)</v>
       </c>
       <c r="J13" s="1" t="str">
@@ -10855,19 +10855,19 @@
         <v>400</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="G14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="H14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="J14" s="1" t="str">
@@ -10907,19 +10907,19 @@
         <v>396</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="G15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="J15" s="1" t="str">
@@ -10959,19 +10959,19 @@
         <v>392</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="G16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="J16" s="1" t="str">
@@ -11011,19 +11011,19 @@
         <v>388</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="G17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="J17" s="1" t="str">
@@ -11063,19 +11063,19 @@
         <v>384</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J18" s="1" t="str">
@@ -11115,19 +11115,19 @@
         <v>380</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J19" s="1" t="str">
@@ -11164,19 +11164,19 @@
         <v>376</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Lignin)</v>
       </c>
       <c r="G20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Lignin)</v>
       </c>
       <c r="H20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Lignin)</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Lignin)</v>
       </c>
       <c r="J20" s="1" t="str">
@@ -11216,19 +11216,19 @@
         <v>372</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J21" s="1" t="str">
@@ -11268,19 +11268,19 @@
         <v>368</v>
       </c>
       <c r="F22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="G22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="H22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="J22" s="1" t="str">
@@ -11320,19 +11320,19 @@
         <v>364</v>
       </c>
       <c r="F23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="G23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="H23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="J23" s="1" t="str">
@@ -11372,19 +11372,19 @@
         <v>360</v>
       </c>
       <c r="F24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="G24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="H24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="J24" s="1" t="str">
@@ -11421,19 +11421,19 @@
         <v>356</v>
       </c>
       <c r="F25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="G25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="H25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="J25" s="1" t="str">
@@ -11473,19 +11473,19 @@
         <v>352</v>
       </c>
       <c r="F26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Metaldehyde Pellets)</v>
       </c>
       <c r="G26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Metaldehyde Pellets)</v>
       </c>
       <c r="H26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Metaldehyde Pellets)</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Metaldehyde Pellets)</v>
       </c>
       <c r="J26" s="1" t="str">
@@ -11525,19 +11525,19 @@
         <v>348</v>
       </c>
       <c r="F27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J27" s="1" t="str">
@@ -11577,19 +11577,19 @@
         <v>344</v>
       </c>
       <c r="F28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraformaldehyde Pellets)</v>
       </c>
       <c r="G28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraformaldehyde Pellets)</v>
       </c>
       <c r="H28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraformaldehyde Pellets)</v>
       </c>
       <c r="I28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraformaldehyde Pellets)</v>
       </c>
       <c r="J28" s="1" t="str">
@@ -11629,19 +11629,19 @@
         <v>340</v>
       </c>
       <c r="F29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraldehyde Pellets)</v>
       </c>
       <c r="G29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraldehyde Pellets)</v>
       </c>
       <c r="H29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraldehyde Pellets)</v>
       </c>
       <c r="I29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraldehyde Pellets)</v>
       </c>
       <c r="J29" s="1" t="str">
@@ -11681,19 +11681,19 @@
         <v>336</v>
       </c>
       <c r="F30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Phenolic Resin)</v>
       </c>
       <c r="G30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Phenolic Resin)</v>
       </c>
       <c r="H30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Phenolic Resin)</v>
       </c>
       <c r="I30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Phenolic Resin)</v>
       </c>
       <c r="J30" s="1" t="str">
@@ -11733,19 +11733,19 @@
         <v>332</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="G31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="H31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="I31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="J31" s="1" t="str">
@@ -11782,19 +11782,19 @@
         <v>328</v>
       </c>
       <c r="F32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly1-Butene Pellets)</v>
       </c>
       <c r="G32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly1-Butene Pellets)</v>
       </c>
       <c r="H32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly1-Butene Pellets)</v>
       </c>
       <c r="I32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly1-Butene Pellets)</v>
       </c>
       <c r="J32" s="1" t="str">
@@ -11831,19 +11831,19 @@
         <v>324</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2,6-Dimethyl-1,4-Phenylene Ether Pellets)</v>
       </c>
       <c r="G33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2,6-Dimethyl-1,4-Phenylene Ether Pellets)</v>
       </c>
       <c r="H33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2,6-Dimethyl-1,4-Phenylene Ether Pellets)</v>
       </c>
       <c r="I33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2,6-Dimethyl-1,4-Phenylene Ether Pellets)</v>
       </c>
       <c r="J33" s="1" t="str">
@@ -11880,19 +11880,19 @@
         <v>320</v>
       </c>
       <c r="F34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="G34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="H34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="I34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="J34" s="1" t="str">
@@ -11929,19 +11929,19 @@
         <v>316</v>
       </c>
       <c r="F35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="G35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="H35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="I35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="J35" s="1" t="str">
@@ -11981,19 +11981,19 @@
         <v>312</v>
       </c>
       <c r="F36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="G36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="H36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="I36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="J36" s="1" t="str">
@@ -12033,19 +12033,19 @@
         <v>308</v>
       </c>
       <c r="F37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="G37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="H37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="I37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="J37" s="1" t="str">
@@ -12085,19 +12085,19 @@
         <v>304</v>
       </c>
       <c r="F38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="G38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="H38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="I38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="J38" s="1" t="str">
@@ -12137,19 +12137,19 @@
         <v>300</v>
       </c>
       <c r="F39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="G39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="H39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="I39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="J39" s="1" t="str">
@@ -12189,19 +12189,19 @@
         <v>296</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="G40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="H40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="I40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="J40" s="1" t="str">
@@ -12241,19 +12241,19 @@
         <v>292</v>
       </c>
       <c r="F41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="G41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="H41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="I41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="J41" s="1" t="str">
@@ -12293,19 +12293,19 @@
         <v>288</v>
       </c>
       <c r="F42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCaprolactone Pellets)</v>
       </c>
       <c r="G42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCaprolactone Pellets)</v>
       </c>
       <c r="H42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCaprolactone Pellets)</v>
       </c>
       <c r="I42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCaprolactone Pellets)</v>
       </c>
       <c r="J42" s="1" t="str">
@@ -12345,19 +12345,19 @@
         <v>284</v>
       </c>
       <c r="F43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCarbonate Pellets)</v>
       </c>
       <c r="G43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCarbonate Pellets)</v>
       </c>
       <c r="H43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCarbonate Pellets)</v>
       </c>
       <c r="I43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCarbonate Pellets)</v>
       </c>
       <c r="J43" s="1" t="str">
@@ -12394,19 +12394,19 @@
         <v>280</v>
       </c>
       <c r="F44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChloroPrene Pellets)</v>
       </c>
       <c r="G44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChloroPrene Pellets)</v>
       </c>
       <c r="H44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChloroPrene Pellets)</v>
       </c>
       <c r="I44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChloroPrene Pellets)</v>
       </c>
       <c r="J44" s="1" t="str">
@@ -12443,19 +12443,19 @@
         <v>276</v>
       </c>
       <c r="F45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="G45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="H45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="I45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="J45" s="1" t="str">
@@ -12495,19 +12495,19 @@
         <v>272</v>
       </c>
       <c r="F46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="G46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="H46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="I46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="J46" s="1" t="str">
@@ -12547,19 +12547,19 @@
         <v>268</v>
       </c>
       <c r="F47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="G47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="H47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="I47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="J47" s="1" t="str">
@@ -12599,19 +12599,19 @@
         <v>264</v>
       </c>
       <c r="F48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEtherImide Pellets)</v>
       </c>
       <c r="G48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEtherImide Pellets)</v>
       </c>
       <c r="H48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEtherImide Pellets)</v>
       </c>
       <c r="I48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEtherImide Pellets)</v>
       </c>
       <c r="J48" s="1" t="str">
@@ -12648,19 +12648,19 @@
         <v>260</v>
       </c>
       <c r="F49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="G49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="H49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="I49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="J49" s="1" t="str">
@@ -12697,19 +12697,19 @@
         <v>256</v>
       </c>
       <c r="F50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="G50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="H50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="I50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="J50" s="1" t="str">
@@ -12749,19 +12749,19 @@
         <v>252</v>
       </c>
       <c r="F51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="G51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="H51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="I51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="J51" s="1" t="str">
@@ -12798,19 +12798,19 @@
         <v>248</v>
       </c>
       <c r="F52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J52" s="1" t="str">
@@ -12850,19 +12850,19 @@
         <v>244</v>
       </c>
       <c r="F53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="G53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="H53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="I53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="J53" s="1" t="str">
@@ -12902,19 +12902,19 @@
         <v>240</v>
       </c>
       <c r="F54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="G54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="H54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="I54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="J54" s="1" t="str">
@@ -12954,19 +12954,19 @@
         <v>236</v>
       </c>
       <c r="F55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="G55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="H55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="I55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="J55" s="1" t="str">
@@ -13006,19 +13006,19 @@
         <v>232</v>
       </c>
       <c r="F56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J56" s="1" t="str">
@@ -13058,19 +13058,19 @@
         <v>228</v>
       </c>
       <c r="F57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="G57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="H57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="I57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="J57" s="1" t="str">
@@ -13110,19 +13110,19 @@
         <v>224</v>
       </c>
       <c r="F58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="G58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="H58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="I58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="J58" s="1" t="str">
@@ -13162,19 +13162,19 @@
         <v>220</v>
       </c>
       <c r="F59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="G59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="H59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="I59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="J59" s="1" t="str">
@@ -13214,19 +13214,19 @@
         <v>216</v>
       </c>
       <c r="F60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="G60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="H60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="I60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="J60" s="1" t="str">
@@ -13266,19 +13266,19 @@
         <v>212</v>
       </c>
       <c r="F61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="G61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="H61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="I61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="J61" s="1" t="str">
@@ -13315,19 +13315,19 @@
         <v>208</v>
       </c>
       <c r="F62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="G62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="H62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="I62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="J62" s="1" t="str">
@@ -13367,19 +13367,19 @@
         <v>204</v>
       </c>
       <c r="F63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyImide Pellets)</v>
       </c>
       <c r="G63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyImide Pellets)</v>
       </c>
       <c r="H63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyImide Pellets)</v>
       </c>
       <c r="I63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyImide Pellets)</v>
       </c>
       <c r="J63" s="1" t="str">
@@ -13416,19 +13416,19 @@
         <v>200</v>
       </c>
       <c r="F64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="G64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="H64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="I64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="J64" s="1" t="str">
@@ -13465,19 +13465,19 @@
         <v>196</v>
       </c>
       <c r="F65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="G65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="H65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="I65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="J65" s="1" t="str">
@@ -13517,19 +13517,19 @@
         <v>192</v>
       </c>
       <c r="F66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButylene Pellets)</v>
       </c>
       <c r="G66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButylene Pellets)</v>
       </c>
       <c r="H66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButylene Pellets)</v>
       </c>
       <c r="I66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButylene Pellets)</v>
       </c>
       <c r="J66" s="1" t="str">
@@ -13569,19 +13569,19 @@
         <v>188</v>
       </c>
       <c r="F67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoPrene Pellets)</v>
       </c>
       <c r="G67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoPrene Pellets)</v>
       </c>
       <c r="H67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoPrene Pellets)</v>
       </c>
       <c r="I67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoPrene Pellets)</v>
       </c>
       <c r="J67" s="1" t="str">
@@ -13621,19 +13621,19 @@
         <v>184</v>
       </c>
       <c r="F68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic Acid Pellets)</v>
       </c>
       <c r="G68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic Acid Pellets)</v>
       </c>
       <c r="H68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic Acid Pellets)</v>
       </c>
       <c r="I68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic Acid Pellets)</v>
       </c>
       <c r="J68" s="1" t="str">
@@ -13670,19 +13670,19 @@
         <v>180</v>
       </c>
       <c r="F69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="G69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="H69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="I69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="J69" s="1" t="str">
@@ -13719,19 +13719,19 @@
         <v>176</v>
       </c>
       <c r="F70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="G70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="H70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="I70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="J70" s="1" t="str">
@@ -13768,19 +13768,19 @@
         <v>172</v>
       </c>
       <c r="F71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="G71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="H71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="I71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="J71" s="1" t="str">
@@ -13817,19 +13817,19 @@
         <v>168</v>
       </c>
       <c r="F72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="G72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="H72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="I72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="J72" s="1" t="str">
@@ -13866,19 +13866,19 @@
         <v>164</v>
       </c>
       <c r="F73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="G73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="H73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="I73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="J73" s="1" t="str">
@@ -13918,19 +13918,19 @@
         <v>160</v>
       </c>
       <c r="F74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="G74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="H74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="I74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="J74" s="1" t="str">
@@ -13967,19 +13967,19 @@
         <v>156</v>
       </c>
       <c r="F75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J75" s="1" t="str">
@@ -14019,19 +14019,19 @@
         <v>152</v>
       </c>
       <c r="F76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyOxymethylene Pellets)</v>
       </c>
       <c r="G76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyOxymethylene Pellets)</v>
       </c>
       <c r="H76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyOxymethylene Pellets)</v>
       </c>
       <c r="I76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyOxymethylene Pellets)</v>
       </c>
       <c r="J76" s="1" t="str">
@@ -14068,19 +14068,19 @@
         <v>148</v>
       </c>
       <c r="F77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J77" s="1" t="str">
@@ -14117,19 +14117,19 @@
         <v>144</v>
       </c>
       <c r="F78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenol Pellets)</v>
       </c>
       <c r="G78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenol Pellets)</v>
       </c>
       <c r="H78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenol Pellets)</v>
       </c>
       <c r="I78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenol Pellets)</v>
       </c>
       <c r="J78" s="1" t="str">
@@ -14166,19 +14166,19 @@
         <v>140</v>
       </c>
       <c r="F79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="G79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="H79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="I79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="J79" s="1" t="str">
@@ -14215,19 +14215,19 @@
         <v>136</v>
       </c>
       <c r="F80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhosphazene Pellets)</v>
       </c>
       <c r="G80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhosphazene Pellets)</v>
       </c>
       <c r="H80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhosphazene Pellets)</v>
       </c>
       <c r="I80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhosphazene Pellets)</v>
       </c>
       <c r="J80" s="1" t="str">
@@ -14264,19 +14264,19 @@
         <v>132</v>
       </c>
       <c r="F81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="G81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="H81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="I81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="J81" s="1" t="str">
@@ -14313,19 +14313,19 @@
         <v>128</v>
       </c>
       <c r="F82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="G82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="H82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="I82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="J82" s="1" t="str">
@@ -14365,19 +14365,19 @@
         <v>124</v>
       </c>
       <c r="F83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="G83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="H83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="I83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="J83" s="1" t="str">
@@ -14417,19 +14417,19 @@
         <v>120</v>
       </c>
       <c r="F84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Pellets)</v>
       </c>
       <c r="G84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Pellets)</v>
       </c>
       <c r="H84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Pellets)</v>
       </c>
       <c r="I84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Pellets)</v>
       </c>
       <c r="J84" s="1" t="str">
@@ -14466,19 +14466,19 @@
         <v>116</v>
       </c>
       <c r="F85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="G85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="H85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="I85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="J85" s="1" t="str">
@@ -14515,19 +14515,19 @@
         <v>112</v>
       </c>
       <c r="F86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="G86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="H86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="I86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="J86" s="1" t="str">
@@ -14567,19 +14567,19 @@
         <v>108</v>
       </c>
       <c r="F87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyStyrene Pellets)</v>
       </c>
       <c r="G87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyStyrene Pellets)</v>
       </c>
       <c r="H87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyStyrene Pellets)</v>
       </c>
       <c r="I87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyStyrene Pellets)</v>
       </c>
       <c r="J87" s="1" t="str">
@@ -14616,19 +14616,19 @@
         <v>104</v>
       </c>
       <c r="F88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J88" s="1" t="str">
@@ -14668,19 +14668,19 @@
         <v>100</v>
       </c>
       <c r="F89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="G89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="H89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="I89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="J89" s="1" t="str">
@@ -14717,19 +14717,19 @@
         <v>96</v>
       </c>
       <c r="F90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="G90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="H90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="I90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="J90" s="1" t="str">
@@ -14766,19 +14766,19 @@
         <v>92</v>
       </c>
       <c r="F91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="G91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="H91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="I91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="J91" s="1" t="str">
@@ -14815,19 +14815,19 @@
         <v>88</v>
       </c>
       <c r="F92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyThiazyl Pellets)</v>
       </c>
       <c r="G92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyThiazyl Pellets)</v>
       </c>
       <c r="H92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyThiazyl Pellets)</v>
       </c>
       <c r="I92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyThiazyl Pellets)</v>
       </c>
       <c r="J92" s="1" t="str">
@@ -14867,19 +14867,19 @@
         <v>84</v>
       </c>
       <c r="F93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="G93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="H93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="I93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="J93" s="1" t="str">
@@ -14919,19 +14919,19 @@
         <v>80</v>
       </c>
       <c r="F94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyUrethane Pellets)</v>
       </c>
       <c r="G94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyUrethane Pellets)</v>
       </c>
       <c r="H94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyUrethane Pellets)</v>
       </c>
       <c r="I94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyUrethane Pellets)</v>
       </c>
       <c r="J94" s="1" t="str">
@@ -14971,19 +14971,19 @@
         <v>76</v>
       </c>
       <c r="F95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="G95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="H95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="I95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="J95" s="1" t="str">
@@ -15023,19 +15023,19 @@
         <v>72</v>
       </c>
       <c r="F96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="G96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="H96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="I96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="J96" s="1" t="str">
@@ -15072,19 +15072,19 @@
         <v>68</v>
       </c>
       <c r="F97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="G97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="H97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="I97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="J97" s="1" t="str">
@@ -15124,19 +15124,19 @@
         <v>64</v>
       </c>
       <c r="F98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="G98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="H98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="I98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="J98" s="1" t="str">
@@ -15176,19 +15176,19 @@
         <v>60</v>
       </c>
       <c r="F99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="G99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="H99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="I99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="J99" s="1" t="str">
@@ -15225,19 +15225,19 @@
         <v>56</v>
       </c>
       <c r="F100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="G100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="H100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="I100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="J100" s="1" t="str">
@@ -15274,19 +15274,19 @@
         <v>52</v>
       </c>
       <c r="F101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="G101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="H101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="I101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="J101" s="1" t="str">
@@ -15323,19 +15323,19 @@
         <v>48</v>
       </c>
       <c r="F102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="G102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="H102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="I102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="J102" s="1" t="str">
@@ -15372,19 +15372,19 @@
         <v>44</v>
       </c>
       <c r="F103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="G103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="H103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="I103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="J103" s="1" t="str">
@@ -15421,19 +15421,19 @@
         <v>40</v>
       </c>
       <c r="F104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="G104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="H104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="I104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="J104" s="1" t="str">
@@ -15470,19 +15470,19 @@
         <v>36</v>
       </c>
       <c r="F105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="G105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="H105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="I105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="J105" s="1" t="str">
@@ -15522,19 +15522,19 @@
         <v>32</v>
       </c>
       <c r="F106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="G106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="H106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="I106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="J106" s="1" t="str">
@@ -15574,19 +15574,19 @@
         <v>28</v>
       </c>
       <c r="F107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J107" s="1" t="str">
@@ -15626,19 +15626,19 @@
         <v>24</v>
       </c>
       <c r="F108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J108" s="1" t="str">
@@ -15675,19 +15675,19 @@
         <v>20</v>
       </c>
       <c r="F109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="G109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="H109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="I109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="J109" s="1" t="str">
@@ -15724,19 +15724,19 @@
         <v>16</v>
       </c>
       <c r="F110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="G110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="H110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="I110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="J110" s="1" t="str">
@@ -15776,19 +15776,19 @@
         <v>12</v>
       </c>
       <c r="F111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="G111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="H111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="I111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="J111" s="1" t="str">
@@ -15825,19 +15825,19 @@
         <v>8</v>
       </c>
       <c r="F112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="G112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="H112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="I112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="J112" s="1" t="str">
@@ -15877,19 +15877,19 @@
         <v>4</v>
       </c>
       <c r="F113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J113" s="1" t="str">
@@ -15929,19 +15929,19 @@
         <v>0</v>
       </c>
       <c r="F114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="G114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="H114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="I114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="J114" s="1" t="str">
@@ -15981,19 +15981,19 @@
         <v>1853</v>
       </c>
       <c r="F115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Polycaprolactam Pellets)</v>
       </c>
       <c r="G115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Polycaprolactam Pellets)</v>
       </c>
       <c r="H115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Polycaprolactam Pellets)</v>
       </c>
       <c r="I115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Polycaprolactam Pellets)</v>
       </c>
       <c r="J115" s="1" t="str">
@@ -16033,19 +16033,19 @@
         <v>2412</v>
       </c>
       <c r="F116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="G116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="H116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="I116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="J116" s="1" t="str">
@@ -16085,19 +16085,19 @@
         <v>2416</v>
       </c>
       <c r="F117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="G117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="H117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="I117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="J117" s="1" t="str">
@@ -16134,19 +16134,19 @@
         <v>2420</v>
       </c>
       <c r="F118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (0)</v>
       </c>
       <c r="G118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (0)</v>
       </c>
       <c r="H118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (0)</v>
       </c>
       <c r="I118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (0)</v>
       </c>
       <c r="J118" s="1">
@@ -16183,19 +16183,19 @@
         <v>2424</v>
       </c>
       <c r="F119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$25, [1]Enums!$A$26)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (0)</v>
       </c>
       <c r="G119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$28, [1]Enums!$A$29)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (0)</v>
       </c>
       <c r="H119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (0)</v>
       </c>
       <c r="I119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (0)</v>
       </c>
       <c r="J119" s="1">
@@ -17175,7 +17175,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I2" s="45" t="str">
-        <f>[1]Enums!$A$134&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Steel</v>
       </c>
       <c r="J2" s="45">
@@ -17223,7 +17223,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I3" s="45" t="str">
-        <f>[1]Enums!$A$134&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Stainless Steel</v>
       </c>
       <c r="J3" s="45">
@@ -17271,7 +17271,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I4" s="45" t="str">
-        <f>[1]Enums!$A$134&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Brass</v>
       </c>
       <c r="J4" s="45">
@@ -17319,7 +17319,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I5" s="45" t="str">
-        <f>[1]Enums!$A$134&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Bronze</v>
       </c>
       <c r="J5" s="45">
@@ -17367,7 +17367,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I6" s="45" t="str">
-        <f>[1]Enums!$A$134&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Tungsten Carbide</v>
       </c>
       <c r="J6" s="45">
@@ -17415,7 +17415,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I7" s="45" t="str">
-        <f>[1]Enums!$A$134&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Nichrome</v>
       </c>
       <c r="J7" s="45">
@@ -17463,7 +17463,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I8" s="45" t="str">
-        <f>[1]Enums!$A$134&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Antimony-Lead</v>
       </c>
       <c r="J8" s="45">
@@ -17511,7 +17511,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I9" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Steel</v>
       </c>
       <c r="J9" s="45">
@@ -17559,7 +17559,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I10" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Stainless Steel</v>
       </c>
       <c r="J10" s="45">
@@ -17607,7 +17607,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I11" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Brass</v>
       </c>
       <c r="J11" s="45">
@@ -17655,7 +17655,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I12" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Bronze</v>
       </c>
       <c r="J12" s="45">
@@ -17703,7 +17703,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I13" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Tungsten Carbide</v>
       </c>
       <c r="J13" s="45">
@@ -17751,7 +17751,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I14" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Nichrome</v>
       </c>
       <c r="J14" s="45">
@@ -17799,7 +17799,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I15" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Antimony-Lead</v>
       </c>
       <c r="J15" s="45">
@@ -17847,7 +17847,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I16" s="45" t="str">
-        <f>[1]Enums!$A$134&amp;" Iron"</f>
+        <f>[1]Enums!$A$135&amp;" Iron"</f>
         <v>Composite Iron</v>
       </c>
       <c r="J16" s="45">
@@ -17895,7 +17895,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I17" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" Iron"</f>
+        <f>[1]Enums!$A$136&amp;" Iron"</f>
         <v>Engineered Iron</v>
       </c>
       <c r="J17" s="45">
@@ -17943,7 +17943,7 @@
         <v>Diamond</v>
       </c>
       <c r="I18" s="45" t="str">
-        <f>[1]Enums!$A$134&amp;" Diamond"</f>
+        <f>[1]Enums!$A$135&amp;" Diamond"</f>
         <v>Composite Diamond</v>
       </c>
       <c r="J18" s="45">
@@ -17991,7 +17991,7 @@
         <v>Diamond</v>
       </c>
       <c r="I19" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" Diamond"</f>
+        <f>[1]Enums!$A$136&amp;" Diamond"</f>
         <v>Engineered Diamond</v>
       </c>
       <c r="J19" s="45">
@@ -18292,7 +18292,7 @@
         <v>Molded Item</v>
       </c>
       <c r="F1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$99</f>
+        <f xml:space="preserve"> [1]Enums!$A$100</f>
         <v>Base Material</v>
       </c>
       <c r="G1" s="30" t="s">
@@ -18320,7 +18320,7 @@
         <v>1812</v>
       </c>
       <c r="C2" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D2</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D2</f>
         <v>Gripped Iron Shovel</v>
       </c>
       <c r="D2" s="24" t="str">
@@ -18332,7 +18332,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F2" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$103</f>
         <v>Iron</v>
       </c>
       <c r="G2" s="24">
@@ -18357,7 +18357,7 @@
         <v>1811</v>
       </c>
       <c r="C3" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D3</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D3</f>
         <v>Gripped Iron Pickaxe</v>
       </c>
       <c r="D3" s="21" t="str">
@@ -18369,7 +18369,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F3" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$103</f>
         <v>Iron</v>
       </c>
       <c r="G3" s="24">
@@ -18394,7 +18394,7 @@
         <v>1810</v>
       </c>
       <c r="C4" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D4</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D4</f>
         <v>Gripped Iron Axe</v>
       </c>
       <c r="D4" s="21" t="str">
@@ -18406,7 +18406,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F4" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$103</f>
         <v>Iron</v>
       </c>
       <c r="G4" s="24">
@@ -18431,7 +18431,7 @@
         <v>1809</v>
       </c>
       <c r="C5" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D5</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D5</f>
         <v>Gripped Iron Sword</v>
       </c>
       <c r="D5" s="21" t="str">
@@ -18443,7 +18443,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F5" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$103</f>
         <v>Iron</v>
       </c>
       <c r="G5" s="24">
@@ -18468,7 +18468,7 @@
         <v>1808</v>
       </c>
       <c r="C6" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D6</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D6</f>
         <v>Gripped Wooden Sword</v>
       </c>
       <c r="D6" s="21" t="str">
@@ -18480,7 +18480,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F6" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$101</f>
         <v>Wooden</v>
       </c>
       <c r="G6" s="24">
@@ -18505,7 +18505,7 @@
         <v>1807</v>
       </c>
       <c r="C7" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D7</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D7</f>
         <v>Gripped Wooden Shovel</v>
       </c>
       <c r="D7" s="21" t="str">
@@ -18517,7 +18517,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F7" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$101</f>
         <v>Wooden</v>
       </c>
       <c r="G7" s="24">
@@ -18542,7 +18542,7 @@
         <v>1806</v>
       </c>
       <c r="C8" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D8</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D8</f>
         <v>Gripped Wooden Pickaxe</v>
       </c>
       <c r="D8" s="21" t="str">
@@ -18554,7 +18554,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F8" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$101</f>
         <v>Wooden</v>
       </c>
       <c r="G8" s="24">
@@ -18579,7 +18579,7 @@
         <v>1805</v>
       </c>
       <c r="C9" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D9</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D9</f>
         <v>Gripped Wooden Axe</v>
       </c>
       <c r="D9" s="21" t="str">
@@ -18591,7 +18591,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F9" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$101</f>
         <v>Wooden</v>
       </c>
       <c r="G9" s="24">
@@ -18616,7 +18616,7 @@
         <v>1804</v>
       </c>
       <c r="C10" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D10</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D10</f>
         <v>Gripped Stone Sword</v>
       </c>
       <c r="D10" s="21" t="str">
@@ -18628,7 +18628,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F10" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$102</f>
         <v>Stone</v>
       </c>
       <c r="G10" s="24">
@@ -18653,7 +18653,7 @@
         <v>1803</v>
       </c>
       <c r="C11" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D11</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D11</f>
         <v>Gripped Stone Shovel</v>
       </c>
       <c r="D11" s="21" t="str">
@@ -18665,7 +18665,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F11" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$102</f>
         <v>Stone</v>
       </c>
       <c r="G11" s="24">
@@ -18690,7 +18690,7 @@
         <v>1802</v>
       </c>
       <c r="C12" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D12</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D12</f>
         <v>Gripped Stone Pickaxe</v>
       </c>
       <c r="D12" s="21" t="str">
@@ -18702,7 +18702,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F12" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$102</f>
         <v>Stone</v>
       </c>
       <c r="G12" s="24">
@@ -18727,7 +18727,7 @@
         <v>1801</v>
       </c>
       <c r="C13" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D13</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D13</f>
         <v>Gripped Stone Axe</v>
       </c>
       <c r="D13" s="21" t="str">
@@ -18739,7 +18739,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F13" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$102</f>
         <v>Stone</v>
       </c>
       <c r="G13" s="24">
@@ -18764,7 +18764,7 @@
         <v>1800</v>
       </c>
       <c r="C14" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D14</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D14</f>
         <v>Gripped Diamond Sword</v>
       </c>
       <c r="D14" s="21" t="str">
@@ -18776,7 +18776,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F14" s="34" t="str">
-        <f>[1]Enums!$A$104</f>
+        <f>[1]Enums!$A$105</f>
         <v>Diamond</v>
       </c>
       <c r="G14" s="24">
@@ -18801,7 +18801,7 @@
         <v>1799</v>
       </c>
       <c r="C15" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D15</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D15</f>
         <v>Gripped Diamond Shovel</v>
       </c>
       <c r="D15" s="21" t="str">
@@ -18813,7 +18813,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F15" s="34" t="str">
-        <f>[1]Enums!$A$104</f>
+        <f>[1]Enums!$A$105</f>
         <v>Diamond</v>
       </c>
       <c r="G15" s="24">
@@ -18838,7 +18838,7 @@
         <v>1798</v>
       </c>
       <c r="C16" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D16</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D16</f>
         <v>Gripped Diamond Pickaxe</v>
       </c>
       <c r="D16" s="21" t="str">
@@ -18850,7 +18850,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F16" s="34" t="str">
-        <f>[1]Enums!$A$104</f>
+        <f>[1]Enums!$A$105</f>
         <v>Diamond</v>
       </c>
       <c r="G16" s="24">
@@ -18875,7 +18875,7 @@
         <v>1797</v>
       </c>
       <c r="C17" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D17</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D17</f>
         <v>Gripped Diamond Axe</v>
       </c>
       <c r="D17" s="21" t="str">
@@ -18887,7 +18887,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F17" s="34" t="str">
-        <f>[1]Enums!$A$104</f>
+        <f>[1]Enums!$A$105</f>
         <v>Diamond</v>
       </c>
       <c r="G17" s="24">
@@ -18912,7 +18912,7 @@
         <v>1796</v>
       </c>
       <c r="C18" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D18</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D18</f>
         <v>Gripped Golden Sword</v>
       </c>
       <c r="D18" s="21" t="str">
@@ -18924,7 +18924,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F18" s="34" t="str">
-        <f>[1]Enums!$A$103</f>
+        <f>[1]Enums!$A$104</f>
         <v>Golden</v>
       </c>
       <c r="G18" s="24">
@@ -18949,7 +18949,7 @@
         <v>1795</v>
       </c>
       <c r="C19" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D19</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D19</f>
         <v>Gripped Golden Shovel</v>
       </c>
       <c r="D19" s="21" t="str">
@@ -18961,7 +18961,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F19" s="34" t="str">
-        <f>[1]Enums!$A$103</f>
+        <f>[1]Enums!$A$104</f>
         <v>Golden</v>
       </c>
       <c r="G19" s="24">
@@ -18986,7 +18986,7 @@
         <v>1794</v>
       </c>
       <c r="C20" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D20</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D20</f>
         <v>Gripped Golden Pickaxe</v>
       </c>
       <c r="D20" s="21" t="str">
@@ -18998,7 +18998,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F20" s="34" t="str">
-        <f>[1]Enums!$A$103</f>
+        <f>[1]Enums!$A$104</f>
         <v>Golden</v>
       </c>
       <c r="G20" s="24">
@@ -19023,7 +19023,7 @@
         <v>1793</v>
       </c>
       <c r="C21" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D21</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D21</f>
         <v>Gripped Golden Axe</v>
       </c>
       <c r="D21" s="21" t="str">
@@ -19035,7 +19035,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F21" s="34" t="str">
-        <f>[1]Enums!$A$103</f>
+        <f>[1]Enums!$A$104</f>
         <v>Golden</v>
       </c>
       <c r="G21" s="24">
@@ -19060,7 +19060,7 @@
         <v>1792</v>
       </c>
       <c r="C22" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D22</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D22</f>
         <v>Gripped Wooden Hoe</v>
       </c>
       <c r="D22" s="21" t="str">
@@ -19072,7 +19072,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F22" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$101</f>
         <v>Wooden</v>
       </c>
       <c r="G22" s="24">
@@ -19097,7 +19097,7 @@
         <v>1791</v>
       </c>
       <c r="C23" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D23</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D23</f>
         <v>Gripped Stone Hoe</v>
       </c>
       <c r="D23" s="21" t="str">
@@ -19109,7 +19109,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F23" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$102</f>
         <v>Stone</v>
       </c>
       <c r="G23" s="24">
@@ -19134,7 +19134,7 @@
         <v>1790</v>
       </c>
       <c r="C24" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D24</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D24</f>
         <v>Gripped Iron Hoe</v>
       </c>
       <c r="D24" s="21" t="str">
@@ -19146,7 +19146,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F24" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$103</f>
         <v>Iron</v>
       </c>
       <c r="G24" s="24">
@@ -19171,7 +19171,7 @@
         <v>1789</v>
       </c>
       <c r="C25" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D25</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D25</f>
         <v>Gripped Diamond Hoe</v>
       </c>
       <c r="D25" s="21" t="str">
@@ -19183,7 +19183,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F25" s="34" t="str">
-        <f>[1]Enums!$A$104</f>
+        <f>[1]Enums!$A$105</f>
         <v>Diamond</v>
       </c>
       <c r="G25" s="24">
@@ -19208,7 +19208,7 @@
         <v>1788</v>
       </c>
       <c r="C26" s="22" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;D26</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;D26</f>
         <v>Gripped Golden Hoe</v>
       </c>
       <c r="D26" s="21" t="str">
@@ -19220,7 +19220,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F26" s="34" t="str">
-        <f>[1]Enums!$A$103</f>
+        <f>[1]Enums!$A$104</f>
         <v>Golden</v>
       </c>
       <c r="G26" s="24">
@@ -19282,7 +19282,7 @@
         <v>1832</v>
       </c>
       <c r="D1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$99</f>
+        <f xml:space="preserve"> [1]Enums!$A$100</f>
         <v>Base Material</v>
       </c>
       <c r="E1" s="36" t="s">
@@ -19328,7 +19328,7 @@
         <v>Wooden Pogo Stick</v>
       </c>
       <c r="D2" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$101</f>
         <v>Wooden</v>
       </c>
       <c r="E2" s="37">
@@ -19365,7 +19365,7 @@
         <v>Stone Pogo Stick</v>
       </c>
       <c r="D3" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$102</f>
         <v>Stone</v>
       </c>
       <c r="E3" s="37">
@@ -19401,7 +19401,7 @@
         <v>Iron Pogo Stick</v>
       </c>
       <c r="D4" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$103</f>
         <v>Iron</v>
       </c>
       <c r="E4" s="37">
@@ -19437,7 +19437,7 @@
         <v>Golden Pogo Stick</v>
       </c>
       <c r="D5" s="34" t="str">
-        <f>[1]Enums!$A$103</f>
+        <f>[1]Enums!$A$104</f>
         <v>Golden</v>
       </c>
       <c r="E5" s="37">
@@ -19473,7 +19473,7 @@
         <v>Diamond Pogo Stick</v>
       </c>
       <c r="D6" s="34" t="str">
-        <f>[1]Enums!$A$104</f>
+        <f>[1]Enums!$A$105</f>
         <v>Diamond</v>
       </c>
       <c r="E6" s="37">
@@ -19509,7 +19509,7 @@
         <v>Magic Pogo Stick</v>
       </c>
       <c r="D7" s="34" t="str">
-        <f>[1]Enums!$A$105</f>
+        <f>[1]Enums!$A$106</f>
         <v>Magic</v>
       </c>
       <c r="E7" s="37">
@@ -19541,11 +19541,11 @@
         <v>1821</v>
       </c>
       <c r="C8" s="34" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;I8</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;I8</f>
         <v>Gripped Wooden Pogo Stick</v>
       </c>
       <c r="D8" s="34" t="str">
-        <f>[1]Enums!$A$100</f>
+        <f>[1]Enums!$A$101</f>
         <v>Wooden</v>
       </c>
       <c r="E8" s="37">
@@ -19585,11 +19585,11 @@
         <v>1820</v>
       </c>
       <c r="C9" s="34" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;I9</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;I9</f>
         <v>Gripped Stone Pogo Stick</v>
       </c>
       <c r="D9" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$102</f>
         <v>Stone</v>
       </c>
       <c r="E9" s="37">
@@ -19629,11 +19629,11 @@
         <v>1819</v>
       </c>
       <c r="C10" s="34" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;I10</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;I10</f>
         <v>Gripped Iron Pogo Stick</v>
       </c>
       <c r="D10" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$103</f>
         <v>Iron</v>
       </c>
       <c r="E10" s="37">
@@ -19673,11 +19673,11 @@
         <v>1818</v>
       </c>
       <c r="C11" s="34" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;I11</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;I11</f>
         <v>Gripped Golden Pogo Stick</v>
       </c>
       <c r="D11" s="34" t="str">
-        <f>[1]Enums!$A$103</f>
+        <f>[1]Enums!$A$104</f>
         <v>Golden</v>
       </c>
       <c r="E11" s="37">
@@ -19717,11 +19717,11 @@
         <v>1817</v>
       </c>
       <c r="C12" s="34" t="str">
-        <f>[1]Enums!$A$96&amp;" "&amp;I12</f>
+        <f>[1]Enums!$A$97&amp;" "&amp;I12</f>
         <v>Gripped Diamond Pogo Stick</v>
       </c>
       <c r="D12" s="34" t="str">
-        <f>[1]Enums!$A$104</f>
+        <f>[1]Enums!$A$105</f>
         <v>Diamond</v>
       </c>
       <c r="E12" s="37">
@@ -37803,7 +37803,7 @@
         <v>590</v>
       </c>
       <c r="D1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$73</f>
+        <f xml:space="preserve"> [1]Enums!$B$74</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="19" t="str">
@@ -37827,7 +37827,7 @@
         <v>Mold (Grip)</v>
       </c>
       <c r="D2" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E2" s="11" t="str">
@@ -37852,7 +37852,7 @@
         <v>Mold (Running Shoes)</v>
       </c>
       <c r="D3" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E3" s="11" t="str">
@@ -37877,7 +37877,7 @@
         <v>Mold (Scuba Fins)</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E4" s="11" t="str">
@@ -37902,7 +37902,7 @@
         <v>Mold (Scuba Mask)</v>
       </c>
       <c r="D5" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E5" s="11" t="str">
@@ -37927,7 +37927,7 @@
         <v>Mold (Gasket)</v>
       </c>
       <c r="D6" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E6" s="11" t="str">
@@ -37952,7 +37952,7 @@
         <v>Mold (Life Preserver)</v>
       </c>
       <c r="D7" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E7" s="11" t="str">
@@ -37977,7 +37977,7 @@
         <v>Metal Die (Fibers)</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Metal Die</v>
       </c>
       <c r="E8" s="11" t="str">
@@ -38002,7 +38002,7 @@
         <v>Metal Die (Tether)</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Metal Die</v>
       </c>
       <c r="E9" s="11" t="str">
@@ -38027,7 +38027,7 @@
         <v>Metal Die (Cord)</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Metal Die</v>
       </c>
       <c r="E10" s="11" t="str">
@@ -38052,7 +38052,7 @@
         <v>Metal Die (Hose)</v>
       </c>
       <c r="D11" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Metal Die</v>
       </c>
       <c r="E11" s="11" t="str">
@@ -38077,7 +38077,7 @@
         <v>Metal Die (Pipe Segment)</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Metal Die</v>
       </c>
       <c r="E12" s="11" t="str">
@@ -38102,7 +38102,7 @@
         <v>Mold (Flashlight Shaft)</v>
       </c>
       <c r="D13" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E13" s="11" t="str">
@@ -38126,7 +38126,7 @@
         <v>Mold (Plastic Brick (1 x 1))</v>
       </c>
       <c r="D14" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E14" t="str">
@@ -38150,7 +38150,7 @@
         <v>Mold (Plastic Brick (1 x 2))</v>
       </c>
       <c r="D15" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E15" t="str">
@@ -38174,7 +38174,7 @@
         <v>Mold (Plastic Brick (1 x 3))</v>
       </c>
       <c r="D16" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E16" t="str">
@@ -38198,7 +38198,7 @@
         <v>Mold (Plastic Brick (1 x 4))</v>
       </c>
       <c r="D17" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E17" t="str">
@@ -38222,7 +38222,7 @@
         <v>Mold (Plastic Brick (2 x 2))</v>
       </c>
       <c r="D18" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E18" t="str">
@@ -38246,7 +38246,7 @@
         <v>Mold (Plastic Brick (2 x 3))</v>
       </c>
       <c r="D19" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E19" t="str">
@@ -38270,7 +38270,7 @@
         <v>Mold (Plastic Brick (2 x 4))</v>
       </c>
       <c r="D20" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E20" t="str">
@@ -38294,7 +38294,7 @@
         <v>Mold (Plastic Brick (3 x 3))</v>
       </c>
       <c r="D21" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E21" t="str">
@@ -38318,7 +38318,7 @@
         <v>Mold (Plastic Brick (3 x 4))</v>
       </c>
       <c r="D22" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E22" t="str">
@@ -38342,7 +38342,7 @@
         <v>Mold (Plastic Brick (4 x 4))</v>
       </c>
       <c r="D23" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E23" t="str">
@@ -38366,7 +38366,7 @@
         <v>Mold (Plastic Brick (1 x 8))</v>
       </c>
       <c r="D24" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E24" t="str">
@@ -38390,7 +38390,7 @@
         <v>Mold (Plastic Brick (2 x 8))</v>
       </c>
       <c r="D25" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E25" t="str">
@@ -38414,7 +38414,7 @@
         <v>Mold (Heated Knife Handle)</v>
       </c>
       <c r="D26" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E26" s="11" t="str">
@@ -38438,7 +38438,7 @@
         <v>Mold (Rubber Sole)</v>
       </c>
       <c r="D27" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E27" s="11" t="str">
@@ -38462,7 +38462,7 @@
         <v>Mold (Battery Case)</v>
       </c>
       <c r="D28" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E28" s="11" t="str">
@@ -38486,7 +38486,7 @@
         <v>Mold (Tool Shaft)</v>
       </c>
       <c r="D29" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E29" t="str">
@@ -38510,7 +38510,7 @@
         <v>Mold (Lighter Body)</v>
       </c>
       <c r="D30" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$77</f>
+        <f xml:space="preserve"> [1]Enums!$B$78</f>
         <v>Mold</v>
       </c>
       <c r="E30" t="str">
@@ -38533,8 +38533,8 @@
   </sheetPr>
   <dimension ref="A1:U156"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:D30"/>
+    <sheetView showZeros="0" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="E152" sqref="E152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added Flood Light and Gaslamp
</commit_message>
<xml_diff>
--- a/config/Polycraft Polymers.xlsx
+++ b/config/Polycraft Polymers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27660" yWindow="0" windowWidth="27240" windowHeight="14310" tabRatio="826"/>
+    <workbookView xWindow="28590" yWindow="0" windowWidth="27240" windowHeight="14310" tabRatio="826"/>
   </bookViews>
   <sheets>
     <sheet name="Pellets" sheetId="1" r:id="rId1"/>
@@ -7886,108 +7886,108 @@
             <v>1.1.2</v>
           </cell>
         </row>
-        <row r="26">
-          <cell r="A26" t="str">
-            <v>Bag</v>
-          </cell>
-        </row>
         <row r="27">
           <cell r="A27" t="str">
+            <v>Bag</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
             <v>Vial</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29" t="str">
-            <v>Sack</v>
           </cell>
         </row>
         <row r="30">
           <cell r="A30" t="str">
+            <v>Sack</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
             <v>Beaker</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32" t="str">
-            <v>Powder Keg</v>
           </cell>
         </row>
         <row r="33">
           <cell r="A33" t="str">
+            <v>Powder Keg</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34" t="str">
             <v>Drum</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35" t="str">
-            <v>Chemical Silo</v>
           </cell>
         </row>
         <row r="36">
           <cell r="A36" t="str">
+            <v>Chemical Silo</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37" t="str">
             <v>Chemical Vat</v>
           </cell>
         </row>
-        <row r="74">
-          <cell r="B74" t="str">
+        <row r="75">
+          <cell r="B75" t="str">
             <v>Mold Type</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="B78" t="str">
-            <v>Mold</v>
           </cell>
         </row>
         <row r="79">
           <cell r="B79" t="str">
+            <v>Mold</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="B80" t="str">
             <v>Metal Die</v>
           </cell>
         </row>
-        <row r="97">
-          <cell r="A97" t="str">
+        <row r="98">
+          <cell r="A98" t="str">
             <v>Gripped</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="A100" t="str">
-            <v>Base Material</v>
           </cell>
         </row>
         <row r="101">
           <cell r="A101" t="str">
-            <v>Wooden</v>
+            <v>Base Material</v>
           </cell>
         </row>
         <row r="102">
           <cell r="A102" t="str">
-            <v>Stone</v>
+            <v>Wooden</v>
           </cell>
         </row>
         <row r="103">
           <cell r="A103" t="str">
-            <v>Iron</v>
+            <v>Stone</v>
           </cell>
         </row>
         <row r="104">
           <cell r="A104" t="str">
-            <v>Golden</v>
+            <v>Iron</v>
           </cell>
         </row>
         <row r="105">
           <cell r="A105" t="str">
-            <v>Diamond</v>
+            <v>Golden</v>
           </cell>
         </row>
         <row r="106">
           <cell r="A106" t="str">
+            <v>Diamond</v>
+          </cell>
+        </row>
+        <row r="107">
+          <cell r="A107" t="str">
             <v>Magic</v>
-          </cell>
-        </row>
-        <row r="135">
-          <cell r="A135" t="str">
-            <v>Composite</v>
           </cell>
         </row>
         <row r="136">
           <cell r="A136" t="str">
+            <v>Composite</v>
+          </cell>
+        </row>
+        <row r="137">
+          <cell r="A137" t="str">
             <v>Engineered</v>
           </cell>
         </row>
@@ -10192,19 +10192,19 @@
         <v>Game ID XL</v>
       </c>
       <c r="F1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$26&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$27&amp;" ("&amp;J1&amp;")"</f>
         <v>Bag (Pellets)</v>
       </c>
       <c r="G1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$29&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$30&amp;" ("&amp;J1&amp;")"</f>
         <v>Sack (Pellets)</v>
       </c>
       <c r="H1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$32&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$33&amp;" ("&amp;J1&amp;")"</f>
         <v>Powder Keg (Pellets)</v>
       </c>
       <c r="I1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$35&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$36&amp;" ("&amp;J1&amp;")"</f>
         <v>Chemical Silo (Pellets)</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -10240,19 +10240,19 @@
         <v>448</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="G2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="H2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="J2" s="1" t="str">
@@ -10292,19 +10292,19 @@
         <v>444</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J3" s="1" t="str">
@@ -10341,19 +10341,19 @@
         <v>440</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Alkyd Resin)</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Alkyd Resin)</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Alkyd Resin)</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Alkyd Resin)</v>
       </c>
       <c r="J4" s="1" t="str">
@@ -10393,19 +10393,19 @@
         <v>436</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J5" s="1" t="str">
@@ -10445,19 +10445,19 @@
         <v>432</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J6" s="1" t="str">
@@ -10497,19 +10497,19 @@
         <v>428</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$26, [1]Enums!$A$26)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$27, [1]Enums!$A$27)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Carbon Fiber)</v>
       </c>
       <c r="G7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$29, [1]Enums!$A$29)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$30, [1]Enums!$A$30)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Carbon Fiber)</v>
       </c>
       <c r="H7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$32, [1]Enums!$A$32)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$33, [1]Enums!$A$33)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Carbon Fiber)</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$35, [1]Enums!$A$35)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$36, [1]Enums!$A$36)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Carbon Fiber)</v>
       </c>
       <c r="J7" s="1" t="str">
@@ -10546,19 +10546,19 @@
         <v>424</v>
       </c>
       <c r="F8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="G8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="J8" s="1" t="str">
@@ -10598,19 +10598,19 @@
         <v>420</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulosic Pellets)</v>
       </c>
       <c r="G9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulosic Pellets)</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulosic Pellets)</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulosic Pellets)</v>
       </c>
       <c r="J9" s="1" t="str">
@@ -10650,19 +10650,19 @@
         <v>416</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chitin Pellets)</v>
       </c>
       <c r="G10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chitin Pellets)</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chitin Pellets)</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chitin Pellets)</v>
       </c>
       <c r="J10" s="1" t="str">
@@ -10702,19 +10702,19 @@
         <v>412</v>
       </c>
       <c r="F11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J11" s="1" t="str">
@@ -10754,19 +10754,19 @@
         <v>408</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Epoxy Resin)</v>
       </c>
       <c r="G12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Epoxy Resin)</v>
       </c>
       <c r="H12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Epoxy Resin)</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Epoxy Resin)</v>
       </c>
       <c r="J12" s="1" t="str">
@@ -10803,19 +10803,19 @@
         <v>404</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethoxylates Pellets)</v>
       </c>
       <c r="G13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethoxylates Pellets)</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethoxylates Pellets)</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethoxylates Pellets)</v>
       </c>
       <c r="J13" s="1" t="str">
@@ -10855,19 +10855,19 @@
         <v>400</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="G14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="H14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="J14" s="1" t="str">
@@ -10907,19 +10907,19 @@
         <v>396</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="G15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="J15" s="1" t="str">
@@ -10959,19 +10959,19 @@
         <v>392</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="G16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="J16" s="1" t="str">
@@ -11011,19 +11011,19 @@
         <v>388</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="G17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="J17" s="1" t="str">
@@ -11063,19 +11063,19 @@
         <v>384</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J18" s="1" t="str">
@@ -11115,19 +11115,19 @@
         <v>380</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J19" s="1" t="str">
@@ -11164,19 +11164,19 @@
         <v>376</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Lignin)</v>
       </c>
       <c r="G20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Lignin)</v>
       </c>
       <c r="H20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Lignin)</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Lignin)</v>
       </c>
       <c r="J20" s="1" t="str">
@@ -11216,19 +11216,19 @@
         <v>372</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J21" s="1" t="str">
@@ -11268,19 +11268,19 @@
         <v>368</v>
       </c>
       <c r="F22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="G22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="H22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="J22" s="1" t="str">
@@ -11320,19 +11320,19 @@
         <v>364</v>
       </c>
       <c r="F23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="G23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="H23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="J23" s="1" t="str">
@@ -11372,19 +11372,19 @@
         <v>360</v>
       </c>
       <c r="F24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="G24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="H24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="J24" s="1" t="str">
@@ -11421,19 +11421,19 @@
         <v>356</v>
       </c>
       <c r="F25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="G25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="H25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="J25" s="1" t="str">
@@ -11473,19 +11473,19 @@
         <v>352</v>
       </c>
       <c r="F26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Metaldehyde Pellets)</v>
       </c>
       <c r="G26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Metaldehyde Pellets)</v>
       </c>
       <c r="H26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Metaldehyde Pellets)</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Metaldehyde Pellets)</v>
       </c>
       <c r="J26" s="1" t="str">
@@ -11525,19 +11525,19 @@
         <v>348</v>
       </c>
       <c r="F27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J27" s="1" t="str">
@@ -11577,19 +11577,19 @@
         <v>344</v>
       </c>
       <c r="F28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraformaldehyde Pellets)</v>
       </c>
       <c r="G28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraformaldehyde Pellets)</v>
       </c>
       <c r="H28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraformaldehyde Pellets)</v>
       </c>
       <c r="I28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraformaldehyde Pellets)</v>
       </c>
       <c r="J28" s="1" t="str">
@@ -11629,19 +11629,19 @@
         <v>340</v>
       </c>
       <c r="F29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraldehyde Pellets)</v>
       </c>
       <c r="G29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraldehyde Pellets)</v>
       </c>
       <c r="H29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraldehyde Pellets)</v>
       </c>
       <c r="I29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraldehyde Pellets)</v>
       </c>
       <c r="J29" s="1" t="str">
@@ -11681,19 +11681,19 @@
         <v>336</v>
       </c>
       <c r="F30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Phenolic Resin)</v>
       </c>
       <c r="G30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Phenolic Resin)</v>
       </c>
       <c r="H30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Phenolic Resin)</v>
       </c>
       <c r="I30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Phenolic Resin)</v>
       </c>
       <c r="J30" s="1" t="str">
@@ -11733,19 +11733,19 @@
         <v>332</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="G31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="H31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="I31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="J31" s="1" t="str">
@@ -11782,19 +11782,19 @@
         <v>328</v>
       </c>
       <c r="F32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly1-Butene Pellets)</v>
       </c>
       <c r="G32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly1-Butene Pellets)</v>
       </c>
       <c r="H32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly1-Butene Pellets)</v>
       </c>
       <c r="I32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly1-Butene Pellets)</v>
       </c>
       <c r="J32" s="1" t="str">
@@ -11831,19 +11831,19 @@
         <v>324</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2,6-Dimethyl-1,4-Phenylene Ether Pellets)</v>
       </c>
       <c r="G33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2,6-Dimethyl-1,4-Phenylene Ether Pellets)</v>
       </c>
       <c r="H33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2,6-Dimethyl-1,4-Phenylene Ether Pellets)</v>
       </c>
       <c r="I33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2,6-Dimethyl-1,4-Phenylene Ether Pellets)</v>
       </c>
       <c r="J33" s="1" t="str">
@@ -11880,19 +11880,19 @@
         <v>320</v>
       </c>
       <c r="F34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="G34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="H34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="I34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="J34" s="1" t="str">
@@ -11929,19 +11929,19 @@
         <v>316</v>
       </c>
       <c r="F35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="G35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="H35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="I35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="J35" s="1" t="str">
@@ -11981,19 +11981,19 @@
         <v>312</v>
       </c>
       <c r="F36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="G36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="H36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="I36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="J36" s="1" t="str">
@@ -12033,19 +12033,19 @@
         <v>308</v>
       </c>
       <c r="F37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="G37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="H37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="I37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="J37" s="1" t="str">
@@ -12085,19 +12085,19 @@
         <v>304</v>
       </c>
       <c r="F38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="G38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="H38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="I38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="J38" s="1" t="str">
@@ -12137,19 +12137,19 @@
         <v>300</v>
       </c>
       <c r="F39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="G39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="H39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="I39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="J39" s="1" t="str">
@@ -12189,19 +12189,19 @@
         <v>296</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="G40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="H40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="I40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="J40" s="1" t="str">
@@ -12241,19 +12241,19 @@
         <v>292</v>
       </c>
       <c r="F41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="G41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="H41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="I41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="J41" s="1" t="str">
@@ -12293,19 +12293,19 @@
         <v>288</v>
       </c>
       <c r="F42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCaprolactone Pellets)</v>
       </c>
       <c r="G42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCaprolactone Pellets)</v>
       </c>
       <c r="H42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCaprolactone Pellets)</v>
       </c>
       <c r="I42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCaprolactone Pellets)</v>
       </c>
       <c r="J42" s="1" t="str">
@@ -12345,19 +12345,19 @@
         <v>284</v>
       </c>
       <c r="F43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCarbonate Pellets)</v>
       </c>
       <c r="G43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCarbonate Pellets)</v>
       </c>
       <c r="H43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCarbonate Pellets)</v>
       </c>
       <c r="I43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCarbonate Pellets)</v>
       </c>
       <c r="J43" s="1" t="str">
@@ -12394,19 +12394,19 @@
         <v>280</v>
       </c>
       <c r="F44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChloroPrene Pellets)</v>
       </c>
       <c r="G44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChloroPrene Pellets)</v>
       </c>
       <c r="H44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChloroPrene Pellets)</v>
       </c>
       <c r="I44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChloroPrene Pellets)</v>
       </c>
       <c r="J44" s="1" t="str">
@@ -12443,19 +12443,19 @@
         <v>276</v>
       </c>
       <c r="F45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="G45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="H45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="I45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="J45" s="1" t="str">
@@ -12495,19 +12495,19 @@
         <v>272</v>
       </c>
       <c r="F46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="G46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="H46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="I46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="J46" s="1" t="str">
@@ -12547,19 +12547,19 @@
         <v>268</v>
       </c>
       <c r="F47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="G47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="H47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="I47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="J47" s="1" t="str">
@@ -12599,19 +12599,19 @@
         <v>264</v>
       </c>
       <c r="F48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEtherImide Pellets)</v>
       </c>
       <c r="G48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEtherImide Pellets)</v>
       </c>
       <c r="H48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEtherImide Pellets)</v>
       </c>
       <c r="I48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEtherImide Pellets)</v>
       </c>
       <c r="J48" s="1" t="str">
@@ -12648,19 +12648,19 @@
         <v>260</v>
       </c>
       <c r="F49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="G49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="H49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="I49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="J49" s="1" t="str">
@@ -12697,19 +12697,19 @@
         <v>256</v>
       </c>
       <c r="F50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="G50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="H50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="I50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="J50" s="1" t="str">
@@ -12749,19 +12749,19 @@
         <v>252</v>
       </c>
       <c r="F51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="G51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="H51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="I51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="J51" s="1" t="str">
@@ -12798,19 +12798,19 @@
         <v>248</v>
       </c>
       <c r="F52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J52" s="1" t="str">
@@ -12850,19 +12850,19 @@
         <v>244</v>
       </c>
       <c r="F53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="G53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="H53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="I53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="J53" s="1" t="str">
@@ -12902,19 +12902,19 @@
         <v>240</v>
       </c>
       <c r="F54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="G54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="H54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="I54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="J54" s="1" t="str">
@@ -12954,19 +12954,19 @@
         <v>236</v>
       </c>
       <c r="F55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="G55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="H55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="I55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="J55" s="1" t="str">
@@ -13006,19 +13006,19 @@
         <v>232</v>
       </c>
       <c r="F56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J56" s="1" t="str">
@@ -13058,19 +13058,19 @@
         <v>228</v>
       </c>
       <c r="F57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="G57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="H57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="I57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="J57" s="1" t="str">
@@ -13110,19 +13110,19 @@
         <v>224</v>
       </c>
       <c r="F58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="G58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="H58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="I58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="J58" s="1" t="str">
@@ -13162,19 +13162,19 @@
         <v>220</v>
       </c>
       <c r="F59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="G59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="H59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="I59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="J59" s="1" t="str">
@@ -13214,19 +13214,19 @@
         <v>216</v>
       </c>
       <c r="F60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="G60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="H60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="I60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="J60" s="1" t="str">
@@ -13266,19 +13266,19 @@
         <v>212</v>
       </c>
       <c r="F61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="G61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="H61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="I61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="J61" s="1" t="str">
@@ -13315,19 +13315,19 @@
         <v>208</v>
       </c>
       <c r="F62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="G62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="H62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="I62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="J62" s="1" t="str">
@@ -13367,19 +13367,19 @@
         <v>204</v>
       </c>
       <c r="F63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyImide Pellets)</v>
       </c>
       <c r="G63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyImide Pellets)</v>
       </c>
       <c r="H63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyImide Pellets)</v>
       </c>
       <c r="I63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyImide Pellets)</v>
       </c>
       <c r="J63" s="1" t="str">
@@ -13416,19 +13416,19 @@
         <v>200</v>
       </c>
       <c r="F64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="G64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="H64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="I64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="J64" s="1" t="str">
@@ -13465,19 +13465,19 @@
         <v>196</v>
       </c>
       <c r="F65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="G65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="H65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="I65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="J65" s="1" t="str">
@@ -13517,19 +13517,19 @@
         <v>192</v>
       </c>
       <c r="F66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButylene Pellets)</v>
       </c>
       <c r="G66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButylene Pellets)</v>
       </c>
       <c r="H66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButylene Pellets)</v>
       </c>
       <c r="I66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButylene Pellets)</v>
       </c>
       <c r="J66" s="1" t="str">
@@ -13569,19 +13569,19 @@
         <v>188</v>
       </c>
       <c r="F67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoPrene Pellets)</v>
       </c>
       <c r="G67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoPrene Pellets)</v>
       </c>
       <c r="H67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoPrene Pellets)</v>
       </c>
       <c r="I67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoPrene Pellets)</v>
       </c>
       <c r="J67" s="1" t="str">
@@ -13621,19 +13621,19 @@
         <v>184</v>
       </c>
       <c r="F68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic Acid Pellets)</v>
       </c>
       <c r="G68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic Acid Pellets)</v>
       </c>
       <c r="H68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic Acid Pellets)</v>
       </c>
       <c r="I68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic Acid Pellets)</v>
       </c>
       <c r="J68" s="1" t="str">
@@ -13670,19 +13670,19 @@
         <v>180</v>
       </c>
       <c r="F69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="G69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="H69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="I69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="J69" s="1" t="str">
@@ -13719,19 +13719,19 @@
         <v>176</v>
       </c>
       <c r="F70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="G70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="H70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="I70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="J70" s="1" t="str">
@@ -13768,19 +13768,19 @@
         <v>172</v>
       </c>
       <c r="F71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="G71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="H71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="I71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="J71" s="1" t="str">
@@ -13817,19 +13817,19 @@
         <v>168</v>
       </c>
       <c r="F72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="G72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="H72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="I72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="J72" s="1" t="str">
@@ -13866,19 +13866,19 @@
         <v>164</v>
       </c>
       <c r="F73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="G73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="H73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="I73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="J73" s="1" t="str">
@@ -13918,19 +13918,19 @@
         <v>160</v>
       </c>
       <c r="F74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="G74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="H74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="I74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="J74" s="1" t="str">
@@ -13967,19 +13967,19 @@
         <v>156</v>
       </c>
       <c r="F75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J75" s="1" t="str">
@@ -14019,19 +14019,19 @@
         <v>152</v>
       </c>
       <c r="F76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyOxymethylene Pellets)</v>
       </c>
       <c r="G76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyOxymethylene Pellets)</v>
       </c>
       <c r="H76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyOxymethylene Pellets)</v>
       </c>
       <c r="I76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyOxymethylene Pellets)</v>
       </c>
       <c r="J76" s="1" t="str">
@@ -14068,19 +14068,19 @@
         <v>148</v>
       </c>
       <c r="F77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J77" s="1" t="str">
@@ -14117,19 +14117,19 @@
         <v>144</v>
       </c>
       <c r="F78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenol Pellets)</v>
       </c>
       <c r="G78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenol Pellets)</v>
       </c>
       <c r="H78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenol Pellets)</v>
       </c>
       <c r="I78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenol Pellets)</v>
       </c>
       <c r="J78" s="1" t="str">
@@ -14166,19 +14166,19 @@
         <v>140</v>
       </c>
       <c r="F79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="G79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="H79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="I79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="J79" s="1" t="str">
@@ -14215,19 +14215,19 @@
         <v>136</v>
       </c>
       <c r="F80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhosphazene Pellets)</v>
       </c>
       <c r="G80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhosphazene Pellets)</v>
       </c>
       <c r="H80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhosphazene Pellets)</v>
       </c>
       <c r="I80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhosphazene Pellets)</v>
       </c>
       <c r="J80" s="1" t="str">
@@ -14264,19 +14264,19 @@
         <v>132</v>
       </c>
       <c r="F81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="G81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="H81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="I81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="J81" s="1" t="str">
@@ -14313,19 +14313,19 @@
         <v>128</v>
       </c>
       <c r="F82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="G82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="H82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="I82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="J82" s="1" t="str">
@@ -14365,19 +14365,19 @@
         <v>124</v>
       </c>
       <c r="F83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="G83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="H83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="I83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="J83" s="1" t="str">
@@ -14417,19 +14417,19 @@
         <v>120</v>
       </c>
       <c r="F84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Pellets)</v>
       </c>
       <c r="G84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Pellets)</v>
       </c>
       <c r="H84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Pellets)</v>
       </c>
       <c r="I84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Pellets)</v>
       </c>
       <c r="J84" s="1" t="str">
@@ -14466,19 +14466,19 @@
         <v>116</v>
       </c>
       <c r="F85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="G85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="H85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="I85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="J85" s="1" t="str">
@@ -14515,19 +14515,19 @@
         <v>112</v>
       </c>
       <c r="F86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="G86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="H86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="I86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="J86" s="1" t="str">
@@ -14567,19 +14567,19 @@
         <v>108</v>
       </c>
       <c r="F87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyStyrene Pellets)</v>
       </c>
       <c r="G87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyStyrene Pellets)</v>
       </c>
       <c r="H87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyStyrene Pellets)</v>
       </c>
       <c r="I87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyStyrene Pellets)</v>
       </c>
       <c r="J87" s="1" t="str">
@@ -14616,19 +14616,19 @@
         <v>104</v>
       </c>
       <c r="F88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J88" s="1" t="str">
@@ -14668,19 +14668,19 @@
         <v>100</v>
       </c>
       <c r="F89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="G89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="H89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="I89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="J89" s="1" t="str">
@@ -14717,19 +14717,19 @@
         <v>96</v>
       </c>
       <c r="F90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="G90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="H90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="I90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="J90" s="1" t="str">
@@ -14766,19 +14766,19 @@
         <v>92</v>
       </c>
       <c r="F91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="G91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="H91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="I91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="J91" s="1" t="str">
@@ -14815,19 +14815,19 @@
         <v>88</v>
       </c>
       <c r="F92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyThiazyl Pellets)</v>
       </c>
       <c r="G92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyThiazyl Pellets)</v>
       </c>
       <c r="H92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyThiazyl Pellets)</v>
       </c>
       <c r="I92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyThiazyl Pellets)</v>
       </c>
       <c r="J92" s="1" t="str">
@@ -14867,19 +14867,19 @@
         <v>84</v>
       </c>
       <c r="F93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="G93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="H93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="I93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="J93" s="1" t="str">
@@ -14919,19 +14919,19 @@
         <v>80</v>
       </c>
       <c r="F94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyUrethane Pellets)</v>
       </c>
       <c r="G94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyUrethane Pellets)</v>
       </c>
       <c r="H94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyUrethane Pellets)</v>
       </c>
       <c r="I94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyUrethane Pellets)</v>
       </c>
       <c r="J94" s="1" t="str">
@@ -14971,19 +14971,19 @@
         <v>76</v>
       </c>
       <c r="F95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="G95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="H95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="I95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="J95" s="1" t="str">
@@ -15023,19 +15023,19 @@
         <v>72</v>
       </c>
       <c r="F96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="G96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="H96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="I96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="J96" s="1" t="str">
@@ -15072,19 +15072,19 @@
         <v>68</v>
       </c>
       <c r="F97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="G97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="H97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="I97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="J97" s="1" t="str">
@@ -15124,19 +15124,19 @@
         <v>64</v>
       </c>
       <c r="F98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="G98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="H98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="I98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="J98" s="1" t="str">
@@ -15176,19 +15176,19 @@
         <v>60</v>
       </c>
       <c r="F99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="G99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="H99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="I99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="J99" s="1" t="str">
@@ -15225,19 +15225,19 @@
         <v>56</v>
       </c>
       <c r="F100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="G100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="H100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="I100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="J100" s="1" t="str">
@@ -15274,19 +15274,19 @@
         <v>52</v>
       </c>
       <c r="F101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="G101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="H101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="I101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="J101" s="1" t="str">
@@ -15323,19 +15323,19 @@
         <v>48</v>
       </c>
       <c r="F102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="G102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="H102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="I102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="J102" s="1" t="str">
@@ -15372,19 +15372,19 @@
         <v>44</v>
       </c>
       <c r="F103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="G103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="H103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="I103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="J103" s="1" t="str">
@@ -15421,19 +15421,19 @@
         <v>40</v>
       </c>
       <c r="F104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="G104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="H104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="I104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="J104" s="1" t="str">
@@ -15470,19 +15470,19 @@
         <v>36</v>
       </c>
       <c r="F105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="G105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="H105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="I105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="J105" s="1" t="str">
@@ -15522,19 +15522,19 @@
         <v>32</v>
       </c>
       <c r="F106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="G106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="H106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="I106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="J106" s="1" t="str">
@@ -15574,19 +15574,19 @@
         <v>28</v>
       </c>
       <c r="F107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J107" s="1" t="str">
@@ -15626,19 +15626,19 @@
         <v>24</v>
       </c>
       <c r="F108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J108" s="1" t="str">
@@ -15675,19 +15675,19 @@
         <v>20</v>
       </c>
       <c r="F109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="G109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="H109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="I109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="J109" s="1" t="str">
@@ -15724,19 +15724,19 @@
         <v>16</v>
       </c>
       <c r="F110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="G110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="H110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="I110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="J110" s="1" t="str">
@@ -15776,19 +15776,19 @@
         <v>12</v>
       </c>
       <c r="F111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="G111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="H111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="I111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="J111" s="1" t="str">
@@ -15825,19 +15825,19 @@
         <v>8</v>
       </c>
       <c r="F112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="G112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="H112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="I112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="J112" s="1" t="str">
@@ -15877,19 +15877,19 @@
         <v>4</v>
       </c>
       <c r="F113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J113" s="1" t="str">
@@ -15929,19 +15929,19 @@
         <v>0</v>
       </c>
       <c r="F114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="G114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="H114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="I114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="J114" s="1" t="str">
@@ -15981,19 +15981,19 @@
         <v>1853</v>
       </c>
       <c r="F115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Polycaprolactam Pellets)</v>
       </c>
       <c r="G115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Polycaprolactam Pellets)</v>
       </c>
       <c r="H115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Polycaprolactam Pellets)</v>
       </c>
       <c r="I115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Polycaprolactam Pellets)</v>
       </c>
       <c r="J115" s="1" t="str">
@@ -16033,19 +16033,19 @@
         <v>2412</v>
       </c>
       <c r="F116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="G116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="H116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="I116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="J116" s="1" t="str">
@@ -16085,19 +16085,19 @@
         <v>2416</v>
       </c>
       <c r="F117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="G117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="H117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="I117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="J117" s="1" t="str">
@@ -16134,19 +16134,19 @@
         <v>2420</v>
       </c>
       <c r="F118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (0)</v>
       </c>
       <c r="G118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (0)</v>
       </c>
       <c r="H118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (0)</v>
       </c>
       <c r="I118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (0)</v>
       </c>
       <c r="J118" s="1">
@@ -16183,19 +16183,19 @@
         <v>2424</v>
       </c>
       <c r="F119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$26, [1]Enums!$A$27)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$27, [1]Enums!$A$28)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (0)</v>
       </c>
       <c r="G119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$29, [1]Enums!$A$30)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (0)</v>
       </c>
       <c r="H119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (0)</v>
       </c>
       <c r="I119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (0)</v>
       </c>
       <c r="J119" s="1">
@@ -17175,7 +17175,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I2" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Steel</v>
       </c>
       <c r="J2" s="45">
@@ -17223,7 +17223,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I3" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Stainless Steel</v>
       </c>
       <c r="J3" s="45">
@@ -17271,7 +17271,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I4" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Brass</v>
       </c>
       <c r="J4" s="45">
@@ -17319,7 +17319,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I5" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Bronze</v>
       </c>
       <c r="J5" s="45">
@@ -17367,7 +17367,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I6" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Tungsten Carbide</v>
       </c>
       <c r="J6" s="45">
@@ -17415,7 +17415,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I7" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Nichrome</v>
       </c>
       <c r="J7" s="45">
@@ -17463,7 +17463,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I8" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Antimony-Lead</v>
       </c>
       <c r="J8" s="45">
@@ -17511,7 +17511,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I9" s="45" t="str">
-        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$137&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Steel</v>
       </c>
       <c r="J9" s="45">
@@ -17559,7 +17559,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I10" s="45" t="str">
-        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$137&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Stainless Steel</v>
       </c>
       <c r="J10" s="45">
@@ -17607,7 +17607,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I11" s="45" t="str">
-        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$137&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Brass</v>
       </c>
       <c r="J11" s="45">
@@ -17655,7 +17655,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I12" s="45" t="str">
-        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$137&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Bronze</v>
       </c>
       <c r="J12" s="45">
@@ -17703,7 +17703,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I13" s="45" t="str">
-        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$137&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Tungsten Carbide</v>
       </c>
       <c r="J13" s="45">
@@ -17751,7 +17751,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I14" s="45" t="str">
-        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$137&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Nichrome</v>
       </c>
       <c r="J14" s="45">
@@ -17799,7 +17799,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I15" s="45" t="str">
-        <f>[1]Enums!$A$136&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$137&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Antimony-Lead</v>
       </c>
       <c r="J15" s="45">
@@ -17847,7 +17847,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I16" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" Iron"</f>
+        <f>[1]Enums!$A$136&amp;" Iron"</f>
         <v>Composite Iron</v>
       </c>
       <c r="J16" s="45">
@@ -17895,7 +17895,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I17" s="45" t="str">
-        <f>[1]Enums!$A$136&amp;" Iron"</f>
+        <f>[1]Enums!$A$137&amp;" Iron"</f>
         <v>Engineered Iron</v>
       </c>
       <c r="J17" s="45">
@@ -17943,7 +17943,7 @@
         <v>Diamond</v>
       </c>
       <c r="I18" s="45" t="str">
-        <f>[1]Enums!$A$135&amp;" Diamond"</f>
+        <f>[1]Enums!$A$136&amp;" Diamond"</f>
         <v>Composite Diamond</v>
       </c>
       <c r="J18" s="45">
@@ -17991,7 +17991,7 @@
         <v>Diamond</v>
       </c>
       <c r="I19" s="45" t="str">
-        <f>[1]Enums!$A$136&amp;" Diamond"</f>
+        <f>[1]Enums!$A$137&amp;" Diamond"</f>
         <v>Engineered Diamond</v>
       </c>
       <c r="J19" s="45">
@@ -18292,7 +18292,7 @@
         <v>Molded Item</v>
       </c>
       <c r="F1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$100</f>
+        <f xml:space="preserve"> [1]Enums!$A$101</f>
         <v>Base Material</v>
       </c>
       <c r="G1" s="30" t="s">
@@ -18320,7 +18320,7 @@
         <v>1812</v>
       </c>
       <c r="C2" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D2</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D2</f>
         <v>Gripped Iron Shovel</v>
       </c>
       <c r="D2" s="24" t="str">
@@ -18332,7 +18332,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F2" s="34" t="str">
-        <f>[1]Enums!$A$103</f>
+        <f>[1]Enums!$A$104</f>
         <v>Iron</v>
       </c>
       <c r="G2" s="24">
@@ -18357,7 +18357,7 @@
         <v>1811</v>
       </c>
       <c r="C3" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D3</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D3</f>
         <v>Gripped Iron Pickaxe</v>
       </c>
       <c r="D3" s="21" t="str">
@@ -18369,7 +18369,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F3" s="34" t="str">
-        <f>[1]Enums!$A$103</f>
+        <f>[1]Enums!$A$104</f>
         <v>Iron</v>
       </c>
       <c r="G3" s="24">
@@ -18394,7 +18394,7 @@
         <v>1810</v>
       </c>
       <c r="C4" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D4</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D4</f>
         <v>Gripped Iron Axe</v>
       </c>
       <c r="D4" s="21" t="str">
@@ -18406,7 +18406,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F4" s="34" t="str">
-        <f>[1]Enums!$A$103</f>
+        <f>[1]Enums!$A$104</f>
         <v>Iron</v>
       </c>
       <c r="G4" s="24">
@@ -18431,7 +18431,7 @@
         <v>1809</v>
       </c>
       <c r="C5" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D5</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D5</f>
         <v>Gripped Iron Sword</v>
       </c>
       <c r="D5" s="21" t="str">
@@ -18443,7 +18443,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F5" s="34" t="str">
-        <f>[1]Enums!$A$103</f>
+        <f>[1]Enums!$A$104</f>
         <v>Iron</v>
       </c>
       <c r="G5" s="24">
@@ -18468,7 +18468,7 @@
         <v>1808</v>
       </c>
       <c r="C6" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D6</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D6</f>
         <v>Gripped Wooden Sword</v>
       </c>
       <c r="D6" s="21" t="str">
@@ -18480,7 +18480,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F6" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$102</f>
         <v>Wooden</v>
       </c>
       <c r="G6" s="24">
@@ -18505,7 +18505,7 @@
         <v>1807</v>
       </c>
       <c r="C7" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D7</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D7</f>
         <v>Gripped Wooden Shovel</v>
       </c>
       <c r="D7" s="21" t="str">
@@ -18517,7 +18517,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F7" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$102</f>
         <v>Wooden</v>
       </c>
       <c r="G7" s="24">
@@ -18542,7 +18542,7 @@
         <v>1806</v>
       </c>
       <c r="C8" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D8</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D8</f>
         <v>Gripped Wooden Pickaxe</v>
       </c>
       <c r="D8" s="21" t="str">
@@ -18554,7 +18554,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F8" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$102</f>
         <v>Wooden</v>
       </c>
       <c r="G8" s="24">
@@ -18579,7 +18579,7 @@
         <v>1805</v>
       </c>
       <c r="C9" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D9</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D9</f>
         <v>Gripped Wooden Axe</v>
       </c>
       <c r="D9" s="21" t="str">
@@ -18591,7 +18591,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F9" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$102</f>
         <v>Wooden</v>
       </c>
       <c r="G9" s="24">
@@ -18616,7 +18616,7 @@
         <v>1804</v>
       </c>
       <c r="C10" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D10</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D10</f>
         <v>Gripped Stone Sword</v>
       </c>
       <c r="D10" s="21" t="str">
@@ -18628,7 +18628,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F10" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$103</f>
         <v>Stone</v>
       </c>
       <c r="G10" s="24">
@@ -18653,7 +18653,7 @@
         <v>1803</v>
       </c>
       <c r="C11" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D11</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D11</f>
         <v>Gripped Stone Shovel</v>
       </c>
       <c r="D11" s="21" t="str">
@@ -18665,7 +18665,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F11" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$103</f>
         <v>Stone</v>
       </c>
       <c r="G11" s="24">
@@ -18690,7 +18690,7 @@
         <v>1802</v>
       </c>
       <c r="C12" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D12</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D12</f>
         <v>Gripped Stone Pickaxe</v>
       </c>
       <c r="D12" s="21" t="str">
@@ -18702,7 +18702,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F12" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$103</f>
         <v>Stone</v>
       </c>
       <c r="G12" s="24">
@@ -18727,7 +18727,7 @@
         <v>1801</v>
       </c>
       <c r="C13" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D13</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D13</f>
         <v>Gripped Stone Axe</v>
       </c>
       <c r="D13" s="21" t="str">
@@ -18739,7 +18739,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F13" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$103</f>
         <v>Stone</v>
       </c>
       <c r="G13" s="24">
@@ -18764,7 +18764,7 @@
         <v>1800</v>
       </c>
       <c r="C14" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D14</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D14</f>
         <v>Gripped Diamond Sword</v>
       </c>
       <c r="D14" s="21" t="str">
@@ -18776,7 +18776,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F14" s="34" t="str">
-        <f>[1]Enums!$A$105</f>
+        <f>[1]Enums!$A$106</f>
         <v>Diamond</v>
       </c>
       <c r="G14" s="24">
@@ -18801,7 +18801,7 @@
         <v>1799</v>
       </c>
       <c r="C15" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D15</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D15</f>
         <v>Gripped Diamond Shovel</v>
       </c>
       <c r="D15" s="21" t="str">
@@ -18813,7 +18813,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F15" s="34" t="str">
-        <f>[1]Enums!$A$105</f>
+        <f>[1]Enums!$A$106</f>
         <v>Diamond</v>
       </c>
       <c r="G15" s="24">
@@ -18838,7 +18838,7 @@
         <v>1798</v>
       </c>
       <c r="C16" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D16</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D16</f>
         <v>Gripped Diamond Pickaxe</v>
       </c>
       <c r="D16" s="21" t="str">
@@ -18850,7 +18850,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F16" s="34" t="str">
-        <f>[1]Enums!$A$105</f>
+        <f>[1]Enums!$A$106</f>
         <v>Diamond</v>
       </c>
       <c r="G16" s="24">
@@ -18875,7 +18875,7 @@
         <v>1797</v>
       </c>
       <c r="C17" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D17</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D17</f>
         <v>Gripped Diamond Axe</v>
       </c>
       <c r="D17" s="21" t="str">
@@ -18887,7 +18887,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F17" s="34" t="str">
-        <f>[1]Enums!$A$105</f>
+        <f>[1]Enums!$A$106</f>
         <v>Diamond</v>
       </c>
       <c r="G17" s="24">
@@ -18912,7 +18912,7 @@
         <v>1796</v>
       </c>
       <c r="C18" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D18</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D18</f>
         <v>Gripped Golden Sword</v>
       </c>
       <c r="D18" s="21" t="str">
@@ -18924,7 +18924,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F18" s="34" t="str">
-        <f>[1]Enums!$A$104</f>
+        <f>[1]Enums!$A$105</f>
         <v>Golden</v>
       </c>
       <c r="G18" s="24">
@@ -18949,7 +18949,7 @@
         <v>1795</v>
       </c>
       <c r="C19" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D19</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D19</f>
         <v>Gripped Golden Shovel</v>
       </c>
       <c r="D19" s="21" t="str">
@@ -18961,7 +18961,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F19" s="34" t="str">
-        <f>[1]Enums!$A$104</f>
+        <f>[1]Enums!$A$105</f>
         <v>Golden</v>
       </c>
       <c r="G19" s="24">
@@ -18986,7 +18986,7 @@
         <v>1794</v>
       </c>
       <c r="C20" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D20</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D20</f>
         <v>Gripped Golden Pickaxe</v>
       </c>
       <c r="D20" s="21" t="str">
@@ -18998,7 +18998,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F20" s="34" t="str">
-        <f>[1]Enums!$A$104</f>
+        <f>[1]Enums!$A$105</f>
         <v>Golden</v>
       </c>
       <c r="G20" s="24">
@@ -19023,7 +19023,7 @@
         <v>1793</v>
       </c>
       <c r="C21" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D21</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D21</f>
         <v>Gripped Golden Axe</v>
       </c>
       <c r="D21" s="21" t="str">
@@ -19035,7 +19035,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F21" s="34" t="str">
-        <f>[1]Enums!$A$104</f>
+        <f>[1]Enums!$A$105</f>
         <v>Golden</v>
       </c>
       <c r="G21" s="24">
@@ -19060,7 +19060,7 @@
         <v>1792</v>
       </c>
       <c r="C22" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D22</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D22</f>
         <v>Gripped Wooden Hoe</v>
       </c>
       <c r="D22" s="21" t="str">
@@ -19072,7 +19072,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F22" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$102</f>
         <v>Wooden</v>
       </c>
       <c r="G22" s="24">
@@ -19097,7 +19097,7 @@
         <v>1791</v>
       </c>
       <c r="C23" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D23</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D23</f>
         <v>Gripped Stone Hoe</v>
       </c>
       <c r="D23" s="21" t="str">
@@ -19109,7 +19109,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F23" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$103</f>
         <v>Stone</v>
       </c>
       <c r="G23" s="24">
@@ -19134,7 +19134,7 @@
         <v>1790</v>
       </c>
       <c r="C24" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D24</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D24</f>
         <v>Gripped Iron Hoe</v>
       </c>
       <c r="D24" s="21" t="str">
@@ -19146,7 +19146,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F24" s="34" t="str">
-        <f>[1]Enums!$A$103</f>
+        <f>[1]Enums!$A$104</f>
         <v>Iron</v>
       </c>
       <c r="G24" s="24">
@@ -19171,7 +19171,7 @@
         <v>1789</v>
       </c>
       <c r="C25" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D25</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D25</f>
         <v>Gripped Diamond Hoe</v>
       </c>
       <c r="D25" s="21" t="str">
@@ -19183,7 +19183,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F25" s="34" t="str">
-        <f>[1]Enums!$A$105</f>
+        <f>[1]Enums!$A$106</f>
         <v>Diamond</v>
       </c>
       <c r="G25" s="24">
@@ -19208,7 +19208,7 @@
         <v>1788</v>
       </c>
       <c r="C26" s="22" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;D26</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;D26</f>
         <v>Gripped Golden Hoe</v>
       </c>
       <c r="D26" s="21" t="str">
@@ -19220,7 +19220,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F26" s="34" t="str">
-        <f>[1]Enums!$A$104</f>
+        <f>[1]Enums!$A$105</f>
         <v>Golden</v>
       </c>
       <c r="G26" s="24">
@@ -19282,7 +19282,7 @@
         <v>1832</v>
       </c>
       <c r="D1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$100</f>
+        <f xml:space="preserve"> [1]Enums!$A$101</f>
         <v>Base Material</v>
       </c>
       <c r="E1" s="36" t="s">
@@ -19328,7 +19328,7 @@
         <v>Wooden Pogo Stick</v>
       </c>
       <c r="D2" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$102</f>
         <v>Wooden</v>
       </c>
       <c r="E2" s="37">
@@ -19365,7 +19365,7 @@
         <v>Stone Pogo Stick</v>
       </c>
       <c r="D3" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$103</f>
         <v>Stone</v>
       </c>
       <c r="E3" s="37">
@@ -19401,7 +19401,7 @@
         <v>Iron Pogo Stick</v>
       </c>
       <c r="D4" s="34" t="str">
-        <f>[1]Enums!$A$103</f>
+        <f>[1]Enums!$A$104</f>
         <v>Iron</v>
       </c>
       <c r="E4" s="37">
@@ -19437,7 +19437,7 @@
         <v>Golden Pogo Stick</v>
       </c>
       <c r="D5" s="34" t="str">
-        <f>[1]Enums!$A$104</f>
+        <f>[1]Enums!$A$105</f>
         <v>Golden</v>
       </c>
       <c r="E5" s="37">
@@ -19473,7 +19473,7 @@
         <v>Diamond Pogo Stick</v>
       </c>
       <c r="D6" s="34" t="str">
-        <f>[1]Enums!$A$105</f>
+        <f>[1]Enums!$A$106</f>
         <v>Diamond</v>
       </c>
       <c r="E6" s="37">
@@ -19509,7 +19509,7 @@
         <v>Magic Pogo Stick</v>
       </c>
       <c r="D7" s="34" t="str">
-        <f>[1]Enums!$A$106</f>
+        <f>[1]Enums!$A$107</f>
         <v>Magic</v>
       </c>
       <c r="E7" s="37">
@@ -19541,11 +19541,11 @@
         <v>1821</v>
       </c>
       <c r="C8" s="34" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;I8</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;I8</f>
         <v>Gripped Wooden Pogo Stick</v>
       </c>
       <c r="D8" s="34" t="str">
-        <f>[1]Enums!$A$101</f>
+        <f>[1]Enums!$A$102</f>
         <v>Wooden</v>
       </c>
       <c r="E8" s="37">
@@ -19585,11 +19585,11 @@
         <v>1820</v>
       </c>
       <c r="C9" s="34" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;I9</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;I9</f>
         <v>Gripped Stone Pogo Stick</v>
       </c>
       <c r="D9" s="34" t="str">
-        <f>[1]Enums!$A$102</f>
+        <f>[1]Enums!$A$103</f>
         <v>Stone</v>
       </c>
       <c r="E9" s="37">
@@ -19629,11 +19629,11 @@
         <v>1819</v>
       </c>
       <c r="C10" s="34" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;I10</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;I10</f>
         <v>Gripped Iron Pogo Stick</v>
       </c>
       <c r="D10" s="34" t="str">
-        <f>[1]Enums!$A$103</f>
+        <f>[1]Enums!$A$104</f>
         <v>Iron</v>
       </c>
       <c r="E10" s="37">
@@ -19673,11 +19673,11 @@
         <v>1818</v>
       </c>
       <c r="C11" s="34" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;I11</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;I11</f>
         <v>Gripped Golden Pogo Stick</v>
       </c>
       <c r="D11" s="34" t="str">
-        <f>[1]Enums!$A$104</f>
+        <f>[1]Enums!$A$105</f>
         <v>Golden</v>
       </c>
       <c r="E11" s="37">
@@ -19717,11 +19717,11 @@
         <v>1817</v>
       </c>
       <c r="C12" s="34" t="str">
-        <f>[1]Enums!$A$97&amp;" "&amp;I12</f>
+        <f>[1]Enums!$A$98&amp;" "&amp;I12</f>
         <v>Gripped Diamond Pogo Stick</v>
       </c>
       <c r="D12" s="34" t="str">
-        <f>[1]Enums!$A$105</f>
+        <f>[1]Enums!$A$106</f>
         <v>Diamond</v>
       </c>
       <c r="E12" s="37">
@@ -37803,7 +37803,7 @@
         <v>590</v>
       </c>
       <c r="D1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$74</f>
+        <f xml:space="preserve"> [1]Enums!$B$75</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="19" t="str">
@@ -37827,7 +37827,7 @@
         <v>Mold (Grip)</v>
       </c>
       <c r="D2" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E2" s="11" t="str">
@@ -37852,7 +37852,7 @@
         <v>Mold (Running Shoes)</v>
       </c>
       <c r="D3" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E3" s="11" t="str">
@@ -37877,7 +37877,7 @@
         <v>Mold (Scuba Fins)</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E4" s="11" t="str">
@@ -37902,7 +37902,7 @@
         <v>Mold (Scuba Mask)</v>
       </c>
       <c r="D5" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E5" s="11" t="str">
@@ -37927,7 +37927,7 @@
         <v>Mold (Gasket)</v>
       </c>
       <c r="D6" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E6" s="11" t="str">
@@ -37952,7 +37952,7 @@
         <v>Mold (Life Preserver)</v>
       </c>
       <c r="D7" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E7" s="11" t="str">
@@ -37977,7 +37977,7 @@
         <v>Metal Die (Fibers)</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$79</f>
+        <f xml:space="preserve"> [1]Enums!$B$80</f>
         <v>Metal Die</v>
       </c>
       <c r="E8" s="11" t="str">
@@ -38002,7 +38002,7 @@
         <v>Metal Die (Tether)</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$79</f>
+        <f xml:space="preserve"> [1]Enums!$B$80</f>
         <v>Metal Die</v>
       </c>
       <c r="E9" s="11" t="str">
@@ -38027,7 +38027,7 @@
         <v>Metal Die (Cord)</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$79</f>
+        <f xml:space="preserve"> [1]Enums!$B$80</f>
         <v>Metal Die</v>
       </c>
       <c r="E10" s="11" t="str">
@@ -38052,7 +38052,7 @@
         <v>Metal Die (Hose)</v>
       </c>
       <c r="D11" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$79</f>
+        <f xml:space="preserve"> [1]Enums!$B$80</f>
         <v>Metal Die</v>
       </c>
       <c r="E11" s="11" t="str">
@@ -38077,7 +38077,7 @@
         <v>Metal Die (Pipe Segment)</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$79</f>
+        <f xml:space="preserve"> [1]Enums!$B$80</f>
         <v>Metal Die</v>
       </c>
       <c r="E12" s="11" t="str">
@@ -38102,7 +38102,7 @@
         <v>Mold (Flashlight Shaft)</v>
       </c>
       <c r="D13" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E13" s="11" t="str">
@@ -38126,7 +38126,7 @@
         <v>Mold (Plastic Brick (1 x 1))</v>
       </c>
       <c r="D14" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E14" t="str">
@@ -38150,7 +38150,7 @@
         <v>Mold (Plastic Brick (1 x 2))</v>
       </c>
       <c r="D15" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E15" t="str">
@@ -38174,7 +38174,7 @@
         <v>Mold (Plastic Brick (1 x 3))</v>
       </c>
       <c r="D16" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E16" t="str">
@@ -38198,7 +38198,7 @@
         <v>Mold (Plastic Brick (1 x 4))</v>
       </c>
       <c r="D17" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E17" t="str">
@@ -38222,7 +38222,7 @@
         <v>Mold (Plastic Brick (2 x 2))</v>
       </c>
       <c r="D18" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E18" t="str">
@@ -38246,7 +38246,7 @@
         <v>Mold (Plastic Brick (2 x 3))</v>
       </c>
       <c r="D19" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E19" t="str">
@@ -38270,7 +38270,7 @@
         <v>Mold (Plastic Brick (2 x 4))</v>
       </c>
       <c r="D20" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E20" t="str">
@@ -38294,7 +38294,7 @@
         <v>Mold (Plastic Brick (3 x 3))</v>
       </c>
       <c r="D21" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E21" t="str">
@@ -38318,7 +38318,7 @@
         <v>Mold (Plastic Brick (3 x 4))</v>
       </c>
       <c r="D22" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E22" t="str">
@@ -38342,7 +38342,7 @@
         <v>Mold (Plastic Brick (4 x 4))</v>
       </c>
       <c r="D23" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E23" t="str">
@@ -38366,7 +38366,7 @@
         <v>Mold (Plastic Brick (1 x 8))</v>
       </c>
       <c r="D24" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E24" t="str">
@@ -38390,7 +38390,7 @@
         <v>Mold (Plastic Brick (2 x 8))</v>
       </c>
       <c r="D25" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E25" t="str">
@@ -38414,7 +38414,7 @@
         <v>Mold (Heated Knife Handle)</v>
       </c>
       <c r="D26" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E26" s="11" t="str">
@@ -38438,7 +38438,7 @@
         <v>Mold (Rubber Sole)</v>
       </c>
       <c r="D27" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E27" s="11" t="str">
@@ -38462,7 +38462,7 @@
         <v>Mold (Battery Case)</v>
       </c>
       <c r="D28" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E28" s="11" t="str">
@@ -38486,7 +38486,7 @@
         <v>Mold (Tool Shaft)</v>
       </c>
       <c r="D29" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E29" t="str">
@@ -38510,7 +38510,7 @@
         <v>Mold (Lighter Body)</v>
       </c>
       <c r="D30" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$78</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold</v>
       </c>
       <c r="E30" t="str">

</xml_diff>

<commit_message>
Added Trading house and exchange rates into the game
</commit_message>
<xml_diff>
--- a/config/Polycraft Polymers.xlsx
+++ b/config/Polycraft Polymers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="826" firstSheet="2" activeTab="13"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="826" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Pellets" sheetId="1" r:id="rId1"/>
@@ -10231,6 +10231,7 @@
       <sheetName val="Internal Objects"/>
       <sheetName val="Ores"/>
       <sheetName val="Ingots"/>
+      <sheetName val="Nuggets"/>
       <sheetName val="Compressed Blocks"/>
       <sheetName val="Catalysts"/>
       <sheetName val="Element Vessels"/>
@@ -10534,6 +10535,7 @@
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -25261,7 +25263,7 @@
   </sheetPr>
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -46310,7 +46312,7 @@
   </sheetPr>
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Working update: forgot to add these files on last commit
</commit_message>
<xml_diff>
--- a/config/Polycraft Polymers.xlsx
+++ b/config/Polycraft Polymers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="826" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="826" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Pellets" sheetId="1" r:id="rId1"/>
@@ -46312,8 +46312,8 @@
   </sheetPr>
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -47139,8 +47139,8 @@
   </sheetPr>
   <dimension ref="A1:U156"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="J159" sqref="J159"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updates from GitHub Interface for Communications
phones, chats, etc.
</commit_message>
<xml_diff>
--- a/config/Polycraft Polymers.xlsx
+++ b/config/Polycraft Polymers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="826" activeTab="7"/>
+    <workbookView xWindow="8370" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="826" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Pellets" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2942" uniqueCount="2708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2946" uniqueCount="2711">
   <si>
     <t>GC</t>
   </si>
@@ -8176,6 +8176,15 @@
   </si>
   <si>
     <t>Silicon Wafer (Ruined)</t>
+  </si>
+  <si>
+    <t>1fu</t>
+  </si>
+  <si>
+    <t>1fv</t>
+  </si>
+  <si>
+    <t>1fw</t>
   </si>
 </sst>
 </file>
@@ -8475,118 +8484,123 @@
             <v>1.3.2</v>
           </cell>
         </row>
-        <row r="30">
-          <cell r="A30" t="str">
-            <v>Bag</v>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>1.3.3</v>
           </cell>
         </row>
         <row r="31">
           <cell r="A31" t="str">
-            <v>Vial</v>
+            <v>Bag</v>
           </cell>
         </row>
-        <row r="33">
-          <cell r="A33" t="str">
-            <v>Sack</v>
+        <row r="32">
+          <cell r="A32" t="str">
+            <v>Vial</v>
           </cell>
         </row>
         <row r="34">
           <cell r="A34" t="str">
-            <v>Beaker</v>
+            <v>Sack</v>
           </cell>
         </row>
-        <row r="36">
-          <cell r="A36" t="str">
-            <v>Powder Keg</v>
+        <row r="35">
+          <cell r="A35" t="str">
+            <v>Beaker</v>
           </cell>
         </row>
         <row r="37">
           <cell r="A37" t="str">
-            <v>Drum</v>
+            <v>Powder Keg</v>
           </cell>
         </row>
-        <row r="39">
-          <cell r="A39" t="str">
-            <v>Chemical Silo</v>
+        <row r="38">
+          <cell r="A38" t="str">
+            <v>Drum</v>
           </cell>
         </row>
         <row r="40">
           <cell r="A40" t="str">
+            <v>Chemical Silo</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41" t="str">
             <v>Chemical Vat</v>
           </cell>
         </row>
-        <row r="79">
-          <cell r="B79" t="str">
+        <row r="80">
+          <cell r="B80" t="str">
             <v>Mold Type</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="B83" t="str">
-            <v>Mold</v>
           </cell>
         </row>
         <row r="84">
           <cell r="B84" t="str">
-            <v>Metal Die</v>
+            <v>Mold</v>
           </cell>
         </row>
-        <row r="91">
-          <cell r="B91" t="str">
-            <v>Wafer</v>
+        <row r="85">
+          <cell r="B85" t="str">
+            <v>Metal Die</v>
           </cell>
         </row>
         <row r="92">
           <cell r="B92" t="str">
+            <v>Wafer</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="B93" t="str">
             <v>Mask</v>
           </cell>
         </row>
-        <row r="107">
-          <cell r="A107" t="str">
+        <row r="108">
+          <cell r="A108" t="str">
             <v>Gripped</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="A110" t="str">
-            <v>Base Material</v>
           </cell>
         </row>
         <row r="111">
           <cell r="A111" t="str">
-            <v>Wooden</v>
+            <v>Base Material</v>
           </cell>
         </row>
         <row r="112">
           <cell r="A112" t="str">
-            <v>Stone</v>
+            <v>Wooden</v>
           </cell>
         </row>
         <row r="113">
           <cell r="A113" t="str">
-            <v>Iron</v>
+            <v>Stone</v>
           </cell>
         </row>
         <row r="114">
           <cell r="A114" t="str">
-            <v>Golden</v>
+            <v>Iron</v>
           </cell>
         </row>
         <row r="115">
           <cell r="A115" t="str">
-            <v>Diamond</v>
+            <v>Golden</v>
           </cell>
         </row>
         <row r="116">
           <cell r="A116" t="str">
-            <v>Magic</v>
+            <v>Diamond</v>
           </cell>
         </row>
-        <row r="145">
-          <cell r="A145" t="str">
-            <v>Composite</v>
+        <row r="117">
+          <cell r="A117" t="str">
+            <v>Magic</v>
           </cell>
         </row>
         <row r="146">
           <cell r="A146" t="str">
+            <v>Composite</v>
+          </cell>
+        </row>
+        <row r="147">
+          <cell r="A147" t="str">
             <v>Engineered</v>
           </cell>
         </row>
@@ -10217,6 +10231,11 @@
             <v>HAM Radio Case</v>
           </cell>
         </row>
+        <row r="34">
+          <cell r="B34" t="str">
+            <v>Flagpole Segment</v>
+          </cell>
+        </row>
       </sheetData>
     </sheetDataSet>
   </externalBook>
@@ -10852,19 +10871,19 @@
         <v>Game ID XL</v>
       </c>
       <c r="F1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$30&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$31&amp;" ("&amp;J1&amp;")"</f>
         <v>Bag (Pellets)</v>
       </c>
       <c r="G1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$33&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$34&amp;" ("&amp;J1&amp;")"</f>
         <v>Sack (Pellets)</v>
       </c>
       <c r="H1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$36&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$37&amp;" ("&amp;J1&amp;")"</f>
         <v>Powder Keg (Pellets)</v>
       </c>
       <c r="I1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$39&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$40&amp;" ("&amp;J1&amp;")"</f>
         <v>Chemical Silo (Pellets)</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -10903,19 +10922,19 @@
         <v>448</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="G2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="H2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="J2" s="1" t="str">
@@ -10955,19 +10974,19 @@
         <v>444</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J3" s="1" t="str">
@@ -11004,19 +11023,19 @@
         <v>440</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Alkyd Resin)</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Alkyd Resin)</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Alkyd Resin)</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Alkyd Resin)</v>
       </c>
       <c r="J4" s="1" t="str">
@@ -11056,19 +11075,19 @@
         <v>436</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J5" s="1" t="str">
@@ -11108,19 +11127,19 @@
         <v>432</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J6" s="1" t="str">
@@ -11160,19 +11179,19 @@
         <v>428</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$30, [1]Enums!$A$30)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$31, [1]Enums!$A$31)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Carbon Fiber)</v>
       </c>
       <c r="G7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$33, [1]Enums!$A$33)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$34, [1]Enums!$A$34)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Carbon Fiber)</v>
       </c>
       <c r="H7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$36, [1]Enums!$A$36)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$37, [1]Enums!$A$37)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Carbon Fiber)</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$39, [1]Enums!$A$39)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$40, [1]Enums!$A$40)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Carbon Fiber)</v>
       </c>
       <c r="J7" s="1" t="str">
@@ -11209,19 +11228,19 @@
         <v>424</v>
       </c>
       <c r="F8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="G8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="J8" s="1" t="str">
@@ -11261,19 +11280,19 @@
         <v>420</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulosic Pellets)</v>
       </c>
       <c r="G9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulosic Pellets)</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulosic Pellets)</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulosic Pellets)</v>
       </c>
       <c r="J9" s="1" t="str">
@@ -11313,19 +11332,19 @@
         <v>416</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chitin Pellets)</v>
       </c>
       <c r="G10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chitin Pellets)</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chitin Pellets)</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chitin Pellets)</v>
       </c>
       <c r="J10" s="1" t="str">
@@ -11365,19 +11384,19 @@
         <v>412</v>
       </c>
       <c r="F11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J11" s="1" t="str">
@@ -11417,19 +11436,19 @@
         <v>408</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Epoxy Resin)</v>
       </c>
       <c r="G12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Epoxy Resin)</v>
       </c>
       <c r="H12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Epoxy Resin)</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Epoxy Resin)</v>
       </c>
       <c r="J12" s="1" t="str">
@@ -11466,19 +11485,19 @@
         <v>404</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethoxylates Pellets)</v>
       </c>
       <c r="G13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethoxylates Pellets)</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethoxylates Pellets)</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethoxylates Pellets)</v>
       </c>
       <c r="J13" s="1" t="str">
@@ -11518,19 +11537,19 @@
         <v>400</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="G14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="H14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="J14" s="1" t="str">
@@ -11570,19 +11589,19 @@
         <v>396</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="G15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="J15" s="1" t="str">
@@ -11622,19 +11641,19 @@
         <v>392</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="G16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="J16" s="1" t="str">
@@ -11674,19 +11693,19 @@
         <v>388</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="G17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="J17" s="1" t="str">
@@ -11726,19 +11745,19 @@
         <v>384</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J18" s="1" t="str">
@@ -11778,19 +11797,19 @@
         <v>380</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J19" s="1" t="str">
@@ -11827,19 +11846,19 @@
         <v>376</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Lignin)</v>
       </c>
       <c r="G20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Lignin)</v>
       </c>
       <c r="H20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Lignin)</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Lignin)</v>
       </c>
       <c r="J20" s="1" t="str">
@@ -11879,19 +11898,19 @@
         <v>372</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J21" s="1" t="str">
@@ -11931,19 +11950,19 @@
         <v>368</v>
       </c>
       <c r="F22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="G22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="H22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="J22" s="1" t="str">
@@ -11983,19 +12002,19 @@
         <v>364</v>
       </c>
       <c r="F23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="G23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="H23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="J23" s="1" t="str">
@@ -12035,19 +12054,19 @@
         <v>360</v>
       </c>
       <c r="F24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="G24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="H24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="J24" s="1" t="str">
@@ -12084,19 +12103,19 @@
         <v>356</v>
       </c>
       <c r="F25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="G25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="H25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="J25" s="1" t="str">
@@ -12136,19 +12155,19 @@
         <v>352</v>
       </c>
       <c r="F26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Metaldehyde Pellets)</v>
       </c>
       <c r="G26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Metaldehyde Pellets)</v>
       </c>
       <c r="H26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Metaldehyde Pellets)</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Metaldehyde Pellets)</v>
       </c>
       <c r="J26" s="1" t="str">
@@ -12188,19 +12207,19 @@
         <v>348</v>
       </c>
       <c r="F27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J27" s="1" t="str">
@@ -12240,19 +12259,19 @@
         <v>344</v>
       </c>
       <c r="F28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraformaldehyde Pellets)</v>
       </c>
       <c r="G28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraformaldehyde Pellets)</v>
       </c>
       <c r="H28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraformaldehyde Pellets)</v>
       </c>
       <c r="I28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraformaldehyde Pellets)</v>
       </c>
       <c r="J28" s="1" t="str">
@@ -12292,19 +12311,19 @@
         <v>340</v>
       </c>
       <c r="F29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraldehyde Pellets)</v>
       </c>
       <c r="G29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraldehyde Pellets)</v>
       </c>
       <c r="H29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraldehyde Pellets)</v>
       </c>
       <c r="I29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraldehyde Pellets)</v>
       </c>
       <c r="J29" s="1" t="str">
@@ -12344,19 +12363,19 @@
         <v>336</v>
       </c>
       <c r="F30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Phenolic Resin)</v>
       </c>
       <c r="G30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Phenolic Resin)</v>
       </c>
       <c r="H30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Phenolic Resin)</v>
       </c>
       <c r="I30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Phenolic Resin)</v>
       </c>
       <c r="J30" s="1" t="str">
@@ -12396,19 +12415,19 @@
         <v>332</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="G31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="H31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="I31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="J31" s="1" t="str">
@@ -12448,19 +12467,19 @@
         <v>328</v>
       </c>
       <c r="F32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly1-Butene Pellets)</v>
       </c>
       <c r="G32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly1-Butene Pellets)</v>
       </c>
       <c r="H32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly1-Butene Pellets)</v>
       </c>
       <c r="I32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly1-Butene Pellets)</v>
       </c>
       <c r="J32" s="1" t="str">
@@ -12500,19 +12519,19 @@
         <v>324</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="G33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="H33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="I33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="J33" s="1" t="str">
@@ -12552,19 +12571,19 @@
         <v>320</v>
       </c>
       <c r="F34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="G34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="H34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="I34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="J34" s="1" t="str">
@@ -12604,19 +12623,19 @@
         <v>316</v>
       </c>
       <c r="F35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="G35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="H35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="I35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="J35" s="1" t="str">
@@ -12656,19 +12675,19 @@
         <v>312</v>
       </c>
       <c r="F36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="G36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="H36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="I36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="J36" s="1" t="str">
@@ -12708,19 +12727,19 @@
         <v>308</v>
       </c>
       <c r="F37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="G37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="H37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="I37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="J37" s="1" t="str">
@@ -12760,19 +12779,19 @@
         <v>304</v>
       </c>
       <c r="F38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="G38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="H38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="I38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="J38" s="1" t="str">
@@ -12812,19 +12831,19 @@
         <v>300</v>
       </c>
       <c r="F39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="G39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="H39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="I39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="J39" s="1" t="str">
@@ -12864,19 +12883,19 @@
         <v>296</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="G40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="H40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="I40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="J40" s="1" t="str">
@@ -12916,19 +12935,19 @@
         <v>292</v>
       </c>
       <c r="F41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="G41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="H41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="I41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="J41" s="1" t="str">
@@ -12968,19 +12987,19 @@
         <v>288</v>
       </c>
       <c r="F42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCaprolactone Pellets)</v>
       </c>
       <c r="G42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCaprolactone Pellets)</v>
       </c>
       <c r="H42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCaprolactone Pellets)</v>
       </c>
       <c r="I42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCaprolactone Pellets)</v>
       </c>
       <c r="J42" s="1" t="str">
@@ -13020,19 +13039,19 @@
         <v>284</v>
       </c>
       <c r="F43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCarbonate Pellets)</v>
       </c>
       <c r="G43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCarbonate Pellets)</v>
       </c>
       <c r="H43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCarbonate Pellets)</v>
       </c>
       <c r="I43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCarbonate Pellets)</v>
       </c>
       <c r="J43" s="1" t="str">
@@ -13072,19 +13091,19 @@
         <v>280</v>
       </c>
       <c r="F44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChloroPrene Pellets)</v>
       </c>
       <c r="G44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChloroPrene Pellets)</v>
       </c>
       <c r="H44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChloroPrene Pellets)</v>
       </c>
       <c r="I44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChloroPrene Pellets)</v>
       </c>
       <c r="J44" s="1" t="str">
@@ -13121,19 +13140,19 @@
         <v>276</v>
       </c>
       <c r="F45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="G45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="H45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="I45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="J45" s="1" t="str">
@@ -13173,19 +13192,19 @@
         <v>272</v>
       </c>
       <c r="F46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="G46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="H46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="I46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="J46" s="1" t="str">
@@ -13225,19 +13244,19 @@
         <v>268</v>
       </c>
       <c r="F47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="G47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="H47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="I47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="J47" s="1" t="str">
@@ -13277,19 +13296,19 @@
         <v>264</v>
       </c>
       <c r="F48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEtherImide Pellets)</v>
       </c>
       <c r="G48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEtherImide Pellets)</v>
       </c>
       <c r="H48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEtherImide Pellets)</v>
       </c>
       <c r="I48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEtherImide Pellets)</v>
       </c>
       <c r="J48" s="1" t="str">
@@ -13326,19 +13345,19 @@
         <v>260</v>
       </c>
       <c r="F49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="G49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="H49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="I49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="J49" s="1" t="str">
@@ -13375,19 +13394,19 @@
         <v>256</v>
       </c>
       <c r="F50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="G50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="H50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="I50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="J50" s="1" t="str">
@@ -13427,19 +13446,19 @@
         <v>252</v>
       </c>
       <c r="F51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="G51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="H51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="I51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="J51" s="1" t="str">
@@ -13476,19 +13495,19 @@
         <v>248</v>
       </c>
       <c r="F52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J52" s="1" t="str">
@@ -13528,19 +13547,19 @@
         <v>244</v>
       </c>
       <c r="F53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="G53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="H53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="I53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="J53" s="1" t="str">
@@ -13580,19 +13599,19 @@
         <v>240</v>
       </c>
       <c r="F54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="G54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="H54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="I54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="J54" s="1" t="str">
@@ -13632,19 +13651,19 @@
         <v>236</v>
       </c>
       <c r="F55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="G55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="H55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="I55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="J55" s="1" t="str">
@@ -13684,19 +13703,19 @@
         <v>232</v>
       </c>
       <c r="F56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J56" s="1" t="str">
@@ -13736,19 +13755,19 @@
         <v>228</v>
       </c>
       <c r="F57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="G57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="H57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="I57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="J57" s="1" t="str">
@@ -13788,19 +13807,19 @@
         <v>224</v>
       </c>
       <c r="F58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="G58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="H58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="I58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="J58" s="1" t="str">
@@ -13840,19 +13859,19 @@
         <v>220</v>
       </c>
       <c r="F59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="G59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="H59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="I59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="J59" s="1" t="str">
@@ -13892,19 +13911,19 @@
         <v>216</v>
       </c>
       <c r="F60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="G60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="H60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="I60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="J60" s="1" t="str">
@@ -13944,19 +13963,19 @@
         <v>212</v>
       </c>
       <c r="F61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="G61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="H61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="I61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="J61" s="1" t="str">
@@ -13993,19 +14012,19 @@
         <v>208</v>
       </c>
       <c r="F62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="G62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="H62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="I62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="J62" s="1" t="str">
@@ -14045,19 +14064,19 @@
         <v>204</v>
       </c>
       <c r="F63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyImide Pellets)</v>
       </c>
       <c r="G63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyImide Pellets)</v>
       </c>
       <c r="H63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyImide Pellets)</v>
       </c>
       <c r="I63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyImide Pellets)</v>
       </c>
       <c r="J63" s="1" t="str">
@@ -14094,19 +14113,19 @@
         <v>200</v>
       </c>
       <c r="F64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="G64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="H64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="I64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="J64" s="1" t="str">
@@ -14143,19 +14162,19 @@
         <v>196</v>
       </c>
       <c r="F65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="G65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="H65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="I65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="J65" s="1" t="str">
@@ -14195,19 +14214,19 @@
         <v>192</v>
       </c>
       <c r="F66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButylene Pellets)</v>
       </c>
       <c r="G66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButylene Pellets)</v>
       </c>
       <c r="H66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButylene Pellets)</v>
       </c>
       <c r="I66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButylene Pellets)</v>
       </c>
       <c r="J66" s="1" t="str">
@@ -14247,19 +14266,19 @@
         <v>188</v>
       </c>
       <c r="F67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoPrene Pellets)</v>
       </c>
       <c r="G67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoPrene Pellets)</v>
       </c>
       <c r="H67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoPrene Pellets)</v>
       </c>
       <c r="I67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoPrene Pellets)</v>
       </c>
       <c r="J67" s="1" t="str">
@@ -14299,19 +14318,19 @@
         <v>184</v>
       </c>
       <c r="F68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic Acid Pellets)</v>
       </c>
       <c r="G68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic Acid Pellets)</v>
       </c>
       <c r="H68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic Acid Pellets)</v>
       </c>
       <c r="I68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic Acid Pellets)</v>
       </c>
       <c r="J68" s="1" t="str">
@@ -14348,19 +14367,19 @@
         <v>180</v>
       </c>
       <c r="F69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="G69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="H69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="I69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="J69" s="1" t="str">
@@ -14400,19 +14419,19 @@
         <v>176</v>
       </c>
       <c r="F70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="G70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="H70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="I70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="J70" s="1" t="str">
@@ -14449,19 +14468,19 @@
         <v>172</v>
       </c>
       <c r="F71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="G71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="H71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="I71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="J71" s="1" t="str">
@@ -14501,19 +14520,19 @@
         <v>168</v>
       </c>
       <c r="F72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="G72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="H72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="I72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="J72" s="1" t="str">
@@ -14553,19 +14572,19 @@
         <v>164</v>
       </c>
       <c r="F73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="G73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="H73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="I73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="J73" s="1" t="str">
@@ -14605,19 +14624,19 @@
         <v>160</v>
       </c>
       <c r="F74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="G74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="H74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="I74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="J74" s="1" t="str">
@@ -14654,19 +14673,19 @@
         <v>156</v>
       </c>
       <c r="F75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J75" s="1" t="str">
@@ -14706,19 +14725,19 @@
         <v>152</v>
       </c>
       <c r="F76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyOxymethylene Pellets)</v>
       </c>
       <c r="G76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyOxymethylene Pellets)</v>
       </c>
       <c r="H76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyOxymethylene Pellets)</v>
       </c>
       <c r="I76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyOxymethylene Pellets)</v>
       </c>
       <c r="J76" s="1" t="str">
@@ -14755,19 +14774,19 @@
         <v>148</v>
       </c>
       <c r="F77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J77" s="1" t="str">
@@ -14807,19 +14826,19 @@
         <v>144</v>
       </c>
       <c r="F78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenol Pellets)</v>
       </c>
       <c r="G78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenol Pellets)</v>
       </c>
       <c r="H78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenol Pellets)</v>
       </c>
       <c r="I78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenol Pellets)</v>
       </c>
       <c r="J78" s="1" t="str">
@@ -14856,19 +14875,19 @@
         <v>140</v>
       </c>
       <c r="F79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="G79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="H79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="I79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="J79" s="1" t="str">
@@ -14905,19 +14924,19 @@
         <v>136</v>
       </c>
       <c r="F80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhosphazene Pellets)</v>
       </c>
       <c r="G80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhosphazene Pellets)</v>
       </c>
       <c r="H80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhosphazene Pellets)</v>
       </c>
       <c r="I80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhosphazene Pellets)</v>
       </c>
       <c r="J80" s="1" t="str">
@@ -14954,19 +14973,19 @@
         <v>132</v>
       </c>
       <c r="F81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="G81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="H81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="I81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="J81" s="1" t="str">
@@ -15003,19 +15022,19 @@
         <v>128</v>
       </c>
       <c r="F82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="G82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="H82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="I82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="J82" s="1" t="str">
@@ -15055,19 +15074,19 @@
         <v>124</v>
       </c>
       <c r="F83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="G83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="H83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="I83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="J83" s="1" t="str">
@@ -15107,19 +15126,19 @@
         <v>120</v>
       </c>
       <c r="F84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Pellets)</v>
       </c>
       <c r="G84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Pellets)</v>
       </c>
       <c r="H84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Pellets)</v>
       </c>
       <c r="I84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Pellets)</v>
       </c>
       <c r="J84" s="1" t="str">
@@ -15156,19 +15175,19 @@
         <v>116</v>
       </c>
       <c r="F85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="G85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="H85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="I85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="J85" s="1" t="str">
@@ -15205,19 +15224,19 @@
         <v>112</v>
       </c>
       <c r="F86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="G86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="H86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="I86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="J86" s="1" t="str">
@@ -15257,19 +15276,19 @@
         <v>108</v>
       </c>
       <c r="F87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyStyrene Pellets)</v>
       </c>
       <c r="G87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyStyrene Pellets)</v>
       </c>
       <c r="H87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyStyrene Pellets)</v>
       </c>
       <c r="I87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyStyrene Pellets)</v>
       </c>
       <c r="J87" s="1" t="str">
@@ -15306,19 +15325,19 @@
         <v>104</v>
       </c>
       <c r="F88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J88" s="1" t="str">
@@ -15358,19 +15377,19 @@
         <v>100</v>
       </c>
       <c r="F89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="G89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="H89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="I89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="J89" s="1" t="str">
@@ -15407,19 +15426,19 @@
         <v>96</v>
       </c>
       <c r="F90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="G90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="H90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="I90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="J90" s="1" t="str">
@@ -15456,19 +15475,19 @@
         <v>92</v>
       </c>
       <c r="F91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="G91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="H91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="I91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="J91" s="1" t="str">
@@ -15505,19 +15524,19 @@
         <v>88</v>
       </c>
       <c r="F92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyThiazyl Pellets)</v>
       </c>
       <c r="G92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyThiazyl Pellets)</v>
       </c>
       <c r="H92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyThiazyl Pellets)</v>
       </c>
       <c r="I92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyThiazyl Pellets)</v>
       </c>
       <c r="J92" s="1" t="str">
@@ -15557,19 +15576,19 @@
         <v>84</v>
       </c>
       <c r="F93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="G93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="H93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="I93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="J93" s="1" t="str">
@@ -15609,19 +15628,19 @@
         <v>80</v>
       </c>
       <c r="F94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyUrethane Pellets)</v>
       </c>
       <c r="G94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyUrethane Pellets)</v>
       </c>
       <c r="H94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyUrethane Pellets)</v>
       </c>
       <c r="I94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyUrethane Pellets)</v>
       </c>
       <c r="J94" s="1" t="str">
@@ -15661,19 +15680,19 @@
         <v>76</v>
       </c>
       <c r="F95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="G95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="H95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="I95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="J95" s="1" t="str">
@@ -15713,19 +15732,19 @@
         <v>72</v>
       </c>
       <c r="F96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="G96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="H96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="I96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="J96" s="1" t="str">
@@ -15762,19 +15781,19 @@
         <v>68</v>
       </c>
       <c r="F97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="G97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="H97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="I97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="J97" s="1" t="str">
@@ -15814,19 +15833,19 @@
         <v>64</v>
       </c>
       <c r="F98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="G98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="H98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="I98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="J98" s="1" t="str">
@@ -15866,19 +15885,19 @@
         <v>60</v>
       </c>
       <c r="F99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="G99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="H99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="I99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="J99" s="1" t="str">
@@ -15915,19 +15934,19 @@
         <v>56</v>
       </c>
       <c r="F100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="G100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="H100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="I100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="J100" s="1" t="str">
@@ -15964,19 +15983,19 @@
         <v>52</v>
       </c>
       <c r="F101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="G101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="H101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="I101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="J101" s="1" t="str">
@@ -16013,19 +16032,19 @@
         <v>48</v>
       </c>
       <c r="F102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="G102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="H102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="I102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="J102" s="1" t="str">
@@ -16062,19 +16081,19 @@
         <v>44</v>
       </c>
       <c r="F103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="G103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="H103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="I103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="J103" s="1" t="str">
@@ -16111,19 +16130,19 @@
         <v>40</v>
       </c>
       <c r="F104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="G104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="H104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="I104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="J104" s="1" t="str">
@@ -16160,19 +16179,19 @@
         <v>36</v>
       </c>
       <c r="F105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="G105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="H105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="I105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="J105" s="1" t="str">
@@ -16212,19 +16231,19 @@
         <v>32</v>
       </c>
       <c r="F106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="G106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="H106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="I106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="J106" s="1" t="str">
@@ -16264,19 +16283,19 @@
         <v>28</v>
       </c>
       <c r="F107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J107" s="1" t="str">
@@ -16316,19 +16335,19 @@
         <v>24</v>
       </c>
       <c r="F108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J108" s="1" t="str">
@@ -16368,19 +16387,19 @@
         <v>20</v>
       </c>
       <c r="F109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="G109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="H109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="I109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="J109" s="1" t="str">
@@ -16417,19 +16436,19 @@
         <v>16</v>
       </c>
       <c r="F110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="G110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="H110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="I110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="J110" s="1" t="str">
@@ -16469,19 +16488,19 @@
         <v>12</v>
       </c>
       <c r="F111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="G111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="H111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="I111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="J111" s="1" t="str">
@@ -16518,19 +16537,19 @@
         <v>8</v>
       </c>
       <c r="F112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="G112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="H112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="I112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="J112" s="1" t="str">
@@ -16570,19 +16589,19 @@
         <v>4</v>
       </c>
       <c r="F113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J113" s="1" t="str">
@@ -16622,19 +16641,19 @@
         <v>0</v>
       </c>
       <c r="F114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="G114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="H114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="I114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="J114" s="1" t="str">
@@ -16674,19 +16693,19 @@
         <v>1853</v>
       </c>
       <c r="F115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Polycaprolactam Pellets)</v>
       </c>
       <c r="G115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Polycaprolactam Pellets)</v>
       </c>
       <c r="H115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Polycaprolactam Pellets)</v>
       </c>
       <c r="I115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Polycaprolactam Pellets)</v>
       </c>
       <c r="J115" s="1" t="str">
@@ -16726,19 +16745,19 @@
         <v>2412</v>
       </c>
       <c r="F116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="G116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="H116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="I116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="J116" s="1" t="str">
@@ -16778,19 +16797,19 @@
         <v>2416</v>
       </c>
       <c r="F117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="G117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="H117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="I117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="J117" s="1" t="str">
@@ -16830,19 +16849,19 @@
         <v>2420</v>
       </c>
       <c r="F118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Negative Photoresist)</v>
       </c>
       <c r="G118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Negative Photoresist)</v>
       </c>
       <c r="H118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Negative Photoresist)</v>
       </c>
       <c r="I118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Negative Photoresist)</v>
       </c>
       <c r="J118" s="1" t="str">
@@ -16882,19 +16901,19 @@
         <v>2424</v>
       </c>
       <c r="F119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Positive Photoresist)</v>
       </c>
       <c r="G119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Positive Photoresist)</v>
       </c>
       <c r="H119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Positive Photoresist)</v>
       </c>
       <c r="I119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Positive Photoresist)</v>
       </c>
       <c r="J119" s="1" t="str">
@@ -17809,11 +17828,11 @@
         <v>2651</v>
       </c>
       <c r="C1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="D1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$79</f>
+        <f xml:space="preserve"> [1]Enums!$B$80</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="19" t="str">
@@ -17849,7 +17868,7 @@
         <v>Mask (Solar Cell)[PR Backplane]</v>
       </c>
       <c r="D2" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E2" s="15" t="str">
@@ -17873,7 +17892,7 @@
         <v>Mask (Solar Cell)[PR Semiconductor]</v>
       </c>
       <c r="D3" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E3" s="15" t="str">
@@ -17897,7 +17916,7 @@
         <v>Mask (Solar Cell)[PR Dielectric]</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E4" s="15" t="str">
@@ -17921,7 +17940,7 @@
         <v>Mask (Solar Cell)[PR Traces]</v>
       </c>
       <c r="D5" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E5" s="15" t="str">
@@ -17945,7 +17964,7 @@
         <v>Mask (Solar Cell)[PR Encapsulation]</v>
       </c>
       <c r="D6" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E6" s="15" t="str">
@@ -17969,7 +17988,7 @@
         <v>Mask (Processor)[PR Backplane]</v>
       </c>
       <c r="D7" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E7" s="15" t="str">
@@ -17993,7 +18012,7 @@
         <v>Mask (Processor)[PR n-Type Semiconductor]</v>
       </c>
       <c r="D8" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E8" s="15" t="str">
@@ -18017,7 +18036,7 @@
         <v>Mask (Processor)[PR p-Type Semiconductor]</v>
       </c>
       <c r="D9" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E9" s="15" t="str">
@@ -18041,7 +18060,7 @@
         <v>Mask (Processor)[PR Dielectric]</v>
       </c>
       <c r="D10" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E10" s="15" t="str">
@@ -18065,7 +18084,7 @@
         <v>Mask (Processor)[PR Inner Traces]</v>
       </c>
       <c r="D11" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E11" s="15" t="str">
@@ -18089,7 +18108,7 @@
         <v>Mask (Processor)[PR Through Vias]</v>
       </c>
       <c r="D12" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E12" s="15" t="str">
@@ -18113,7 +18132,7 @@
         <v>Mask (Processor)[PR Outer Traces]</v>
       </c>
       <c r="D13" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E13" s="15" t="str">
@@ -18137,7 +18156,7 @@
         <v>Mask (Processor)[PR Encapsulation]</v>
       </c>
       <c r="D14" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E14" s="15" t="str">
@@ -18161,7 +18180,7 @@
         <v>Mask (Temperature Sensor)[PR Backplane]</v>
       </c>
       <c r="D15" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E15" s="15" t="str">
@@ -18185,7 +18204,7 @@
         <v>Mask (Temperature Sensor)[PR Semiconductor]</v>
       </c>
       <c r="D16" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E16" s="15" t="str">
@@ -18209,7 +18228,7 @@
         <v>Mask (Temperature Sensor)[PR Dielectric]</v>
       </c>
       <c r="D17" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E17" s="15" t="str">
@@ -18233,7 +18252,7 @@
         <v>Mask (Temperature Sensor)[PR Traces]</v>
       </c>
       <c r="D18" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E18" s="15" t="str">
@@ -18257,7 +18276,7 @@
         <v>Mask (Temperature Sensor)[PR Encapsulation]</v>
       </c>
       <c r="D19" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E19" s="15" t="str">
@@ -18281,7 +18300,7 @@
         <v>Mask (Pressure Sensor)[PR Backplane]</v>
       </c>
       <c r="D20" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E20" s="15" t="str">
@@ -18305,7 +18324,7 @@
         <v>Mask (Pressure Sensor)[PR Semiconductor]</v>
       </c>
       <c r="D21" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E21" s="15" t="str">
@@ -18329,7 +18348,7 @@
         <v>Mask (Pressure Sensor)[PR Dielectric]</v>
       </c>
       <c r="D22" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E22" s="15" t="str">
@@ -18353,7 +18372,7 @@
         <v>Mask (Pressure Sensor)[PR Traces]</v>
       </c>
       <c r="D23" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E23" s="15" t="str">
@@ -18377,7 +18396,7 @@
         <v>Mask (Pressure Sensor)[PR Encapsulation]</v>
       </c>
       <c r="D24" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E24" s="15" t="str">
@@ -18401,7 +18420,7 @@
         <v>Mask (Low Power Radio)[PR Backplane]</v>
       </c>
       <c r="D25" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E25" s="15" t="str">
@@ -18425,7 +18444,7 @@
         <v>Mask (Low Power Radio)[PR n-Type Semiconductor]</v>
       </c>
       <c r="D26" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E26" s="15" t="str">
@@ -18449,7 +18468,7 @@
         <v>Mask (Low Power Radio)[PR p-Type Semiconductor]</v>
       </c>
       <c r="D27" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E27" s="15" t="str">
@@ -18473,7 +18492,7 @@
         <v>Mask (Low Power Radio)[PR Dielectric]</v>
       </c>
       <c r="D28" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E28" s="15" t="str">
@@ -18497,7 +18516,7 @@
         <v>Mask (Low Power Radio)[PR Inner Traces]</v>
       </c>
       <c r="D29" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E29" s="15" t="str">
@@ -18521,7 +18540,7 @@
         <v>Mask (Low Power Radio)[PR Through Vias]</v>
       </c>
       <c r="D30" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E30" s="15" t="str">
@@ -18545,7 +18564,7 @@
         <v>Mask (Low Power Radio)[PR Outer Traces]</v>
       </c>
       <c r="D31" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E31" s="15" t="str">
@@ -18569,7 +18588,7 @@
         <v>Mask (Low Power Radio)[PR Encapsulation]</v>
       </c>
       <c r="D32" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E32" s="15" t="str">
@@ -18593,7 +18612,7 @@
         <v>Mask (DSP)[PR Backplane]</v>
       </c>
       <c r="D33" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E33" s="15" t="str">
@@ -18617,7 +18636,7 @@
         <v>Mask (DSP)[PR n-Type Semiconductor]</v>
       </c>
       <c r="D34" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E34" s="15" t="str">
@@ -18641,7 +18660,7 @@
         <v>Mask (DSP)[PR p-Type Semiconductor]</v>
       </c>
       <c r="D35" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E35" s="15" t="str">
@@ -18665,7 +18684,7 @@
         <v>Mask (DSP)[PR Dielectric]</v>
       </c>
       <c r="D36" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E36" s="15" t="str">
@@ -18689,7 +18708,7 @@
         <v>Mask (DSP)[PR Inner Traces]</v>
       </c>
       <c r="D37" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E37" s="15" t="str">
@@ -18713,7 +18732,7 @@
         <v>Mask (DSP)[PR Through Vias]</v>
       </c>
       <c r="D38" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E38" s="15" t="str">
@@ -18737,7 +18756,7 @@
         <v>Mask (DSP)[PR Outer Traces]</v>
       </c>
       <c r="D39" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E39" s="15" t="str">
@@ -18761,7 +18780,7 @@
         <v>Mask (DSP)[PR Encapsulation]</v>
       </c>
       <c r="D40" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E40" s="15" t="str">
@@ -18785,7 +18804,7 @@
         <v>Mask (Digital Analog Convertor)[PR Backplane]</v>
       </c>
       <c r="D41" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E41" s="15" t="str">
@@ -18809,7 +18828,7 @@
         <v>Mask (Digital Analog Convertor)[PR Semiconductor]</v>
       </c>
       <c r="D42" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E42" s="15" t="str">
@@ -18833,7 +18852,7 @@
         <v>Mask (Digital Analog Convertor)[PR Dielectric]</v>
       </c>
       <c r="D43" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E43" s="15" t="str">
@@ -18857,7 +18876,7 @@
         <v>Mask (Digital Analog Convertor)[PR Traces]</v>
       </c>
       <c r="D44" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E44" s="15" t="str">
@@ -18881,7 +18900,7 @@
         <v>Mask (Digital Analog Convertor)[PR Encapsulation]</v>
       </c>
       <c r="D45" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E45" s="15" t="str">
@@ -18905,7 +18924,7 @@
         <v>Mask (Amplifier)[PR Backplane]</v>
       </c>
       <c r="D46" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E46" s="15" t="str">
@@ -18929,7 +18948,7 @@
         <v>Mask (Amplifier)[PR Semiconductor]</v>
       </c>
       <c r="D47" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E47" s="15" t="str">
@@ -18953,7 +18972,7 @@
         <v>Mask (Amplifier)[PR Dielectric]</v>
       </c>
       <c r="D48" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E48" s="15" t="str">
@@ -18977,7 +18996,7 @@
         <v>Mask (Amplifier)[PR Traces]</v>
       </c>
       <c r="D49" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E49" s="15" t="str">
@@ -19001,7 +19020,7 @@
         <v>Mask (Amplifier)[PR Encapsulation]</v>
       </c>
       <c r="D50" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E50" s="15" t="str">
@@ -19025,7 +19044,7 @@
         <v>Mask (OLED Array)[PR Backplane]</v>
       </c>
       <c r="D51" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E51" s="15" t="str">
@@ -19049,7 +19068,7 @@
         <v>Mask (OLED Array)[PR Semiconductor]</v>
       </c>
       <c r="D52" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E52" s="15" t="str">
@@ -19073,7 +19092,7 @@
         <v>Mask (OLED Array)[PR Dielectric]</v>
       </c>
       <c r="D53" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E53" s="15" t="str">
@@ -19097,7 +19116,7 @@
         <v>Mask (OLED Array)[PR Traces]</v>
       </c>
       <c r="D54" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E54" s="15" t="str">
@@ -19121,7 +19140,7 @@
         <v>Mask (OLED Array)[PR Encapsulation]</v>
       </c>
       <c r="D55" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$93</f>
         <v>Mask</v>
       </c>
       <c r="E55" s="15" t="str">
@@ -19174,7 +19193,7 @@
   </sheetPr>
   <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -25388,7 +25407,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I2" s="45" t="str">
-        <f>[1]Enums!$A$145&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Steel</v>
       </c>
       <c r="J2" s="45">
@@ -25436,7 +25455,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I3" s="45" t="str">
-        <f>[1]Enums!$A$145&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Stainless Steel</v>
       </c>
       <c r="J3" s="45">
@@ -25484,7 +25503,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I4" s="45" t="str">
-        <f>[1]Enums!$A$145&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Brass</v>
       </c>
       <c r="J4" s="45">
@@ -25532,7 +25551,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I5" s="45" t="str">
-        <f>[1]Enums!$A$145&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Bronze</v>
       </c>
       <c r="J5" s="45">
@@ -25580,7 +25599,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I6" s="45" t="str">
-        <f>[1]Enums!$A$145&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Tungsten Carbide</v>
       </c>
       <c r="J6" s="45">
@@ -25628,7 +25647,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I7" s="45" t="str">
-        <f>[1]Enums!$A$145&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Nichrome</v>
       </c>
       <c r="J7" s="45">
@@ -25676,7 +25695,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I8" s="45" t="str">
-        <f>[1]Enums!$A$145&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Antimony-Lead</v>
       </c>
       <c r="J8" s="45">
@@ -25724,7 +25743,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I9" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Steel</v>
       </c>
       <c r="J9" s="45">
@@ -25772,7 +25791,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I10" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Stainless Steel</v>
       </c>
       <c r="J10" s="45">
@@ -25820,7 +25839,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I11" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Brass</v>
       </c>
       <c r="J11" s="45">
@@ -25868,7 +25887,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I12" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Bronze</v>
       </c>
       <c r="J12" s="45">
@@ -25916,7 +25935,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I13" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Tungsten Carbide</v>
       </c>
       <c r="J13" s="45">
@@ -25964,7 +25983,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I14" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Nichrome</v>
       </c>
       <c r="J14" s="45">
@@ -26012,7 +26031,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I15" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Antimony-Lead</v>
       </c>
       <c r="J15" s="45">
@@ -26060,7 +26079,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I16" s="45" t="str">
-        <f>[1]Enums!$A$145&amp;" Iron"</f>
+        <f>[1]Enums!$A$146&amp;" Iron"</f>
         <v>Composite Iron</v>
       </c>
       <c r="J16" s="45">
@@ -26108,7 +26127,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I17" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" Iron"</f>
+        <f>[1]Enums!$A$147&amp;" Iron"</f>
         <v>Engineered Iron</v>
       </c>
       <c r="J17" s="45">
@@ -26156,7 +26175,7 @@
         <v>Diamond</v>
       </c>
       <c r="I18" s="45" t="str">
-        <f>[1]Enums!$A$145&amp;" Diamond"</f>
+        <f>[1]Enums!$A$146&amp;" Diamond"</f>
         <v>Composite Diamond</v>
       </c>
       <c r="J18" s="45">
@@ -26204,7 +26223,7 @@
         <v>Diamond</v>
       </c>
       <c r="I19" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" Diamond"</f>
+        <f>[1]Enums!$A$147&amp;" Diamond"</f>
         <v>Engineered Diamond</v>
       </c>
       <c r="J19" s="45">
@@ -26505,7 +26524,7 @@
         <v>Molded Item</v>
       </c>
       <c r="F1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$110</f>
+        <f xml:space="preserve"> [1]Enums!$A$111</f>
         <v>Base Material</v>
       </c>
       <c r="G1" s="30" t="s">
@@ -26533,7 +26552,7 @@
         <v>1812</v>
       </c>
       <c r="C2" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D2</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D2</f>
         <v>Gripped Iron Shovel</v>
       </c>
       <c r="D2" s="24" t="str">
@@ -26545,7 +26564,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F2" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$114</f>
         <v>Iron</v>
       </c>
       <c r="G2" s="24">
@@ -26570,7 +26589,7 @@
         <v>1811</v>
       </c>
       <c r="C3" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D3</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D3</f>
         <v>Gripped Iron Pickaxe</v>
       </c>
       <c r="D3" s="21" t="str">
@@ -26582,7 +26601,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F3" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$114</f>
         <v>Iron</v>
       </c>
       <c r="G3" s="24">
@@ -26607,7 +26626,7 @@
         <v>1810</v>
       </c>
       <c r="C4" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D4</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D4</f>
         <v>Gripped Iron Axe</v>
       </c>
       <c r="D4" s="21" t="str">
@@ -26619,7 +26638,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F4" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$114</f>
         <v>Iron</v>
       </c>
       <c r="G4" s="24">
@@ -26644,7 +26663,7 @@
         <v>1809</v>
       </c>
       <c r="C5" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D5</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D5</f>
         <v>Gripped Iron Sword</v>
       </c>
       <c r="D5" s="21" t="str">
@@ -26656,7 +26675,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F5" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$114</f>
         <v>Iron</v>
       </c>
       <c r="G5" s="24">
@@ -26681,7 +26700,7 @@
         <v>1808</v>
       </c>
       <c r="C6" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D6</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D6</f>
         <v>Gripped Wooden Sword</v>
       </c>
       <c r="D6" s="21" t="str">
@@ -26693,7 +26712,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F6" s="34" t="str">
-        <f>[1]Enums!$A$111</f>
+        <f>[1]Enums!$A$112</f>
         <v>Wooden</v>
       </c>
       <c r="G6" s="24">
@@ -26718,7 +26737,7 @@
         <v>1807</v>
       </c>
       <c r="C7" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D7</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D7</f>
         <v>Gripped Wooden Shovel</v>
       </c>
       <c r="D7" s="21" t="str">
@@ -26730,7 +26749,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F7" s="34" t="str">
-        <f>[1]Enums!$A$111</f>
+        <f>[1]Enums!$A$112</f>
         <v>Wooden</v>
       </c>
       <c r="G7" s="24">
@@ -26755,7 +26774,7 @@
         <v>1806</v>
       </c>
       <c r="C8" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D8</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D8</f>
         <v>Gripped Wooden Pickaxe</v>
       </c>
       <c r="D8" s="21" t="str">
@@ -26767,7 +26786,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F8" s="34" t="str">
-        <f>[1]Enums!$A$111</f>
+        <f>[1]Enums!$A$112</f>
         <v>Wooden</v>
       </c>
       <c r="G8" s="24">
@@ -26792,7 +26811,7 @@
         <v>1805</v>
       </c>
       <c r="C9" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D9</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D9</f>
         <v>Gripped Wooden Axe</v>
       </c>
       <c r="D9" s="21" t="str">
@@ -26804,7 +26823,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F9" s="34" t="str">
-        <f>[1]Enums!$A$111</f>
+        <f>[1]Enums!$A$112</f>
         <v>Wooden</v>
       </c>
       <c r="G9" s="24">
@@ -26829,7 +26848,7 @@
         <v>1804</v>
       </c>
       <c r="C10" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D10</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D10</f>
         <v>Gripped Stone Sword</v>
       </c>
       <c r="D10" s="21" t="str">
@@ -26841,7 +26860,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F10" s="34" t="str">
-        <f>[1]Enums!$A$112</f>
+        <f>[1]Enums!$A$113</f>
         <v>Stone</v>
       </c>
       <c r="G10" s="24">
@@ -26866,7 +26885,7 @@
         <v>1803</v>
       </c>
       <c r="C11" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D11</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D11</f>
         <v>Gripped Stone Shovel</v>
       </c>
       <c r="D11" s="21" t="str">
@@ -26878,7 +26897,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F11" s="34" t="str">
-        <f>[1]Enums!$A$112</f>
+        <f>[1]Enums!$A$113</f>
         <v>Stone</v>
       </c>
       <c r="G11" s="24">
@@ -26903,7 +26922,7 @@
         <v>1802</v>
       </c>
       <c r="C12" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D12</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D12</f>
         <v>Gripped Stone Pickaxe</v>
       </c>
       <c r="D12" s="21" t="str">
@@ -26915,7 +26934,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F12" s="34" t="str">
-        <f>[1]Enums!$A$112</f>
+        <f>[1]Enums!$A$113</f>
         <v>Stone</v>
       </c>
       <c r="G12" s="24">
@@ -26940,7 +26959,7 @@
         <v>1801</v>
       </c>
       <c r="C13" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D13</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D13</f>
         <v>Gripped Stone Axe</v>
       </c>
       <c r="D13" s="21" t="str">
@@ -26952,7 +26971,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F13" s="34" t="str">
-        <f>[1]Enums!$A$112</f>
+        <f>[1]Enums!$A$113</f>
         <v>Stone</v>
       </c>
       <c r="G13" s="24">
@@ -26977,7 +26996,7 @@
         <v>1800</v>
       </c>
       <c r="C14" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D14</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D14</f>
         <v>Gripped Diamond Sword</v>
       </c>
       <c r="D14" s="21" t="str">
@@ -26989,7 +27008,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F14" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Diamond</v>
       </c>
       <c r="G14" s="24">
@@ -27014,7 +27033,7 @@
         <v>1799</v>
       </c>
       <c r="C15" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D15</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D15</f>
         <v>Gripped Diamond Shovel</v>
       </c>
       <c r="D15" s="21" t="str">
@@ -27026,7 +27045,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F15" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Diamond</v>
       </c>
       <c r="G15" s="24">
@@ -27051,7 +27070,7 @@
         <v>1798</v>
       </c>
       <c r="C16" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D16</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D16</f>
         <v>Gripped Diamond Pickaxe</v>
       </c>
       <c r="D16" s="21" t="str">
@@ -27063,7 +27082,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F16" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Diamond</v>
       </c>
       <c r="G16" s="24">
@@ -27088,7 +27107,7 @@
         <v>1797</v>
       </c>
       <c r="C17" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D17</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D17</f>
         <v>Gripped Diamond Axe</v>
       </c>
       <c r="D17" s="21" t="str">
@@ -27100,7 +27119,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F17" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Diamond</v>
       </c>
       <c r="G17" s="24">
@@ -27125,7 +27144,7 @@
         <v>1796</v>
       </c>
       <c r="C18" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D18</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D18</f>
         <v>Gripped Golden Sword</v>
       </c>
       <c r="D18" s="21" t="str">
@@ -27137,7 +27156,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F18" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$115</f>
         <v>Golden</v>
       </c>
       <c r="G18" s="24">
@@ -27162,7 +27181,7 @@
         <v>1795</v>
       </c>
       <c r="C19" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D19</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D19</f>
         <v>Gripped Golden Shovel</v>
       </c>
       <c r="D19" s="21" t="str">
@@ -27174,7 +27193,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F19" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$115</f>
         <v>Golden</v>
       </c>
       <c r="G19" s="24">
@@ -27199,7 +27218,7 @@
         <v>1794</v>
       </c>
       <c r="C20" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D20</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D20</f>
         <v>Gripped Golden Pickaxe</v>
       </c>
       <c r="D20" s="21" t="str">
@@ -27211,7 +27230,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F20" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$115</f>
         <v>Golden</v>
       </c>
       <c r="G20" s="24">
@@ -27236,7 +27255,7 @@
         <v>1793</v>
       </c>
       <c r="C21" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D21</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D21</f>
         <v>Gripped Golden Axe</v>
       </c>
       <c r="D21" s="21" t="str">
@@ -27248,7 +27267,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F21" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$115</f>
         <v>Golden</v>
       </c>
       <c r="G21" s="24">
@@ -27273,7 +27292,7 @@
         <v>1792</v>
       </c>
       <c r="C22" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D22</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D22</f>
         <v>Gripped Wooden Hoe</v>
       </c>
       <c r="D22" s="21" t="str">
@@ -27285,7 +27304,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F22" s="34" t="str">
-        <f>[1]Enums!$A$111</f>
+        <f>[1]Enums!$A$112</f>
         <v>Wooden</v>
       </c>
       <c r="G22" s="24">
@@ -27310,7 +27329,7 @@
         <v>1791</v>
       </c>
       <c r="C23" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D23</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D23</f>
         <v>Gripped Stone Hoe</v>
       </c>
       <c r="D23" s="21" t="str">
@@ -27322,7 +27341,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F23" s="34" t="str">
-        <f>[1]Enums!$A$112</f>
+        <f>[1]Enums!$A$113</f>
         <v>Stone</v>
       </c>
       <c r="G23" s="24">
@@ -27347,7 +27366,7 @@
         <v>1790</v>
       </c>
       <c r="C24" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D24</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D24</f>
         <v>Gripped Iron Hoe</v>
       </c>
       <c r="D24" s="21" t="str">
@@ -27359,7 +27378,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F24" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$114</f>
         <v>Iron</v>
       </c>
       <c r="G24" s="24">
@@ -27384,7 +27403,7 @@
         <v>1789</v>
       </c>
       <c r="C25" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D25</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D25</f>
         <v>Gripped Diamond Hoe</v>
       </c>
       <c r="D25" s="21" t="str">
@@ -27396,7 +27415,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F25" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Diamond</v>
       </c>
       <c r="G25" s="24">
@@ -27421,7 +27440,7 @@
         <v>1788</v>
       </c>
       <c r="C26" s="22" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;D26</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;D26</f>
         <v>Gripped Golden Hoe</v>
       </c>
       <c r="D26" s="21" t="str">
@@ -27433,7 +27452,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F26" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$115</f>
         <v>Golden</v>
       </c>
       <c r="G26" s="24">
@@ -27495,7 +27514,7 @@
         <v>1832</v>
       </c>
       <c r="D1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$110</f>
+        <f xml:space="preserve"> [1]Enums!$A$111</f>
         <v>Base Material</v>
       </c>
       <c r="E1" s="36" t="s">
@@ -27541,7 +27560,7 @@
         <v>Wooden Pogo Stick</v>
       </c>
       <c r="D2" s="34" t="str">
-        <f>[1]Enums!$A$111</f>
+        <f>[1]Enums!$A$112</f>
         <v>Wooden</v>
       </c>
       <c r="E2" s="37">
@@ -27578,7 +27597,7 @@
         <v>Stone Pogo Stick</v>
       </c>
       <c r="D3" s="34" t="str">
-        <f>[1]Enums!$A$112</f>
+        <f>[1]Enums!$A$113</f>
         <v>Stone</v>
       </c>
       <c r="E3" s="37">
@@ -27614,7 +27633,7 @@
         <v>Iron Pogo Stick</v>
       </c>
       <c r="D4" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$114</f>
         <v>Iron</v>
       </c>
       <c r="E4" s="37">
@@ -27650,7 +27669,7 @@
         <v>Golden Pogo Stick</v>
       </c>
       <c r="D5" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$115</f>
         <v>Golden</v>
       </c>
       <c r="E5" s="37">
@@ -27686,7 +27705,7 @@
         <v>Diamond Pogo Stick</v>
       </c>
       <c r="D6" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Diamond</v>
       </c>
       <c r="E6" s="37">
@@ -27722,7 +27741,7 @@
         <v>Magic Pogo Stick</v>
       </c>
       <c r="D7" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$117</f>
         <v>Magic</v>
       </c>
       <c r="E7" s="37">
@@ -27754,11 +27773,11 @@
         <v>1821</v>
       </c>
       <c r="C8" s="34" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;I8</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;I8</f>
         <v>Gripped Wooden Pogo Stick</v>
       </c>
       <c r="D8" s="34" t="str">
-        <f>[1]Enums!$A$111</f>
+        <f>[1]Enums!$A$112</f>
         <v>Wooden</v>
       </c>
       <c r="E8" s="37">
@@ -27798,11 +27817,11 @@
         <v>1820</v>
       </c>
       <c r="C9" s="34" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;I9</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;I9</f>
         <v>Gripped Stone Pogo Stick</v>
       </c>
       <c r="D9" s="34" t="str">
-        <f>[1]Enums!$A$112</f>
+        <f>[1]Enums!$A$113</f>
         <v>Stone</v>
       </c>
       <c r="E9" s="37">
@@ -27842,11 +27861,11 @@
         <v>1819</v>
       </c>
       <c r="C10" s="34" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;I10</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;I10</f>
         <v>Gripped Iron Pogo Stick</v>
       </c>
       <c r="D10" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$114</f>
         <v>Iron</v>
       </c>
       <c r="E10" s="37">
@@ -27886,11 +27905,11 @@
         <v>1818</v>
       </c>
       <c r="C11" s="34" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;I11</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;I11</f>
         <v>Gripped Golden Pogo Stick</v>
       </c>
       <c r="D11" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$115</f>
         <v>Golden</v>
       </c>
       <c r="E11" s="37">
@@ -27930,11 +27949,11 @@
         <v>1817</v>
       </c>
       <c r="C12" s="34" t="str">
-        <f>[1]Enums!$A$107&amp;" "&amp;I12</f>
+        <f>[1]Enums!$A$108&amp;" "&amp;I12</f>
         <v>Gripped Diamond Pogo Stick</v>
       </c>
       <c r="D12" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Diamond</v>
       </c>
       <c r="E12" s="37">
@@ -46325,10 +46344,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -46352,7 +46371,7 @@
         <v>590</v>
       </c>
       <c r="D1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$79</f>
+        <f xml:space="preserve"> [1]Enums!$B$80</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="19" t="str">
@@ -46372,11 +46391,11 @@
         <v>1756</v>
       </c>
       <c r="C2" s="10" t="str">
-        <f t="shared" ref="C2:C33" si="0">D2&amp;" ("&amp;E2&amp;")"</f>
+        <f t="shared" ref="C2:C32" si="0">D2&amp;" ("&amp;E2&amp;")"</f>
         <v>Mold (Grip)</v>
       </c>
       <c r="D2" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E2" s="11" t="str">
@@ -46401,7 +46420,7 @@
         <v>Mold (Running Shoes)</v>
       </c>
       <c r="D3" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E3" s="11" t="str">
@@ -46426,7 +46445,7 @@
         <v>Mold (Scuba Fins)</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E4" s="11" t="str">
@@ -46451,7 +46470,7 @@
         <v>Mold (Scuba Mask)</v>
       </c>
       <c r="D5" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E5" s="11" t="str">
@@ -46476,7 +46495,7 @@
         <v>Mold (Gasket)</v>
       </c>
       <c r="D6" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E6" s="11" t="str">
@@ -46501,7 +46520,7 @@
         <v>Mold (Life Preserver)</v>
       </c>
       <c r="D7" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E7" s="11" t="str">
@@ -46526,7 +46545,7 @@
         <v>Metal Die (Fibers)</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$85</f>
         <v>Metal Die</v>
       </c>
       <c r="E8" s="11" t="str">
@@ -46551,7 +46570,7 @@
         <v>Metal Die (Tether)</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$85</f>
         <v>Metal Die</v>
       </c>
       <c r="E9" s="11" t="str">
@@ -46576,7 +46595,7 @@
         <v>Metal Die (Cord)</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$85</f>
         <v>Metal Die</v>
       </c>
       <c r="E10" s="11" t="str">
@@ -46601,7 +46620,7 @@
         <v>Metal Die (Hose)</v>
       </c>
       <c r="D11" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$85</f>
         <v>Metal Die</v>
       </c>
       <c r="E11" s="11" t="str">
@@ -46626,7 +46645,7 @@
         <v>Metal Die (Pipe Segment)</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$85</f>
         <v>Metal Die</v>
       </c>
       <c r="E12" s="11" t="str">
@@ -46651,7 +46670,7 @@
         <v>Mold (Flashlight Shaft)</v>
       </c>
       <c r="D13" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E13" s="11" t="str">
@@ -46675,7 +46694,7 @@
         <v>Mold (Plastic Brick (1 x 1))</v>
       </c>
       <c r="D14" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E14" t="str">
@@ -46699,7 +46718,7 @@
         <v>Mold (Plastic Brick (1 x 2))</v>
       </c>
       <c r="D15" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E15" t="str">
@@ -46723,7 +46742,7 @@
         <v>Mold (Plastic Brick (1 x 3))</v>
       </c>
       <c r="D16" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E16" t="str">
@@ -46747,7 +46766,7 @@
         <v>Mold (Plastic Brick (1 x 4))</v>
       </c>
       <c r="D17" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E17" t="str">
@@ -46771,7 +46790,7 @@
         <v>Mold (Plastic Brick (2 x 2))</v>
       </c>
       <c r="D18" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E18" t="str">
@@ -46795,7 +46814,7 @@
         <v>Mold (Plastic Brick (2 x 3))</v>
       </c>
       <c r="D19" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E19" t="str">
@@ -46819,7 +46838,7 @@
         <v>Mold (Plastic Brick (2 x 4))</v>
       </c>
       <c r="D20" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E20" t="str">
@@ -46843,7 +46862,7 @@
         <v>Mold (Plastic Brick (3 x 3))</v>
       </c>
       <c r="D21" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E21" t="str">
@@ -46867,7 +46886,7 @@
         <v>Mold (Plastic Brick (3 x 4))</v>
       </c>
       <c r="D22" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E22" t="str">
@@ -46891,7 +46910,7 @@
         <v>Mold (Plastic Brick (4 x 4))</v>
       </c>
       <c r="D23" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E23" t="str">
@@ -46915,7 +46934,7 @@
         <v>Mold (Plastic Brick (1 x 8))</v>
       </c>
       <c r="D24" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E24" t="str">
@@ -46939,7 +46958,7 @@
         <v>Mold (Plastic Brick (2 x 8))</v>
       </c>
       <c r="D25" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E25" t="str">
@@ -46963,7 +46982,7 @@
         <v>Mold (Heated Knife Handle)</v>
       </c>
       <c r="D26" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E26" s="11" t="str">
@@ -46987,7 +47006,7 @@
         <v>Mold (Rubber Sole)</v>
       </c>
       <c r="D27" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E27" s="11" t="str">
@@ -47011,7 +47030,7 @@
         <v>Mold (Battery Case)</v>
       </c>
       <c r="D28" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E28" s="11" t="str">
@@ -47035,7 +47054,7 @@
         <v>Mold (Tool Shaft)</v>
       </c>
       <c r="D29" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E29" t="str">
@@ -47059,7 +47078,7 @@
         <v>Mold (Lighter Body)</v>
       </c>
       <c r="D30" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E30" t="str">
@@ -47083,7 +47102,7 @@
         <v>Mold (Cell Phone Case)</v>
       </c>
       <c r="D31" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E31" t="str">
@@ -47107,7 +47126,7 @@
         <v>Mold (Walky Talky Case)</v>
       </c>
       <c r="D32" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E32" t="str">
@@ -47127,11 +47146,11 @@
         <v>2689</v>
       </c>
       <c r="C33" s="10" t="str">
-        <f t="shared" si="0"/>
+        <f>D33&amp;" ("&amp;E33&amp;")"</f>
         <v>Mold (HAM Radio Case)</v>
       </c>
       <c r="D33" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold</v>
       </c>
       <c r="E33" t="str">
@@ -47139,6 +47158,30 @@
         <v>HAM Radio Case</v>
       </c>
       <c r="F33">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="str">
+        <f>[1]Enums!$A$22</f>
+        <v>1.3.3</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C34" s="10" t="str">
+        <f>D34&amp;" ("&amp;E34&amp;")"</f>
+        <v>Mold (Flagpole Segment)</v>
+      </c>
+      <c r="D34" s="10" t="str">
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <v>Mold</v>
+      </c>
+      <c r="E34" t="str">
+        <f>'[1]Polymer Objects'!$B34</f>
+        <v>Flagpole Segment</v>
+      </c>
+      <c r="F34">
         <v>8192</v>
       </c>
     </row>
@@ -47152,10 +47195,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:U156"/>
+  <dimension ref="A1:U157"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="I140" sqref="I140"/>
+    <sheetView showZeros="0" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="H162" sqref="H162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -53468,8 +53511,85 @@
       </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A156" s="23"/>
-      <c r="C156" s="22"/>
+      <c r="A156" s="23" t="str">
+        <f>[1]Enums!$A$22</f>
+        <v>1.3.3</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>2709</v>
+      </c>
+      <c r="C156" s="22" t="str">
+        <f xml:space="preserve"> VLOOKUP(D156, Molds!C:E, 3, FALSE)&amp;" ("&amp;F156&amp;")"</f>
+        <v>Flagpole Segment (PEEK)</v>
+      </c>
+      <c r="D156" s="24" t="str">
+        <f xml:space="preserve"> Molds!$C$34</f>
+        <v>Mold (Flagpole Segment)</v>
+      </c>
+      <c r="E156" s="21" t="str">
+        <f>Pellets!$F$47</f>
+        <v>Bag (PolyEther Ether Ketone Pellets)</v>
+      </c>
+      <c r="F156" s="21" t="str">
+        <f>VLOOKUP(E80, Pellets!F:M,8,FALSE)</f>
+        <v>PEEK</v>
+      </c>
+      <c r="G156" s="21">
+        <v>8</v>
+      </c>
+      <c r="H156" s="21">
+        <v>10</v>
+      </c>
+      <c r="I156" s="21">
+        <v>64</v>
+      </c>
+      <c r="J156" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A157" s="23" t="str">
+        <f>[1]Enums!$A$22</f>
+        <v>1.3.3</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>2710</v>
+      </c>
+      <c r="C157" s="22" t="str">
+        <f xml:space="preserve"> VLOOKUP(D157, Molds!C:E, 3, FALSE)&amp;" ("&amp;F157&amp;")"</f>
+        <v>Flagpole Segment (Carbon Fiber Composite)</v>
+      </c>
+      <c r="D157" s="24" t="str">
+        <f xml:space="preserve"> Molds!$C$34</f>
+        <v>Mold (Flagpole Segment)</v>
+      </c>
+      <c r="E157" s="21" t="str">
+        <f>Pellets!$F$116</f>
+        <v>Vial (Epoxy-Carbon Fiber Resin)</v>
+      </c>
+      <c r="F157" s="21" t="str">
+        <f>LEFT(VLOOKUP(E157, Pellets!F:M, 8,FALSE), FIND("(", VLOOKUP(E157, Pellets!F:M, 8,FALSE))-8)&amp;" Composite"</f>
+        <v>Carbon Fiber Composite</v>
+      </c>
+      <c r="G157" s="21">
+        <v>8</v>
+      </c>
+      <c r="H157" s="21">
+        <v>10</v>
+      </c>
+      <c r="I157" s="21">
+        <v>64</v>
+      </c>
+      <c r="J157" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K157" s="42" t="s">
+        <v>2504</v>
+      </c>
+      <c r="L157" s="21" t="str">
+        <f>Pellets!$F$117</f>
+        <v>Vial (Phenolic-Carbon Fiber Resin)</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -53512,7 +53632,7 @@
         <v>2518</v>
       </c>
       <c r="D1" s="53" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$79</f>
+        <f xml:space="preserve"> [1]Enums!$B$80</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="20" t="s">
@@ -53546,7 +53666,7 @@
         <v>Wafer (Solar Cell)</v>
       </c>
       <c r="D2" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$91</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Wafer</v>
       </c>
       <c r="E2" s="49" t="s">
@@ -53573,7 +53693,7 @@
         <v>Wafer (Processor)</v>
       </c>
       <c r="D3" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$91</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Wafer</v>
       </c>
       <c r="E3" s="49" t="s">
@@ -53600,7 +53720,7 @@
         <v>Wafer (Temperature Sensor)</v>
       </c>
       <c r="D4" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$91</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Wafer</v>
       </c>
       <c r="E4" s="49" t="s">
@@ -53627,7 +53747,7 @@
         <v>Wafer (Pressure Sensor)</v>
       </c>
       <c r="D5" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$91</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Wafer</v>
       </c>
       <c r="E5" s="49" t="s">
@@ -53654,7 +53774,7 @@
         <v>Wafer (Low Power Radio)</v>
       </c>
       <c r="D6" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$91</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Wafer</v>
       </c>
       <c r="E6" s="49" t="s">
@@ -53681,7 +53801,7 @@
         <v>Wafer (DSP)</v>
       </c>
       <c r="D7" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$91</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Wafer</v>
       </c>
       <c r="E7" s="49" t="s">
@@ -53708,7 +53828,7 @@
         <v>Wafer (Digital Analog Convertor)</v>
       </c>
       <c r="D8" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$91</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Wafer</v>
       </c>
       <c r="E8" s="49" t="s">
@@ -53735,7 +53855,7 @@
         <v>Wafer (Amplifier)</v>
       </c>
       <c r="D9" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$91</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Wafer</v>
       </c>
       <c r="E9" s="49" t="s">
@@ -53762,7 +53882,7 @@
         <v>Wafer (OLED Array)</v>
       </c>
       <c r="D10" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$91</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Wafer</v>
       </c>
       <c r="E10" s="49" t="s">

</xml_diff>

<commit_message>
Revert "Updates from GitHub Interface for Communications"
This reverts commit 5b8d47613fc54df1e353b79ae96d7ede4f75282e.
</commit_message>
<xml_diff>
--- a/config/Polycraft Polymers.xlsx
+++ b/config/Polycraft Polymers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="826" activeTab="10"/>
+    <workbookView xWindow="6510" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="826" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Pellets" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2946" uniqueCount="2711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2942" uniqueCount="2708">
   <si>
     <t>GC</t>
   </si>
@@ -8176,15 +8176,6 @@
   </si>
   <si>
     <t>Silicon Wafer (Ruined)</t>
-  </si>
-  <si>
-    <t>1fu</t>
-  </si>
-  <si>
-    <t>1fv</t>
-  </si>
-  <si>
-    <t>1fw</t>
   </si>
 </sst>
 </file>
@@ -8484,123 +8475,118 @@
             <v>1.3.2</v>
           </cell>
         </row>
-        <row r="22">
-          <cell r="A22" t="str">
-            <v>1.3.3</v>
+        <row r="30">
+          <cell r="A30" t="str">
+            <v>Bag</v>
           </cell>
         </row>
         <row r="31">
           <cell r="A31" t="str">
-            <v>Bag</v>
+            <v>Vial</v>
           </cell>
         </row>
-        <row r="32">
-          <cell r="A32" t="str">
-            <v>Vial</v>
+        <row r="33">
+          <cell r="A33" t="str">
+            <v>Sack</v>
           </cell>
         </row>
         <row r="34">
           <cell r="A34" t="str">
-            <v>Sack</v>
+            <v>Beaker</v>
           </cell>
         </row>
-        <row r="35">
-          <cell r="A35" t="str">
-            <v>Beaker</v>
+        <row r="36">
+          <cell r="A36" t="str">
+            <v>Powder Keg</v>
           </cell>
         </row>
         <row r="37">
           <cell r="A37" t="str">
-            <v>Powder Keg</v>
+            <v>Drum</v>
           </cell>
         </row>
-        <row r="38">
-          <cell r="A38" t="str">
-            <v>Drum</v>
+        <row r="39">
+          <cell r="A39" t="str">
+            <v>Chemical Silo</v>
           </cell>
         </row>
         <row r="40">
           <cell r="A40" t="str">
-            <v>Chemical Silo</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41" t="str">
             <v>Chemical Vat</v>
           </cell>
         </row>
-        <row r="80">
-          <cell r="B80" t="str">
+        <row r="79">
+          <cell r="B79" t="str">
             <v>Mold Type</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="B83" t="str">
+            <v>Mold</v>
           </cell>
         </row>
         <row r="84">
           <cell r="B84" t="str">
-            <v>Mold</v>
+            <v>Metal Die</v>
           </cell>
         </row>
-        <row r="85">
-          <cell r="B85" t="str">
-            <v>Metal Die</v>
+        <row r="91">
+          <cell r="B91" t="str">
+            <v>Wafer</v>
           </cell>
         </row>
         <row r="92">
           <cell r="B92" t="str">
-            <v>Wafer</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="B93" t="str">
             <v>Mask</v>
           </cell>
         </row>
-        <row r="108">
-          <cell r="A108" t="str">
+        <row r="107">
+          <cell r="A107" t="str">
             <v>Gripped</v>
+          </cell>
+        </row>
+        <row r="110">
+          <cell r="A110" t="str">
+            <v>Base Material</v>
           </cell>
         </row>
         <row r="111">
           <cell r="A111" t="str">
-            <v>Base Material</v>
+            <v>Wooden</v>
           </cell>
         </row>
         <row r="112">
           <cell r="A112" t="str">
-            <v>Wooden</v>
+            <v>Stone</v>
           </cell>
         </row>
         <row r="113">
           <cell r="A113" t="str">
-            <v>Stone</v>
+            <v>Iron</v>
           </cell>
         </row>
         <row r="114">
           <cell r="A114" t="str">
-            <v>Iron</v>
+            <v>Golden</v>
           </cell>
         </row>
         <row r="115">
           <cell r="A115" t="str">
-            <v>Golden</v>
+            <v>Diamond</v>
           </cell>
         </row>
         <row r="116">
           <cell r="A116" t="str">
-            <v>Diamond</v>
+            <v>Magic</v>
           </cell>
         </row>
-        <row r="117">
-          <cell r="A117" t="str">
-            <v>Magic</v>
+        <row r="145">
+          <cell r="A145" t="str">
+            <v>Composite</v>
           </cell>
         </row>
         <row r="146">
           <cell r="A146" t="str">
-            <v>Composite</v>
-          </cell>
-        </row>
-        <row r="147">
-          <cell r="A147" t="str">
             <v>Engineered</v>
           </cell>
         </row>
@@ -10231,11 +10217,6 @@
             <v>HAM Radio Case</v>
           </cell>
         </row>
-        <row r="34">
-          <cell r="B34" t="str">
-            <v>Flagpole Segment</v>
-          </cell>
-        </row>
       </sheetData>
     </sheetDataSet>
   </externalBook>
@@ -10871,19 +10852,19 @@
         <v>Game ID XL</v>
       </c>
       <c r="F1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$31&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$30&amp;" ("&amp;J1&amp;")"</f>
         <v>Bag (Pellets)</v>
       </c>
       <c r="G1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$34&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$33&amp;" ("&amp;J1&amp;")"</f>
         <v>Sack (Pellets)</v>
       </c>
       <c r="H1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$37&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$36&amp;" ("&amp;J1&amp;")"</f>
         <v>Powder Keg (Pellets)</v>
       </c>
       <c r="I1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$40&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$39&amp;" ("&amp;J1&amp;")"</f>
         <v>Chemical Silo (Pellets)</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -10922,19 +10903,19 @@
         <v>448</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="G2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="H2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="J2" s="1" t="str">
@@ -10974,19 +10955,19 @@
         <v>444</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J3" s="1" t="str">
@@ -11023,19 +11004,19 @@
         <v>440</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Alkyd Resin)</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Alkyd Resin)</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Alkyd Resin)</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Alkyd Resin)</v>
       </c>
       <c r="J4" s="1" t="str">
@@ -11075,19 +11056,19 @@
         <v>436</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J5" s="1" t="str">
@@ -11127,19 +11108,19 @@
         <v>432</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J6" s="1" t="str">
@@ -11179,19 +11160,19 @@
         <v>428</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$31, [1]Enums!$A$31)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$30, [1]Enums!$A$30)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Carbon Fiber)</v>
       </c>
       <c r="G7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$34, [1]Enums!$A$34)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$33, [1]Enums!$A$33)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Carbon Fiber)</v>
       </c>
       <c r="H7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$37, [1]Enums!$A$37)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$36, [1]Enums!$A$36)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Carbon Fiber)</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$40, [1]Enums!$A$40)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$39, [1]Enums!$A$39)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Carbon Fiber)</v>
       </c>
       <c r="J7" s="1" t="str">
@@ -11228,19 +11209,19 @@
         <v>424</v>
       </c>
       <c r="F8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="G8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="J8" s="1" t="str">
@@ -11280,19 +11261,19 @@
         <v>420</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulosic Pellets)</v>
       </c>
       <c r="G9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulosic Pellets)</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulosic Pellets)</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulosic Pellets)</v>
       </c>
       <c r="J9" s="1" t="str">
@@ -11332,19 +11313,19 @@
         <v>416</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chitin Pellets)</v>
       </c>
       <c r="G10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chitin Pellets)</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chitin Pellets)</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chitin Pellets)</v>
       </c>
       <c r="J10" s="1" t="str">
@@ -11384,19 +11365,19 @@
         <v>412</v>
       </c>
       <c r="F11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J11" s="1" t="str">
@@ -11436,19 +11417,19 @@
         <v>408</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Epoxy Resin)</v>
       </c>
       <c r="G12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Epoxy Resin)</v>
       </c>
       <c r="H12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Epoxy Resin)</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Epoxy Resin)</v>
       </c>
       <c r="J12" s="1" t="str">
@@ -11485,19 +11466,19 @@
         <v>404</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethoxylates Pellets)</v>
       </c>
       <c r="G13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethoxylates Pellets)</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethoxylates Pellets)</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethoxylates Pellets)</v>
       </c>
       <c r="J13" s="1" t="str">
@@ -11537,19 +11518,19 @@
         <v>400</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="G14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="H14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="J14" s="1" t="str">
@@ -11589,19 +11570,19 @@
         <v>396</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="G15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="J15" s="1" t="str">
@@ -11641,19 +11622,19 @@
         <v>392</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="G16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="J16" s="1" t="str">
@@ -11693,19 +11674,19 @@
         <v>388</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="G17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="J17" s="1" t="str">
@@ -11745,19 +11726,19 @@
         <v>384</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J18" s="1" t="str">
@@ -11797,19 +11778,19 @@
         <v>380</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J19" s="1" t="str">
@@ -11846,19 +11827,19 @@
         <v>376</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Lignin)</v>
       </c>
       <c r="G20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Lignin)</v>
       </c>
       <c r="H20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Lignin)</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Lignin)</v>
       </c>
       <c r="J20" s="1" t="str">
@@ -11898,19 +11879,19 @@
         <v>372</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J21" s="1" t="str">
@@ -11950,19 +11931,19 @@
         <v>368</v>
       </c>
       <c r="F22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="G22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="H22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="J22" s="1" t="str">
@@ -12002,19 +11983,19 @@
         <v>364</v>
       </c>
       <c r="F23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="G23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="H23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="J23" s="1" t="str">
@@ -12054,19 +12035,19 @@
         <v>360</v>
       </c>
       <c r="F24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="G24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="H24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="J24" s="1" t="str">
@@ -12103,19 +12084,19 @@
         <v>356</v>
       </c>
       <c r="F25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="G25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="H25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="J25" s="1" t="str">
@@ -12155,19 +12136,19 @@
         <v>352</v>
       </c>
       <c r="F26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Metaldehyde Pellets)</v>
       </c>
       <c r="G26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Metaldehyde Pellets)</v>
       </c>
       <c r="H26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Metaldehyde Pellets)</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Metaldehyde Pellets)</v>
       </c>
       <c r="J26" s="1" t="str">
@@ -12207,19 +12188,19 @@
         <v>348</v>
       </c>
       <c r="F27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J27" s="1" t="str">
@@ -12259,19 +12240,19 @@
         <v>344</v>
       </c>
       <c r="F28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraformaldehyde Pellets)</v>
       </c>
       <c r="G28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraformaldehyde Pellets)</v>
       </c>
       <c r="H28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraformaldehyde Pellets)</v>
       </c>
       <c r="I28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraformaldehyde Pellets)</v>
       </c>
       <c r="J28" s="1" t="str">
@@ -12311,19 +12292,19 @@
         <v>340</v>
       </c>
       <c r="F29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraldehyde Pellets)</v>
       </c>
       <c r="G29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraldehyde Pellets)</v>
       </c>
       <c r="H29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraldehyde Pellets)</v>
       </c>
       <c r="I29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraldehyde Pellets)</v>
       </c>
       <c r="J29" s="1" t="str">
@@ -12363,19 +12344,19 @@
         <v>336</v>
       </c>
       <c r="F30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Phenolic Resin)</v>
       </c>
       <c r="G30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Phenolic Resin)</v>
       </c>
       <c r="H30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Phenolic Resin)</v>
       </c>
       <c r="I30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Phenolic Resin)</v>
       </c>
       <c r="J30" s="1" t="str">
@@ -12415,19 +12396,19 @@
         <v>332</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="G31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="H31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="I31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="J31" s="1" t="str">
@@ -12467,19 +12448,19 @@
         <v>328</v>
       </c>
       <c r="F32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly1-Butene Pellets)</v>
       </c>
       <c r="G32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly1-Butene Pellets)</v>
       </c>
       <c r="H32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly1-Butene Pellets)</v>
       </c>
       <c r="I32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly1-Butene Pellets)</v>
       </c>
       <c r="J32" s="1" t="str">
@@ -12519,19 +12500,19 @@
         <v>324</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="G33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="H33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="I33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="J33" s="1" t="str">
@@ -12571,19 +12552,19 @@
         <v>320</v>
       </c>
       <c r="F34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="G34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="H34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="I34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="J34" s="1" t="str">
@@ -12623,19 +12604,19 @@
         <v>316</v>
       </c>
       <c r="F35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="G35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="H35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="I35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="J35" s="1" t="str">
@@ -12675,19 +12656,19 @@
         <v>312</v>
       </c>
       <c r="F36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="G36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="H36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="I36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="J36" s="1" t="str">
@@ -12727,19 +12708,19 @@
         <v>308</v>
       </c>
       <c r="F37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="G37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="H37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="I37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="J37" s="1" t="str">
@@ -12779,19 +12760,19 @@
         <v>304</v>
       </c>
       <c r="F38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="G38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="H38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="I38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="J38" s="1" t="str">
@@ -12831,19 +12812,19 @@
         <v>300</v>
       </c>
       <c r="F39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="G39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="H39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="I39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="J39" s="1" t="str">
@@ -12883,19 +12864,19 @@
         <v>296</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="G40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="H40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="I40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="J40" s="1" t="str">
@@ -12935,19 +12916,19 @@
         <v>292</v>
       </c>
       <c r="F41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="G41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="H41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="I41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="J41" s="1" t="str">
@@ -12987,19 +12968,19 @@
         <v>288</v>
       </c>
       <c r="F42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCaprolactone Pellets)</v>
       </c>
       <c r="G42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCaprolactone Pellets)</v>
       </c>
       <c r="H42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCaprolactone Pellets)</v>
       </c>
       <c r="I42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCaprolactone Pellets)</v>
       </c>
       <c r="J42" s="1" t="str">
@@ -13039,19 +13020,19 @@
         <v>284</v>
       </c>
       <c r="F43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCarbonate Pellets)</v>
       </c>
       <c r="G43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCarbonate Pellets)</v>
       </c>
       <c r="H43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCarbonate Pellets)</v>
       </c>
       <c r="I43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCarbonate Pellets)</v>
       </c>
       <c r="J43" s="1" t="str">
@@ -13091,19 +13072,19 @@
         <v>280</v>
       </c>
       <c r="F44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChloroPrene Pellets)</v>
       </c>
       <c r="G44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChloroPrene Pellets)</v>
       </c>
       <c r="H44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChloroPrene Pellets)</v>
       </c>
       <c r="I44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChloroPrene Pellets)</v>
       </c>
       <c r="J44" s="1" t="str">
@@ -13140,19 +13121,19 @@
         <v>276</v>
       </c>
       <c r="F45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="G45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="H45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="I45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="J45" s="1" t="str">
@@ -13192,19 +13173,19 @@
         <v>272</v>
       </c>
       <c r="F46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="G46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="H46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="I46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="J46" s="1" t="str">
@@ -13244,19 +13225,19 @@
         <v>268</v>
       </c>
       <c r="F47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="G47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="H47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="I47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="J47" s="1" t="str">
@@ -13296,19 +13277,19 @@
         <v>264</v>
       </c>
       <c r="F48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEtherImide Pellets)</v>
       </c>
       <c r="G48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEtherImide Pellets)</v>
       </c>
       <c r="H48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEtherImide Pellets)</v>
       </c>
       <c r="I48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEtherImide Pellets)</v>
       </c>
       <c r="J48" s="1" t="str">
@@ -13345,19 +13326,19 @@
         <v>260</v>
       </c>
       <c r="F49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="G49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="H49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="I49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="J49" s="1" t="str">
@@ -13394,19 +13375,19 @@
         <v>256</v>
       </c>
       <c r="F50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="G50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="H50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="I50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="J50" s="1" t="str">
@@ -13446,19 +13427,19 @@
         <v>252</v>
       </c>
       <c r="F51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="G51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="H51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="I51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="J51" s="1" t="str">
@@ -13495,19 +13476,19 @@
         <v>248</v>
       </c>
       <c r="F52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J52" s="1" t="str">
@@ -13547,19 +13528,19 @@
         <v>244</v>
       </c>
       <c r="F53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="G53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="H53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="I53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="J53" s="1" t="str">
@@ -13599,19 +13580,19 @@
         <v>240</v>
       </c>
       <c r="F54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="G54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="H54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="I54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="J54" s="1" t="str">
@@ -13651,19 +13632,19 @@
         <v>236</v>
       </c>
       <c r="F55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="G55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="H55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="I55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="J55" s="1" t="str">
@@ -13703,19 +13684,19 @@
         <v>232</v>
       </c>
       <c r="F56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J56" s="1" t="str">
@@ -13755,19 +13736,19 @@
         <v>228</v>
       </c>
       <c r="F57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="G57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="H57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="I57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="J57" s="1" t="str">
@@ -13807,19 +13788,19 @@
         <v>224</v>
       </c>
       <c r="F58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="G58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="H58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="I58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="J58" s="1" t="str">
@@ -13859,19 +13840,19 @@
         <v>220</v>
       </c>
       <c r="F59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="G59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="H59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="I59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="J59" s="1" t="str">
@@ -13911,19 +13892,19 @@
         <v>216</v>
       </c>
       <c r="F60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="G60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="H60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="I60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="J60" s="1" t="str">
@@ -13963,19 +13944,19 @@
         <v>212</v>
       </c>
       <c r="F61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="G61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="H61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="I61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="J61" s="1" t="str">
@@ -14012,19 +13993,19 @@
         <v>208</v>
       </c>
       <c r="F62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="G62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="H62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="I62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="J62" s="1" t="str">
@@ -14064,19 +14045,19 @@
         <v>204</v>
       </c>
       <c r="F63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyImide Pellets)</v>
       </c>
       <c r="G63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyImide Pellets)</v>
       </c>
       <c r="H63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyImide Pellets)</v>
       </c>
       <c r="I63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyImide Pellets)</v>
       </c>
       <c r="J63" s="1" t="str">
@@ -14113,19 +14094,19 @@
         <v>200</v>
       </c>
       <c r="F64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="G64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="H64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="I64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="J64" s="1" t="str">
@@ -14162,19 +14143,19 @@
         <v>196</v>
       </c>
       <c r="F65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="G65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="H65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="I65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="J65" s="1" t="str">
@@ -14214,19 +14195,19 @@
         <v>192</v>
       </c>
       <c r="F66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButylene Pellets)</v>
       </c>
       <c r="G66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButylene Pellets)</v>
       </c>
       <c r="H66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButylene Pellets)</v>
       </c>
       <c r="I66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButylene Pellets)</v>
       </c>
       <c r="J66" s="1" t="str">
@@ -14266,19 +14247,19 @@
         <v>188</v>
       </c>
       <c r="F67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoPrene Pellets)</v>
       </c>
       <c r="G67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoPrene Pellets)</v>
       </c>
       <c r="H67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoPrene Pellets)</v>
       </c>
       <c r="I67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoPrene Pellets)</v>
       </c>
       <c r="J67" s="1" t="str">
@@ -14318,19 +14299,19 @@
         <v>184</v>
       </c>
       <c r="F68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic Acid Pellets)</v>
       </c>
       <c r="G68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic Acid Pellets)</v>
       </c>
       <c r="H68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic Acid Pellets)</v>
       </c>
       <c r="I68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic Acid Pellets)</v>
       </c>
       <c r="J68" s="1" t="str">
@@ -14367,19 +14348,19 @@
         <v>180</v>
       </c>
       <c r="F69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="G69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="H69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="I69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="J69" s="1" t="str">
@@ -14419,19 +14400,19 @@
         <v>176</v>
       </c>
       <c r="F70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="G70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="H70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="I70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="J70" s="1" t="str">
@@ -14468,19 +14449,19 @@
         <v>172</v>
       </c>
       <c r="F71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="G71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="H71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="I71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="J71" s="1" t="str">
@@ -14520,19 +14501,19 @@
         <v>168</v>
       </c>
       <c r="F72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="G72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="H72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="I72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="J72" s="1" t="str">
@@ -14572,19 +14553,19 @@
         <v>164</v>
       </c>
       <c r="F73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="G73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="H73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="I73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="J73" s="1" t="str">
@@ -14624,19 +14605,19 @@
         <v>160</v>
       </c>
       <c r="F74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="G74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="H74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="I74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="J74" s="1" t="str">
@@ -14673,19 +14654,19 @@
         <v>156</v>
       </c>
       <c r="F75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J75" s="1" t="str">
@@ -14725,19 +14706,19 @@
         <v>152</v>
       </c>
       <c r="F76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyOxymethylene Pellets)</v>
       </c>
       <c r="G76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyOxymethylene Pellets)</v>
       </c>
       <c r="H76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyOxymethylene Pellets)</v>
       </c>
       <c r="I76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyOxymethylene Pellets)</v>
       </c>
       <c r="J76" s="1" t="str">
@@ -14774,19 +14755,19 @@
         <v>148</v>
       </c>
       <c r="F77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J77" s="1" t="str">
@@ -14826,19 +14807,19 @@
         <v>144</v>
       </c>
       <c r="F78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenol Pellets)</v>
       </c>
       <c r="G78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenol Pellets)</v>
       </c>
       <c r="H78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenol Pellets)</v>
       </c>
       <c r="I78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenol Pellets)</v>
       </c>
       <c r="J78" s="1" t="str">
@@ -14875,19 +14856,19 @@
         <v>140</v>
       </c>
       <c r="F79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="G79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="H79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="I79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="J79" s="1" t="str">
@@ -14924,19 +14905,19 @@
         <v>136</v>
       </c>
       <c r="F80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhosphazene Pellets)</v>
       </c>
       <c r="G80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhosphazene Pellets)</v>
       </c>
       <c r="H80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhosphazene Pellets)</v>
       </c>
       <c r="I80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhosphazene Pellets)</v>
       </c>
       <c r="J80" s="1" t="str">
@@ -14973,19 +14954,19 @@
         <v>132</v>
       </c>
       <c r="F81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="G81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="H81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="I81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="J81" s="1" t="str">
@@ -15022,19 +15003,19 @@
         <v>128</v>
       </c>
       <c r="F82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="G82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="H82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="I82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="J82" s="1" t="str">
@@ -15074,19 +15055,19 @@
         <v>124</v>
       </c>
       <c r="F83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="G83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="H83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="I83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="J83" s="1" t="str">
@@ -15126,19 +15107,19 @@
         <v>120</v>
       </c>
       <c r="F84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Pellets)</v>
       </c>
       <c r="G84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Pellets)</v>
       </c>
       <c r="H84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Pellets)</v>
       </c>
       <c r="I84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Pellets)</v>
       </c>
       <c r="J84" s="1" t="str">
@@ -15175,19 +15156,19 @@
         <v>116</v>
       </c>
       <c r="F85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="G85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="H85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="I85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="J85" s="1" t="str">
@@ -15224,19 +15205,19 @@
         <v>112</v>
       </c>
       <c r="F86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="G86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="H86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="I86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="J86" s="1" t="str">
@@ -15276,19 +15257,19 @@
         <v>108</v>
       </c>
       <c r="F87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyStyrene Pellets)</v>
       </c>
       <c r="G87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyStyrene Pellets)</v>
       </c>
       <c r="H87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyStyrene Pellets)</v>
       </c>
       <c r="I87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyStyrene Pellets)</v>
       </c>
       <c r="J87" s="1" t="str">
@@ -15325,19 +15306,19 @@
         <v>104</v>
       </c>
       <c r="F88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J88" s="1" t="str">
@@ -15377,19 +15358,19 @@
         <v>100</v>
       </c>
       <c r="F89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="G89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="H89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="I89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="J89" s="1" t="str">
@@ -15426,19 +15407,19 @@
         <v>96</v>
       </c>
       <c r="F90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="G90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="H90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="I90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="J90" s="1" t="str">
@@ -15475,19 +15456,19 @@
         <v>92</v>
       </c>
       <c r="F91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="G91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="H91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="I91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="J91" s="1" t="str">
@@ -15524,19 +15505,19 @@
         <v>88</v>
       </c>
       <c r="F92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyThiazyl Pellets)</v>
       </c>
       <c r="G92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyThiazyl Pellets)</v>
       </c>
       <c r="H92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyThiazyl Pellets)</v>
       </c>
       <c r="I92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyThiazyl Pellets)</v>
       </c>
       <c r="J92" s="1" t="str">
@@ -15576,19 +15557,19 @@
         <v>84</v>
       </c>
       <c r="F93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="G93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="H93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="I93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="J93" s="1" t="str">
@@ -15628,19 +15609,19 @@
         <v>80</v>
       </c>
       <c r="F94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyUrethane Pellets)</v>
       </c>
       <c r="G94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyUrethane Pellets)</v>
       </c>
       <c r="H94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyUrethane Pellets)</v>
       </c>
       <c r="I94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyUrethane Pellets)</v>
       </c>
       <c r="J94" s="1" t="str">
@@ -15680,19 +15661,19 @@
         <v>76</v>
       </c>
       <c r="F95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="G95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="H95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="I95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="J95" s="1" t="str">
@@ -15732,19 +15713,19 @@
         <v>72</v>
       </c>
       <c r="F96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="G96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="H96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="I96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="J96" s="1" t="str">
@@ -15781,19 +15762,19 @@
         <v>68</v>
       </c>
       <c r="F97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="G97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="H97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="I97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="J97" s="1" t="str">
@@ -15833,19 +15814,19 @@
         <v>64</v>
       </c>
       <c r="F98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="G98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="H98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="I98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="J98" s="1" t="str">
@@ -15885,19 +15866,19 @@
         <v>60</v>
       </c>
       <c r="F99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="G99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="H99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="I99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="J99" s="1" t="str">
@@ -15934,19 +15915,19 @@
         <v>56</v>
       </c>
       <c r="F100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="G100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="H100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="I100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="J100" s="1" t="str">
@@ -15983,19 +15964,19 @@
         <v>52</v>
       </c>
       <c r="F101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="G101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="H101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="I101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="J101" s="1" t="str">
@@ -16032,19 +16013,19 @@
         <v>48</v>
       </c>
       <c r="F102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="G102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="H102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="I102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="J102" s="1" t="str">
@@ -16081,19 +16062,19 @@
         <v>44</v>
       </c>
       <c r="F103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="G103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="H103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="I103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="J103" s="1" t="str">
@@ -16130,19 +16111,19 @@
         <v>40</v>
       </c>
       <c r="F104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="G104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="H104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="I104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="J104" s="1" t="str">
@@ -16179,19 +16160,19 @@
         <v>36</v>
       </c>
       <c r="F105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="G105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="H105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="I105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="J105" s="1" t="str">
@@ -16231,19 +16212,19 @@
         <v>32</v>
       </c>
       <c r="F106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="G106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="H106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="I106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="J106" s="1" t="str">
@@ -16283,19 +16264,19 @@
         <v>28</v>
       </c>
       <c r="F107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J107" s="1" t="str">
@@ -16335,19 +16316,19 @@
         <v>24</v>
       </c>
       <c r="F108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J108" s="1" t="str">
@@ -16387,19 +16368,19 @@
         <v>20</v>
       </c>
       <c r="F109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="G109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="H109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="I109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="J109" s="1" t="str">
@@ -16436,19 +16417,19 @@
         <v>16</v>
       </c>
       <c r="F110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="G110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="H110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="I110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="J110" s="1" t="str">
@@ -16488,19 +16469,19 @@
         <v>12</v>
       </c>
       <c r="F111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="G111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="H111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="I111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="J111" s="1" t="str">
@@ -16537,19 +16518,19 @@
         <v>8</v>
       </c>
       <c r="F112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="G112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="H112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="I112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="J112" s="1" t="str">
@@ -16589,19 +16570,19 @@
         <v>4</v>
       </c>
       <c r="F113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J113" s="1" t="str">
@@ -16641,19 +16622,19 @@
         <v>0</v>
       </c>
       <c r="F114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="G114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="H114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="I114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="J114" s="1" t="str">
@@ -16693,19 +16674,19 @@
         <v>1853</v>
       </c>
       <c r="F115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Polycaprolactam Pellets)</v>
       </c>
       <c r="G115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Polycaprolactam Pellets)</v>
       </c>
       <c r="H115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Polycaprolactam Pellets)</v>
       </c>
       <c r="I115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Polycaprolactam Pellets)</v>
       </c>
       <c r="J115" s="1" t="str">
@@ -16745,19 +16726,19 @@
         <v>2412</v>
       </c>
       <c r="F116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="G116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="H116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="I116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="J116" s="1" t="str">
@@ -16797,19 +16778,19 @@
         <v>2416</v>
       </c>
       <c r="F117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="G117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="H117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="I117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="J117" s="1" t="str">
@@ -16849,19 +16830,19 @@
         <v>2420</v>
       </c>
       <c r="F118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Negative Photoresist)</v>
       </c>
       <c r="G118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Negative Photoresist)</v>
       </c>
       <c r="H118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Negative Photoresist)</v>
       </c>
       <c r="I118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Negative Photoresist)</v>
       </c>
       <c r="J118" s="1" t="str">
@@ -16901,19 +16882,19 @@
         <v>2424</v>
       </c>
       <c r="F119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$31, [1]Enums!$A$32)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$30, [1]Enums!$A$31)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Positive Photoresist)</v>
       </c>
       <c r="G119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Positive Photoresist)</v>
       </c>
       <c r="H119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Positive Photoresist)</v>
       </c>
       <c r="I119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Positive Photoresist)</v>
       </c>
       <c r="J119" s="1" t="str">
@@ -17828,11 +17809,11 @@
         <v>2651</v>
       </c>
       <c r="C1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="D1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$80</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="19" t="str">
@@ -17868,7 +17849,7 @@
         <v>Mask (Solar Cell)[PR Backplane]</v>
       </c>
       <c r="D2" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E2" s="15" t="str">
@@ -17892,7 +17873,7 @@
         <v>Mask (Solar Cell)[PR Semiconductor]</v>
       </c>
       <c r="D3" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E3" s="15" t="str">
@@ -17916,7 +17897,7 @@
         <v>Mask (Solar Cell)[PR Dielectric]</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E4" s="15" t="str">
@@ -17940,7 +17921,7 @@
         <v>Mask (Solar Cell)[PR Traces]</v>
       </c>
       <c r="D5" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E5" s="15" t="str">
@@ -17964,7 +17945,7 @@
         <v>Mask (Solar Cell)[PR Encapsulation]</v>
       </c>
       <c r="D6" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E6" s="15" t="str">
@@ -17988,7 +17969,7 @@
         <v>Mask (Processor)[PR Backplane]</v>
       </c>
       <c r="D7" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E7" s="15" t="str">
@@ -18012,7 +17993,7 @@
         <v>Mask (Processor)[PR n-Type Semiconductor]</v>
       </c>
       <c r="D8" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E8" s="15" t="str">
@@ -18036,7 +18017,7 @@
         <v>Mask (Processor)[PR p-Type Semiconductor]</v>
       </c>
       <c r="D9" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E9" s="15" t="str">
@@ -18060,7 +18041,7 @@
         <v>Mask (Processor)[PR Dielectric]</v>
       </c>
       <c r="D10" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E10" s="15" t="str">
@@ -18084,7 +18065,7 @@
         <v>Mask (Processor)[PR Inner Traces]</v>
       </c>
       <c r="D11" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E11" s="15" t="str">
@@ -18108,7 +18089,7 @@
         <v>Mask (Processor)[PR Through Vias]</v>
       </c>
       <c r="D12" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E12" s="15" t="str">
@@ -18132,7 +18113,7 @@
         <v>Mask (Processor)[PR Outer Traces]</v>
       </c>
       <c r="D13" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E13" s="15" t="str">
@@ -18156,7 +18137,7 @@
         <v>Mask (Processor)[PR Encapsulation]</v>
       </c>
       <c r="D14" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E14" s="15" t="str">
@@ -18180,7 +18161,7 @@
         <v>Mask (Temperature Sensor)[PR Backplane]</v>
       </c>
       <c r="D15" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E15" s="15" t="str">
@@ -18204,7 +18185,7 @@
         <v>Mask (Temperature Sensor)[PR Semiconductor]</v>
       </c>
       <c r="D16" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E16" s="15" t="str">
@@ -18228,7 +18209,7 @@
         <v>Mask (Temperature Sensor)[PR Dielectric]</v>
       </c>
       <c r="D17" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E17" s="15" t="str">
@@ -18252,7 +18233,7 @@
         <v>Mask (Temperature Sensor)[PR Traces]</v>
       </c>
       <c r="D18" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E18" s="15" t="str">
@@ -18276,7 +18257,7 @@
         <v>Mask (Temperature Sensor)[PR Encapsulation]</v>
       </c>
       <c r="D19" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E19" s="15" t="str">
@@ -18300,7 +18281,7 @@
         <v>Mask (Pressure Sensor)[PR Backplane]</v>
       </c>
       <c r="D20" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E20" s="15" t="str">
@@ -18324,7 +18305,7 @@
         <v>Mask (Pressure Sensor)[PR Semiconductor]</v>
       </c>
       <c r="D21" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E21" s="15" t="str">
@@ -18348,7 +18329,7 @@
         <v>Mask (Pressure Sensor)[PR Dielectric]</v>
       </c>
       <c r="D22" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E22" s="15" t="str">
@@ -18372,7 +18353,7 @@
         <v>Mask (Pressure Sensor)[PR Traces]</v>
       </c>
       <c r="D23" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E23" s="15" t="str">
@@ -18396,7 +18377,7 @@
         <v>Mask (Pressure Sensor)[PR Encapsulation]</v>
       </c>
       <c r="D24" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E24" s="15" t="str">
@@ -18420,7 +18401,7 @@
         <v>Mask (Low Power Radio)[PR Backplane]</v>
       </c>
       <c r="D25" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E25" s="15" t="str">
@@ -18444,7 +18425,7 @@
         <v>Mask (Low Power Radio)[PR n-Type Semiconductor]</v>
       </c>
       <c r="D26" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E26" s="15" t="str">
@@ -18468,7 +18449,7 @@
         <v>Mask (Low Power Radio)[PR p-Type Semiconductor]</v>
       </c>
       <c r="D27" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E27" s="15" t="str">
@@ -18492,7 +18473,7 @@
         <v>Mask (Low Power Radio)[PR Dielectric]</v>
       </c>
       <c r="D28" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E28" s="15" t="str">
@@ -18516,7 +18497,7 @@
         <v>Mask (Low Power Radio)[PR Inner Traces]</v>
       </c>
       <c r="D29" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E29" s="15" t="str">
@@ -18540,7 +18521,7 @@
         <v>Mask (Low Power Radio)[PR Through Vias]</v>
       </c>
       <c r="D30" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E30" s="15" t="str">
@@ -18564,7 +18545,7 @@
         <v>Mask (Low Power Radio)[PR Outer Traces]</v>
       </c>
       <c r="D31" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E31" s="15" t="str">
@@ -18588,7 +18569,7 @@
         <v>Mask (Low Power Radio)[PR Encapsulation]</v>
       </c>
       <c r="D32" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E32" s="15" t="str">
@@ -18612,7 +18593,7 @@
         <v>Mask (DSP)[PR Backplane]</v>
       </c>
       <c r="D33" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E33" s="15" t="str">
@@ -18636,7 +18617,7 @@
         <v>Mask (DSP)[PR n-Type Semiconductor]</v>
       </c>
       <c r="D34" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E34" s="15" t="str">
@@ -18660,7 +18641,7 @@
         <v>Mask (DSP)[PR p-Type Semiconductor]</v>
       </c>
       <c r="D35" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E35" s="15" t="str">
@@ -18684,7 +18665,7 @@
         <v>Mask (DSP)[PR Dielectric]</v>
       </c>
       <c r="D36" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E36" s="15" t="str">
@@ -18708,7 +18689,7 @@
         <v>Mask (DSP)[PR Inner Traces]</v>
       </c>
       <c r="D37" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E37" s="15" t="str">
@@ -18732,7 +18713,7 @@
         <v>Mask (DSP)[PR Through Vias]</v>
       </c>
       <c r="D38" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E38" s="15" t="str">
@@ -18756,7 +18737,7 @@
         <v>Mask (DSP)[PR Outer Traces]</v>
       </c>
       <c r="D39" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E39" s="15" t="str">
@@ -18780,7 +18761,7 @@
         <v>Mask (DSP)[PR Encapsulation]</v>
       </c>
       <c r="D40" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E40" s="15" t="str">
@@ -18804,7 +18785,7 @@
         <v>Mask (Digital Analog Convertor)[PR Backplane]</v>
       </c>
       <c r="D41" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E41" s="15" t="str">
@@ -18828,7 +18809,7 @@
         <v>Mask (Digital Analog Convertor)[PR Semiconductor]</v>
       </c>
       <c r="D42" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E42" s="15" t="str">
@@ -18852,7 +18833,7 @@
         <v>Mask (Digital Analog Convertor)[PR Dielectric]</v>
       </c>
       <c r="D43" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E43" s="15" t="str">
@@ -18876,7 +18857,7 @@
         <v>Mask (Digital Analog Convertor)[PR Traces]</v>
       </c>
       <c r="D44" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E44" s="15" t="str">
@@ -18900,7 +18881,7 @@
         <v>Mask (Digital Analog Convertor)[PR Encapsulation]</v>
       </c>
       <c r="D45" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E45" s="15" t="str">
@@ -18924,7 +18905,7 @@
         <v>Mask (Amplifier)[PR Backplane]</v>
       </c>
       <c r="D46" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E46" s="15" t="str">
@@ -18948,7 +18929,7 @@
         <v>Mask (Amplifier)[PR Semiconductor]</v>
       </c>
       <c r="D47" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E47" s="15" t="str">
@@ -18972,7 +18953,7 @@
         <v>Mask (Amplifier)[PR Dielectric]</v>
       </c>
       <c r="D48" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E48" s="15" t="str">
@@ -18996,7 +18977,7 @@
         <v>Mask (Amplifier)[PR Traces]</v>
       </c>
       <c r="D49" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E49" s="15" t="str">
@@ -19020,7 +19001,7 @@
         <v>Mask (Amplifier)[PR Encapsulation]</v>
       </c>
       <c r="D50" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E50" s="15" t="str">
@@ -19044,7 +19025,7 @@
         <v>Mask (OLED Array)[PR Backplane]</v>
       </c>
       <c r="D51" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E51" s="15" t="str">
@@ -19068,7 +19049,7 @@
         <v>Mask (OLED Array)[PR Semiconductor]</v>
       </c>
       <c r="D52" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E52" s="15" t="str">
@@ -19092,7 +19073,7 @@
         <v>Mask (OLED Array)[PR Dielectric]</v>
       </c>
       <c r="D53" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E53" s="15" t="str">
@@ -19116,7 +19097,7 @@
         <v>Mask (OLED Array)[PR Traces]</v>
       </c>
       <c r="D54" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E54" s="15" t="str">
@@ -19140,7 +19121,7 @@
         <v>Mask (OLED Array)[PR Encapsulation]</v>
       </c>
       <c r="D55" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$92</f>
         <v>Mask</v>
       </c>
       <c r="E55" s="15" t="str">
@@ -19193,7 +19174,7 @@
   </sheetPr>
   <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -25407,7 +25388,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I2" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$145&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Steel</v>
       </c>
       <c r="J2" s="45">
@@ -25455,7 +25436,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I3" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$145&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Stainless Steel</v>
       </c>
       <c r="J3" s="45">
@@ -25503,7 +25484,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I4" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$145&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Brass</v>
       </c>
       <c r="J4" s="45">
@@ -25551,7 +25532,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I5" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$145&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Bronze</v>
       </c>
       <c r="J5" s="45">
@@ -25599,7 +25580,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I6" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$145&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Tungsten Carbide</v>
       </c>
       <c r="J6" s="45">
@@ -25647,7 +25628,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I7" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$145&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Nichrome</v>
       </c>
       <c r="J7" s="45">
@@ -25695,7 +25676,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I8" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$145&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Antimony-Lead</v>
       </c>
       <c r="J8" s="45">
@@ -25743,7 +25724,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I9" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Steel</v>
       </c>
       <c r="J9" s="45">
@@ -25791,7 +25772,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I10" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Stainless Steel</v>
       </c>
       <c r="J10" s="45">
@@ -25839,7 +25820,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I11" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Brass</v>
       </c>
       <c r="J11" s="45">
@@ -25887,7 +25868,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I12" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Bronze</v>
       </c>
       <c r="J12" s="45">
@@ -25935,7 +25916,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I13" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Tungsten Carbide</v>
       </c>
       <c r="J13" s="45">
@@ -25983,7 +25964,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I14" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Nichrome</v>
       </c>
       <c r="J14" s="45">
@@ -26031,7 +26012,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I15" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$146&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Antimony-Lead</v>
       </c>
       <c r="J15" s="45">
@@ -26079,7 +26060,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I16" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" Iron"</f>
+        <f>[1]Enums!$A$145&amp;" Iron"</f>
         <v>Composite Iron</v>
       </c>
       <c r="J16" s="45">
@@ -26127,7 +26108,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I17" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" Iron"</f>
+        <f>[1]Enums!$A$146&amp;" Iron"</f>
         <v>Engineered Iron</v>
       </c>
       <c r="J17" s="45">
@@ -26175,7 +26156,7 @@
         <v>Diamond</v>
       </c>
       <c r="I18" s="45" t="str">
-        <f>[1]Enums!$A$146&amp;" Diamond"</f>
+        <f>[1]Enums!$A$145&amp;" Diamond"</f>
         <v>Composite Diamond</v>
       </c>
       <c r="J18" s="45">
@@ -26223,7 +26204,7 @@
         <v>Diamond</v>
       </c>
       <c r="I19" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" Diamond"</f>
+        <f>[1]Enums!$A$146&amp;" Diamond"</f>
         <v>Engineered Diamond</v>
       </c>
       <c r="J19" s="45">
@@ -26524,7 +26505,7 @@
         <v>Molded Item</v>
       </c>
       <c r="F1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$111</f>
+        <f xml:space="preserve"> [1]Enums!$A$110</f>
         <v>Base Material</v>
       </c>
       <c r="G1" s="30" t="s">
@@ -26552,7 +26533,7 @@
         <v>1812</v>
       </c>
       <c r="C2" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D2</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D2</f>
         <v>Gripped Iron Shovel</v>
       </c>
       <c r="D2" s="24" t="str">
@@ -26564,7 +26545,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F2" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$113</f>
         <v>Iron</v>
       </c>
       <c r="G2" s="24">
@@ -26589,7 +26570,7 @@
         <v>1811</v>
       </c>
       <c r="C3" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D3</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D3</f>
         <v>Gripped Iron Pickaxe</v>
       </c>
       <c r="D3" s="21" t="str">
@@ -26601,7 +26582,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F3" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$113</f>
         <v>Iron</v>
       </c>
       <c r="G3" s="24">
@@ -26626,7 +26607,7 @@
         <v>1810</v>
       </c>
       <c r="C4" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D4</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D4</f>
         <v>Gripped Iron Axe</v>
       </c>
       <c r="D4" s="21" t="str">
@@ -26638,7 +26619,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F4" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$113</f>
         <v>Iron</v>
       </c>
       <c r="G4" s="24">
@@ -26663,7 +26644,7 @@
         <v>1809</v>
       </c>
       <c r="C5" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D5</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D5</f>
         <v>Gripped Iron Sword</v>
       </c>
       <c r="D5" s="21" t="str">
@@ -26675,7 +26656,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F5" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$113</f>
         <v>Iron</v>
       </c>
       <c r="G5" s="24">
@@ -26700,7 +26681,7 @@
         <v>1808</v>
       </c>
       <c r="C6" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D6</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D6</f>
         <v>Gripped Wooden Sword</v>
       </c>
       <c r="D6" s="21" t="str">
@@ -26712,7 +26693,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F6" s="34" t="str">
-        <f>[1]Enums!$A$112</f>
+        <f>[1]Enums!$A$111</f>
         <v>Wooden</v>
       </c>
       <c r="G6" s="24">
@@ -26737,7 +26718,7 @@
         <v>1807</v>
       </c>
       <c r="C7" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D7</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D7</f>
         <v>Gripped Wooden Shovel</v>
       </c>
       <c r="D7" s="21" t="str">
@@ -26749,7 +26730,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F7" s="34" t="str">
-        <f>[1]Enums!$A$112</f>
+        <f>[1]Enums!$A$111</f>
         <v>Wooden</v>
       </c>
       <c r="G7" s="24">
@@ -26774,7 +26755,7 @@
         <v>1806</v>
       </c>
       <c r="C8" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D8</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D8</f>
         <v>Gripped Wooden Pickaxe</v>
       </c>
       <c r="D8" s="21" t="str">
@@ -26786,7 +26767,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F8" s="34" t="str">
-        <f>[1]Enums!$A$112</f>
+        <f>[1]Enums!$A$111</f>
         <v>Wooden</v>
       </c>
       <c r="G8" s="24">
@@ -26811,7 +26792,7 @@
         <v>1805</v>
       </c>
       <c r="C9" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D9</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D9</f>
         <v>Gripped Wooden Axe</v>
       </c>
       <c r="D9" s="21" t="str">
@@ -26823,7 +26804,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F9" s="34" t="str">
-        <f>[1]Enums!$A$112</f>
+        <f>[1]Enums!$A$111</f>
         <v>Wooden</v>
       </c>
       <c r="G9" s="24">
@@ -26848,7 +26829,7 @@
         <v>1804</v>
       </c>
       <c r="C10" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D10</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D10</f>
         <v>Gripped Stone Sword</v>
       </c>
       <c r="D10" s="21" t="str">
@@ -26860,7 +26841,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F10" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$112</f>
         <v>Stone</v>
       </c>
       <c r="G10" s="24">
@@ -26885,7 +26866,7 @@
         <v>1803</v>
       </c>
       <c r="C11" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D11</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D11</f>
         <v>Gripped Stone Shovel</v>
       </c>
       <c r="D11" s="21" t="str">
@@ -26897,7 +26878,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F11" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$112</f>
         <v>Stone</v>
       </c>
       <c r="G11" s="24">
@@ -26922,7 +26903,7 @@
         <v>1802</v>
       </c>
       <c r="C12" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D12</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D12</f>
         <v>Gripped Stone Pickaxe</v>
       </c>
       <c r="D12" s="21" t="str">
@@ -26934,7 +26915,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F12" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$112</f>
         <v>Stone</v>
       </c>
       <c r="G12" s="24">
@@ -26959,7 +26940,7 @@
         <v>1801</v>
       </c>
       <c r="C13" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D13</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D13</f>
         <v>Gripped Stone Axe</v>
       </c>
       <c r="D13" s="21" t="str">
@@ -26971,7 +26952,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F13" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$112</f>
         <v>Stone</v>
       </c>
       <c r="G13" s="24">
@@ -26996,7 +26977,7 @@
         <v>1800</v>
       </c>
       <c r="C14" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D14</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D14</f>
         <v>Gripped Diamond Sword</v>
       </c>
       <c r="D14" s="21" t="str">
@@ -27008,7 +26989,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F14" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$115</f>
         <v>Diamond</v>
       </c>
       <c r="G14" s="24">
@@ -27033,7 +27014,7 @@
         <v>1799</v>
       </c>
       <c r="C15" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D15</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D15</f>
         <v>Gripped Diamond Shovel</v>
       </c>
       <c r="D15" s="21" t="str">
@@ -27045,7 +27026,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F15" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$115</f>
         <v>Diamond</v>
       </c>
       <c r="G15" s="24">
@@ -27070,7 +27051,7 @@
         <v>1798</v>
       </c>
       <c r="C16" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D16</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D16</f>
         <v>Gripped Diamond Pickaxe</v>
       </c>
       <c r="D16" s="21" t="str">
@@ -27082,7 +27063,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F16" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$115</f>
         <v>Diamond</v>
       </c>
       <c r="G16" s="24">
@@ -27107,7 +27088,7 @@
         <v>1797</v>
       </c>
       <c r="C17" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D17</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D17</f>
         <v>Gripped Diamond Axe</v>
       </c>
       <c r="D17" s="21" t="str">
@@ -27119,7 +27100,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F17" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$115</f>
         <v>Diamond</v>
       </c>
       <c r="G17" s="24">
@@ -27144,7 +27125,7 @@
         <v>1796</v>
       </c>
       <c r="C18" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D18</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D18</f>
         <v>Gripped Golden Sword</v>
       </c>
       <c r="D18" s="21" t="str">
@@ -27156,7 +27137,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F18" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$114</f>
         <v>Golden</v>
       </c>
       <c r="G18" s="24">
@@ -27181,7 +27162,7 @@
         <v>1795</v>
       </c>
       <c r="C19" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D19</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D19</f>
         <v>Gripped Golden Shovel</v>
       </c>
       <c r="D19" s="21" t="str">
@@ -27193,7 +27174,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F19" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$114</f>
         <v>Golden</v>
       </c>
       <c r="G19" s="24">
@@ -27218,7 +27199,7 @@
         <v>1794</v>
       </c>
       <c r="C20" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D20</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D20</f>
         <v>Gripped Golden Pickaxe</v>
       </c>
       <c r="D20" s="21" t="str">
@@ -27230,7 +27211,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F20" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$114</f>
         <v>Golden</v>
       </c>
       <c r="G20" s="24">
@@ -27255,7 +27236,7 @@
         <v>1793</v>
       </c>
       <c r="C21" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D21</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D21</f>
         <v>Gripped Golden Axe</v>
       </c>
       <c r="D21" s="21" t="str">
@@ -27267,7 +27248,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F21" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$114</f>
         <v>Golden</v>
       </c>
       <c r="G21" s="24">
@@ -27292,7 +27273,7 @@
         <v>1792</v>
       </c>
       <c r="C22" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D22</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D22</f>
         <v>Gripped Wooden Hoe</v>
       </c>
       <c r="D22" s="21" t="str">
@@ -27304,7 +27285,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F22" s="34" t="str">
-        <f>[1]Enums!$A$112</f>
+        <f>[1]Enums!$A$111</f>
         <v>Wooden</v>
       </c>
       <c r="G22" s="24">
@@ -27329,7 +27310,7 @@
         <v>1791</v>
       </c>
       <c r="C23" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D23</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D23</f>
         <v>Gripped Stone Hoe</v>
       </c>
       <c r="D23" s="21" t="str">
@@ -27341,7 +27322,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F23" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$112</f>
         <v>Stone</v>
       </c>
       <c r="G23" s="24">
@@ -27366,7 +27347,7 @@
         <v>1790</v>
       </c>
       <c r="C24" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D24</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D24</f>
         <v>Gripped Iron Hoe</v>
       </c>
       <c r="D24" s="21" t="str">
@@ -27378,7 +27359,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F24" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$113</f>
         <v>Iron</v>
       </c>
       <c r="G24" s="24">
@@ -27403,7 +27384,7 @@
         <v>1789</v>
       </c>
       <c r="C25" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D25</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D25</f>
         <v>Gripped Diamond Hoe</v>
       </c>
       <c r="D25" s="21" t="str">
@@ -27415,7 +27396,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F25" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$115</f>
         <v>Diamond</v>
       </c>
       <c r="G25" s="24">
@@ -27440,7 +27421,7 @@
         <v>1788</v>
       </c>
       <c r="C26" s="22" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;D26</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;D26</f>
         <v>Gripped Golden Hoe</v>
       </c>
       <c r="D26" s="21" t="str">
@@ -27452,7 +27433,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F26" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$114</f>
         <v>Golden</v>
       </c>
       <c r="G26" s="24">
@@ -27514,7 +27495,7 @@
         <v>1832</v>
       </c>
       <c r="D1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$111</f>
+        <f xml:space="preserve"> [1]Enums!$A$110</f>
         <v>Base Material</v>
       </c>
       <c r="E1" s="36" t="s">
@@ -27560,7 +27541,7 @@
         <v>Wooden Pogo Stick</v>
       </c>
       <c r="D2" s="34" t="str">
-        <f>[1]Enums!$A$112</f>
+        <f>[1]Enums!$A$111</f>
         <v>Wooden</v>
       </c>
       <c r="E2" s="37">
@@ -27597,7 +27578,7 @@
         <v>Stone Pogo Stick</v>
       </c>
       <c r="D3" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$112</f>
         <v>Stone</v>
       </c>
       <c r="E3" s="37">
@@ -27633,7 +27614,7 @@
         <v>Iron Pogo Stick</v>
       </c>
       <c r="D4" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$113</f>
         <v>Iron</v>
       </c>
       <c r="E4" s="37">
@@ -27669,7 +27650,7 @@
         <v>Golden Pogo Stick</v>
       </c>
       <c r="D5" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$114</f>
         <v>Golden</v>
       </c>
       <c r="E5" s="37">
@@ -27705,7 +27686,7 @@
         <v>Diamond Pogo Stick</v>
       </c>
       <c r="D6" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$115</f>
         <v>Diamond</v>
       </c>
       <c r="E6" s="37">
@@ -27741,7 +27722,7 @@
         <v>Magic Pogo Stick</v>
       </c>
       <c r="D7" s="34" t="str">
-        <f>[1]Enums!$A$117</f>
+        <f>[1]Enums!$A$116</f>
         <v>Magic</v>
       </c>
       <c r="E7" s="37">
@@ -27773,11 +27754,11 @@
         <v>1821</v>
       </c>
       <c r="C8" s="34" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;I8</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;I8</f>
         <v>Gripped Wooden Pogo Stick</v>
       </c>
       <c r="D8" s="34" t="str">
-        <f>[1]Enums!$A$112</f>
+        <f>[1]Enums!$A$111</f>
         <v>Wooden</v>
       </c>
       <c r="E8" s="37">
@@ -27817,11 +27798,11 @@
         <v>1820</v>
       </c>
       <c r="C9" s="34" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;I9</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;I9</f>
         <v>Gripped Stone Pogo Stick</v>
       </c>
       <c r="D9" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$112</f>
         <v>Stone</v>
       </c>
       <c r="E9" s="37">
@@ -27861,11 +27842,11 @@
         <v>1819</v>
       </c>
       <c r="C10" s="34" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;I10</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;I10</f>
         <v>Gripped Iron Pogo Stick</v>
       </c>
       <c r="D10" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$113</f>
         <v>Iron</v>
       </c>
       <c r="E10" s="37">
@@ -27905,11 +27886,11 @@
         <v>1818</v>
       </c>
       <c r="C11" s="34" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;I11</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;I11</f>
         <v>Gripped Golden Pogo Stick</v>
       </c>
       <c r="D11" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$114</f>
         <v>Golden</v>
       </c>
       <c r="E11" s="37">
@@ -27949,11 +27930,11 @@
         <v>1817</v>
       </c>
       <c r="C12" s="34" t="str">
-        <f>[1]Enums!$A$108&amp;" "&amp;I12</f>
+        <f>[1]Enums!$A$107&amp;" "&amp;I12</f>
         <v>Gripped Diamond Pogo Stick</v>
       </c>
       <c r="D12" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$115</f>
         <v>Diamond</v>
       </c>
       <c r="E12" s="37">
@@ -46344,10 +46325,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -46371,7 +46352,7 @@
         <v>590</v>
       </c>
       <c r="D1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$80</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="19" t="str">
@@ -46391,11 +46372,11 @@
         <v>1756</v>
       </c>
       <c r="C2" s="10" t="str">
-        <f t="shared" ref="C2:C32" si="0">D2&amp;" ("&amp;E2&amp;")"</f>
+        <f t="shared" ref="C2:C33" si="0">D2&amp;" ("&amp;E2&amp;")"</f>
         <v>Mold (Grip)</v>
       </c>
       <c r="D2" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E2" s="11" t="str">
@@ -46420,7 +46401,7 @@
         <v>Mold (Running Shoes)</v>
       </c>
       <c r="D3" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E3" s="11" t="str">
@@ -46445,7 +46426,7 @@
         <v>Mold (Scuba Fins)</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E4" s="11" t="str">
@@ -46470,7 +46451,7 @@
         <v>Mold (Scuba Mask)</v>
       </c>
       <c r="D5" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E5" s="11" t="str">
@@ -46495,7 +46476,7 @@
         <v>Mold (Gasket)</v>
       </c>
       <c r="D6" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E6" s="11" t="str">
@@ -46520,7 +46501,7 @@
         <v>Mold (Life Preserver)</v>
       </c>
       <c r="D7" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E7" s="11" t="str">
@@ -46545,7 +46526,7 @@
         <v>Metal Die (Fibers)</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Metal Die</v>
       </c>
       <c r="E8" s="11" t="str">
@@ -46570,7 +46551,7 @@
         <v>Metal Die (Tether)</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Metal Die</v>
       </c>
       <c r="E9" s="11" t="str">
@@ -46595,7 +46576,7 @@
         <v>Metal Die (Cord)</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Metal Die</v>
       </c>
       <c r="E10" s="11" t="str">
@@ -46620,7 +46601,7 @@
         <v>Metal Die (Hose)</v>
       </c>
       <c r="D11" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Metal Die</v>
       </c>
       <c r="E11" s="11" t="str">
@@ -46645,7 +46626,7 @@
         <v>Metal Die (Pipe Segment)</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Metal Die</v>
       </c>
       <c r="E12" s="11" t="str">
@@ -46670,7 +46651,7 @@
         <v>Mold (Flashlight Shaft)</v>
       </c>
       <c r="D13" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E13" s="11" t="str">
@@ -46694,7 +46675,7 @@
         <v>Mold (Plastic Brick (1 x 1))</v>
       </c>
       <c r="D14" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E14" t="str">
@@ -46718,7 +46699,7 @@
         <v>Mold (Plastic Brick (1 x 2))</v>
       </c>
       <c r="D15" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E15" t="str">
@@ -46742,7 +46723,7 @@
         <v>Mold (Plastic Brick (1 x 3))</v>
       </c>
       <c r="D16" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E16" t="str">
@@ -46766,7 +46747,7 @@
         <v>Mold (Plastic Brick (1 x 4))</v>
       </c>
       <c r="D17" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E17" t="str">
@@ -46790,7 +46771,7 @@
         <v>Mold (Plastic Brick (2 x 2))</v>
       </c>
       <c r="D18" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E18" t="str">
@@ -46814,7 +46795,7 @@
         <v>Mold (Plastic Brick (2 x 3))</v>
       </c>
       <c r="D19" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E19" t="str">
@@ -46838,7 +46819,7 @@
         <v>Mold (Plastic Brick (2 x 4))</v>
       </c>
       <c r="D20" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E20" t="str">
@@ -46862,7 +46843,7 @@
         <v>Mold (Plastic Brick (3 x 3))</v>
       </c>
       <c r="D21" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E21" t="str">
@@ -46886,7 +46867,7 @@
         <v>Mold (Plastic Brick (3 x 4))</v>
       </c>
       <c r="D22" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E22" t="str">
@@ -46910,7 +46891,7 @@
         <v>Mold (Plastic Brick (4 x 4))</v>
       </c>
       <c r="D23" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E23" t="str">
@@ -46934,7 +46915,7 @@
         <v>Mold (Plastic Brick (1 x 8))</v>
       </c>
       <c r="D24" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E24" t="str">
@@ -46958,7 +46939,7 @@
         <v>Mold (Plastic Brick (2 x 8))</v>
       </c>
       <c r="D25" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E25" t="str">
@@ -46982,7 +46963,7 @@
         <v>Mold (Heated Knife Handle)</v>
       </c>
       <c r="D26" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E26" s="11" t="str">
@@ -47006,7 +46987,7 @@
         <v>Mold (Rubber Sole)</v>
       </c>
       <c r="D27" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E27" s="11" t="str">
@@ -47030,7 +47011,7 @@
         <v>Mold (Battery Case)</v>
       </c>
       <c r="D28" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E28" s="11" t="str">
@@ -47054,7 +47035,7 @@
         <v>Mold (Tool Shaft)</v>
       </c>
       <c r="D29" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E29" t="str">
@@ -47078,7 +47059,7 @@
         <v>Mold (Lighter Body)</v>
       </c>
       <c r="D30" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E30" t="str">
@@ -47102,7 +47083,7 @@
         <v>Mold (Cell Phone Case)</v>
       </c>
       <c r="D31" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E31" t="str">
@@ -47126,7 +47107,7 @@
         <v>Mold (Walky Talky Case)</v>
       </c>
       <c r="D32" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E32" t="str">
@@ -47146,11 +47127,11 @@
         <v>2689</v>
       </c>
       <c r="C33" s="10" t="str">
-        <f>D33&amp;" ("&amp;E33&amp;")"</f>
+        <f t="shared" si="0"/>
         <v>Mold (HAM Radio Case)</v>
       </c>
       <c r="D33" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$83</f>
         <v>Mold</v>
       </c>
       <c r="E33" t="str">
@@ -47158,30 +47139,6 @@
         <v>HAM Radio Case</v>
       </c>
       <c r="F33">
-        <v>8192</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="str">
-        <f>[1]Enums!$A$22</f>
-        <v>1.3.3</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>2708</v>
-      </c>
-      <c r="C34" s="10" t="str">
-        <f>D34&amp;" ("&amp;E34&amp;")"</f>
-        <v>Mold (Flagpole Segment)</v>
-      </c>
-      <c r="D34" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
-        <v>Mold</v>
-      </c>
-      <c r="E34" t="str">
-        <f>'[1]Polymer Objects'!$B34</f>
-        <v>Flagpole Segment</v>
-      </c>
-      <c r="F34">
         <v>8192</v>
       </c>
     </row>
@@ -47195,10 +47152,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:U157"/>
+  <dimension ref="A1:U156"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="H162" sqref="H162"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="I140" sqref="I140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -53511,85 +53468,8 @@
       </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A156" s="23" t="str">
-        <f>[1]Enums!$A$22</f>
-        <v>1.3.3</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>2709</v>
-      </c>
-      <c r="C156" s="22" t="str">
-        <f xml:space="preserve"> VLOOKUP(D156, Molds!C:E, 3, FALSE)&amp;" ("&amp;F156&amp;")"</f>
-        <v>Flagpole Segment (PEEK)</v>
-      </c>
-      <c r="D156" s="24" t="str">
-        <f xml:space="preserve"> Molds!$C$34</f>
-        <v>Mold (Flagpole Segment)</v>
-      </c>
-      <c r="E156" s="21" t="str">
-        <f>Pellets!$F$47</f>
-        <v>Bag (PolyEther Ether Ketone Pellets)</v>
-      </c>
-      <c r="F156" s="21" t="str">
-        <f>VLOOKUP(E80, Pellets!F:M,8,FALSE)</f>
-        <v>PEEK</v>
-      </c>
-      <c r="G156" s="21">
-        <v>8</v>
-      </c>
-      <c r="H156" s="21">
-        <v>10</v>
-      </c>
-      <c r="I156" s="21">
-        <v>64</v>
-      </c>
-      <c r="J156" s="24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A157" s="23" t="str">
-        <f>[1]Enums!$A$22</f>
-        <v>1.3.3</v>
-      </c>
-      <c r="B157" s="3" t="s">
-        <v>2710</v>
-      </c>
-      <c r="C157" s="22" t="str">
-        <f xml:space="preserve"> VLOOKUP(D157, Molds!C:E, 3, FALSE)&amp;" ("&amp;F157&amp;")"</f>
-        <v>Flagpole Segment (Carbon Fiber Composite)</v>
-      </c>
-      <c r="D157" s="24" t="str">
-        <f xml:space="preserve"> Molds!$C$34</f>
-        <v>Mold (Flagpole Segment)</v>
-      </c>
-      <c r="E157" s="21" t="str">
-        <f>Pellets!$F$116</f>
-        <v>Vial (Epoxy-Carbon Fiber Resin)</v>
-      </c>
-      <c r="F157" s="21" t="str">
-        <f>LEFT(VLOOKUP(E157, Pellets!F:M, 8,FALSE), FIND("(", VLOOKUP(E157, Pellets!F:M, 8,FALSE))-8)&amp;" Composite"</f>
-        <v>Carbon Fiber Composite</v>
-      </c>
-      <c r="G157" s="21">
-        <v>8</v>
-      </c>
-      <c r="H157" s="21">
-        <v>10</v>
-      </c>
-      <c r="I157" s="21">
-        <v>64</v>
-      </c>
-      <c r="J157" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="K157" s="42" t="s">
-        <v>2504</v>
-      </c>
-      <c r="L157" s="21" t="str">
-        <f>Pellets!$F$117</f>
-        <v>Vial (Phenolic-Carbon Fiber Resin)</v>
-      </c>
+      <c r="A156" s="23"/>
+      <c r="C156" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -53632,7 +53512,7 @@
         <v>2518</v>
       </c>
       <c r="D1" s="53" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$80</f>
+        <f xml:space="preserve"> [1]Enums!$B$79</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="20" t="s">
@@ -53666,7 +53546,7 @@
         <v>Wafer (Solar Cell)</v>
       </c>
       <c r="D2" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$91</f>
         <v>Wafer</v>
       </c>
       <c r="E2" s="49" t="s">
@@ -53693,7 +53573,7 @@
         <v>Wafer (Processor)</v>
       </c>
       <c r="D3" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$91</f>
         <v>Wafer</v>
       </c>
       <c r="E3" s="49" t="s">
@@ -53720,7 +53600,7 @@
         <v>Wafer (Temperature Sensor)</v>
       </c>
       <c r="D4" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$91</f>
         <v>Wafer</v>
       </c>
       <c r="E4" s="49" t="s">
@@ -53747,7 +53627,7 @@
         <v>Wafer (Pressure Sensor)</v>
       </c>
       <c r="D5" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$91</f>
         <v>Wafer</v>
       </c>
       <c r="E5" s="49" t="s">
@@ -53774,7 +53654,7 @@
         <v>Wafer (Low Power Radio)</v>
       </c>
       <c r="D6" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$91</f>
         <v>Wafer</v>
       </c>
       <c r="E6" s="49" t="s">
@@ -53801,7 +53681,7 @@
         <v>Wafer (DSP)</v>
       </c>
       <c r="D7" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$91</f>
         <v>Wafer</v>
       </c>
       <c r="E7" s="49" t="s">
@@ -53828,7 +53708,7 @@
         <v>Wafer (Digital Analog Convertor)</v>
       </c>
       <c r="D8" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$91</f>
         <v>Wafer</v>
       </c>
       <c r="E8" s="49" t="s">
@@ -53855,7 +53735,7 @@
         <v>Wafer (Amplifier)</v>
       </c>
       <c r="D9" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$91</f>
         <v>Wafer</v>
       </c>
       <c r="E9" s="49" t="s">
@@ -53882,7 +53762,7 @@
         <v>Wafer (OLED Array)</v>
       </c>
       <c r="D10" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$92</f>
+        <f xml:space="preserve"> [1]Enums!$B$91</f>
         <v>Wafer</v>
       </c>
       <c r="E10" s="49" t="s">

</xml_diff>

<commit_message>
1.3.5 Update with working Air Quality Detector
</commit_message>
<xml_diff>
--- a/config/Polycraft Polymers.xlsx
+++ b/config/Polycraft Polymers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="826" activeTab="2"/>
+    <workbookView xWindow="10230" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="826" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Pellets" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2942" uniqueCount="2708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2944" uniqueCount="2710">
   <si>
     <t>GC</t>
   </si>
@@ -8175,6 +8175,12 @@
   </si>
   <si>
     <t>Silicon Wafer (Ruined)</t>
+  </si>
+  <si>
+    <t>1bZ</t>
+  </si>
+  <si>
+    <t>1fu</t>
   </si>
 </sst>
 </file>
@@ -8474,118 +8480,123 @@
             <v>1.3.2</v>
           </cell>
         </row>
-        <row r="32">
-          <cell r="A32" t="str">
-            <v>Bag</v>
+        <row r="24">
+          <cell r="A24" t="str">
+            <v>1.3.5</v>
           </cell>
         </row>
         <row r="33">
           <cell r="A33" t="str">
-            <v>Vial</v>
+            <v>Bag</v>
           </cell>
         </row>
-        <row r="35">
-          <cell r="A35" t="str">
-            <v>Sack</v>
+        <row r="34">
+          <cell r="A34" t="str">
+            <v>Vial</v>
           </cell>
         </row>
         <row r="36">
           <cell r="A36" t="str">
-            <v>Beaker</v>
+            <v>Sack</v>
           </cell>
         </row>
-        <row r="38">
-          <cell r="A38" t="str">
-            <v>Powder Keg</v>
+        <row r="37">
+          <cell r="A37" t="str">
+            <v>Beaker</v>
           </cell>
         </row>
         <row r="39">
           <cell r="A39" t="str">
-            <v>Drum</v>
+            <v>Powder Keg</v>
           </cell>
         </row>
-        <row r="41">
-          <cell r="A41" t="str">
-            <v>Chemical Silo</v>
+        <row r="40">
+          <cell r="A40" t="str">
+            <v>Drum</v>
           </cell>
         </row>
         <row r="42">
           <cell r="A42" t="str">
+            <v>Chemical Silo</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43" t="str">
             <v>Chemical Vat</v>
           </cell>
         </row>
-        <row r="81">
-          <cell r="B81" t="str">
+        <row r="82">
+          <cell r="B82" t="str">
             <v>Mold Type</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="B85" t="str">
-            <v>Mold</v>
           </cell>
         </row>
         <row r="86">
           <cell r="B86" t="str">
-            <v>Metal Die</v>
+            <v>Mold</v>
           </cell>
         </row>
-        <row r="93">
-          <cell r="B93" t="str">
-            <v>Wafer</v>
+        <row r="87">
+          <cell r="B87" t="str">
+            <v>Metal Die</v>
           </cell>
         </row>
         <row r="94">
           <cell r="B94" t="str">
+            <v>Wafer</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="B95" t="str">
             <v>Mask</v>
           </cell>
         </row>
-        <row r="109">
-          <cell r="A109" t="str">
+        <row r="110">
+          <cell r="A110" t="str">
             <v>Gripped</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="A112" t="str">
-            <v>Base Material</v>
           </cell>
         </row>
         <row r="113">
           <cell r="A113" t="str">
-            <v>Wooden</v>
+            <v>Base Material</v>
           </cell>
         </row>
         <row r="114">
           <cell r="A114" t="str">
-            <v>Stone</v>
+            <v>Wooden</v>
           </cell>
         </row>
         <row r="115">
           <cell r="A115" t="str">
-            <v>Iron</v>
+            <v>Stone</v>
           </cell>
         </row>
         <row r="116">
           <cell r="A116" t="str">
-            <v>Golden</v>
+            <v>Iron</v>
           </cell>
         </row>
         <row r="117">
           <cell r="A117" t="str">
-            <v>Diamond</v>
+            <v>Golden</v>
           </cell>
         </row>
         <row r="118">
           <cell r="A118" t="str">
-            <v>Magic</v>
+            <v>Diamond</v>
           </cell>
         </row>
-        <row r="147">
-          <cell r="A147" t="str">
-            <v>Composite</v>
+        <row r="119">
+          <cell r="A119" t="str">
+            <v>Magic</v>
           </cell>
         </row>
         <row r="148">
           <cell r="A148" t="str">
+            <v>Composite</v>
+          </cell>
+        </row>
+        <row r="149">
+          <cell r="A149" t="str">
             <v>Engineered</v>
           </cell>
         </row>
@@ -10216,6 +10227,11 @@
             <v>HAM Radio Case</v>
           </cell>
         </row>
+        <row r="34">
+          <cell r="B34" t="str">
+            <v>Air Quality Detector Case</v>
+          </cell>
+        </row>
       </sheetData>
     </sheetDataSet>
   </externalBook>
@@ -10851,19 +10867,19 @@
         <v>Game ID XL</v>
       </c>
       <c r="F1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$32&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$33&amp;" ("&amp;J1&amp;")"</f>
         <v>Bag (Pellets)</v>
       </c>
       <c r="G1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$35&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$36&amp;" ("&amp;J1&amp;")"</f>
         <v>Sack (Pellets)</v>
       </c>
       <c r="H1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$38&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$39&amp;" ("&amp;J1&amp;")"</f>
         <v>Powder Keg (Pellets)</v>
       </c>
       <c r="I1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$41&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$42&amp;" ("&amp;J1&amp;")"</f>
         <v>Chemical Silo (Pellets)</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -10902,19 +10918,19 @@
         <v>448</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="G2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="H2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="J2" s="1" t="str">
@@ -10954,19 +10970,19 @@
         <v>444</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J3" s="1" t="str">
@@ -11003,19 +11019,19 @@
         <v>440</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Alkyd Resin)</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Alkyd Resin)</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Alkyd Resin)</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Alkyd Resin)</v>
       </c>
       <c r="J4" s="1" t="str">
@@ -11055,19 +11071,19 @@
         <v>436</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J5" s="1" t="str">
@@ -11107,19 +11123,19 @@
         <v>432</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J6" s="1" t="str">
@@ -11159,19 +11175,19 @@
         <v>428</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$32, [1]Enums!$A$32)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$33, [1]Enums!$A$33)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Carbon Fiber)</v>
       </c>
       <c r="G7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$35, [1]Enums!$A$35)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$36, [1]Enums!$A$36)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Carbon Fiber)</v>
       </c>
       <c r="H7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$38, [1]Enums!$A$38)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$39, [1]Enums!$A$39)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Carbon Fiber)</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$41, [1]Enums!$A$41)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$42, [1]Enums!$A$42)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Carbon Fiber)</v>
       </c>
       <c r="J7" s="1" t="str">
@@ -11208,19 +11224,19 @@
         <v>424</v>
       </c>
       <c r="F8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="G8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="J8" s="1" t="str">
@@ -11260,19 +11276,19 @@
         <v>420</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulosic Pellets)</v>
       </c>
       <c r="G9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulosic Pellets)</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulosic Pellets)</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulosic Pellets)</v>
       </c>
       <c r="J9" s="1" t="str">
@@ -11312,19 +11328,19 @@
         <v>416</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chitin Pellets)</v>
       </c>
       <c r="G10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chitin Pellets)</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chitin Pellets)</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chitin Pellets)</v>
       </c>
       <c r="J10" s="1" t="str">
@@ -11364,19 +11380,19 @@
         <v>412</v>
       </c>
       <c r="F11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J11" s="1" t="str">
@@ -11416,19 +11432,19 @@
         <v>408</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Epoxy Resin)</v>
       </c>
       <c r="G12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Epoxy Resin)</v>
       </c>
       <c r="H12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Epoxy Resin)</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Epoxy Resin)</v>
       </c>
       <c r="J12" s="1" t="str">
@@ -11465,19 +11481,19 @@
         <v>404</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethoxylates Pellets)</v>
       </c>
       <c r="G13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethoxylates Pellets)</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethoxylates Pellets)</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethoxylates Pellets)</v>
       </c>
       <c r="J13" s="1" t="str">
@@ -11517,19 +11533,19 @@
         <v>400</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="G14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="H14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="J14" s="1" t="str">
@@ -11569,19 +11585,19 @@
         <v>396</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="G15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="J15" s="1" t="str">
@@ -11621,19 +11637,19 @@
         <v>392</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="G16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="J16" s="1" t="str">
@@ -11673,19 +11689,19 @@
         <v>388</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="G17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="J17" s="1" t="str">
@@ -11725,19 +11741,19 @@
         <v>384</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J18" s="1" t="str">
@@ -11777,19 +11793,19 @@
         <v>380</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J19" s="1" t="str">
@@ -11826,19 +11842,19 @@
         <v>376</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Lignin)</v>
       </c>
       <c r="G20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Lignin)</v>
       </c>
       <c r="H20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Lignin)</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Lignin)</v>
       </c>
       <c r="J20" s="1" t="str">
@@ -11878,19 +11894,19 @@
         <v>372</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J21" s="1" t="str">
@@ -11930,19 +11946,19 @@
         <v>368</v>
       </c>
       <c r="F22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="G22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="H22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="J22" s="1" t="str">
@@ -11982,19 +11998,19 @@
         <v>364</v>
       </c>
       <c r="F23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="G23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="H23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="J23" s="1" t="str">
@@ -12034,19 +12050,19 @@
         <v>360</v>
       </c>
       <c r="F24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="G24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="H24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="J24" s="1" t="str">
@@ -12083,19 +12099,19 @@
         <v>356</v>
       </c>
       <c r="F25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="G25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="H25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="J25" s="1" t="str">
@@ -12135,19 +12151,19 @@
         <v>352</v>
       </c>
       <c r="F26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Metaldehyde Pellets)</v>
       </c>
       <c r="G26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Metaldehyde Pellets)</v>
       </c>
       <c r="H26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Metaldehyde Pellets)</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Metaldehyde Pellets)</v>
       </c>
       <c r="J26" s="1" t="str">
@@ -12187,19 +12203,19 @@
         <v>348</v>
       </c>
       <c r="F27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J27" s="1" t="str">
@@ -12239,19 +12255,19 @@
         <v>344</v>
       </c>
       <c r="F28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraformaldehyde Pellets)</v>
       </c>
       <c r="G28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraformaldehyde Pellets)</v>
       </c>
       <c r="H28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraformaldehyde Pellets)</v>
       </c>
       <c r="I28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraformaldehyde Pellets)</v>
       </c>
       <c r="J28" s="1" t="str">
@@ -12291,19 +12307,19 @@
         <v>340</v>
       </c>
       <c r="F29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraldehyde Pellets)</v>
       </c>
       <c r="G29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraldehyde Pellets)</v>
       </c>
       <c r="H29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraldehyde Pellets)</v>
       </c>
       <c r="I29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraldehyde Pellets)</v>
       </c>
       <c r="J29" s="1" t="str">
@@ -12343,19 +12359,19 @@
         <v>336</v>
       </c>
       <c r="F30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Phenolic Resin)</v>
       </c>
       <c r="G30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Phenolic Resin)</v>
       </c>
       <c r="H30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Phenolic Resin)</v>
       </c>
       <c r="I30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Phenolic Resin)</v>
       </c>
       <c r="J30" s="1" t="str">
@@ -12395,19 +12411,19 @@
         <v>332</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="G31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="H31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="I31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="J31" s="1" t="str">
@@ -12447,19 +12463,19 @@
         <v>328</v>
       </c>
       <c r="F32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly1-Butene Pellets)</v>
       </c>
       <c r="G32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly1-Butene Pellets)</v>
       </c>
       <c r="H32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly1-Butene Pellets)</v>
       </c>
       <c r="I32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly1-Butene Pellets)</v>
       </c>
       <c r="J32" s="1" t="str">
@@ -12499,19 +12515,19 @@
         <v>324</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="G33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="H33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="I33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="J33" s="1" t="str">
@@ -12551,19 +12567,19 @@
         <v>320</v>
       </c>
       <c r="F34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="G34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="H34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="I34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="J34" s="1" t="str">
@@ -12603,19 +12619,19 @@
         <v>316</v>
       </c>
       <c r="F35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="G35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="H35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="I35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="J35" s="1" t="str">
@@ -12655,19 +12671,19 @@
         <v>312</v>
       </c>
       <c r="F36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="G36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="H36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="I36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="J36" s="1" t="str">
@@ -12707,19 +12723,19 @@
         <v>308</v>
       </c>
       <c r="F37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="G37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="H37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="I37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="J37" s="1" t="str">
@@ -12759,19 +12775,19 @@
         <v>304</v>
       </c>
       <c r="F38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="G38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="H38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="I38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="J38" s="1" t="str">
@@ -12811,19 +12827,19 @@
         <v>300</v>
       </c>
       <c r="F39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="G39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="H39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="I39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="J39" s="1" t="str">
@@ -12863,19 +12879,19 @@
         <v>296</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="G40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="H40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="I40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="J40" s="1" t="str">
@@ -12915,19 +12931,19 @@
         <v>292</v>
       </c>
       <c r="F41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="G41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="H41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="I41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="J41" s="1" t="str">
@@ -12967,19 +12983,19 @@
         <v>288</v>
       </c>
       <c r="F42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCaprolactone Pellets)</v>
       </c>
       <c r="G42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCaprolactone Pellets)</v>
       </c>
       <c r="H42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCaprolactone Pellets)</v>
       </c>
       <c r="I42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCaprolactone Pellets)</v>
       </c>
       <c r="J42" s="1" t="str">
@@ -13019,19 +13035,19 @@
         <v>284</v>
       </c>
       <c r="F43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCarbonate Pellets)</v>
       </c>
       <c r="G43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCarbonate Pellets)</v>
       </c>
       <c r="H43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCarbonate Pellets)</v>
       </c>
       <c r="I43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCarbonate Pellets)</v>
       </c>
       <c r="J43" s="1" t="str">
@@ -13071,19 +13087,19 @@
         <v>280</v>
       </c>
       <c r="F44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChloroPrene Pellets)</v>
       </c>
       <c r="G44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChloroPrene Pellets)</v>
       </c>
       <c r="H44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChloroPrene Pellets)</v>
       </c>
       <c r="I44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChloroPrene Pellets)</v>
       </c>
       <c r="J44" s="1" t="str">
@@ -13120,19 +13136,19 @@
         <v>276</v>
       </c>
       <c r="F45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="G45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="H45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="I45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="J45" s="1" t="str">
@@ -13172,19 +13188,19 @@
         <v>272</v>
       </c>
       <c r="F46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="G46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="H46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="I46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="J46" s="1" t="str">
@@ -13224,19 +13240,19 @@
         <v>268</v>
       </c>
       <c r="F47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="G47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="H47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="I47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="J47" s="1" t="str">
@@ -13276,19 +13292,19 @@
         <v>264</v>
       </c>
       <c r="F48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEtherImide Pellets)</v>
       </c>
       <c r="G48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEtherImide Pellets)</v>
       </c>
       <c r="H48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEtherImide Pellets)</v>
       </c>
       <c r="I48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEtherImide Pellets)</v>
       </c>
       <c r="J48" s="1" t="str">
@@ -13325,19 +13341,19 @@
         <v>260</v>
       </c>
       <c r="F49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="G49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="H49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="I49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="J49" s="1" t="str">
@@ -13374,19 +13390,19 @@
         <v>256</v>
       </c>
       <c r="F50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="G50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="H50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="I50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="J50" s="1" t="str">
@@ -13426,19 +13442,19 @@
         <v>252</v>
       </c>
       <c r="F51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="G51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="H51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="I51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="J51" s="1" t="str">
@@ -13475,19 +13491,19 @@
         <v>248</v>
       </c>
       <c r="F52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J52" s="1" t="str">
@@ -13527,19 +13543,19 @@
         <v>244</v>
       </c>
       <c r="F53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="G53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="H53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="I53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="J53" s="1" t="str">
@@ -13579,19 +13595,19 @@
         <v>240</v>
       </c>
       <c r="F54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="G54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="H54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="I54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="J54" s="1" t="str">
@@ -13631,19 +13647,19 @@
         <v>236</v>
       </c>
       <c r="F55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="G55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="H55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="I55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="J55" s="1" t="str">
@@ -13683,19 +13699,19 @@
         <v>232</v>
       </c>
       <c r="F56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J56" s="1" t="str">
@@ -13735,19 +13751,19 @@
         <v>228</v>
       </c>
       <c r="F57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="G57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="H57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="I57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="J57" s="1" t="str">
@@ -13787,19 +13803,19 @@
         <v>224</v>
       </c>
       <c r="F58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="G58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="H58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="I58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="J58" s="1" t="str">
@@ -13839,19 +13855,19 @@
         <v>220</v>
       </c>
       <c r="F59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="G59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="H59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="I59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="J59" s="1" t="str">
@@ -13891,19 +13907,19 @@
         <v>216</v>
       </c>
       <c r="F60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="G60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="H60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="I60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="J60" s="1" t="str">
@@ -13943,19 +13959,19 @@
         <v>212</v>
       </c>
       <c r="F61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="G61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="H61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="I61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="J61" s="1" t="str">
@@ -13992,19 +14008,19 @@
         <v>208</v>
       </c>
       <c r="F62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="G62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="H62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="I62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="J62" s="1" t="str">
@@ -14044,19 +14060,19 @@
         <v>204</v>
       </c>
       <c r="F63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyImide Pellets)</v>
       </c>
       <c r="G63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyImide Pellets)</v>
       </c>
       <c r="H63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyImide Pellets)</v>
       </c>
       <c r="I63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyImide Pellets)</v>
       </c>
       <c r="J63" s="1" t="str">
@@ -14093,19 +14109,19 @@
         <v>200</v>
       </c>
       <c r="F64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="G64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="H64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="I64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="J64" s="1" t="str">
@@ -14142,19 +14158,19 @@
         <v>196</v>
       </c>
       <c r="F65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="G65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="H65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="I65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="J65" s="1" t="str">
@@ -14194,19 +14210,19 @@
         <v>192</v>
       </c>
       <c r="F66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButylene Pellets)</v>
       </c>
       <c r="G66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButylene Pellets)</v>
       </c>
       <c r="H66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButylene Pellets)</v>
       </c>
       <c r="I66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButylene Pellets)</v>
       </c>
       <c r="J66" s="1" t="str">
@@ -14246,19 +14262,19 @@
         <v>188</v>
       </c>
       <c r="F67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoPrene Pellets)</v>
       </c>
       <c r="G67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoPrene Pellets)</v>
       </c>
       <c r="H67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoPrene Pellets)</v>
       </c>
       <c r="I67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoPrene Pellets)</v>
       </c>
       <c r="J67" s="1" t="str">
@@ -14298,19 +14314,19 @@
         <v>184</v>
       </c>
       <c r="F68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic Acid Pellets)</v>
       </c>
       <c r="G68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic Acid Pellets)</v>
       </c>
       <c r="H68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic Acid Pellets)</v>
       </c>
       <c r="I68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic Acid Pellets)</v>
       </c>
       <c r="J68" s="1" t="str">
@@ -14347,19 +14363,19 @@
         <v>180</v>
       </c>
       <c r="F69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="G69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="H69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="I69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="J69" s="1" t="str">
@@ -14399,19 +14415,19 @@
         <v>176</v>
       </c>
       <c r="F70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="G70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="H70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="I70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="J70" s="1" t="str">
@@ -14448,19 +14464,19 @@
         <v>172</v>
       </c>
       <c r="F71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="G71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="H71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="I71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="J71" s="1" t="str">
@@ -14500,19 +14516,19 @@
         <v>168</v>
       </c>
       <c r="F72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="G72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="H72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="I72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="J72" s="1" t="str">
@@ -14552,19 +14568,19 @@
         <v>164</v>
       </c>
       <c r="F73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="G73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="H73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="I73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="J73" s="1" t="str">
@@ -14604,19 +14620,19 @@
         <v>160</v>
       </c>
       <c r="F74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="G74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="H74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="I74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="J74" s="1" t="str">
@@ -14653,19 +14669,19 @@
         <v>156</v>
       </c>
       <c r="F75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J75" s="1" t="str">
@@ -14705,19 +14721,19 @@
         <v>152</v>
       </c>
       <c r="F76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyOxymethylene Pellets)</v>
       </c>
       <c r="G76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyOxymethylene Pellets)</v>
       </c>
       <c r="H76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyOxymethylene Pellets)</v>
       </c>
       <c r="I76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyOxymethylene Pellets)</v>
       </c>
       <c r="J76" s="1" t="str">
@@ -14754,19 +14770,19 @@
         <v>148</v>
       </c>
       <c r="F77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J77" s="1" t="str">
@@ -14806,19 +14822,19 @@
         <v>144</v>
       </c>
       <c r="F78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenol Pellets)</v>
       </c>
       <c r="G78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenol Pellets)</v>
       </c>
       <c r="H78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenol Pellets)</v>
       </c>
       <c r="I78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenol Pellets)</v>
       </c>
       <c r="J78" s="1" t="str">
@@ -14855,19 +14871,19 @@
         <v>140</v>
       </c>
       <c r="F79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="G79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="H79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="I79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="J79" s="1" t="str">
@@ -14904,19 +14920,19 @@
         <v>136</v>
       </c>
       <c r="F80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhosphazene Pellets)</v>
       </c>
       <c r="G80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhosphazene Pellets)</v>
       </c>
       <c r="H80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhosphazene Pellets)</v>
       </c>
       <c r="I80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhosphazene Pellets)</v>
       </c>
       <c r="J80" s="1" t="str">
@@ -14953,19 +14969,19 @@
         <v>132</v>
       </c>
       <c r="F81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="G81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="H81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="I81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="J81" s="1" t="str">
@@ -15002,19 +15018,19 @@
         <v>128</v>
       </c>
       <c r="F82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="G82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="H82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="I82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="J82" s="1" t="str">
@@ -15054,19 +15070,19 @@
         <v>124</v>
       </c>
       <c r="F83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="G83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="H83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="I83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="J83" s="1" t="str">
@@ -15106,19 +15122,19 @@
         <v>120</v>
       </c>
       <c r="F84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Pellets)</v>
       </c>
       <c r="G84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Pellets)</v>
       </c>
       <c r="H84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Pellets)</v>
       </c>
       <c r="I84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Pellets)</v>
       </c>
       <c r="J84" s="1" t="str">
@@ -15155,19 +15171,19 @@
         <v>116</v>
       </c>
       <c r="F85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="G85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="H85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="I85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="J85" s="1" t="str">
@@ -15204,19 +15220,19 @@
         <v>112</v>
       </c>
       <c r="F86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="G86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="H86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="I86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="J86" s="1" t="str">
@@ -15256,19 +15272,19 @@
         <v>108</v>
       </c>
       <c r="F87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyStyrene Pellets)</v>
       </c>
       <c r="G87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyStyrene Pellets)</v>
       </c>
       <c r="H87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyStyrene Pellets)</v>
       </c>
       <c r="I87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyStyrene Pellets)</v>
       </c>
       <c r="J87" s="1" t="str">
@@ -15305,19 +15321,19 @@
         <v>104</v>
       </c>
       <c r="F88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J88" s="1" t="str">
@@ -15357,19 +15373,19 @@
         <v>100</v>
       </c>
       <c r="F89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="G89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="H89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="I89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="J89" s="1" t="str">
@@ -15406,19 +15422,19 @@
         <v>96</v>
       </c>
       <c r="F90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="G90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="H90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="I90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="J90" s="1" t="str">
@@ -15455,19 +15471,19 @@
         <v>92</v>
       </c>
       <c r="F91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="G91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="H91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="I91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="J91" s="1" t="str">
@@ -15504,19 +15520,19 @@
         <v>88</v>
       </c>
       <c r="F92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyThiazyl Pellets)</v>
       </c>
       <c r="G92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyThiazyl Pellets)</v>
       </c>
       <c r="H92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyThiazyl Pellets)</v>
       </c>
       <c r="I92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyThiazyl Pellets)</v>
       </c>
       <c r="J92" s="1" t="str">
@@ -15556,19 +15572,19 @@
         <v>84</v>
       </c>
       <c r="F93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="G93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="H93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="I93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="J93" s="1" t="str">
@@ -15608,19 +15624,19 @@
         <v>80</v>
       </c>
       <c r="F94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyUrethane Pellets)</v>
       </c>
       <c r="G94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyUrethane Pellets)</v>
       </c>
       <c r="H94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyUrethane Pellets)</v>
       </c>
       <c r="I94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyUrethane Pellets)</v>
       </c>
       <c r="J94" s="1" t="str">
@@ -15660,19 +15676,19 @@
         <v>76</v>
       </c>
       <c r="F95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="G95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="H95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="I95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="J95" s="1" t="str">
@@ -15712,19 +15728,19 @@
         <v>72</v>
       </c>
       <c r="F96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="G96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="H96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="I96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="J96" s="1" t="str">
@@ -15761,19 +15777,19 @@
         <v>68</v>
       </c>
       <c r="F97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="G97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="H97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="I97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="J97" s="1" t="str">
@@ -15813,19 +15829,19 @@
         <v>64</v>
       </c>
       <c r="F98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="G98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="H98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="I98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="J98" s="1" t="str">
@@ -15865,19 +15881,19 @@
         <v>60</v>
       </c>
       <c r="F99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="G99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="H99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="I99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="J99" s="1" t="str">
@@ -15914,19 +15930,19 @@
         <v>56</v>
       </c>
       <c r="F100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="G100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="H100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="I100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="J100" s="1" t="str">
@@ -15963,19 +15979,19 @@
         <v>52</v>
       </c>
       <c r="F101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="G101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="H101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="I101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="J101" s="1" t="str">
@@ -16012,19 +16028,19 @@
         <v>48</v>
       </c>
       <c r="F102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="G102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="H102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="I102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="J102" s="1" t="str">
@@ -16061,19 +16077,19 @@
         <v>44</v>
       </c>
       <c r="F103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="G103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="H103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="I103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="J103" s="1" t="str">
@@ -16110,19 +16126,19 @@
         <v>40</v>
       </c>
       <c r="F104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="G104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="H104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="I104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="J104" s="1" t="str">
@@ -16159,19 +16175,19 @@
         <v>36</v>
       </c>
       <c r="F105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="G105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="H105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="I105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="J105" s="1" t="str">
@@ -16211,19 +16227,19 @@
         <v>32</v>
       </c>
       <c r="F106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="G106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="H106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="I106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="J106" s="1" t="str">
@@ -16263,19 +16279,19 @@
         <v>28</v>
       </c>
       <c r="F107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J107" s="1" t="str">
@@ -16315,19 +16331,19 @@
         <v>24</v>
       </c>
       <c r="F108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J108" s="1" t="str">
@@ -16367,19 +16383,19 @@
         <v>20</v>
       </c>
       <c r="F109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="G109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="H109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="I109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="J109" s="1" t="str">
@@ -16416,19 +16432,19 @@
         <v>16</v>
       </c>
       <c r="F110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="G110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="H110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="I110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="J110" s="1" t="str">
@@ -16468,19 +16484,19 @@
         <v>12</v>
       </c>
       <c r="F111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="G111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="H111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="I111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="J111" s="1" t="str">
@@ -16517,19 +16533,19 @@
         <v>8</v>
       </c>
       <c r="F112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="G112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="H112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="I112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="J112" s="1" t="str">
@@ -16569,19 +16585,19 @@
         <v>4</v>
       </c>
       <c r="F113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J113" s="1" t="str">
@@ -16621,19 +16637,19 @@
         <v>0</v>
       </c>
       <c r="F114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="G114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="H114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="I114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="J114" s="1" t="str">
@@ -16673,19 +16689,19 @@
         <v>1853</v>
       </c>
       <c r="F115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Polycaprolactam Pellets)</v>
       </c>
       <c r="G115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Polycaprolactam Pellets)</v>
       </c>
       <c r="H115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Polycaprolactam Pellets)</v>
       </c>
       <c r="I115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Polycaprolactam Pellets)</v>
       </c>
       <c r="J115" s="1" t="str">
@@ -16725,19 +16741,19 @@
         <v>2412</v>
       </c>
       <c r="F116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="G116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="H116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="I116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="J116" s="1" t="str">
@@ -16777,19 +16793,19 @@
         <v>2416</v>
       </c>
       <c r="F117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="G117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="H117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="I117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="J117" s="1" t="str">
@@ -16829,19 +16845,19 @@
         <v>2420</v>
       </c>
       <c r="F118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Negative Photoresist)</v>
       </c>
       <c r="G118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Negative Photoresist)</v>
       </c>
       <c r="H118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Negative Photoresist)</v>
       </c>
       <c r="I118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Negative Photoresist)</v>
       </c>
       <c r="J118" s="1" t="str">
@@ -16881,19 +16897,19 @@
         <v>2424</v>
       </c>
       <c r="F119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$32, [1]Enums!$A$33)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$33, [1]Enums!$A$34)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Positive Photoresist)</v>
       </c>
       <c r="G119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Positive Photoresist)</v>
       </c>
       <c r="H119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Positive Photoresist)</v>
       </c>
       <c r="I119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Positive Photoresist)</v>
       </c>
       <c r="J119" s="1" t="str">
@@ -17808,11 +17824,11 @@
         <v>2651</v>
       </c>
       <c r="C1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="D1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$81</f>
+        <f xml:space="preserve"> [1]Enums!$B$82</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="19" t="str">
@@ -17848,7 +17864,7 @@
         <v>Mask (Solar Cell)[PR Backplane]</v>
       </c>
       <c r="D2" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E2" s="15" t="str">
@@ -17872,7 +17888,7 @@
         <v>Mask (Solar Cell)[PR Semiconductor]</v>
       </c>
       <c r="D3" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E3" s="15" t="str">
@@ -17896,7 +17912,7 @@
         <v>Mask (Solar Cell)[PR Dielectric]</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E4" s="15" t="str">
@@ -17920,7 +17936,7 @@
         <v>Mask (Solar Cell)[PR Traces]</v>
       </c>
       <c r="D5" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E5" s="15" t="str">
@@ -17944,7 +17960,7 @@
         <v>Mask (Solar Cell)[PR Encapsulation]</v>
       </c>
       <c r="D6" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E6" s="15" t="str">
@@ -17968,7 +17984,7 @@
         <v>Mask (Processor)[PR Backplane]</v>
       </c>
       <c r="D7" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E7" s="15" t="str">
@@ -17992,7 +18008,7 @@
         <v>Mask (Processor)[PR n-Type Semiconductor]</v>
       </c>
       <c r="D8" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E8" s="15" t="str">
@@ -18016,7 +18032,7 @@
         <v>Mask (Processor)[PR p-Type Semiconductor]</v>
       </c>
       <c r="D9" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E9" s="15" t="str">
@@ -18040,7 +18056,7 @@
         <v>Mask (Processor)[PR Dielectric]</v>
       </c>
       <c r="D10" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E10" s="15" t="str">
@@ -18064,7 +18080,7 @@
         <v>Mask (Processor)[PR Inner Traces]</v>
       </c>
       <c r="D11" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E11" s="15" t="str">
@@ -18088,7 +18104,7 @@
         <v>Mask (Processor)[PR Through Vias]</v>
       </c>
       <c r="D12" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E12" s="15" t="str">
@@ -18112,7 +18128,7 @@
         <v>Mask (Processor)[PR Outer Traces]</v>
       </c>
       <c r="D13" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E13" s="15" t="str">
@@ -18136,7 +18152,7 @@
         <v>Mask (Processor)[PR Encapsulation]</v>
       </c>
       <c r="D14" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E14" s="15" t="str">
@@ -18160,7 +18176,7 @@
         <v>Mask (Temperature Sensor)[PR Backplane]</v>
       </c>
       <c r="D15" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E15" s="15" t="str">
@@ -18184,7 +18200,7 @@
         <v>Mask (Temperature Sensor)[PR Semiconductor]</v>
       </c>
       <c r="D16" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E16" s="15" t="str">
@@ -18208,7 +18224,7 @@
         <v>Mask (Temperature Sensor)[PR Dielectric]</v>
       </c>
       <c r="D17" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E17" s="15" t="str">
@@ -18232,7 +18248,7 @@
         <v>Mask (Temperature Sensor)[PR Traces]</v>
       </c>
       <c r="D18" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E18" s="15" t="str">
@@ -18256,7 +18272,7 @@
         <v>Mask (Temperature Sensor)[PR Encapsulation]</v>
       </c>
       <c r="D19" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E19" s="15" t="str">
@@ -18280,7 +18296,7 @@
         <v>Mask (Pressure Sensor)[PR Backplane]</v>
       </c>
       <c r="D20" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E20" s="15" t="str">
@@ -18304,7 +18320,7 @@
         <v>Mask (Pressure Sensor)[PR Semiconductor]</v>
       </c>
       <c r="D21" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E21" s="15" t="str">
@@ -18328,7 +18344,7 @@
         <v>Mask (Pressure Sensor)[PR Dielectric]</v>
       </c>
       <c r="D22" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E22" s="15" t="str">
@@ -18352,7 +18368,7 @@
         <v>Mask (Pressure Sensor)[PR Traces]</v>
       </c>
       <c r="D23" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E23" s="15" t="str">
@@ -18376,7 +18392,7 @@
         <v>Mask (Pressure Sensor)[PR Encapsulation]</v>
       </c>
       <c r="D24" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E24" s="15" t="str">
@@ -18400,7 +18416,7 @@
         <v>Mask (Low Power Radio)[PR Backplane]</v>
       </c>
       <c r="D25" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E25" s="15" t="str">
@@ -18424,7 +18440,7 @@
         <v>Mask (Low Power Radio)[PR n-Type Semiconductor]</v>
       </c>
       <c r="D26" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E26" s="15" t="str">
@@ -18448,7 +18464,7 @@
         <v>Mask (Low Power Radio)[PR p-Type Semiconductor]</v>
       </c>
       <c r="D27" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E27" s="15" t="str">
@@ -18472,7 +18488,7 @@
         <v>Mask (Low Power Radio)[PR Dielectric]</v>
       </c>
       <c r="D28" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E28" s="15" t="str">
@@ -18496,7 +18512,7 @@
         <v>Mask (Low Power Radio)[PR Inner Traces]</v>
       </c>
       <c r="D29" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E29" s="15" t="str">
@@ -18520,7 +18536,7 @@
         <v>Mask (Low Power Radio)[PR Through Vias]</v>
       </c>
       <c r="D30" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E30" s="15" t="str">
@@ -18544,7 +18560,7 @@
         <v>Mask (Low Power Radio)[PR Outer Traces]</v>
       </c>
       <c r="D31" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E31" s="15" t="str">
@@ -18568,7 +18584,7 @@
         <v>Mask (Low Power Radio)[PR Encapsulation]</v>
       </c>
       <c r="D32" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E32" s="15" t="str">
@@ -18592,7 +18608,7 @@
         <v>Mask (DSP)[PR Backplane]</v>
       </c>
       <c r="D33" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E33" s="15" t="str">
@@ -18616,7 +18632,7 @@
         <v>Mask (DSP)[PR n-Type Semiconductor]</v>
       </c>
       <c r="D34" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E34" s="15" t="str">
@@ -18640,7 +18656,7 @@
         <v>Mask (DSP)[PR p-Type Semiconductor]</v>
       </c>
       <c r="D35" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E35" s="15" t="str">
@@ -18664,7 +18680,7 @@
         <v>Mask (DSP)[PR Dielectric]</v>
       </c>
       <c r="D36" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E36" s="15" t="str">
@@ -18688,7 +18704,7 @@
         <v>Mask (DSP)[PR Inner Traces]</v>
       </c>
       <c r="D37" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E37" s="15" t="str">
@@ -18712,7 +18728,7 @@
         <v>Mask (DSP)[PR Through Vias]</v>
       </c>
       <c r="D38" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E38" s="15" t="str">
@@ -18736,7 +18752,7 @@
         <v>Mask (DSP)[PR Outer Traces]</v>
       </c>
       <c r="D39" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E39" s="15" t="str">
@@ -18760,7 +18776,7 @@
         <v>Mask (DSP)[PR Encapsulation]</v>
       </c>
       <c r="D40" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E40" s="15" t="str">
@@ -18784,7 +18800,7 @@
         <v>Mask (Digital Analog Convertor)[PR Backplane]</v>
       </c>
       <c r="D41" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E41" s="15" t="str">
@@ -18808,7 +18824,7 @@
         <v>Mask (Digital Analog Convertor)[PR Semiconductor]</v>
       </c>
       <c r="D42" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E42" s="15" t="str">
@@ -18832,7 +18848,7 @@
         <v>Mask (Digital Analog Convertor)[PR Dielectric]</v>
       </c>
       <c r="D43" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E43" s="15" t="str">
@@ -18856,7 +18872,7 @@
         <v>Mask (Digital Analog Convertor)[PR Traces]</v>
       </c>
       <c r="D44" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E44" s="15" t="str">
@@ -18880,7 +18896,7 @@
         <v>Mask (Digital Analog Convertor)[PR Encapsulation]</v>
       </c>
       <c r="D45" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E45" s="15" t="str">
@@ -18904,7 +18920,7 @@
         <v>Mask (Amplifier)[PR Backplane]</v>
       </c>
       <c r="D46" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E46" s="15" t="str">
@@ -18928,7 +18944,7 @@
         <v>Mask (Amplifier)[PR Semiconductor]</v>
       </c>
       <c r="D47" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E47" s="15" t="str">
@@ -18952,7 +18968,7 @@
         <v>Mask (Amplifier)[PR Dielectric]</v>
       </c>
       <c r="D48" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E48" s="15" t="str">
@@ -18976,7 +18992,7 @@
         <v>Mask (Amplifier)[PR Traces]</v>
       </c>
       <c r="D49" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E49" s="15" t="str">
@@ -19000,7 +19016,7 @@
         <v>Mask (Amplifier)[PR Encapsulation]</v>
       </c>
       <c r="D50" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E50" s="15" t="str">
@@ -19024,7 +19040,7 @@
         <v>Mask (OLED Array)[PR Backplane]</v>
       </c>
       <c r="D51" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E51" s="15" t="str">
@@ -19048,7 +19064,7 @@
         <v>Mask (OLED Array)[PR Semiconductor]</v>
       </c>
       <c r="D52" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E52" s="15" t="str">
@@ -19072,7 +19088,7 @@
         <v>Mask (OLED Array)[PR Dielectric]</v>
       </c>
       <c r="D53" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E53" s="15" t="str">
@@ -19096,7 +19112,7 @@
         <v>Mask (OLED Array)[PR Traces]</v>
       </c>
       <c r="D54" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E54" s="15" t="str">
@@ -19120,7 +19136,7 @@
         <v>Mask (OLED Array)[PR Encapsulation]</v>
       </c>
       <c r="D55" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$94</f>
+        <f xml:space="preserve"> [1]Enums!$B$95</f>
         <v>Mask</v>
       </c>
       <c r="E55" s="15" t="str">
@@ -25370,7 +25386,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I2" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$148&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Steel</v>
       </c>
       <c r="J2" s="45">
@@ -25418,7 +25434,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I3" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$148&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Stainless Steel</v>
       </c>
       <c r="J3" s="45">
@@ -25466,7 +25482,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I4" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$148&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Brass</v>
       </c>
       <c r="J4" s="45">
@@ -25514,7 +25530,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I5" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$148&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Bronze</v>
       </c>
       <c r="J5" s="45">
@@ -25562,7 +25578,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I6" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$148&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Tungsten Carbide</v>
       </c>
       <c r="J6" s="45">
@@ -25610,7 +25626,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I7" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$148&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Nichrome</v>
       </c>
       <c r="J7" s="45">
@@ -25658,7 +25674,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I8" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$148&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Antimony-Lead</v>
       </c>
       <c r="J8" s="45">
@@ -25706,7 +25722,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I9" s="45" t="str">
-        <f>[1]Enums!$A$148&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$149&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Steel</v>
       </c>
       <c r="J9" s="45">
@@ -25754,7 +25770,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I10" s="45" t="str">
-        <f>[1]Enums!$A$148&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$149&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Stainless Steel</v>
       </c>
       <c r="J10" s="45">
@@ -25802,7 +25818,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I11" s="45" t="str">
-        <f>[1]Enums!$A$148&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$149&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Brass</v>
       </c>
       <c r="J11" s="45">
@@ -25850,7 +25866,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I12" s="45" t="str">
-        <f>[1]Enums!$A$148&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$149&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Bronze</v>
       </c>
       <c r="J12" s="45">
@@ -25898,7 +25914,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I13" s="45" t="str">
-        <f>[1]Enums!$A$148&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$149&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Tungsten Carbide</v>
       </c>
       <c r="J13" s="45">
@@ -25946,7 +25962,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I14" s="45" t="str">
-        <f>[1]Enums!$A$148&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$149&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Nichrome</v>
       </c>
       <c r="J14" s="45">
@@ -25994,7 +26010,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I15" s="45" t="str">
-        <f>[1]Enums!$A$148&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$149&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Antimony-Lead</v>
       </c>
       <c r="J15" s="45">
@@ -26042,7 +26058,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I16" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" Iron"</f>
+        <f>[1]Enums!$A$148&amp;" Iron"</f>
         <v>Composite Iron</v>
       </c>
       <c r="J16" s="45">
@@ -26090,7 +26106,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I17" s="45" t="str">
-        <f>[1]Enums!$A$148&amp;" Iron"</f>
+        <f>[1]Enums!$A$149&amp;" Iron"</f>
         <v>Engineered Iron</v>
       </c>
       <c r="J17" s="45">
@@ -26138,7 +26154,7 @@
         <v>Diamond</v>
       </c>
       <c r="I18" s="45" t="str">
-        <f>[1]Enums!$A$147&amp;" Diamond"</f>
+        <f>[1]Enums!$A$148&amp;" Diamond"</f>
         <v>Composite Diamond</v>
       </c>
       <c r="J18" s="45">
@@ -26186,7 +26202,7 @@
         <v>Diamond</v>
       </c>
       <c r="I19" s="45" t="str">
-        <f>[1]Enums!$A$148&amp;" Diamond"</f>
+        <f>[1]Enums!$A$149&amp;" Diamond"</f>
         <v>Engineered Diamond</v>
       </c>
       <c r="J19" s="45">
@@ -26487,7 +26503,7 @@
         <v>Molded Item</v>
       </c>
       <c r="F1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$112</f>
+        <f xml:space="preserve"> [1]Enums!$A$113</f>
         <v>Base Material</v>
       </c>
       <c r="G1" s="30" t="s">
@@ -26515,7 +26531,7 @@
         <v>1812</v>
       </c>
       <c r="C2" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D2</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D2</f>
         <v>Gripped Iron Shovel</v>
       </c>
       <c r="D2" s="24" t="str">
@@ -26527,7 +26543,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F2" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Iron</v>
       </c>
       <c r="G2" s="24">
@@ -26552,7 +26568,7 @@
         <v>1811</v>
       </c>
       <c r="C3" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D3</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D3</f>
         <v>Gripped Iron Pickaxe</v>
       </c>
       <c r="D3" s="21" t="str">
@@ -26564,7 +26580,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F3" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Iron</v>
       </c>
       <c r="G3" s="24">
@@ -26589,7 +26605,7 @@
         <v>1810</v>
       </c>
       <c r="C4" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D4</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D4</f>
         <v>Gripped Iron Axe</v>
       </c>
       <c r="D4" s="21" t="str">
@@ -26601,7 +26617,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F4" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Iron</v>
       </c>
       <c r="G4" s="24">
@@ -26626,7 +26642,7 @@
         <v>1809</v>
       </c>
       <c r="C5" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D5</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D5</f>
         <v>Gripped Iron Sword</v>
       </c>
       <c r="D5" s="21" t="str">
@@ -26638,7 +26654,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F5" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Iron</v>
       </c>
       <c r="G5" s="24">
@@ -26663,7 +26679,7 @@
         <v>1808</v>
       </c>
       <c r="C6" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D6</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D6</f>
         <v>Gripped Wooden Sword</v>
       </c>
       <c r="D6" s="21" t="str">
@@ -26675,7 +26691,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F6" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$114</f>
         <v>Wooden</v>
       </c>
       <c r="G6" s="24">
@@ -26700,7 +26716,7 @@
         <v>1807</v>
       </c>
       <c r="C7" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D7</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D7</f>
         <v>Gripped Wooden Shovel</v>
       </c>
       <c r="D7" s="21" t="str">
@@ -26712,7 +26728,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F7" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$114</f>
         <v>Wooden</v>
       </c>
       <c r="G7" s="24">
@@ -26737,7 +26753,7 @@
         <v>1806</v>
       </c>
       <c r="C8" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D8</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D8</f>
         <v>Gripped Wooden Pickaxe</v>
       </c>
       <c r="D8" s="21" t="str">
@@ -26749,7 +26765,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F8" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$114</f>
         <v>Wooden</v>
       </c>
       <c r="G8" s="24">
@@ -26774,7 +26790,7 @@
         <v>1805</v>
       </c>
       <c r="C9" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D9</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D9</f>
         <v>Gripped Wooden Axe</v>
       </c>
       <c r="D9" s="21" t="str">
@@ -26786,7 +26802,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F9" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$114</f>
         <v>Wooden</v>
       </c>
       <c r="G9" s="24">
@@ -26811,7 +26827,7 @@
         <v>1804</v>
       </c>
       <c r="C10" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D10</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D10</f>
         <v>Gripped Stone Sword</v>
       </c>
       <c r="D10" s="21" t="str">
@@ -26823,7 +26839,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F10" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$115</f>
         <v>Stone</v>
       </c>
       <c r="G10" s="24">
@@ -26848,7 +26864,7 @@
         <v>1803</v>
       </c>
       <c r="C11" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D11</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D11</f>
         <v>Gripped Stone Shovel</v>
       </c>
       <c r="D11" s="21" t="str">
@@ -26860,7 +26876,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F11" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$115</f>
         <v>Stone</v>
       </c>
       <c r="G11" s="24">
@@ -26885,7 +26901,7 @@
         <v>1802</v>
       </c>
       <c r="C12" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D12</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D12</f>
         <v>Gripped Stone Pickaxe</v>
       </c>
       <c r="D12" s="21" t="str">
@@ -26897,7 +26913,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F12" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$115</f>
         <v>Stone</v>
       </c>
       <c r="G12" s="24">
@@ -26922,7 +26938,7 @@
         <v>1801</v>
       </c>
       <c r="C13" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D13</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D13</f>
         <v>Gripped Stone Axe</v>
       </c>
       <c r="D13" s="21" t="str">
@@ -26934,7 +26950,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F13" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$115</f>
         <v>Stone</v>
       </c>
       <c r="G13" s="24">
@@ -26959,7 +26975,7 @@
         <v>1800</v>
       </c>
       <c r="C14" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D14</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D14</f>
         <v>Gripped Diamond Sword</v>
       </c>
       <c r="D14" s="21" t="str">
@@ -26971,7 +26987,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F14" s="34" t="str">
-        <f>[1]Enums!$A$117</f>
+        <f>[1]Enums!$A$118</f>
         <v>Diamond</v>
       </c>
       <c r="G14" s="24">
@@ -26996,7 +27012,7 @@
         <v>1799</v>
       </c>
       <c r="C15" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D15</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D15</f>
         <v>Gripped Diamond Shovel</v>
       </c>
       <c r="D15" s="21" t="str">
@@ -27008,7 +27024,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F15" s="34" t="str">
-        <f>[1]Enums!$A$117</f>
+        <f>[1]Enums!$A$118</f>
         <v>Diamond</v>
       </c>
       <c r="G15" s="24">
@@ -27033,7 +27049,7 @@
         <v>1798</v>
       </c>
       <c r="C16" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D16</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D16</f>
         <v>Gripped Diamond Pickaxe</v>
       </c>
       <c r="D16" s="21" t="str">
@@ -27045,7 +27061,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F16" s="34" t="str">
-        <f>[1]Enums!$A$117</f>
+        <f>[1]Enums!$A$118</f>
         <v>Diamond</v>
       </c>
       <c r="G16" s="24">
@@ -27070,7 +27086,7 @@
         <v>1797</v>
       </c>
       <c r="C17" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D17</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D17</f>
         <v>Gripped Diamond Axe</v>
       </c>
       <c r="D17" s="21" t="str">
@@ -27082,7 +27098,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F17" s="34" t="str">
-        <f>[1]Enums!$A$117</f>
+        <f>[1]Enums!$A$118</f>
         <v>Diamond</v>
       </c>
       <c r="G17" s="24">
@@ -27107,7 +27123,7 @@
         <v>1796</v>
       </c>
       <c r="C18" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D18</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D18</f>
         <v>Gripped Golden Sword</v>
       </c>
       <c r="D18" s="21" t="str">
@@ -27119,7 +27135,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F18" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$117</f>
         <v>Golden</v>
       </c>
       <c r="G18" s="24">
@@ -27144,7 +27160,7 @@
         <v>1795</v>
       </c>
       <c r="C19" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D19</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D19</f>
         <v>Gripped Golden Shovel</v>
       </c>
       <c r="D19" s="21" t="str">
@@ -27156,7 +27172,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F19" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$117</f>
         <v>Golden</v>
       </c>
       <c r="G19" s="24">
@@ -27181,7 +27197,7 @@
         <v>1794</v>
       </c>
       <c r="C20" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D20</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D20</f>
         <v>Gripped Golden Pickaxe</v>
       </c>
       <c r="D20" s="21" t="str">
@@ -27193,7 +27209,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F20" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$117</f>
         <v>Golden</v>
       </c>
       <c r="G20" s="24">
@@ -27218,7 +27234,7 @@
         <v>1793</v>
       </c>
       <c r="C21" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D21</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D21</f>
         <v>Gripped Golden Axe</v>
       </c>
       <c r="D21" s="21" t="str">
@@ -27230,7 +27246,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F21" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$117</f>
         <v>Golden</v>
       </c>
       <c r="G21" s="24">
@@ -27255,7 +27271,7 @@
         <v>1792</v>
       </c>
       <c r="C22" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D22</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D22</f>
         <v>Gripped Wooden Hoe</v>
       </c>
       <c r="D22" s="21" t="str">
@@ -27267,7 +27283,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F22" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$114</f>
         <v>Wooden</v>
       </c>
       <c r="G22" s="24">
@@ -27292,7 +27308,7 @@
         <v>1791</v>
       </c>
       <c r="C23" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D23</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D23</f>
         <v>Gripped Stone Hoe</v>
       </c>
       <c r="D23" s="21" t="str">
@@ -27304,7 +27320,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F23" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$115</f>
         <v>Stone</v>
       </c>
       <c r="G23" s="24">
@@ -27329,7 +27345,7 @@
         <v>1790</v>
       </c>
       <c r="C24" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D24</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D24</f>
         <v>Gripped Iron Hoe</v>
       </c>
       <c r="D24" s="21" t="str">
@@ -27341,7 +27357,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F24" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Iron</v>
       </c>
       <c r="G24" s="24">
@@ -27366,7 +27382,7 @@
         <v>1789</v>
       </c>
       <c r="C25" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D25</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D25</f>
         <v>Gripped Diamond Hoe</v>
       </c>
       <c r="D25" s="21" t="str">
@@ -27378,7 +27394,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F25" s="34" t="str">
-        <f>[1]Enums!$A$117</f>
+        <f>[1]Enums!$A$118</f>
         <v>Diamond</v>
       </c>
       <c r="G25" s="24">
@@ -27403,7 +27419,7 @@
         <v>1788</v>
       </c>
       <c r="C26" s="22" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;D26</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;D26</f>
         <v>Gripped Golden Hoe</v>
       </c>
       <c r="D26" s="21" t="str">
@@ -27415,7 +27431,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F26" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$117</f>
         <v>Golden</v>
       </c>
       <c r="G26" s="24">
@@ -27477,7 +27493,7 @@
         <v>1832</v>
       </c>
       <c r="D1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$112</f>
+        <f xml:space="preserve"> [1]Enums!$A$113</f>
         <v>Base Material</v>
       </c>
       <c r="E1" s="36" t="s">
@@ -27523,7 +27539,7 @@
         <v>Wooden Pogo Stick</v>
       </c>
       <c r="D2" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$114</f>
         <v>Wooden</v>
       </c>
       <c r="E2" s="37">
@@ -27560,7 +27576,7 @@
         <v>Stone Pogo Stick</v>
       </c>
       <c r="D3" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$115</f>
         <v>Stone</v>
       </c>
       <c r="E3" s="37">
@@ -27596,7 +27612,7 @@
         <v>Iron Pogo Stick</v>
       </c>
       <c r="D4" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Iron</v>
       </c>
       <c r="E4" s="37">
@@ -27632,7 +27648,7 @@
         <v>Golden Pogo Stick</v>
       </c>
       <c r="D5" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$117</f>
         <v>Golden</v>
       </c>
       <c r="E5" s="37">
@@ -27668,7 +27684,7 @@
         <v>Diamond Pogo Stick</v>
       </c>
       <c r="D6" s="34" t="str">
-        <f>[1]Enums!$A$117</f>
+        <f>[1]Enums!$A$118</f>
         <v>Diamond</v>
       </c>
       <c r="E6" s="37">
@@ -27704,7 +27720,7 @@
         <v>Magic Pogo Stick</v>
       </c>
       <c r="D7" s="34" t="str">
-        <f>[1]Enums!$A$118</f>
+        <f>[1]Enums!$A$119</f>
         <v>Magic</v>
       </c>
       <c r="E7" s="37">
@@ -27736,11 +27752,11 @@
         <v>1821</v>
       </c>
       <c r="C8" s="34" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;I8</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;I8</f>
         <v>Gripped Wooden Pogo Stick</v>
       </c>
       <c r="D8" s="34" t="str">
-        <f>[1]Enums!$A$113</f>
+        <f>[1]Enums!$A$114</f>
         <v>Wooden</v>
       </c>
       <c r="E8" s="37">
@@ -27780,11 +27796,11 @@
         <v>1820</v>
       </c>
       <c r="C9" s="34" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;I9</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;I9</f>
         <v>Gripped Stone Pogo Stick</v>
       </c>
       <c r="D9" s="34" t="str">
-        <f>[1]Enums!$A$114</f>
+        <f>[1]Enums!$A$115</f>
         <v>Stone</v>
       </c>
       <c r="E9" s="37">
@@ -27824,11 +27840,11 @@
         <v>1819</v>
       </c>
       <c r="C10" s="34" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;I10</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;I10</f>
         <v>Gripped Iron Pogo Stick</v>
       </c>
       <c r="D10" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Iron</v>
       </c>
       <c r="E10" s="37">
@@ -27868,11 +27884,11 @@
         <v>1818</v>
       </c>
       <c r="C11" s="34" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;I11</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;I11</f>
         <v>Gripped Golden Pogo Stick</v>
       </c>
       <c r="D11" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$117</f>
         <v>Golden</v>
       </c>
       <c r="E11" s="37">
@@ -27912,11 +27928,11 @@
         <v>1817</v>
       </c>
       <c r="C12" s="34" t="str">
-        <f>[1]Enums!$A$109&amp;" "&amp;I12</f>
+        <f>[1]Enums!$A$110&amp;" "&amp;I12</f>
         <v>Gripped Diamond Pogo Stick</v>
       </c>
       <c r="D12" s="34" t="str">
-        <f>[1]Enums!$A$117</f>
+        <f>[1]Enums!$A$118</f>
         <v>Diamond</v>
       </c>
       <c r="E12" s="37">
@@ -29596,8 +29612,8 @@
   </sheetPr>
   <dimension ref="A1:G333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="G127" sqref="G127"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -46307,17 +46323,17 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="28.7109375" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -46334,7 +46350,7 @@
         <v>590</v>
       </c>
       <c r="D1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$81</f>
+        <f xml:space="preserve"> [1]Enums!$B$82</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="19" t="str">
@@ -46354,11 +46370,11 @@
         <v>1756</v>
       </c>
       <c r="C2" s="10" t="str">
-        <f t="shared" ref="C2:C33" si="0">D2&amp;" ("&amp;E2&amp;")"</f>
+        <f t="shared" ref="C2:C34" si="0">D2&amp;" ("&amp;E2&amp;")"</f>
         <v>Mold (Grip)</v>
       </c>
       <c r="D2" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E2" s="11" t="str">
@@ -46383,7 +46399,7 @@
         <v>Mold (Running Shoes)</v>
       </c>
       <c r="D3" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E3" s="11" t="str">
@@ -46408,7 +46424,7 @@
         <v>Mold (Scuba Fins)</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E4" s="11" t="str">
@@ -46433,7 +46449,7 @@
         <v>Mold (Scuba Mask)</v>
       </c>
       <c r="D5" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E5" s="11" t="str">
@@ -46458,7 +46474,7 @@
         <v>Mold (Gasket)</v>
       </c>
       <c r="D6" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E6" s="11" t="str">
@@ -46483,7 +46499,7 @@
         <v>Mold (Life Preserver)</v>
       </c>
       <c r="D7" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E7" s="11" t="str">
@@ -46508,7 +46524,7 @@
         <v>Metal Die (Fibers)</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$86</f>
+        <f xml:space="preserve"> [1]Enums!$B$87</f>
         <v>Metal Die</v>
       </c>
       <c r="E8" s="11" t="str">
@@ -46533,7 +46549,7 @@
         <v>Metal Die (Tether)</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$86</f>
+        <f xml:space="preserve"> [1]Enums!$B$87</f>
         <v>Metal Die</v>
       </c>
       <c r="E9" s="11" t="str">
@@ -46558,7 +46574,7 @@
         <v>Metal Die (Cord)</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$86</f>
+        <f xml:space="preserve"> [1]Enums!$B$87</f>
         <v>Metal Die</v>
       </c>
       <c r="E10" s="11" t="str">
@@ -46583,7 +46599,7 @@
         <v>Metal Die (Hose)</v>
       </c>
       <c r="D11" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$86</f>
+        <f xml:space="preserve"> [1]Enums!$B$87</f>
         <v>Metal Die</v>
       </c>
       <c r="E11" s="11" t="str">
@@ -46608,7 +46624,7 @@
         <v>Metal Die (Pipe Segment)</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$86</f>
+        <f xml:space="preserve"> [1]Enums!$B$87</f>
         <v>Metal Die</v>
       </c>
       <c r="E12" s="11" t="str">
@@ -46633,7 +46649,7 @@
         <v>Mold (Flashlight Shaft)</v>
       </c>
       <c r="D13" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E13" s="11" t="str">
@@ -46657,7 +46673,7 @@
         <v>Mold (Plastic Brick (1 x 1))</v>
       </c>
       <c r="D14" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E14" t="str">
@@ -46681,7 +46697,7 @@
         <v>Mold (Plastic Brick (1 x 2))</v>
       </c>
       <c r="D15" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E15" t="str">
@@ -46705,7 +46721,7 @@
         <v>Mold (Plastic Brick (1 x 3))</v>
       </c>
       <c r="D16" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E16" t="str">
@@ -46729,7 +46745,7 @@
         <v>Mold (Plastic Brick (1 x 4))</v>
       </c>
       <c r="D17" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E17" t="str">
@@ -46753,7 +46769,7 @@
         <v>Mold (Plastic Brick (2 x 2))</v>
       </c>
       <c r="D18" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E18" t="str">
@@ -46777,7 +46793,7 @@
         <v>Mold (Plastic Brick (2 x 3))</v>
       </c>
       <c r="D19" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E19" t="str">
@@ -46801,7 +46817,7 @@
         <v>Mold (Plastic Brick (2 x 4))</v>
       </c>
       <c r="D20" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E20" t="str">
@@ -46825,7 +46841,7 @@
         <v>Mold (Plastic Brick (3 x 3))</v>
       </c>
       <c r="D21" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E21" t="str">
@@ -46849,7 +46865,7 @@
         <v>Mold (Plastic Brick (3 x 4))</v>
       </c>
       <c r="D22" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E22" t="str">
@@ -46873,7 +46889,7 @@
         <v>Mold (Plastic Brick (4 x 4))</v>
       </c>
       <c r="D23" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E23" t="str">
@@ -46897,7 +46913,7 @@
         <v>Mold (Plastic Brick (1 x 8))</v>
       </c>
       <c r="D24" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E24" t="str">
@@ -46921,7 +46937,7 @@
         <v>Mold (Plastic Brick (2 x 8))</v>
       </c>
       <c r="D25" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E25" t="str">
@@ -46945,7 +46961,7 @@
         <v>Mold (Heated Knife Handle)</v>
       </c>
       <c r="D26" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E26" s="11" t="str">
@@ -46969,7 +46985,7 @@
         <v>Mold (Rubber Sole)</v>
       </c>
       <c r="D27" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E27" s="11" t="str">
@@ -46993,7 +47009,7 @@
         <v>Mold (Battery Case)</v>
       </c>
       <c r="D28" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E28" s="11" t="str">
@@ -47017,7 +47033,7 @@
         <v>Mold (Tool Shaft)</v>
       </c>
       <c r="D29" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E29" t="str">
@@ -47041,7 +47057,7 @@
         <v>Mold (Lighter Body)</v>
       </c>
       <c r="D30" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E30" t="str">
@@ -47065,7 +47081,7 @@
         <v>Mold (Cell Phone Case)</v>
       </c>
       <c r="D31" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E31" t="str">
@@ -47089,7 +47105,7 @@
         <v>Mold (Walky Talky Case)</v>
       </c>
       <c r="D32" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E32" t="str">
@@ -47113,7 +47129,7 @@
         <v>Mold (HAM Radio Case)</v>
       </c>
       <c r="D33" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$85</f>
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
         <v>Mold</v>
       </c>
       <c r="E33" t="str">
@@ -47121,6 +47137,30 @@
         <v>HAM Radio Case</v>
       </c>
       <c r="F33">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="str">
+        <f>[1]Enums!$A$24</f>
+        <v>1.3.5</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>2709</v>
+      </c>
+      <c r="C34" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Mold (Air Quality Detector Case)</v>
+      </c>
+      <c r="D34" s="10" t="str">
+        <f xml:space="preserve"> [1]Enums!$B$86</f>
+        <v>Mold</v>
+      </c>
+      <c r="E34" t="str">
+        <f>'[1]Polymer Objects'!$B34</f>
+        <v>Air Quality Detector Case</v>
+      </c>
+      <c r="F34">
         <v>8192</v>
       </c>
     </row>
@@ -47136,15 +47176,15 @@
   </sheetPr>
   <dimension ref="A1:U156"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="E150" sqref="E150"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="J159" sqref="J159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="8.85546875" style="21"/>
     <col min="3" max="3" width="46.7109375" style="21" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" style="21" customWidth="1"/>
     <col min="5" max="5" width="37.85546875" style="21" customWidth="1"/>
     <col min="6" max="6" width="23.7109375" style="21" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" style="21" customWidth="1"/>
@@ -53450,8 +53490,41 @@
       </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A156" s="23"/>
-      <c r="C156" s="22"/>
+      <c r="A156" s="23" t="str">
+        <f>[1]Enums!$A$24</f>
+        <v>1.3.5</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C156" s="22" t="str">
+        <f xml:space="preserve"> VLOOKUP(D156, Molds!C:E, 3, FALSE)&amp;" ("&amp;F156&amp;")"</f>
+        <v>Air Quality Detector Case (PS)</v>
+      </c>
+      <c r="D156" s="24" t="str">
+        <f xml:space="preserve"> Molds!$C$34</f>
+        <v>Mold (Air Quality Detector Case)</v>
+      </c>
+      <c r="E156" s="21" t="str">
+        <f>Pellets!F87</f>
+        <v>Bag (PolyStyrene Pellets)</v>
+      </c>
+      <c r="F156" s="21" t="str">
+        <f>VLOOKUP(E156, Pellets!F:M, 8,FALSE)</f>
+        <v>PS</v>
+      </c>
+      <c r="G156" s="21">
+        <v>16</v>
+      </c>
+      <c r="H156" s="21">
+        <v>10</v>
+      </c>
+      <c r="I156" s="21">
+        <v>64</v>
+      </c>
+      <c r="J156" s="21" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -53494,7 +53567,7 @@
         <v>2518</v>
       </c>
       <c r="D1" s="53" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$81</f>
+        <f xml:space="preserve"> [1]Enums!$B$82</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="20" t="s">
@@ -53528,7 +53601,7 @@
         <v>Wafer (Solar Cell)</v>
       </c>
       <c r="D2" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$94</f>
         <v>Wafer</v>
       </c>
       <c r="E2" s="49" t="s">
@@ -53555,7 +53628,7 @@
         <v>Wafer (Processor)</v>
       </c>
       <c r="D3" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$94</f>
         <v>Wafer</v>
       </c>
       <c r="E3" s="49" t="s">
@@ -53582,7 +53655,7 @@
         <v>Wafer (Temperature Sensor)</v>
       </c>
       <c r="D4" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$94</f>
         <v>Wafer</v>
       </c>
       <c r="E4" s="49" t="s">
@@ -53609,7 +53682,7 @@
         <v>Wafer (Pressure Sensor)</v>
       </c>
       <c r="D5" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$94</f>
         <v>Wafer</v>
       </c>
       <c r="E5" s="49" t="s">
@@ -53636,7 +53709,7 @@
         <v>Wafer (Low Power Radio)</v>
       </c>
       <c r="D6" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$94</f>
         <v>Wafer</v>
       </c>
       <c r="E6" s="49" t="s">
@@ -53663,7 +53736,7 @@
         <v>Wafer (DSP)</v>
       </c>
       <c r="D7" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$94</f>
         <v>Wafer</v>
       </c>
       <c r="E7" s="49" t="s">
@@ -53690,7 +53763,7 @@
         <v>Wafer (Digital Analog Convertor)</v>
       </c>
       <c r="D8" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$94</f>
         <v>Wafer</v>
       </c>
       <c r="E8" s="49" t="s">
@@ -53717,7 +53790,7 @@
         <v>Wafer (Amplifier)</v>
       </c>
       <c r="D9" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$94</f>
         <v>Wafer</v>
       </c>
       <c r="E9" s="49" t="s">
@@ -53744,7 +53817,7 @@
         <v>Wafer (OLED Array)</v>
       </c>
       <c r="D10" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$93</f>
+        <f xml:space="preserve"> [1]Enums!$B$94</f>
         <v>Wafer</v>
       </c>
       <c r="E10" s="49" t="s">

</xml_diff>

<commit_message>
Updated to 1.3.7 - fixed lowercase player names and updated recipes and experience code.
</commit_message>
<xml_diff>
--- a/config/Polycraft Polymers.xlsx
+++ b/config/Polycraft Polymers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12090" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="826" activeTab="2"/>
+    <workbookView xWindow="13020" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="826" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pellets" sheetId="1" r:id="rId1"/>
@@ -8485,118 +8485,118 @@
             <v>1.3.5</v>
           </cell>
         </row>
-        <row r="34">
-          <cell r="A34" t="str">
+        <row r="35">
+          <cell r="A35" t="str">
             <v>Bag</v>
           </cell>
         </row>
-        <row r="35">
-          <cell r="A35" t="str">
+        <row r="36">
+          <cell r="A36" t="str">
             <v>Vial</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37" t="str">
-            <v>Sack</v>
           </cell>
         </row>
         <row r="38">
           <cell r="A38" t="str">
-            <v>Beaker</v>
+            <v>Sack</v>
           </cell>
         </row>
-        <row r="40">
-          <cell r="A40" t="str">
-            <v>Powder Keg</v>
+        <row r="39">
+          <cell r="A39" t="str">
+            <v>Beaker</v>
           </cell>
         </row>
         <row r="41">
           <cell r="A41" t="str">
-            <v>Drum</v>
+            <v>Powder Keg</v>
           </cell>
         </row>
-        <row r="43">
-          <cell r="A43" t="str">
-            <v>Chemical Silo</v>
+        <row r="42">
+          <cell r="A42" t="str">
+            <v>Drum</v>
           </cell>
         </row>
         <row r="44">
           <cell r="A44" t="str">
+            <v>Chemical Silo</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45" t="str">
             <v>Chemical Vat</v>
           </cell>
         </row>
-        <row r="83">
-          <cell r="B83" t="str">
+        <row r="84">
+          <cell r="B84" t="str">
             <v>Mold Type</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="B87" t="str">
-            <v>Mold</v>
           </cell>
         </row>
         <row r="88">
           <cell r="B88" t="str">
-            <v>Metal Die</v>
+            <v>Mold</v>
           </cell>
         </row>
-        <row r="95">
-          <cell r="B95" t="str">
-            <v>Wafer</v>
+        <row r="89">
+          <cell r="B89" t="str">
+            <v>Metal Die</v>
           </cell>
         </row>
         <row r="96">
           <cell r="B96" t="str">
+            <v>Wafer</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="B97" t="str">
             <v>Mask</v>
           </cell>
         </row>
-        <row r="111">
-          <cell r="A111" t="str">
+        <row r="112">
+          <cell r="A112" t="str">
             <v>Gripped</v>
-          </cell>
-        </row>
-        <row r="114">
-          <cell r="A114" t="str">
-            <v>Base Material</v>
           </cell>
         </row>
         <row r="115">
           <cell r="A115" t="str">
-            <v>Wooden</v>
+            <v>Base Material</v>
           </cell>
         </row>
         <row r="116">
           <cell r="A116" t="str">
-            <v>Stone</v>
+            <v>Wooden</v>
           </cell>
         </row>
         <row r="117">
           <cell r="A117" t="str">
-            <v>Iron</v>
+            <v>Stone</v>
           </cell>
         </row>
         <row r="118">
           <cell r="A118" t="str">
-            <v>Golden</v>
+            <v>Iron</v>
           </cell>
         </row>
         <row r="119">
           <cell r="A119" t="str">
-            <v>Diamond</v>
+            <v>Golden</v>
           </cell>
         </row>
         <row r="120">
           <cell r="A120" t="str">
-            <v>Magic</v>
+            <v>Diamond</v>
           </cell>
         </row>
-        <row r="149">
-          <cell r="A149" t="str">
-            <v>Composite</v>
+        <row r="121">
+          <cell r="A121" t="str">
+            <v>Magic</v>
           </cell>
         </row>
         <row r="150">
           <cell r="A150" t="str">
+            <v>Composite</v>
+          </cell>
+        </row>
+        <row r="151">
+          <cell r="A151" t="str">
             <v>Engineered</v>
           </cell>
         </row>
@@ -10867,19 +10867,19 @@
         <v>Game ID XL</v>
       </c>
       <c r="F1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$34&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$35&amp;" ("&amp;J1&amp;")"</f>
         <v>Bag (Pellets)</v>
       </c>
       <c r="G1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$37&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$38&amp;" ("&amp;J1&amp;")"</f>
         <v>Sack (Pellets)</v>
       </c>
       <c r="H1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$40&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$41&amp;" ("&amp;J1&amp;")"</f>
         <v>Powder Keg (Pellets)</v>
       </c>
       <c r="I1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$43&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$44&amp;" ("&amp;J1&amp;")"</f>
         <v>Chemical Silo (Pellets)</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -10918,19 +10918,19 @@
         <v>448</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="G2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="H2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="J2" s="1" t="str">
@@ -10970,19 +10970,19 @@
         <v>444</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J3" s="1" t="str">
@@ -11019,19 +11019,19 @@
         <v>440</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Alkyd Resin)</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Alkyd Resin)</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Alkyd Resin)</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Alkyd Resin)</v>
       </c>
       <c r="J4" s="1" t="str">
@@ -11071,19 +11071,19 @@
         <v>436</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J5" s="1" t="str">
@@ -11123,19 +11123,19 @@
         <v>432</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J6" s="1" t="str">
@@ -11175,19 +11175,19 @@
         <v>428</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$34, [1]Enums!$A$34)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$35, [1]Enums!$A$35)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Carbon Fiber)</v>
       </c>
       <c r="G7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$37, [1]Enums!$A$37)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$38, [1]Enums!$A$38)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Carbon Fiber)</v>
       </c>
       <c r="H7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$40, [1]Enums!$A$40)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$41, [1]Enums!$A$41)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Carbon Fiber)</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$43, [1]Enums!$A$43)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$44, [1]Enums!$A$44)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Carbon Fiber)</v>
       </c>
       <c r="J7" s="1" t="str">
@@ -11224,19 +11224,19 @@
         <v>424</v>
       </c>
       <c r="F8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="G8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="J8" s="1" t="str">
@@ -11276,19 +11276,19 @@
         <v>420</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulosic Pellets)</v>
       </c>
       <c r="G9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulosic Pellets)</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulosic Pellets)</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulosic Pellets)</v>
       </c>
       <c r="J9" s="1" t="str">
@@ -11328,19 +11328,19 @@
         <v>416</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chitin Pellets)</v>
       </c>
       <c r="G10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chitin Pellets)</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chitin Pellets)</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chitin Pellets)</v>
       </c>
       <c r="J10" s="1" t="str">
@@ -11380,19 +11380,19 @@
         <v>412</v>
       </c>
       <c r="F11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J11" s="1" t="str">
@@ -11432,19 +11432,19 @@
         <v>408</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Epoxy Resin)</v>
       </c>
       <c r="G12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Epoxy Resin)</v>
       </c>
       <c r="H12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Epoxy Resin)</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Epoxy Resin)</v>
       </c>
       <c r="J12" s="1" t="str">
@@ -11481,19 +11481,19 @@
         <v>404</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethoxylates Pellets)</v>
       </c>
       <c r="G13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethoxylates Pellets)</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethoxylates Pellets)</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethoxylates Pellets)</v>
       </c>
       <c r="J13" s="1" t="str">
@@ -11533,19 +11533,19 @@
         <v>400</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="G14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="H14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="J14" s="1" t="str">
@@ -11585,19 +11585,19 @@
         <v>396</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="G15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="J15" s="1" t="str">
@@ -11637,19 +11637,19 @@
         <v>392</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="G16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="J16" s="1" t="str">
@@ -11689,19 +11689,19 @@
         <v>388</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="G17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="J17" s="1" t="str">
@@ -11741,19 +11741,19 @@
         <v>384</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J18" s="1" t="str">
@@ -11793,19 +11793,19 @@
         <v>380</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J19" s="1" t="str">
@@ -11842,19 +11842,19 @@
         <v>376</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Lignin)</v>
       </c>
       <c r="G20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Lignin)</v>
       </c>
       <c r="H20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Lignin)</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Lignin)</v>
       </c>
       <c r="J20" s="1" t="str">
@@ -11894,19 +11894,19 @@
         <v>372</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J21" s="1" t="str">
@@ -11946,19 +11946,19 @@
         <v>368</v>
       </c>
       <c r="F22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="G22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="H22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="J22" s="1" t="str">
@@ -11998,19 +11998,19 @@
         <v>364</v>
       </c>
       <c r="F23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="G23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="H23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="J23" s="1" t="str">
@@ -12050,19 +12050,19 @@
         <v>360</v>
       </c>
       <c r="F24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="G24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="H24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="J24" s="1" t="str">
@@ -12099,19 +12099,19 @@
         <v>356</v>
       </c>
       <c r="F25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="G25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="H25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="J25" s="1" t="str">
@@ -12151,19 +12151,19 @@
         <v>352</v>
       </c>
       <c r="F26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Metaldehyde Pellets)</v>
       </c>
       <c r="G26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Metaldehyde Pellets)</v>
       </c>
       <c r="H26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Metaldehyde Pellets)</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Metaldehyde Pellets)</v>
       </c>
       <c r="J26" s="1" t="str">
@@ -12203,19 +12203,19 @@
         <v>348</v>
       </c>
       <c r="F27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J27" s="1" t="str">
@@ -12255,19 +12255,19 @@
         <v>344</v>
       </c>
       <c r="F28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraformaldehyde Pellets)</v>
       </c>
       <c r="G28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraformaldehyde Pellets)</v>
       </c>
       <c r="H28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraformaldehyde Pellets)</v>
       </c>
       <c r="I28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraformaldehyde Pellets)</v>
       </c>
       <c r="J28" s="1" t="str">
@@ -12307,19 +12307,19 @@
         <v>340</v>
       </c>
       <c r="F29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraldehyde Pellets)</v>
       </c>
       <c r="G29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraldehyde Pellets)</v>
       </c>
       <c r="H29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraldehyde Pellets)</v>
       </c>
       <c r="I29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraldehyde Pellets)</v>
       </c>
       <c r="J29" s="1" t="str">
@@ -12359,19 +12359,19 @@
         <v>336</v>
       </c>
       <c r="F30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Phenolic Resin)</v>
       </c>
       <c r="G30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Phenolic Resin)</v>
       </c>
       <c r="H30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Phenolic Resin)</v>
       </c>
       <c r="I30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Phenolic Resin)</v>
       </c>
       <c r="J30" s="1" t="str">
@@ -12411,19 +12411,19 @@
         <v>332</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="G31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="H31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="I31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="J31" s="1" t="str">
@@ -12463,19 +12463,19 @@
         <v>328</v>
       </c>
       <c r="F32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly1-Butene Pellets)</v>
       </c>
       <c r="G32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly1-Butene Pellets)</v>
       </c>
       <c r="H32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly1-Butene Pellets)</v>
       </c>
       <c r="I32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly1-Butene Pellets)</v>
       </c>
       <c r="J32" s="1" t="str">
@@ -12515,19 +12515,19 @@
         <v>324</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="G33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="H33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="I33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="J33" s="1" t="str">
@@ -12567,19 +12567,19 @@
         <v>320</v>
       </c>
       <c r="F34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="G34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="H34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="I34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="J34" s="1" t="str">
@@ -12619,19 +12619,19 @@
         <v>316</v>
       </c>
       <c r="F35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="G35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="H35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="I35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="J35" s="1" t="str">
@@ -12671,19 +12671,19 @@
         <v>312</v>
       </c>
       <c r="F36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="G36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="H36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="I36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="J36" s="1" t="str">
@@ -12723,19 +12723,19 @@
         <v>308</v>
       </c>
       <c r="F37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="G37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="H37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="I37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="J37" s="1" t="str">
@@ -12775,19 +12775,19 @@
         <v>304</v>
       </c>
       <c r="F38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="G38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="H38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="I38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="J38" s="1" t="str">
@@ -12827,19 +12827,19 @@
         <v>300</v>
       </c>
       <c r="F39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="G39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="H39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="I39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="J39" s="1" t="str">
@@ -12879,19 +12879,19 @@
         <v>296</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="G40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="H40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="I40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="J40" s="1" t="str">
@@ -12931,19 +12931,19 @@
         <v>292</v>
       </c>
       <c r="F41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="G41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="H41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="I41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="J41" s="1" t="str">
@@ -12983,19 +12983,19 @@
         <v>288</v>
       </c>
       <c r="F42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCaprolactone Pellets)</v>
       </c>
       <c r="G42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCaprolactone Pellets)</v>
       </c>
       <c r="H42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCaprolactone Pellets)</v>
       </c>
       <c r="I42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCaprolactone Pellets)</v>
       </c>
       <c r="J42" s="1" t="str">
@@ -13035,19 +13035,19 @@
         <v>284</v>
       </c>
       <c r="F43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCarbonate Pellets)</v>
       </c>
       <c r="G43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCarbonate Pellets)</v>
       </c>
       <c r="H43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCarbonate Pellets)</v>
       </c>
       <c r="I43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCarbonate Pellets)</v>
       </c>
       <c r="J43" s="1" t="str">
@@ -13087,19 +13087,19 @@
         <v>280</v>
       </c>
       <c r="F44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChloroPrene Pellets)</v>
       </c>
       <c r="G44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChloroPrene Pellets)</v>
       </c>
       <c r="H44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChloroPrene Pellets)</v>
       </c>
       <c r="I44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChloroPrene Pellets)</v>
       </c>
       <c r="J44" s="1" t="str">
@@ -13136,19 +13136,19 @@
         <v>276</v>
       </c>
       <c r="F45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="G45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="H45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="I45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="J45" s="1" t="str">
@@ -13188,19 +13188,19 @@
         <v>272</v>
       </c>
       <c r="F46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="G46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="H46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="I46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="J46" s="1" t="str">
@@ -13240,19 +13240,19 @@
         <v>268</v>
       </c>
       <c r="F47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="G47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="H47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="I47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="J47" s="1" t="str">
@@ -13292,19 +13292,19 @@
         <v>264</v>
       </c>
       <c r="F48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEtherImide Pellets)</v>
       </c>
       <c r="G48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEtherImide Pellets)</v>
       </c>
       <c r="H48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEtherImide Pellets)</v>
       </c>
       <c r="I48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEtherImide Pellets)</v>
       </c>
       <c r="J48" s="1" t="str">
@@ -13341,19 +13341,19 @@
         <v>260</v>
       </c>
       <c r="F49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="G49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="H49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="I49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="J49" s="1" t="str">
@@ -13390,19 +13390,19 @@
         <v>256</v>
       </c>
       <c r="F50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="G50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="H50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="I50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="J50" s="1" t="str">
@@ -13442,19 +13442,19 @@
         <v>252</v>
       </c>
       <c r="F51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="G51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="H51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="I51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="J51" s="1" t="str">
@@ -13491,19 +13491,19 @@
         <v>248</v>
       </c>
       <c r="F52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J52" s="1" t="str">
@@ -13543,19 +13543,19 @@
         <v>244</v>
       </c>
       <c r="F53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="G53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="H53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="I53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="J53" s="1" t="str">
@@ -13595,19 +13595,19 @@
         <v>240</v>
       </c>
       <c r="F54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="G54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="H54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="I54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="J54" s="1" t="str">
@@ -13647,19 +13647,19 @@
         <v>236</v>
       </c>
       <c r="F55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="G55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="H55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="I55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="J55" s="1" t="str">
@@ -13699,19 +13699,19 @@
         <v>232</v>
       </c>
       <c r="F56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J56" s="1" t="str">
@@ -13751,19 +13751,19 @@
         <v>228</v>
       </c>
       <c r="F57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="G57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="H57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="I57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="J57" s="1" t="str">
@@ -13803,19 +13803,19 @@
         <v>224</v>
       </c>
       <c r="F58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="G58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="H58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="I58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="J58" s="1" t="str">
@@ -13855,19 +13855,19 @@
         <v>220</v>
       </c>
       <c r="F59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="G59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="H59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="I59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="J59" s="1" t="str">
@@ -13907,19 +13907,19 @@
         <v>216</v>
       </c>
       <c r="F60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="G60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="H60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="I60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="J60" s="1" t="str">
@@ -13959,19 +13959,19 @@
         <v>212</v>
       </c>
       <c r="F61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="G61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="H61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="I61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="J61" s="1" t="str">
@@ -14008,19 +14008,19 @@
         <v>208</v>
       </c>
       <c r="F62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="G62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="H62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="I62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="J62" s="1" t="str">
@@ -14060,19 +14060,19 @@
         <v>204</v>
       </c>
       <c r="F63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyImide Pellets)</v>
       </c>
       <c r="G63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyImide Pellets)</v>
       </c>
       <c r="H63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyImide Pellets)</v>
       </c>
       <c r="I63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyImide Pellets)</v>
       </c>
       <c r="J63" s="1" t="str">
@@ -14109,19 +14109,19 @@
         <v>200</v>
       </c>
       <c r="F64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="G64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="H64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="I64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="J64" s="1" t="str">
@@ -14158,19 +14158,19 @@
         <v>196</v>
       </c>
       <c r="F65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="G65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="H65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="I65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="J65" s="1" t="str">
@@ -14210,19 +14210,19 @@
         <v>192</v>
       </c>
       <c r="F66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButylene Pellets)</v>
       </c>
       <c r="G66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButylene Pellets)</v>
       </c>
       <c r="H66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButylene Pellets)</v>
       </c>
       <c r="I66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButylene Pellets)</v>
       </c>
       <c r="J66" s="1" t="str">
@@ -14262,19 +14262,19 @@
         <v>188</v>
       </c>
       <c r="F67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoPrene Pellets)</v>
       </c>
       <c r="G67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoPrene Pellets)</v>
       </c>
       <c r="H67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoPrene Pellets)</v>
       </c>
       <c r="I67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoPrene Pellets)</v>
       </c>
       <c r="J67" s="1" t="str">
@@ -14314,19 +14314,19 @@
         <v>184</v>
       </c>
       <c r="F68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic Acid Pellets)</v>
       </c>
       <c r="G68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic Acid Pellets)</v>
       </c>
       <c r="H68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic Acid Pellets)</v>
       </c>
       <c r="I68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic Acid Pellets)</v>
       </c>
       <c r="J68" s="1" t="str">
@@ -14363,19 +14363,19 @@
         <v>180</v>
       </c>
       <c r="F69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="G69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="H69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="I69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="J69" s="1" t="str">
@@ -14415,19 +14415,19 @@
         <v>176</v>
       </c>
       <c r="F70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="G70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="H70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="I70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="J70" s="1" t="str">
@@ -14464,19 +14464,19 @@
         <v>172</v>
       </c>
       <c r="F71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="G71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="H71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="I71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="J71" s="1" t="str">
@@ -14516,19 +14516,19 @@
         <v>168</v>
       </c>
       <c r="F72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="G72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="H72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="I72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="J72" s="1" t="str">
@@ -14568,19 +14568,19 @@
         <v>164</v>
       </c>
       <c r="F73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="G73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="H73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="I73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="J73" s="1" t="str">
@@ -14620,19 +14620,19 @@
         <v>160</v>
       </c>
       <c r="F74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="G74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="H74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="I74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="J74" s="1" t="str">
@@ -14669,19 +14669,19 @@
         <v>156</v>
       </c>
       <c r="F75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J75" s="1" t="str">
@@ -14721,19 +14721,19 @@
         <v>152</v>
       </c>
       <c r="F76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyOxymethylene Pellets)</v>
       </c>
       <c r="G76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyOxymethylene Pellets)</v>
       </c>
       <c r="H76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyOxymethylene Pellets)</v>
       </c>
       <c r="I76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyOxymethylene Pellets)</v>
       </c>
       <c r="J76" s="1" t="str">
@@ -14770,19 +14770,19 @@
         <v>148</v>
       </c>
       <c r="F77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J77" s="1" t="str">
@@ -14822,19 +14822,19 @@
         <v>144</v>
       </c>
       <c r="F78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenol Pellets)</v>
       </c>
       <c r="G78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenol Pellets)</v>
       </c>
       <c r="H78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenol Pellets)</v>
       </c>
       <c r="I78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenol Pellets)</v>
       </c>
       <c r="J78" s="1" t="str">
@@ -14871,19 +14871,19 @@
         <v>140</v>
       </c>
       <c r="F79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="G79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="H79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="I79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="J79" s="1" t="str">
@@ -14920,19 +14920,19 @@
         <v>136</v>
       </c>
       <c r="F80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhosphazene Pellets)</v>
       </c>
       <c r="G80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhosphazene Pellets)</v>
       </c>
       <c r="H80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhosphazene Pellets)</v>
       </c>
       <c r="I80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhosphazene Pellets)</v>
       </c>
       <c r="J80" s="1" t="str">
@@ -14969,19 +14969,19 @@
         <v>132</v>
       </c>
       <c r="F81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="G81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="H81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="I81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="J81" s="1" t="str">
@@ -15018,19 +15018,19 @@
         <v>128</v>
       </c>
       <c r="F82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="G82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="H82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="I82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="J82" s="1" t="str">
@@ -15070,19 +15070,19 @@
         <v>124</v>
       </c>
       <c r="F83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="G83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="H83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="I83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="J83" s="1" t="str">
@@ -15122,19 +15122,19 @@
         <v>120</v>
       </c>
       <c r="F84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Pellets)</v>
       </c>
       <c r="G84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Pellets)</v>
       </c>
       <c r="H84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Pellets)</v>
       </c>
       <c r="I84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Pellets)</v>
       </c>
       <c r="J84" s="1" t="str">
@@ -15171,19 +15171,19 @@
         <v>116</v>
       </c>
       <c r="F85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="G85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="H85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="I85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="J85" s="1" t="str">
@@ -15220,19 +15220,19 @@
         <v>112</v>
       </c>
       <c r="F86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="G86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="H86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="I86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="J86" s="1" t="str">
@@ -15272,19 +15272,19 @@
         <v>108</v>
       </c>
       <c r="F87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyStyrene Pellets)</v>
       </c>
       <c r="G87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyStyrene Pellets)</v>
       </c>
       <c r="H87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyStyrene Pellets)</v>
       </c>
       <c r="I87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyStyrene Pellets)</v>
       </c>
       <c r="J87" s="1" t="str">
@@ -15321,19 +15321,19 @@
         <v>104</v>
       </c>
       <c r="F88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J88" s="1" t="str">
@@ -15373,19 +15373,19 @@
         <v>100</v>
       </c>
       <c r="F89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="G89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="H89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="I89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="J89" s="1" t="str">
@@ -15422,19 +15422,19 @@
         <v>96</v>
       </c>
       <c r="F90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="G90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="H90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="I90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="J90" s="1" t="str">
@@ -15471,19 +15471,19 @@
         <v>92</v>
       </c>
       <c r="F91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="G91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="H91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="I91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="J91" s="1" t="str">
@@ -15520,19 +15520,19 @@
         <v>88</v>
       </c>
       <c r="F92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyThiazyl Pellets)</v>
       </c>
       <c r="G92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyThiazyl Pellets)</v>
       </c>
       <c r="H92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyThiazyl Pellets)</v>
       </c>
       <c r="I92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyThiazyl Pellets)</v>
       </c>
       <c r="J92" s="1" t="str">
@@ -15572,19 +15572,19 @@
         <v>84</v>
       </c>
       <c r="F93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="G93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="H93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="I93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="J93" s="1" t="str">
@@ -15624,19 +15624,19 @@
         <v>80</v>
       </c>
       <c r="F94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyUrethane Pellets)</v>
       </c>
       <c r="G94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyUrethane Pellets)</v>
       </c>
       <c r="H94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyUrethane Pellets)</v>
       </c>
       <c r="I94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyUrethane Pellets)</v>
       </c>
       <c r="J94" s="1" t="str">
@@ -15676,19 +15676,19 @@
         <v>76</v>
       </c>
       <c r="F95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="G95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="H95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="I95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="J95" s="1" t="str">
@@ -15728,19 +15728,19 @@
         <v>72</v>
       </c>
       <c r="F96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="G96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="H96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="I96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="J96" s="1" t="str">
@@ -15777,19 +15777,19 @@
         <v>68</v>
       </c>
       <c r="F97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="G97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="H97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="I97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="J97" s="1" t="str">
@@ -15829,19 +15829,19 @@
         <v>64</v>
       </c>
       <c r="F98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="G98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="H98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="I98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="J98" s="1" t="str">
@@ -15881,19 +15881,19 @@
         <v>60</v>
       </c>
       <c r="F99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="G99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="H99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="I99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="J99" s="1" t="str">
@@ -15930,19 +15930,19 @@
         <v>56</v>
       </c>
       <c r="F100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="G100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="H100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="I100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="J100" s="1" t="str">
@@ -15979,19 +15979,19 @@
         <v>52</v>
       </c>
       <c r="F101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="G101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="H101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="I101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="J101" s="1" t="str">
@@ -16028,19 +16028,19 @@
         <v>48</v>
       </c>
       <c r="F102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="G102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="H102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="I102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="J102" s="1" t="str">
@@ -16077,19 +16077,19 @@
         <v>44</v>
       </c>
       <c r="F103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="G103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="H103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="I103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="J103" s="1" t="str">
@@ -16126,19 +16126,19 @@
         <v>40</v>
       </c>
       <c r="F104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="G104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="H104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="I104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="J104" s="1" t="str">
@@ -16175,19 +16175,19 @@
         <v>36</v>
       </c>
       <c r="F105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="G105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="H105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="I105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="J105" s="1" t="str">
@@ -16227,19 +16227,19 @@
         <v>32</v>
       </c>
       <c r="F106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="G106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="H106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="I106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="J106" s="1" t="str">
@@ -16279,19 +16279,19 @@
         <v>28</v>
       </c>
       <c r="F107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J107" s="1" t="str">
@@ -16331,19 +16331,19 @@
         <v>24</v>
       </c>
       <c r="F108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J108" s="1" t="str">
@@ -16383,19 +16383,19 @@
         <v>20</v>
       </c>
       <c r="F109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="G109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="H109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="I109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="J109" s="1" t="str">
@@ -16432,19 +16432,19 @@
         <v>16</v>
       </c>
       <c r="F110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="G110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="H110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="I110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="J110" s="1" t="str">
@@ -16484,19 +16484,19 @@
         <v>12</v>
       </c>
       <c r="F111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="G111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="H111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="I111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="J111" s="1" t="str">
@@ -16533,19 +16533,19 @@
         <v>8</v>
       </c>
       <c r="F112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="G112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="H112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="I112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="J112" s="1" t="str">
@@ -16585,19 +16585,19 @@
         <v>4</v>
       </c>
       <c r="F113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J113" s="1" t="str">
@@ -16637,19 +16637,19 @@
         <v>0</v>
       </c>
       <c r="F114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="G114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="H114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="I114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="J114" s="1" t="str">
@@ -16689,19 +16689,19 @@
         <v>1853</v>
       </c>
       <c r="F115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Polycaprolactam Pellets)</v>
       </c>
       <c r="G115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Polycaprolactam Pellets)</v>
       </c>
       <c r="H115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Polycaprolactam Pellets)</v>
       </c>
       <c r="I115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Polycaprolactam Pellets)</v>
       </c>
       <c r="J115" s="1" t="str">
@@ -16741,19 +16741,19 @@
         <v>2412</v>
       </c>
       <c r="F116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="G116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="H116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="I116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="J116" s="1" t="str">
@@ -16793,19 +16793,19 @@
         <v>2416</v>
       </c>
       <c r="F117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="G117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="H117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="I117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="J117" s="1" t="str">
@@ -16845,19 +16845,19 @@
         <v>2420</v>
       </c>
       <c r="F118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Negative Photoresist)</v>
       </c>
       <c r="G118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Negative Photoresist)</v>
       </c>
       <c r="H118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Negative Photoresist)</v>
       </c>
       <c r="I118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Negative Photoresist)</v>
       </c>
       <c r="J118" s="1" t="str">
@@ -16897,19 +16897,19 @@
         <v>2424</v>
       </c>
       <c r="F119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$34, [1]Enums!$A$35)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Positive Photoresist)</v>
       </c>
       <c r="G119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$37, [1]Enums!$A$38)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Positive Photoresist)</v>
       </c>
       <c r="H119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$40, [1]Enums!$A$41)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Positive Photoresist)</v>
       </c>
       <c r="I119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$43, [1]Enums!$A$44)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Positive Photoresist)</v>
       </c>
       <c r="J119" s="1" t="str">
@@ -17824,11 +17824,11 @@
         <v>2651</v>
       </c>
       <c r="C1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="D1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="19" t="str">
@@ -17864,7 +17864,7 @@
         <v>Mask (Solar Cell)(PR Backplane)</v>
       </c>
       <c r="D2" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E2" s="15" t="str">
@@ -17888,7 +17888,7 @@
         <v>Mask (Solar Cell)(PR Semiconductor)</v>
       </c>
       <c r="D3" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E3" s="15" t="str">
@@ -17912,7 +17912,7 @@
         <v>Mask (Solar Cell)(PR Dielectric)</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E4" s="15" t="str">
@@ -17936,7 +17936,7 @@
         <v>Mask (Solar Cell)(PR Traces)</v>
       </c>
       <c r="D5" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E5" s="15" t="str">
@@ -17960,7 +17960,7 @@
         <v>Mask (Solar Cell)(PR Encapsulation)</v>
       </c>
       <c r="D6" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E6" s="15" t="str">
@@ -17984,7 +17984,7 @@
         <v>Mask (Processor)(PR Backplane)</v>
       </c>
       <c r="D7" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E7" s="15" t="str">
@@ -18008,7 +18008,7 @@
         <v>Mask (Processor)(PR n-Type Semiconductor)</v>
       </c>
       <c r="D8" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E8" s="15" t="str">
@@ -18032,7 +18032,7 @@
         <v>Mask (Processor)(PR p-Type Semiconductor)</v>
       </c>
       <c r="D9" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E9" s="15" t="str">
@@ -18056,7 +18056,7 @@
         <v>Mask (Processor)(PR Dielectric)</v>
       </c>
       <c r="D10" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E10" s="15" t="str">
@@ -18080,7 +18080,7 @@
         <v>Mask (Processor)(PR Inner Traces)</v>
       </c>
       <c r="D11" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E11" s="15" t="str">
@@ -18104,7 +18104,7 @@
         <v>Mask (Processor)(PR Through Vias)</v>
       </c>
       <c r="D12" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E12" s="15" t="str">
@@ -18128,7 +18128,7 @@
         <v>Mask (Processor)(PR Outer Traces)</v>
       </c>
       <c r="D13" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E13" s="15" t="str">
@@ -18152,7 +18152,7 @@
         <v>Mask (Processor)(PR Encapsulation)</v>
       </c>
       <c r="D14" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E14" s="15" t="str">
@@ -18176,7 +18176,7 @@
         <v>Mask (Temperature Sensor)(PR Backplane)</v>
       </c>
       <c r="D15" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E15" s="15" t="str">
@@ -18200,7 +18200,7 @@
         <v>Mask (Temperature Sensor)(PR Semiconductor)</v>
       </c>
       <c r="D16" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E16" s="15" t="str">
@@ -18224,7 +18224,7 @@
         <v>Mask (Temperature Sensor)(PR Dielectric)</v>
       </c>
       <c r="D17" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E17" s="15" t="str">
@@ -18248,7 +18248,7 @@
         <v>Mask (Temperature Sensor)(PR Traces)</v>
       </c>
       <c r="D18" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E18" s="15" t="str">
@@ -18272,7 +18272,7 @@
         <v>Mask (Temperature Sensor)(PR Encapsulation)</v>
       </c>
       <c r="D19" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E19" s="15" t="str">
@@ -18296,7 +18296,7 @@
         <v>Mask (Pressure Sensor)(PR Backplane)</v>
       </c>
       <c r="D20" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E20" s="15" t="str">
@@ -18320,7 +18320,7 @@
         <v>Mask (Pressure Sensor)(PR Semiconductor)</v>
       </c>
       <c r="D21" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E21" s="15" t="str">
@@ -18344,7 +18344,7 @@
         <v>Mask (Pressure Sensor)(PR Dielectric)</v>
       </c>
       <c r="D22" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E22" s="15" t="str">
@@ -18368,7 +18368,7 @@
         <v>Mask (Pressure Sensor)(PR Traces)</v>
       </c>
       <c r="D23" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E23" s="15" t="str">
@@ -18392,7 +18392,7 @@
         <v>Mask (Pressure Sensor)(PR Encapsulation)</v>
       </c>
       <c r="D24" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E24" s="15" t="str">
@@ -18416,7 +18416,7 @@
         <v>Mask (Low Power Radio)(PR Backplane)</v>
       </c>
       <c r="D25" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E25" s="15" t="str">
@@ -18440,7 +18440,7 @@
         <v>Mask (Low Power Radio)(PR n-Type Semiconductor)</v>
       </c>
       <c r="D26" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E26" s="15" t="str">
@@ -18464,7 +18464,7 @@
         <v>Mask (Low Power Radio)(PR p-Type Semiconductor)</v>
       </c>
       <c r="D27" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E27" s="15" t="str">
@@ -18488,7 +18488,7 @@
         <v>Mask (Low Power Radio)(PR Dielectric)</v>
       </c>
       <c r="D28" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E28" s="15" t="str">
@@ -18512,7 +18512,7 @@
         <v>Mask (Low Power Radio)(PR Inner Traces)</v>
       </c>
       <c r="D29" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E29" s="15" t="str">
@@ -18536,7 +18536,7 @@
         <v>Mask (Low Power Radio)(PR Through Vias)</v>
       </c>
       <c r="D30" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E30" s="15" t="str">
@@ -18560,7 +18560,7 @@
         <v>Mask (Low Power Radio)(PR Outer Traces)</v>
       </c>
       <c r="D31" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E31" s="15" t="str">
@@ -18584,7 +18584,7 @@
         <v>Mask (Low Power Radio)(PR Encapsulation)</v>
       </c>
       <c r="D32" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E32" s="15" t="str">
@@ -18608,7 +18608,7 @@
         <v>Mask (DSP)(PR Backplane)</v>
       </c>
       <c r="D33" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E33" s="15" t="str">
@@ -18632,7 +18632,7 @@
         <v>Mask (DSP)(PR n-Type Semiconductor)</v>
       </c>
       <c r="D34" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E34" s="15" t="str">
@@ -18656,7 +18656,7 @@
         <v>Mask (DSP)(PR p-Type Semiconductor)</v>
       </c>
       <c r="D35" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E35" s="15" t="str">
@@ -18680,7 +18680,7 @@
         <v>Mask (DSP)(PR Dielectric)</v>
       </c>
       <c r="D36" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E36" s="15" t="str">
@@ -18704,7 +18704,7 @@
         <v>Mask (DSP)(PR Inner Traces)</v>
       </c>
       <c r="D37" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E37" s="15" t="str">
@@ -18728,7 +18728,7 @@
         <v>Mask (DSP)(PR Through Vias)</v>
       </c>
       <c r="D38" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E38" s="15" t="str">
@@ -18752,7 +18752,7 @@
         <v>Mask (DSP)(PR Outer Traces)</v>
       </c>
       <c r="D39" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E39" s="15" t="str">
@@ -18776,7 +18776,7 @@
         <v>Mask (DSP)(PR Encapsulation)</v>
       </c>
       <c r="D40" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E40" s="15" t="str">
@@ -18800,7 +18800,7 @@
         <v>Mask (Digital Analog Convertor)(PR Backplane)</v>
       </c>
       <c r="D41" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E41" s="15" t="str">
@@ -18824,7 +18824,7 @@
         <v>Mask (Digital Analog Convertor)(PR Semiconductor)</v>
       </c>
       <c r="D42" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E42" s="15" t="str">
@@ -18848,7 +18848,7 @@
         <v>Mask (Digital Analog Convertor)(PR Dielectric)</v>
       </c>
       <c r="D43" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E43" s="15" t="str">
@@ -18872,7 +18872,7 @@
         <v>Mask (Digital Analog Convertor)(PR Traces)</v>
       </c>
       <c r="D44" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E44" s="15" t="str">
@@ -18896,7 +18896,7 @@
         <v>Mask (Digital Analog Convertor)(PR Encapsulation)</v>
       </c>
       <c r="D45" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E45" s="15" t="str">
@@ -18920,7 +18920,7 @@
         <v>Mask (Amplifier)(PR Backplane)</v>
       </c>
       <c r="D46" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E46" s="15" t="str">
@@ -18944,7 +18944,7 @@
         <v>Mask (Amplifier)(PR Semiconductor)</v>
       </c>
       <c r="D47" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E47" s="15" t="str">
@@ -18968,7 +18968,7 @@
         <v>Mask (Amplifier)(PR Dielectric)</v>
       </c>
       <c r="D48" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E48" s="15" t="str">
@@ -18992,7 +18992,7 @@
         <v>Mask (Amplifier)(PR Traces)</v>
       </c>
       <c r="D49" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E49" s="15" t="str">
@@ -19016,7 +19016,7 @@
         <v>Mask (Amplifier)(PR Encapsulation)</v>
       </c>
       <c r="D50" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E50" s="15" t="str">
@@ -19040,7 +19040,7 @@
         <v>Mask (OLED Array)(PR Backplane)</v>
       </c>
       <c r="D51" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E51" s="15" t="str">
@@ -19064,7 +19064,7 @@
         <v>Mask (OLED Array)(PR Semiconductor)</v>
       </c>
       <c r="D52" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E52" s="15" t="str">
@@ -19088,7 +19088,7 @@
         <v>Mask (OLED Array)(PR Dielectric)</v>
       </c>
       <c r="D53" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E53" s="15" t="str">
@@ -19112,7 +19112,7 @@
         <v>Mask (OLED Array)(PR Traces)</v>
       </c>
       <c r="D54" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E54" s="15" t="str">
@@ -19136,7 +19136,7 @@
         <v>Mask (OLED Array)(PR Encapsulation)</v>
       </c>
       <c r="D55" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$96</f>
+        <f xml:space="preserve"> [1]Enums!$B$97</f>
         <v>Mask</v>
       </c>
       <c r="E55" s="15" t="str">
@@ -25386,7 +25386,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I2" s="45" t="str">
-        <f>[1]Enums!$A$149&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Steel</v>
       </c>
       <c r="J2" s="45">
@@ -25434,7 +25434,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I3" s="45" t="str">
-        <f>[1]Enums!$A$149&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Stainless Steel</v>
       </c>
       <c r="J3" s="45">
@@ -25482,7 +25482,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I4" s="45" t="str">
-        <f>[1]Enums!$A$149&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Brass</v>
       </c>
       <c r="J4" s="45">
@@ -25530,7 +25530,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I5" s="45" t="str">
-        <f>[1]Enums!$A$149&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Bronze</v>
       </c>
       <c r="J5" s="45">
@@ -25578,7 +25578,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I6" s="45" t="str">
-        <f>[1]Enums!$A$149&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Tungsten Carbide</v>
       </c>
       <c r="J6" s="45">
@@ -25626,7 +25626,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I7" s="45" t="str">
-        <f>[1]Enums!$A$149&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Nichrome</v>
       </c>
       <c r="J7" s="45">
@@ -25674,7 +25674,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I8" s="45" t="str">
-        <f>[1]Enums!$A$149&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Antimony-Lead</v>
       </c>
       <c r="J8" s="45">
@@ -25722,7 +25722,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I9" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Steel</v>
       </c>
       <c r="J9" s="45">
@@ -25770,7 +25770,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I10" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Stainless Steel</v>
       </c>
       <c r="J10" s="45">
@@ -25818,7 +25818,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I11" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Brass</v>
       </c>
       <c r="J11" s="45">
@@ -25866,7 +25866,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I12" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Bronze</v>
       </c>
       <c r="J12" s="45">
@@ -25914,7 +25914,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I13" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Tungsten Carbide</v>
       </c>
       <c r="J13" s="45">
@@ -25962,7 +25962,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I14" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Nichrome</v>
       </c>
       <c r="J14" s="45">
@@ -26010,7 +26010,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I15" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Antimony-Lead</v>
       </c>
       <c r="J15" s="45">
@@ -26058,7 +26058,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I16" s="45" t="str">
-        <f>[1]Enums!$A$149&amp;" Iron"</f>
+        <f>[1]Enums!$A$150&amp;" Iron"</f>
         <v>Composite Iron</v>
       </c>
       <c r="J16" s="45">
@@ -26106,7 +26106,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I17" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" Iron"</f>
+        <f>[1]Enums!$A$151&amp;" Iron"</f>
         <v>Engineered Iron</v>
       </c>
       <c r="J17" s="45">
@@ -26154,7 +26154,7 @@
         <v>Diamond</v>
       </c>
       <c r="I18" s="45" t="str">
-        <f>[1]Enums!$A$149&amp;" Diamond"</f>
+        <f>[1]Enums!$A$150&amp;" Diamond"</f>
         <v>Composite Diamond</v>
       </c>
       <c r="J18" s="45">
@@ -26202,7 +26202,7 @@
         <v>Diamond</v>
       </c>
       <c r="I19" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" Diamond"</f>
+        <f>[1]Enums!$A$151&amp;" Diamond"</f>
         <v>Engineered Diamond</v>
       </c>
       <c r="J19" s="45">
@@ -26503,7 +26503,7 @@
         <v>Molded Item</v>
       </c>
       <c r="F1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$114</f>
+        <f xml:space="preserve"> [1]Enums!$A$115</f>
         <v>Base Material</v>
       </c>
       <c r="G1" s="30" t="s">
@@ -26531,7 +26531,7 @@
         <v>1812</v>
       </c>
       <c r="C2" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D2</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D2</f>
         <v>Gripped Iron Shovel</v>
       </c>
       <c r="D2" s="24" t="str">
@@ -26543,7 +26543,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F2" s="34" t="str">
-        <f>[1]Enums!$A$117</f>
+        <f>[1]Enums!$A$118</f>
         <v>Iron</v>
       </c>
       <c r="G2" s="24">
@@ -26568,7 +26568,7 @@
         <v>1811</v>
       </c>
       <c r="C3" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D3</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D3</f>
         <v>Gripped Iron Pickaxe</v>
       </c>
       <c r="D3" s="21" t="str">
@@ -26580,7 +26580,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F3" s="34" t="str">
-        <f>[1]Enums!$A$117</f>
+        <f>[1]Enums!$A$118</f>
         <v>Iron</v>
       </c>
       <c r="G3" s="24">
@@ -26605,7 +26605,7 @@
         <v>1810</v>
       </c>
       <c r="C4" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D4</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D4</f>
         <v>Gripped Iron Axe</v>
       </c>
       <c r="D4" s="21" t="str">
@@ -26617,7 +26617,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F4" s="34" t="str">
-        <f>[1]Enums!$A$117</f>
+        <f>[1]Enums!$A$118</f>
         <v>Iron</v>
       </c>
       <c r="G4" s="24">
@@ -26642,7 +26642,7 @@
         <v>1809</v>
       </c>
       <c r="C5" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D5</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D5</f>
         <v>Gripped Iron Sword</v>
       </c>
       <c r="D5" s="21" t="str">
@@ -26654,7 +26654,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F5" s="34" t="str">
-        <f>[1]Enums!$A$117</f>
+        <f>[1]Enums!$A$118</f>
         <v>Iron</v>
       </c>
       <c r="G5" s="24">
@@ -26679,7 +26679,7 @@
         <v>1808</v>
       </c>
       <c r="C6" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D6</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D6</f>
         <v>Gripped Wooden Sword</v>
       </c>
       <c r="D6" s="21" t="str">
@@ -26691,7 +26691,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F6" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Wooden</v>
       </c>
       <c r="G6" s="24">
@@ -26716,7 +26716,7 @@
         <v>1807</v>
       </c>
       <c r="C7" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D7</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D7</f>
         <v>Gripped Wooden Shovel</v>
       </c>
       <c r="D7" s="21" t="str">
@@ -26728,7 +26728,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F7" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Wooden</v>
       </c>
       <c r="G7" s="24">
@@ -26753,7 +26753,7 @@
         <v>1806</v>
       </c>
       <c r="C8" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D8</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D8</f>
         <v>Gripped Wooden Pickaxe</v>
       </c>
       <c r="D8" s="21" t="str">
@@ -26765,7 +26765,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F8" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Wooden</v>
       </c>
       <c r="G8" s="24">
@@ -26790,7 +26790,7 @@
         <v>1805</v>
       </c>
       <c r="C9" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D9</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D9</f>
         <v>Gripped Wooden Axe</v>
       </c>
       <c r="D9" s="21" t="str">
@@ -26802,7 +26802,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F9" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Wooden</v>
       </c>
       <c r="G9" s="24">
@@ -26827,7 +26827,7 @@
         <v>1804</v>
       </c>
       <c r="C10" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D10</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D10</f>
         <v>Gripped Stone Sword</v>
       </c>
       <c r="D10" s="21" t="str">
@@ -26839,7 +26839,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F10" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$117</f>
         <v>Stone</v>
       </c>
       <c r="G10" s="24">
@@ -26864,7 +26864,7 @@
         <v>1803</v>
       </c>
       <c r="C11" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D11</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D11</f>
         <v>Gripped Stone Shovel</v>
       </c>
       <c r="D11" s="21" t="str">
@@ -26876,7 +26876,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F11" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$117</f>
         <v>Stone</v>
       </c>
       <c r="G11" s="24">
@@ -26901,7 +26901,7 @@
         <v>1802</v>
       </c>
       <c r="C12" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D12</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D12</f>
         <v>Gripped Stone Pickaxe</v>
       </c>
       <c r="D12" s="21" t="str">
@@ -26913,7 +26913,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F12" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$117</f>
         <v>Stone</v>
       </c>
       <c r="G12" s="24">
@@ -26938,7 +26938,7 @@
         <v>1801</v>
       </c>
       <c r="C13" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D13</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D13</f>
         <v>Gripped Stone Axe</v>
       </c>
       <c r="D13" s="21" t="str">
@@ -26950,7 +26950,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F13" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$117</f>
         <v>Stone</v>
       </c>
       <c r="G13" s="24">
@@ -26975,7 +26975,7 @@
         <v>1800</v>
       </c>
       <c r="C14" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D14</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D14</f>
         <v>Gripped Diamond Sword</v>
       </c>
       <c r="D14" s="21" t="str">
@@ -26987,7 +26987,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F14" s="34" t="str">
-        <f>[1]Enums!$A$119</f>
+        <f>[1]Enums!$A$120</f>
         <v>Diamond</v>
       </c>
       <c r="G14" s="24">
@@ -27012,7 +27012,7 @@
         <v>1799</v>
       </c>
       <c r="C15" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D15</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D15</f>
         <v>Gripped Diamond Shovel</v>
       </c>
       <c r="D15" s="21" t="str">
@@ -27024,7 +27024,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F15" s="34" t="str">
-        <f>[1]Enums!$A$119</f>
+        <f>[1]Enums!$A$120</f>
         <v>Diamond</v>
       </c>
       <c r="G15" s="24">
@@ -27049,7 +27049,7 @@
         <v>1798</v>
       </c>
       <c r="C16" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D16</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D16</f>
         <v>Gripped Diamond Pickaxe</v>
       </c>
       <c r="D16" s="21" t="str">
@@ -27061,7 +27061,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F16" s="34" t="str">
-        <f>[1]Enums!$A$119</f>
+        <f>[1]Enums!$A$120</f>
         <v>Diamond</v>
       </c>
       <c r="G16" s="24">
@@ -27086,7 +27086,7 @@
         <v>1797</v>
       </c>
       <c r="C17" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D17</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D17</f>
         <v>Gripped Diamond Axe</v>
       </c>
       <c r="D17" s="21" t="str">
@@ -27098,7 +27098,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F17" s="34" t="str">
-        <f>[1]Enums!$A$119</f>
+        <f>[1]Enums!$A$120</f>
         <v>Diamond</v>
       </c>
       <c r="G17" s="24">
@@ -27123,7 +27123,7 @@
         <v>1796</v>
       </c>
       <c r="C18" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D18</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D18</f>
         <v>Gripped Golden Sword</v>
       </c>
       <c r="D18" s="21" t="str">
@@ -27135,7 +27135,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F18" s="34" t="str">
-        <f>[1]Enums!$A$118</f>
+        <f>[1]Enums!$A$119</f>
         <v>Golden</v>
       </c>
       <c r="G18" s="24">
@@ -27160,7 +27160,7 @@
         <v>1795</v>
       </c>
       <c r="C19" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D19</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D19</f>
         <v>Gripped Golden Shovel</v>
       </c>
       <c r="D19" s="21" t="str">
@@ -27172,7 +27172,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F19" s="34" t="str">
-        <f>[1]Enums!$A$118</f>
+        <f>[1]Enums!$A$119</f>
         <v>Golden</v>
       </c>
       <c r="G19" s="24">
@@ -27197,7 +27197,7 @@
         <v>1794</v>
       </c>
       <c r="C20" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D20</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D20</f>
         <v>Gripped Golden Pickaxe</v>
       </c>
       <c r="D20" s="21" t="str">
@@ -27209,7 +27209,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F20" s="34" t="str">
-        <f>[1]Enums!$A$118</f>
+        <f>[1]Enums!$A$119</f>
         <v>Golden</v>
       </c>
       <c r="G20" s="24">
@@ -27234,7 +27234,7 @@
         <v>1793</v>
       </c>
       <c r="C21" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D21</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D21</f>
         <v>Gripped Golden Axe</v>
       </c>
       <c r="D21" s="21" t="str">
@@ -27246,7 +27246,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F21" s="34" t="str">
-        <f>[1]Enums!$A$118</f>
+        <f>[1]Enums!$A$119</f>
         <v>Golden</v>
       </c>
       <c r="G21" s="24">
@@ -27271,7 +27271,7 @@
         <v>1792</v>
       </c>
       <c r="C22" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D22</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D22</f>
         <v>Gripped Wooden Hoe</v>
       </c>
       <c r="D22" s="21" t="str">
@@ -27283,7 +27283,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F22" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Wooden</v>
       </c>
       <c r="G22" s="24">
@@ -27308,7 +27308,7 @@
         <v>1791</v>
       </c>
       <c r="C23" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D23</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D23</f>
         <v>Gripped Stone Hoe</v>
       </c>
       <c r="D23" s="21" t="str">
@@ -27320,7 +27320,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F23" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$117</f>
         <v>Stone</v>
       </c>
       <c r="G23" s="24">
@@ -27345,7 +27345,7 @@
         <v>1790</v>
       </c>
       <c r="C24" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D24</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D24</f>
         <v>Gripped Iron Hoe</v>
       </c>
       <c r="D24" s="21" t="str">
@@ -27357,7 +27357,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F24" s="34" t="str">
-        <f>[1]Enums!$A$117</f>
+        <f>[1]Enums!$A$118</f>
         <v>Iron</v>
       </c>
       <c r="G24" s="24">
@@ -27382,7 +27382,7 @@
         <v>1789</v>
       </c>
       <c r="C25" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D25</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D25</f>
         <v>Gripped Diamond Hoe</v>
       </c>
       <c r="D25" s="21" t="str">
@@ -27394,7 +27394,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F25" s="34" t="str">
-        <f>[1]Enums!$A$119</f>
+        <f>[1]Enums!$A$120</f>
         <v>Diamond</v>
       </c>
       <c r="G25" s="24">
@@ -27419,7 +27419,7 @@
         <v>1788</v>
       </c>
       <c r="C26" s="22" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;D26</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;D26</f>
         <v>Gripped Golden Hoe</v>
       </c>
       <c r="D26" s="21" t="str">
@@ -27431,7 +27431,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F26" s="34" t="str">
-        <f>[1]Enums!$A$118</f>
+        <f>[1]Enums!$A$119</f>
         <v>Golden</v>
       </c>
       <c r="G26" s="24">
@@ -27493,7 +27493,7 @@
         <v>1832</v>
       </c>
       <c r="D1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$114</f>
+        <f xml:space="preserve"> [1]Enums!$A$115</f>
         <v>Base Material</v>
       </c>
       <c r="E1" s="36" t="s">
@@ -27539,7 +27539,7 @@
         <v>Wooden Pogo Stick</v>
       </c>
       <c r="D2" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Wooden</v>
       </c>
       <c r="E2" s="37">
@@ -27576,7 +27576,7 @@
         <v>Stone Pogo Stick</v>
       </c>
       <c r="D3" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$117</f>
         <v>Stone</v>
       </c>
       <c r="E3" s="37">
@@ -27612,7 +27612,7 @@
         <v>Iron Pogo Stick</v>
       </c>
       <c r="D4" s="34" t="str">
-        <f>[1]Enums!$A$117</f>
+        <f>[1]Enums!$A$118</f>
         <v>Iron</v>
       </c>
       <c r="E4" s="37">
@@ -27648,7 +27648,7 @@
         <v>Golden Pogo Stick</v>
       </c>
       <c r="D5" s="34" t="str">
-        <f>[1]Enums!$A$118</f>
+        <f>[1]Enums!$A$119</f>
         <v>Golden</v>
       </c>
       <c r="E5" s="37">
@@ -27684,7 +27684,7 @@
         <v>Diamond Pogo Stick</v>
       </c>
       <c r="D6" s="34" t="str">
-        <f>[1]Enums!$A$119</f>
+        <f>[1]Enums!$A$120</f>
         <v>Diamond</v>
       </c>
       <c r="E6" s="37">
@@ -27720,7 +27720,7 @@
         <v>Magic Pogo Stick</v>
       </c>
       <c r="D7" s="34" t="str">
-        <f>[1]Enums!$A$120</f>
+        <f>[1]Enums!$A$121</f>
         <v>Magic</v>
       </c>
       <c r="E7" s="37">
@@ -27752,11 +27752,11 @@
         <v>1821</v>
       </c>
       <c r="C8" s="34" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;I8</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;I8</f>
         <v>Gripped Wooden Pogo Stick</v>
       </c>
       <c r="D8" s="34" t="str">
-        <f>[1]Enums!$A$115</f>
+        <f>[1]Enums!$A$116</f>
         <v>Wooden</v>
       </c>
       <c r="E8" s="37">
@@ -27796,11 +27796,11 @@
         <v>1820</v>
       </c>
       <c r="C9" s="34" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;I9</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;I9</f>
         <v>Gripped Stone Pogo Stick</v>
       </c>
       <c r="D9" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$117</f>
         <v>Stone</v>
       </c>
       <c r="E9" s="37">
@@ -27840,11 +27840,11 @@
         <v>1819</v>
       </c>
       <c r="C10" s="34" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;I10</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;I10</f>
         <v>Gripped Iron Pogo Stick</v>
       </c>
       <c r="D10" s="34" t="str">
-        <f>[1]Enums!$A$117</f>
+        <f>[1]Enums!$A$118</f>
         <v>Iron</v>
       </c>
       <c r="E10" s="37">
@@ -27884,11 +27884,11 @@
         <v>1818</v>
       </c>
       <c r="C11" s="34" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;I11</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;I11</f>
         <v>Gripped Golden Pogo Stick</v>
       </c>
       <c r="D11" s="34" t="str">
-        <f>[1]Enums!$A$118</f>
+        <f>[1]Enums!$A$119</f>
         <v>Golden</v>
       </c>
       <c r="E11" s="37">
@@ -27928,11 +27928,11 @@
         <v>1817</v>
       </c>
       <c r="C12" s="34" t="str">
-        <f>[1]Enums!$A$111&amp;" "&amp;I12</f>
+        <f>[1]Enums!$A$112&amp;" "&amp;I12</f>
         <v>Gripped Diamond Pogo Stick</v>
       </c>
       <c r="D12" s="34" t="str">
-        <f>[1]Enums!$A$119</f>
+        <f>[1]Enums!$A$120</f>
         <v>Diamond</v>
       </c>
       <c r="E12" s="37">
@@ -29612,8 +29612,8 @@
   </sheetPr>
   <dimension ref="A1:G333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="P71" sqref="P71"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -46350,7 +46350,7 @@
         <v>590</v>
       </c>
       <c r="D1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="19" t="str">
@@ -46374,7 +46374,7 @@
         <v>Mold (Grip)</v>
       </c>
       <c r="D2" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E2" s="11" t="str">
@@ -46399,7 +46399,7 @@
         <v>Mold (Running Shoes)</v>
       </c>
       <c r="D3" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E3" s="11" t="str">
@@ -46424,7 +46424,7 @@
         <v>Mold (Scuba Fins)</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E4" s="11" t="str">
@@ -46449,7 +46449,7 @@
         <v>Mold (Scuba Mask)</v>
       </c>
       <c r="D5" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E5" s="11" t="str">
@@ -46474,7 +46474,7 @@
         <v>Mold (Gasket)</v>
       </c>
       <c r="D6" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E6" s="11" t="str">
@@ -46499,7 +46499,7 @@
         <v>Mold (Life Preserver)</v>
       </c>
       <c r="D7" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E7" s="11" t="str">
@@ -46524,7 +46524,7 @@
         <v>Metal Die (Fibers)</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$88</f>
+        <f xml:space="preserve"> [1]Enums!$B$89</f>
         <v>Metal Die</v>
       </c>
       <c r="E8" s="11" t="str">
@@ -46549,7 +46549,7 @@
         <v>Metal Die (Tether)</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$88</f>
+        <f xml:space="preserve"> [1]Enums!$B$89</f>
         <v>Metal Die</v>
       </c>
       <c r="E9" s="11" t="str">
@@ -46574,7 +46574,7 @@
         <v>Metal Die (Cord)</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$88</f>
+        <f xml:space="preserve"> [1]Enums!$B$89</f>
         <v>Metal Die</v>
       </c>
       <c r="E10" s="11" t="str">
@@ -46599,7 +46599,7 @@
         <v>Metal Die (Hose)</v>
       </c>
       <c r="D11" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$88</f>
+        <f xml:space="preserve"> [1]Enums!$B$89</f>
         <v>Metal Die</v>
       </c>
       <c r="E11" s="11" t="str">
@@ -46624,7 +46624,7 @@
         <v>Metal Die (Pipe Segment)</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$88</f>
+        <f xml:space="preserve"> [1]Enums!$B$89</f>
         <v>Metal Die</v>
       </c>
       <c r="E12" s="11" t="str">
@@ -46649,7 +46649,7 @@
         <v>Mold (Flashlight Shaft)</v>
       </c>
       <c r="D13" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E13" s="11" t="str">
@@ -46673,7 +46673,7 @@
         <v>Mold (Plastic Brick (1 x 1))</v>
       </c>
       <c r="D14" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E14" t="str">
@@ -46697,7 +46697,7 @@
         <v>Mold (Plastic Brick (1 x 2))</v>
       </c>
       <c r="D15" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E15" t="str">
@@ -46721,7 +46721,7 @@
         <v>Mold (Plastic Brick (1 x 3))</v>
       </c>
       <c r="D16" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E16" t="str">
@@ -46745,7 +46745,7 @@
         <v>Mold (Plastic Brick (1 x 4))</v>
       </c>
       <c r="D17" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E17" t="str">
@@ -46769,7 +46769,7 @@
         <v>Mold (Plastic Brick (2 x 2))</v>
       </c>
       <c r="D18" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E18" t="str">
@@ -46793,7 +46793,7 @@
         <v>Mold (Plastic Brick (2 x 3))</v>
       </c>
       <c r="D19" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E19" t="str">
@@ -46817,7 +46817,7 @@
         <v>Mold (Plastic Brick (2 x 4))</v>
       </c>
       <c r="D20" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E20" t="str">
@@ -46841,7 +46841,7 @@
         <v>Mold (Plastic Brick (3 x 3))</v>
       </c>
       <c r="D21" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E21" t="str">
@@ -46865,7 +46865,7 @@
         <v>Mold (Plastic Brick (3 x 4))</v>
       </c>
       <c r="D22" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E22" t="str">
@@ -46889,7 +46889,7 @@
         <v>Mold (Plastic Brick (4 x 4))</v>
       </c>
       <c r="D23" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E23" t="str">
@@ -46913,7 +46913,7 @@
         <v>Mold (Plastic Brick (1 x 8))</v>
       </c>
       <c r="D24" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E24" t="str">
@@ -46937,7 +46937,7 @@
         <v>Mold (Plastic Brick (2 x 8))</v>
       </c>
       <c r="D25" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E25" t="str">
@@ -46961,7 +46961,7 @@
         <v>Mold (Heated Knife Handle)</v>
       </c>
       <c r="D26" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E26" s="11" t="str">
@@ -46985,7 +46985,7 @@
         <v>Mold (Rubber Sole)</v>
       </c>
       <c r="D27" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E27" s="11" t="str">
@@ -47009,7 +47009,7 @@
         <v>Mold (Battery Case)</v>
       </c>
       <c r="D28" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E28" s="11" t="str">
@@ -47033,7 +47033,7 @@
         <v>Mold (Tool Shaft)</v>
       </c>
       <c r="D29" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E29" t="str">
@@ -47057,7 +47057,7 @@
         <v>Mold (Lighter Body)</v>
       </c>
       <c r="D30" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E30" t="str">
@@ -47081,7 +47081,7 @@
         <v>Mold (Cell Phone Case)</v>
       </c>
       <c r="D31" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E31" t="str">
@@ -47105,7 +47105,7 @@
         <v>Mold (Walky Talky Case)</v>
       </c>
       <c r="D32" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E32" t="str">
@@ -47129,7 +47129,7 @@
         <v>Mold (HAM Radio Case)</v>
       </c>
       <c r="D33" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E33" t="str">
@@ -47153,7 +47153,7 @@
         <v>Mold (Air Quality Detector Case)</v>
       </c>
       <c r="D34" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$87</f>
+        <f xml:space="preserve"> [1]Enums!$B$88</f>
         <v>Mold</v>
       </c>
       <c r="E34" t="str">
@@ -47176,8 +47176,8 @@
   </sheetPr>
   <dimension ref="A1:U156"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+    <sheetView showZeros="0" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -53567,7 +53567,7 @@
         <v>2518</v>
       </c>
       <c r="D1" s="53" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$83</f>
+        <f xml:space="preserve"> [1]Enums!$B$84</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="20" t="s">
@@ -53601,7 +53601,7 @@
         <v>Wafer (Solar Cell)</v>
       </c>
       <c r="D2" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$95</f>
+        <f xml:space="preserve"> [1]Enums!$B$96</f>
         <v>Wafer</v>
       </c>
       <c r="E2" s="49" t="s">
@@ -53628,7 +53628,7 @@
         <v>Wafer (Processor)</v>
       </c>
       <c r="D3" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$95</f>
+        <f xml:space="preserve"> [1]Enums!$B$96</f>
         <v>Wafer</v>
       </c>
       <c r="E3" s="49" t="s">
@@ -53655,7 +53655,7 @@
         <v>Wafer (Temperature Sensor)</v>
       </c>
       <c r="D4" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$95</f>
+        <f xml:space="preserve"> [1]Enums!$B$96</f>
         <v>Wafer</v>
       </c>
       <c r="E4" s="49" t="s">
@@ -53682,7 +53682,7 @@
         <v>Wafer (Pressure Sensor)</v>
       </c>
       <c r="D5" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$95</f>
+        <f xml:space="preserve"> [1]Enums!$B$96</f>
         <v>Wafer</v>
       </c>
       <c r="E5" s="49" t="s">
@@ -53709,7 +53709,7 @@
         <v>Wafer (Low Power Radio)</v>
       </c>
       <c r="D6" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$95</f>
+        <f xml:space="preserve"> [1]Enums!$B$96</f>
         <v>Wafer</v>
       </c>
       <c r="E6" s="49" t="s">
@@ -53736,7 +53736,7 @@
         <v>Wafer (DSP)</v>
       </c>
       <c r="D7" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$95</f>
+        <f xml:space="preserve"> [1]Enums!$B$96</f>
         <v>Wafer</v>
       </c>
       <c r="E7" s="49" t="s">
@@ -53763,7 +53763,7 @@
         <v>Wafer (Digital Analog Convertor)</v>
       </c>
       <c r="D8" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$95</f>
+        <f xml:space="preserve"> [1]Enums!$B$96</f>
         <v>Wafer</v>
       </c>
       <c r="E8" s="49" t="s">
@@ -53790,7 +53790,7 @@
         <v>Wafer (Amplifier)</v>
       </c>
       <c r="D9" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$95</f>
+        <f xml:space="preserve"> [1]Enums!$B$96</f>
         <v>Wafer</v>
       </c>
       <c r="E9" s="49" t="s">
@@ -53817,7 +53817,7 @@
         <v>Wafer (OLED Array)</v>
       </c>
       <c r="D10" s="50" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$95</f>
+        <f xml:space="preserve"> [1]Enums!$B$96</f>
         <v>Wafer</v>
       </c>
       <c r="E10" s="49" t="s">

</xml_diff>

<commit_message>
Update to 1.3.8 Added BioTechnology into the game; removed phase shifter, removed magic pogo stick; limited entity spawns
</commit_message>
<xml_diff>
--- a/config/Polycraft Polymers.xlsx
+++ b/config/Polycraft Polymers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="826" activeTab="2"/>
+    <workbookView xWindow="13950" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="826" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pellets" sheetId="1" r:id="rId1"/>
@@ -8485,118 +8485,118 @@
             <v>1.3.5</v>
           </cell>
         </row>
-        <row r="35">
-          <cell r="A35" t="str">
+        <row r="36">
+          <cell r="A36" t="str">
             <v>Bag</v>
           </cell>
         </row>
-        <row r="36">
-          <cell r="A36" t="str">
+        <row r="37">
+          <cell r="A37" t="str">
             <v>Vial</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38" t="str">
-            <v>Sack</v>
           </cell>
         </row>
         <row r="39">
           <cell r="A39" t="str">
-            <v>Beaker</v>
+            <v>Sack</v>
           </cell>
         </row>
-        <row r="41">
-          <cell r="A41" t="str">
-            <v>Powder Keg</v>
+        <row r="40">
+          <cell r="A40" t="str">
+            <v>Beaker</v>
           </cell>
         </row>
         <row r="42">
           <cell r="A42" t="str">
-            <v>Drum</v>
+            <v>Powder Keg</v>
           </cell>
         </row>
-        <row r="44">
-          <cell r="A44" t="str">
-            <v>Chemical Silo</v>
+        <row r="43">
+          <cell r="A43" t="str">
+            <v>Drum</v>
           </cell>
         </row>
         <row r="45">
           <cell r="A45" t="str">
+            <v>Chemical Silo</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46" t="str">
             <v>Chemical Vat</v>
           </cell>
         </row>
-        <row r="84">
-          <cell r="B84" t="str">
+        <row r="85">
+          <cell r="B85" t="str">
             <v>Mold Type</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="B88" t="str">
-            <v>Mold</v>
           </cell>
         </row>
         <row r="89">
           <cell r="B89" t="str">
-            <v>Metal Die</v>
+            <v>Mold</v>
           </cell>
         </row>
-        <row r="96">
-          <cell r="B96" t="str">
-            <v>Wafer</v>
+        <row r="90">
+          <cell r="B90" t="str">
+            <v>Metal Die</v>
           </cell>
         </row>
         <row r="97">
           <cell r="B97" t="str">
+            <v>Wafer</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="B98" t="str">
             <v>Mask</v>
           </cell>
         </row>
-        <row r="112">
-          <cell r="A112" t="str">
+        <row r="113">
+          <cell r="A113" t="str">
             <v>Gripped</v>
-          </cell>
-        </row>
-        <row r="115">
-          <cell r="A115" t="str">
-            <v>Base Material</v>
           </cell>
         </row>
         <row r="116">
           <cell r="A116" t="str">
-            <v>Wooden</v>
+            <v>Base Material</v>
           </cell>
         </row>
         <row r="117">
           <cell r="A117" t="str">
-            <v>Stone</v>
+            <v>Wooden</v>
           </cell>
         </row>
         <row r="118">
           <cell r="A118" t="str">
-            <v>Iron</v>
+            <v>Stone</v>
           </cell>
         </row>
         <row r="119">
           <cell r="A119" t="str">
-            <v>Golden</v>
+            <v>Iron</v>
           </cell>
         </row>
         <row r="120">
           <cell r="A120" t="str">
-            <v>Diamond</v>
+            <v>Golden</v>
           </cell>
         </row>
         <row r="121">
           <cell r="A121" t="str">
-            <v>Magic</v>
+            <v>Diamond</v>
           </cell>
         </row>
-        <row r="150">
-          <cell r="A150" t="str">
-            <v>Composite</v>
+        <row r="122">
+          <cell r="A122" t="str">
+            <v>Magic</v>
           </cell>
         </row>
         <row r="151">
           <cell r="A151" t="str">
+            <v>Composite</v>
+          </cell>
+        </row>
+        <row r="152">
+          <cell r="A152" t="str">
             <v>Engineered</v>
           </cell>
         </row>
@@ -10248,6 +10248,8 @@
       <sheetName val="Ingots"/>
       <sheetName val="Nuggets"/>
       <sheetName val="Compressed Blocks"/>
+      <sheetName val="DNA Sampler"/>
+      <sheetName val="Cell Culture"/>
       <sheetName val="Catalysts"/>
       <sheetName val="Element Vessels"/>
       <sheetName val="Compound Vessels"/>
@@ -10551,6 +10553,8 @@
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -10867,19 +10871,19 @@
         <v>Game ID XL</v>
       </c>
       <c r="F1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$35&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$36&amp;" ("&amp;J1&amp;")"</f>
         <v>Bag (Pellets)</v>
       </c>
       <c r="G1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$38&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$39&amp;" ("&amp;J1&amp;")"</f>
         <v>Sack (Pellets)</v>
       </c>
       <c r="H1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$41&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$42&amp;" ("&amp;J1&amp;")"</f>
         <v>Powder Keg (Pellets)</v>
       </c>
       <c r="I1" s="5" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$44&amp;" ("&amp;J1&amp;")"</f>
+        <f xml:space="preserve"> [1]Enums!$A$45&amp;" ("&amp;J1&amp;")"</f>
         <v>Chemical Silo (Pellets)</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -10918,19 +10922,19 @@
         <v>448</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="G2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="H2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f>IF($N2, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N2, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J2&amp;IF($N2, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Acrylic-Formaldehyde Resin)</v>
       </c>
       <c r="J2" s="1" t="str">
@@ -10970,19 +10974,19 @@
         <v>444</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f>IF($N3, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N3, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J3&amp;IF($N3, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Acrylonitrile-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J3" s="1" t="str">
@@ -11019,19 +11023,19 @@
         <v>440</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Alkyd Resin)</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Alkyd Resin)</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Alkyd Resin)</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>IF($N4, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N4, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J4&amp;IF($N4, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Alkyd Resin)</v>
       </c>
       <c r="J4" s="1" t="str">
@@ -11071,19 +11075,19 @@
         <v>436</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f>IF($N5, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N5, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J5&amp;IF($N5, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Amorphous PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J5" s="1" t="str">
@@ -11123,19 +11127,19 @@
         <v>432</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f>IF($N6, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N6, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J6&amp;IF($N6, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Bromine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J6" s="1" t="str">
@@ -11175,19 +11179,19 @@
         <v>428</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$35, [1]Enums!$A$35)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$36, [1]Enums!$A$36)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Carbon Fiber)</v>
       </c>
       <c r="G7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$38, [1]Enums!$A$38)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$39, [1]Enums!$A$39)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Carbon Fiber)</v>
       </c>
       <c r="H7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$41, [1]Enums!$A$41)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$42, [1]Enums!$A$42)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Carbon Fiber)</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f>IF($N7, [1]Enums!$A$44, [1]Enums!$A$44)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N7, [1]Enums!$A$45, [1]Enums!$A$45)&amp;" ("&amp;$J7&amp;IF($N7, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Carbon Fiber)</v>
       </c>
       <c r="J7" s="1" t="str">
@@ -11224,19 +11228,19 @@
         <v>424</v>
       </c>
       <c r="F8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="G8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f>IF($N8, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N8, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J8&amp;IF($N8, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulose Triacetate Pellets)</v>
       </c>
       <c r="J8" s="1" t="str">
@@ -11276,19 +11280,19 @@
         <v>420</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Cellulosic Pellets)</v>
       </c>
       <c r="G9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Cellulosic Pellets)</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Cellulosic Pellets)</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f>IF($N9, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N9, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J9&amp;IF($N9, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Cellulosic Pellets)</v>
       </c>
       <c r="J9" s="1" t="str">
@@ -11328,19 +11332,19 @@
         <v>416</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chitin Pellets)</v>
       </c>
       <c r="G10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chitin Pellets)</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chitin Pellets)</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f>IF($N10, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N10, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J10&amp;IF($N10, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chitin Pellets)</v>
       </c>
       <c r="J10" s="1" t="str">
@@ -11380,19 +11384,19 @@
         <v>412</v>
       </c>
       <c r="F11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f>IF($N11, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N11, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J11&amp;IF($N11, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Chlorine Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J11" s="1" t="str">
@@ -11432,19 +11436,19 @@
         <v>408</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Epoxy Resin)</v>
       </c>
       <c r="G12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Epoxy Resin)</v>
       </c>
       <c r="H12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Epoxy Resin)</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f>IF($N12, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N12, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J12&amp;IF($N12, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Epoxy Resin)</v>
       </c>
       <c r="J12" s="1" t="str">
@@ -11481,19 +11485,19 @@
         <v>404</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethoxylates Pellets)</v>
       </c>
       <c r="G13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethoxylates Pellets)</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethoxylates Pellets)</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f>IF($N13, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N13, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J13&amp;IF($N13, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethoxylates Pellets)</v>
       </c>
       <c r="J13" s="1" t="str">
@@ -11533,19 +11537,19 @@
         <v>400</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="G14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="H14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f>IF($N14, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N14, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J14&amp;IF($N14, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene Monomer Pellets)</v>
       </c>
       <c r="J14" s="1" t="str">
@@ -11585,19 +11589,19 @@
         <v>396</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="G15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f>IF($N15, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N15, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J15&amp;IF($N15, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Propylene-Diene Monomer Pellets)</v>
       </c>
       <c r="J15" s="1" t="str">
@@ -11637,19 +11641,19 @@
         <v>392</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="G16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f>IF($N16, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N16, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J16&amp;IF($N16, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ethylene-Vinyl Acetate Pellets)</v>
       </c>
       <c r="J16" s="1" t="str">
@@ -11689,19 +11693,19 @@
         <v>388</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="G17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f>IF($N17, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N17, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J17&amp;IF($N17, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (High Density PolyEthylene Pellets)</v>
       </c>
       <c r="J17" s="1" t="str">
@@ -11741,19 +11745,19 @@
         <v>384</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f>IF($N18, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N18, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J18&amp;IF($N18, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Hydrogenated Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J18" s="1" t="str">
@@ -11793,19 +11797,19 @@
         <v>380</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="G19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="H19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f>IF($N19, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N19, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J19&amp;IF($N19, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Isobutylene-Isoprene Rubber Pellets)</v>
       </c>
       <c r="J19" s="1" t="str">
@@ -11842,19 +11846,19 @@
         <v>376</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Lignin)</v>
       </c>
       <c r="G20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Lignin)</v>
       </c>
       <c r="H20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Lignin)</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f>IF($N20, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N20, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J20&amp;IF($N20, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Lignin)</v>
       </c>
       <c r="J20" s="1" t="str">
@@ -11894,19 +11898,19 @@
         <v>372</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f>IF($N21, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N21, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J21&amp;IF($N21, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Linear Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J21" s="1" t="str">
@@ -11946,19 +11950,19 @@
         <v>368</v>
       </c>
       <c r="F22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="G22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="H22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f>IF($N22, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N22, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J22&amp;IF($N22, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Liquid Crystal Polymer Pellets)</v>
       </c>
       <c r="J22" s="1" t="str">
@@ -11998,19 +12002,19 @@
         <v>364</v>
       </c>
       <c r="F23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="G23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="H23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f>IF($N23, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N23, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J23&amp;IF($N23, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Low Density PolyEthylene Pellets)</v>
       </c>
       <c r="J23" s="1" t="str">
@@ -12050,19 +12054,19 @@
         <v>360</v>
       </c>
       <c r="F24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="G24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="H24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f>IF($N24, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N24, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J24&amp;IF($N24, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Medium Density PolyEthylene Pellets)</v>
       </c>
       <c r="J24" s="1" t="str">
@@ -12099,19 +12103,19 @@
         <v>356</v>
       </c>
       <c r="F25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="G25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="H25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f>IF($N25, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N25, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J25&amp;IF($N25, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Melamine-Formaldehyde Polymers)</v>
       </c>
       <c r="J25" s="1" t="str">
@@ -12151,19 +12155,19 @@
         <v>352</v>
       </c>
       <c r="F26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Metaldehyde Pellets)</v>
       </c>
       <c r="G26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Metaldehyde Pellets)</v>
       </c>
       <c r="H26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Metaldehyde Pellets)</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f>IF($N26, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N26, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J26&amp;IF($N26, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Metaldehyde Pellets)</v>
       </c>
       <c r="J26" s="1" t="str">
@@ -12203,19 +12207,19 @@
         <v>348</v>
       </c>
       <c r="F27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I27" s="1" t="str">
-        <f>IF($N27, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N27, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J27&amp;IF($N27, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Nitrile-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J27" s="1" t="str">
@@ -12255,19 +12259,19 @@
         <v>344</v>
       </c>
       <c r="F28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraformaldehyde Pellets)</v>
       </c>
       <c r="G28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraformaldehyde Pellets)</v>
       </c>
       <c r="H28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraformaldehyde Pellets)</v>
       </c>
       <c r="I28" s="1" t="str">
-        <f>IF($N28, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N28, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J28&amp;IF($N28, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraformaldehyde Pellets)</v>
       </c>
       <c r="J28" s="1" t="str">
@@ -12307,19 +12311,19 @@
         <v>340</v>
       </c>
       <c r="F29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Paraldehyde Pellets)</v>
       </c>
       <c r="G29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Paraldehyde Pellets)</v>
       </c>
       <c r="H29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Paraldehyde Pellets)</v>
       </c>
       <c r="I29" s="1" t="str">
-        <f>IF($N29, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N29, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J29&amp;IF($N29, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Paraldehyde Pellets)</v>
       </c>
       <c r="J29" s="1" t="str">
@@ -12359,19 +12363,19 @@
         <v>336</v>
       </c>
       <c r="F30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Phenolic Resin)</v>
       </c>
       <c r="G30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Phenolic Resin)</v>
       </c>
       <c r="H30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Phenolic Resin)</v>
       </c>
       <c r="I30" s="1" t="str">
-        <f>IF($N30, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N30, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J30&amp;IF($N30, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Phenolic Resin)</v>
       </c>
       <c r="J30" s="1" t="str">
@@ -12411,19 +12415,19 @@
         <v>332</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="G31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="H31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="I31" s="1" t="str">
-        <f>IF($N31, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N31, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J31&amp;IF($N31, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly(3-Hydroxybutyrate-Co-3-Hydroxyvalerate) Pellets)</v>
       </c>
       <c r="J31" s="1" t="str">
@@ -12463,19 +12467,19 @@
         <v>328</v>
       </c>
       <c r="F32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly1-Butene Pellets)</v>
       </c>
       <c r="G32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly1-Butene Pellets)</v>
       </c>
       <c r="H32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly1-Butene Pellets)</v>
       </c>
       <c r="I32" s="1" t="str">
-        <f>IF($N32, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N32, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J32&amp;IF($N32, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly1-Butene Pellets)</v>
       </c>
       <c r="J32" s="1" t="str">
@@ -12515,19 +12519,19 @@
         <v>324</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="G33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="H33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="I33" s="1" t="str">
-        <f>IF($N33, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N33, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J33&amp;IF($N33, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2-6-Dimethyl-1-4-Phenylene Ether Pellets)</v>
       </c>
       <c r="J33" s="1" t="str">
@@ -12567,19 +12571,19 @@
         <v>320</v>
       </c>
       <c r="F34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="G34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="H34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="I34" s="1" t="str">
-        <f>IF($N34, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N34, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J34&amp;IF($N34, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly-2-Hydroxy Butyrate Pellets)</v>
       </c>
       <c r="J34" s="1" t="str">
@@ -12619,19 +12623,19 @@
         <v>316</v>
       </c>
       <c r="F35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="G35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="H35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="I35" s="1" t="str">
-        <f>IF($N35, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N35, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J35&amp;IF($N35, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Poly2-Hydroxyethyl Methacrylate Pellets)</v>
       </c>
       <c r="J35" s="1" t="str">
@@ -12671,19 +12675,19 @@
         <v>312</v>
       </c>
       <c r="F36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="G36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="H36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="I36" s="1" t="str">
-        <f>IF($N36, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N36, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J36&amp;IF($N36, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylic Acid Pellets)</v>
       </c>
       <c r="J36" s="1" t="str">
@@ -12723,19 +12727,19 @@
         <v>308</v>
       </c>
       <c r="F37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="G37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="H37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="I37" s="1" t="str">
-        <f>IF($N37, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N37, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J37&amp;IF($N37, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyAcrylonitrile Pellets)</v>
       </c>
       <c r="J37" s="1" t="str">
@@ -12775,19 +12779,19 @@
         <v>304</v>
       </c>
       <c r="F38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="G38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="H38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="I38" s="1" t="str">
-        <f>IF($N38, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N38, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J38&amp;IF($N38, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (low-cis) Pellets)</v>
       </c>
       <c r="J38" s="1" t="str">
@@ -12827,19 +12831,19 @@
         <v>300</v>
       </c>
       <c r="F39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="G39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="H39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="I39" s="1" t="str">
-        <f>IF($N39, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N39, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J39&amp;IF($N39, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButadiene (high-cis) Pellets)</v>
       </c>
       <c r="J39" s="1" t="str">
@@ -12879,19 +12883,19 @@
         <v>296</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="G40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="H40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="I40" s="1" t="str">
-        <f>IF($N40, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N40, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J40&amp;IF($N40, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Succinate Pellets)</v>
       </c>
       <c r="J40" s="1" t="str">
@@ -12931,19 +12935,19 @@
         <v>292</v>
       </c>
       <c r="F41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="G41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="H41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="I41" s="1" t="str">
-        <f>IF($N41, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N41, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J41&amp;IF($N41, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyButylene Terephthalate Pellets)</v>
       </c>
       <c r="J41" s="1" t="str">
@@ -12983,19 +12987,19 @@
         <v>288</v>
       </c>
       <c r="F42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCaprolactone Pellets)</v>
       </c>
       <c r="G42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCaprolactone Pellets)</v>
       </c>
       <c r="H42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCaprolactone Pellets)</v>
       </c>
       <c r="I42" s="1" t="str">
-        <f>IF($N42, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N42, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J42&amp;IF($N42, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCaprolactone Pellets)</v>
       </c>
       <c r="J42" s="1" t="str">
@@ -13035,19 +13039,19 @@
         <v>284</v>
       </c>
       <c r="F43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyCarbonate Pellets)</v>
       </c>
       <c r="G43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyCarbonate Pellets)</v>
       </c>
       <c r="H43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyCarbonate Pellets)</v>
       </c>
       <c r="I43" s="1" t="str">
-        <f>IF($N43, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N43, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J43&amp;IF($N43, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyCarbonate Pellets)</v>
       </c>
       <c r="J43" s="1" t="str">
@@ -13087,19 +13091,19 @@
         <v>280</v>
       </c>
       <c r="F44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChloroPrene Pellets)</v>
       </c>
       <c r="G44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChloroPrene Pellets)</v>
       </c>
       <c r="H44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChloroPrene Pellets)</v>
       </c>
       <c r="I44" s="1" t="str">
-        <f>IF($N44, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N44, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J44&amp;IF($N44, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChloroPrene Pellets)</v>
       </c>
       <c r="J44" s="1" t="str">
@@ -13136,19 +13140,19 @@
         <v>276</v>
       </c>
       <c r="F45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="G45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="H45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="I45" s="1" t="str">
-        <f>IF($N45, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N45, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J45&amp;IF($N45, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyChlorotrifluoroethylene Pellets)</v>
       </c>
       <c r="J45" s="1" t="str">
@@ -13188,19 +13192,19 @@
         <v>272</v>
       </c>
       <c r="F46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="G46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="H46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="I46" s="1" t="str">
-        <f>IF($N46, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N46, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J46&amp;IF($N46, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyDiMethylSiloxane Pellets)</v>
       </c>
       <c r="J46" s="1" t="str">
@@ -13240,19 +13244,19 @@
         <v>268</v>
       </c>
       <c r="F47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="G47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="H47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="I47" s="1" t="str">
-        <f>IF($N47, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N47, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J47&amp;IF($N47, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEther Ether Ketone Pellets)</v>
       </c>
       <c r="J47" s="1" t="str">
@@ -13292,19 +13296,19 @@
         <v>264</v>
       </c>
       <c r="F48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEtherImide Pellets)</v>
       </c>
       <c r="G48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEtherImide Pellets)</v>
       </c>
       <c r="H48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEtherImide Pellets)</v>
       </c>
       <c r="I48" s="1" t="str">
-        <f>IF($N48, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N48, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J48&amp;IF($N48, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEtherImide Pellets)</v>
       </c>
       <c r="J48" s="1" t="str">
@@ -13341,19 +13345,19 @@
         <v>260</v>
       </c>
       <c r="F49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="G49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="H49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="I49" s="1" t="str">
-        <f>IF($N49, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N49, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J49&amp;IF($N49, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthyl Acrylate Pellets)</v>
       </c>
       <c r="J49" s="1" t="str">
@@ -13390,19 +13394,19 @@
         <v>256</v>
       </c>
       <c r="F50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="G50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="H50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="I50" s="1" t="str">
-        <f>IF($N50, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N50, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J50&amp;IF($N50, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Adipate Pellets)</v>
       </c>
       <c r="J50" s="1" t="str">
@@ -13442,19 +13446,19 @@
         <v>252</v>
       </c>
       <c r="F51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="G51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="H51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="I51" s="1" t="str">
-        <f>IF($N51, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N51, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J51&amp;IF($N51, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Glycol Pellets)</v>
       </c>
       <c r="J51" s="1" t="str">
@@ -13491,19 +13495,19 @@
         <v>248</v>
       </c>
       <c r="F52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I52" s="1" t="str">
-        <f>IF($N52, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N52, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J52&amp;IF($N52, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J52" s="1" t="str">
@@ -13543,19 +13547,19 @@
         <v>244</v>
       </c>
       <c r="F53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="G53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="H53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="I53" s="1" t="str">
-        <f>IF($N53, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N53, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J53&amp;IF($N53, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Naphthalate Pellets)</v>
       </c>
       <c r="J53" s="1" t="str">
@@ -13595,19 +13599,19 @@
         <v>240</v>
       </c>
       <c r="F54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="G54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="H54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="I54" s="1" t="str">
-        <f>IF($N54, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N54, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J54&amp;IF($N54, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Oxide Pellets)</v>
       </c>
       <c r="J54" s="1" t="str">
@@ -13647,19 +13651,19 @@
         <v>236</v>
       </c>
       <c r="F55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="G55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="H55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="I55" s="1" t="str">
-        <f>IF($N55, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N55, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J55&amp;IF($N55, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Sulphide Pellets)</v>
       </c>
       <c r="J55" s="1" t="str">
@@ -13699,19 +13703,19 @@
         <v>232</v>
       </c>
       <c r="F56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="G56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="H56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="I56" s="1" t="str">
-        <f>IF($N56, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N56, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J56&amp;IF($N56, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Pellets)</v>
       </c>
       <c r="J56" s="1" t="str">
@@ -13751,19 +13755,19 @@
         <v>228</v>
       </c>
       <c r="F57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="G57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="H57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="I57" s="1" t="str">
-        <f>IF($N57, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N57, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J57&amp;IF($N57, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyEthylene Terephthalate Glycol-Modified Pellets)</v>
       </c>
       <c r="J57" s="1" t="str">
@@ -13803,19 +13807,19 @@
         <v>224</v>
       </c>
       <c r="F58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="G58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="H58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="I58" s="1" t="str">
-        <f>IF($N58, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N58, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J58&amp;IF($N58, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyGlycolic Acid Pellets)</v>
       </c>
       <c r="J58" s="1" t="str">
@@ -13855,19 +13859,19 @@
         <v>220</v>
       </c>
       <c r="F59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="G59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="H59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="I59" s="1" t="str">
-        <f>IF($N59, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N59, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J59&amp;IF($N59, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Adipamide Pellets)</v>
       </c>
       <c r="J59" s="1" t="str">
@@ -13907,19 +13911,19 @@
         <v>216</v>
       </c>
       <c r="F60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="G60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="H60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="I60" s="1" t="str">
-        <f>IF($N60, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N60, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J60&amp;IF($N60, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHexamethylene Sebacamide Pellets)</v>
       </c>
       <c r="J60" s="1" t="str">
@@ -13959,19 +13963,19 @@
         <v>212</v>
       </c>
       <c r="F61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="G61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="H61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="I61" s="1" t="str">
-        <f>IF($N61, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N61, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J61&amp;IF($N61, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxyalkanoate Pellets)</v>
       </c>
       <c r="J61" s="1" t="str">
@@ -14008,19 +14012,19 @@
         <v>208</v>
       </c>
       <c r="F62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="G62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="H62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="I62" s="1" t="str">
-        <f>IF($N62, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N62, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J62&amp;IF($N62, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyHydroxybutyrate-Co-Hydroxyvalerate Pellets)</v>
       </c>
       <c r="J62" s="1" t="str">
@@ -14060,19 +14064,19 @@
         <v>204</v>
       </c>
       <c r="F63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyImide Pellets)</v>
       </c>
       <c r="G63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyImide Pellets)</v>
       </c>
       <c r="H63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyImide Pellets)</v>
       </c>
       <c r="I63" s="1" t="str">
-        <f>IF($N63, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N63, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J63&amp;IF($N63, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyImide Pellets)</v>
       </c>
       <c r="J63" s="1" t="str">
@@ -14109,19 +14113,19 @@
         <v>200</v>
       </c>
       <c r="F64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="G64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="H64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="I64" s="1" t="str">
-        <f>IF($N64, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N64, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J64&amp;IF($N64, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoBorynl Acrylate Pellets)</v>
       </c>
       <c r="J64" s="1" t="str">
@@ -14158,19 +14162,19 @@
         <v>196</v>
       </c>
       <c r="F65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="G65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="H65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="I65" s="1" t="str">
-        <f>IF($N65, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N65, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J65&amp;IF($N65, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButyl Acrylate Pellets)</v>
       </c>
       <c r="J65" s="1" t="str">
@@ -14210,19 +14214,19 @@
         <v>192</v>
       </c>
       <c r="F66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoButylene Pellets)</v>
       </c>
       <c r="G66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoButylene Pellets)</v>
       </c>
       <c r="H66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoButylene Pellets)</v>
       </c>
       <c r="I66" s="1" t="str">
-        <f>IF($N66, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N66, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J66&amp;IF($N66, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoButylene Pellets)</v>
       </c>
       <c r="J66" s="1" t="str">
@@ -14262,19 +14266,19 @@
         <v>188</v>
       </c>
       <c r="F67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyIsoPrene Pellets)</v>
       </c>
       <c r="G67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyIsoPrene Pellets)</v>
       </c>
       <c r="H67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyIsoPrene Pellets)</v>
       </c>
       <c r="I67" s="1" t="str">
-        <f>IF($N67, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N67, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J67&amp;IF($N67, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyIsoPrene Pellets)</v>
       </c>
       <c r="J67" s="1" t="str">
@@ -14314,19 +14318,19 @@
         <v>184</v>
       </c>
       <c r="F68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic Acid Pellets)</v>
       </c>
       <c r="G68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic Acid Pellets)</v>
       </c>
       <c r="H68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic Acid Pellets)</v>
       </c>
       <c r="I68" s="1" t="str">
-        <f>IF($N68, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N68, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J68&amp;IF($N68, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic Acid Pellets)</v>
       </c>
       <c r="J68" s="1" t="str">
@@ -14363,19 +14367,19 @@
         <v>180</v>
       </c>
       <c r="F69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="G69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="H69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="I69" s="1" t="str">
-        <f>IF($N69, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N69, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J69&amp;IF($N69, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyLactic-Co-Glycolic Acid Pellets)</v>
       </c>
       <c r="J69" s="1" t="str">
@@ -14415,19 +14419,19 @@
         <v>176</v>
       </c>
       <c r="F70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="G70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="H70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="I70" s="1" t="str">
-        <f>IF($N70, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N70, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J70&amp;IF($N70, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Acrylate Pellets)</v>
       </c>
       <c r="J70" s="1" t="str">
@@ -14464,19 +14468,19 @@
         <v>172</v>
       </c>
       <c r="F71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="G71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="H71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="I71" s="1" t="str">
-        <f>IF($N71, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N71, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J71&amp;IF($N71, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Cyanoacrylate Pellets)</v>
       </c>
       <c r="J71" s="1" t="str">
@@ -14516,19 +14520,19 @@
         <v>168</v>
       </c>
       <c r="F72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="G72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="H72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="I72" s="1" t="str">
-        <f>IF($N72, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N72, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J72&amp;IF($N72, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyMethyl Methacrylate Pellets)</v>
       </c>
       <c r="J72" s="1" t="str">
@@ -14568,19 +14572,19 @@
         <v>164</v>
       </c>
       <c r="F73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="G73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="H73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="I73" s="1" t="str">
-        <f>IF($N73, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N73, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J73&amp;IF($N73, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Methyl Styrene Pellets)</v>
       </c>
       <c r="J73" s="1" t="str">
@@ -14620,19 +14624,19 @@
         <v>160</v>
       </c>
       <c r="F74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="G74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="H74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="I74" s="1" t="str">
-        <f>IF($N74, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N74, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J74&amp;IF($N74, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyM-Phenylene Isophthalamide Pellets)</v>
       </c>
       <c r="J74" s="1" t="str">
@@ -14669,19 +14673,19 @@
         <v>156</v>
       </c>
       <c r="F75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I75" s="1" t="str">
-        <f>IF($N75, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N75, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J75&amp;IF($N75, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyN-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J75" s="1" t="str">
@@ -14721,19 +14725,19 @@
         <v>152</v>
       </c>
       <c r="F76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyOxymethylene Pellets)</v>
       </c>
       <c r="G76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyOxymethylene Pellets)</v>
       </c>
       <c r="H76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyOxymethylene Pellets)</v>
       </c>
       <c r="I76" s="1" t="str">
-        <f>IF($N76, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N76, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J76&amp;IF($N76, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyOxymethylene Pellets)</v>
       </c>
       <c r="J76" s="1" t="str">
@@ -14770,19 +14774,19 @@
         <v>148</v>
       </c>
       <c r="F77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="G77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="H77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="I77" s="1" t="str">
-        <f>IF($N77, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N77, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J77&amp;IF($N77, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPentamethylene Hexamethylene Dicarbamate Pellets)</v>
       </c>
       <c r="J77" s="1" t="str">
@@ -14822,19 +14826,19 @@
         <v>144</v>
       </c>
       <c r="F78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenol Pellets)</v>
       </c>
       <c r="G78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenol Pellets)</v>
       </c>
       <c r="H78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenol Pellets)</v>
       </c>
       <c r="I78" s="1" t="str">
-        <f>IF($N78, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N78, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J78&amp;IF($N78, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenol Pellets)</v>
       </c>
       <c r="J78" s="1" t="str">
@@ -14871,19 +14875,19 @@
         <v>140</v>
       </c>
       <c r="F79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="G79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="H79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="I79" s="1" t="str">
-        <f>IF($N79, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N79, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J79&amp;IF($N79, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhenylene Oxide Pellets)</v>
       </c>
       <c r="J79" s="1" t="str">
@@ -14920,19 +14924,19 @@
         <v>136</v>
       </c>
       <c r="F80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPhosphazene Pellets)</v>
       </c>
       <c r="G80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPhosphazene Pellets)</v>
       </c>
       <c r="H80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPhosphazene Pellets)</v>
       </c>
       <c r="I80" s="1" t="str">
-        <f>IF($N80, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N80, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J80&amp;IF($N80, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPhosphazene Pellets)</v>
       </c>
       <c r="J80" s="1" t="str">
@@ -14969,19 +14973,19 @@
         <v>132</v>
       </c>
       <c r="F81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="G81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="H81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="I81" s="1" t="str">
-        <f>IF($N81, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N81, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J81&amp;IF($N81, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Methyl Styrene Pellets)</v>
       </c>
       <c r="J81" s="1" t="str">
@@ -15018,19 +15022,19 @@
         <v>128</v>
       </c>
       <c r="F82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="G82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="H82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="I82" s="1" t="str">
-        <f>IF($N82, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N82, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J82&amp;IF($N82, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Sulphide Pellets)</v>
       </c>
       <c r="J82" s="1" t="str">
@@ -15070,19 +15074,19 @@
         <v>124</v>
       </c>
       <c r="F83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="G83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="H83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="I83" s="1" t="str">
-        <f>IF($N83, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N83, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J83&amp;IF($N83, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyP-Phenylene Terephthalamide Pellets)</v>
       </c>
       <c r="J83" s="1" t="str">
@@ -15122,19 +15126,19 @@
         <v>120</v>
       </c>
       <c r="F84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Pellets)</v>
       </c>
       <c r="G84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Pellets)</v>
       </c>
       <c r="H84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Pellets)</v>
       </c>
       <c r="I84" s="1" t="str">
-        <f>IF($N84, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N84, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J84&amp;IF($N84, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Pellets)</v>
       </c>
       <c r="J84" s="1" t="str">
@@ -15171,19 +15175,19 @@
         <v>116</v>
       </c>
       <c r="F85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="G85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="H85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="I85" s="1" t="str">
-        <f>IF($N85, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N85, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J85&amp;IF($N85, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Glycol Pellets)</v>
       </c>
       <c r="J85" s="1" t="str">
@@ -15220,19 +15224,19 @@
         <v>112</v>
       </c>
       <c r="F86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="G86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="H86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="I86" s="1" t="str">
-        <f>IF($N86, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N86, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J86&amp;IF($N86, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyPropylene Oxide Pellets)</v>
       </c>
       <c r="J86" s="1" t="str">
@@ -15272,19 +15276,19 @@
         <v>108</v>
       </c>
       <c r="F87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyStyrene Pellets)</v>
       </c>
       <c r="G87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyStyrene Pellets)</v>
       </c>
       <c r="H87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyStyrene Pellets)</v>
       </c>
       <c r="I87" s="1" t="str">
-        <f>IF($N87, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N87, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J87&amp;IF($N87, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyStyrene Pellets)</v>
       </c>
       <c r="J87" s="1" t="str">
@@ -15321,19 +15325,19 @@
         <v>104</v>
       </c>
       <c r="F88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="G88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="H88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="I88" s="1" t="str">
-        <f>IF($N88, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N88, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J88&amp;IF($N88, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTert-Butyl Acrylate Pellets)</v>
       </c>
       <c r="J88" s="1" t="str">
@@ -15373,19 +15377,19 @@
         <v>100</v>
       </c>
       <c r="F89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="G89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="H89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="I89" s="1" t="str">
-        <f>IF($N89, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N89, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J89&amp;IF($N89, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetraFluoroEthylene Pellets)</v>
       </c>
       <c r="J89" s="1" t="str">
@@ -15422,19 +15426,19 @@
         <v>96</v>
       </c>
       <c r="F90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="G90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="H90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="I90" s="1" t="str">
-        <f>IF($N90, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N90, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J90&amp;IF($N90, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Ether Glycol Pellets)</v>
       </c>
       <c r="J90" s="1" t="str">
@@ -15471,19 +15475,19 @@
         <v>92</v>
       </c>
       <c r="F91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="G91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="H91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="I91" s="1" t="str">
-        <f>IF($N91, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N91, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J91&amp;IF($N91, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTetramethylene Glycol Pellets)</v>
       </c>
       <c r="J91" s="1" t="str">
@@ -15520,19 +15524,19 @@
         <v>88</v>
       </c>
       <c r="F92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyThiazyl Pellets)</v>
       </c>
       <c r="G92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyThiazyl Pellets)</v>
       </c>
       <c r="H92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyThiazyl Pellets)</v>
       </c>
       <c r="I92" s="1" t="str">
-        <f>IF($N92, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N92, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J92&amp;IF($N92, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyThiazyl Pellets)</v>
       </c>
       <c r="J92" s="1" t="str">
@@ -15572,19 +15576,19 @@
         <v>84</v>
       </c>
       <c r="F93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="G93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="H93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="I93" s="1" t="str">
-        <f>IF($N93, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N93, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J93&amp;IF($N93, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyTrimethylene Terephthalate Pellets)</v>
       </c>
       <c r="J93" s="1" t="str">
@@ -15624,19 +15628,19 @@
         <v>80</v>
       </c>
       <c r="F94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyUrethane Pellets)</v>
       </c>
       <c r="G94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyUrethane Pellets)</v>
       </c>
       <c r="H94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyUrethane Pellets)</v>
       </c>
       <c r="I94" s="1" t="str">
-        <f>IF($N94, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N94, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J94&amp;IF($N94, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyUrethane Pellets)</v>
       </c>
       <c r="J94" s="1" t="str">
@@ -15676,19 +15680,19 @@
         <v>76</v>
       </c>
       <c r="F95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="G95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="H95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="I95" s="1" t="str">
-        <f>IF($N95, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N95, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J95&amp;IF($N95, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Acetate Pellets)</v>
       </c>
       <c r="J95" s="1" t="str">
@@ -15728,19 +15732,19 @@
         <v>72</v>
       </c>
       <c r="F96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="G96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="H96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="I96" s="1" t="str">
-        <f>IF($N96, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N96, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J96&amp;IF($N96, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Alcohol Pellets)</v>
       </c>
       <c r="J96" s="1" t="str">
@@ -15777,19 +15781,19 @@
         <v>68</v>
       </c>
       <c r="F97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="G97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="H97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="I97" s="1" t="str">
-        <f>IF($N97, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N97, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J97&amp;IF($N97, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Butyral Pellets)</v>
       </c>
       <c r="J97" s="1" t="str">
@@ -15829,19 +15833,19 @@
         <v>64</v>
       </c>
       <c r="F98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="G98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="H98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="I98" s="1" t="str">
-        <f>IF($N98, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N98, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J98&amp;IF($N98, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Pellets)</v>
       </c>
       <c r="J98" s="1" t="str">
@@ -15881,19 +15885,19 @@
         <v>60</v>
       </c>
       <c r="F99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="G99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="H99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="I99" s="1" t="str">
-        <f>IF($N99, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N99, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J99&amp;IF($N99, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Chloride Acetate Pellets)</v>
       </c>
       <c r="J99" s="1" t="str">
@@ -15930,19 +15934,19 @@
         <v>56</v>
       </c>
       <c r="F100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="G100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="H100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="I100" s="1" t="str">
-        <f>IF($N100, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N100, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J100&amp;IF($N100, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Fluoride Pellets)</v>
       </c>
       <c r="J100" s="1" t="str">
@@ -15979,19 +15983,19 @@
         <v>52</v>
       </c>
       <c r="F101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="G101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="H101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="I101" s="1" t="str">
-        <f>IF($N101, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N101, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J101&amp;IF($N101, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Formal Pellets)</v>
       </c>
       <c r="J101" s="1" t="str">
@@ -16028,19 +16032,19 @@
         <v>48</v>
       </c>
       <c r="F102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="G102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="H102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="I102" s="1" t="str">
-        <f>IF($N102, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N102, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J102&amp;IF($N102, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinyl Methyl Ether Pellets)</v>
       </c>
       <c r="J102" s="1" t="str">
@@ -16077,19 +16081,19 @@
         <v>44</v>
       </c>
       <c r="F103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="G103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="H103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="I103" s="1" t="str">
-        <f>IF($N103, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N103, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J103&amp;IF($N103, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Dichloride Pellets)</v>
       </c>
       <c r="J103" s="1" t="str">
@@ -16126,19 +16130,19 @@
         <v>40</v>
       </c>
       <c r="F104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="G104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="H104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="I104" s="1" t="str">
-        <f>IF($N104, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N104, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J104&amp;IF($N104, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride Pellets)</v>
       </c>
       <c r="J104" s="1" t="str">
@@ -16175,19 +16179,19 @@
         <v>36</v>
       </c>
       <c r="F105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="G105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="H105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="I105" s="1" t="str">
-        <f>IF($N105, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N105, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J105&amp;IF($N105, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (PolyVinylidene Fluoride-Trifluoroethylene Pellets)</v>
       </c>
       <c r="J105" s="1" t="str">
@@ -16227,19 +16231,19 @@
         <v>32</v>
       </c>
       <c r="F106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="G106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="H106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="I106" s="1" t="str">
-        <f>IF($N106, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N106, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J106&amp;IF($N106, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Acrylonitrile Pellets)</v>
       </c>
       <c r="J106" s="1" t="str">
@@ -16279,19 +16283,19 @@
         <v>28</v>
       </c>
       <c r="F107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="G107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="H107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="I107" s="1" t="str">
-        <f>IF($N107, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N107, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J107&amp;IF($N107, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene Rubber Pellets)</v>
       </c>
       <c r="J107" s="1" t="str">
@@ -16331,19 +16335,19 @@
         <v>24</v>
       </c>
       <c r="F108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="G108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="H108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="I108" s="1" t="str">
-        <f>IF($N108, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N108, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J108&amp;IF($N108, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Butadiene-Styrene Pellets)</v>
       </c>
       <c r="J108" s="1" t="str">
@@ -16383,19 +16387,19 @@
         <v>20</v>
       </c>
       <c r="F109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="G109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="H109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="I109" s="1" t="str">
-        <f>IF($N109, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N109, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J109&amp;IF($N109, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Isoprene-Styrene Pellets)</v>
       </c>
       <c r="J109" s="1" t="str">
@@ -16432,19 +16436,19 @@
         <v>16</v>
       </c>
       <c r="F110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="G110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="H110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="I110" s="1" t="str">
-        <f>IF($N110, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N110, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J110&amp;IF($N110, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Styrene-Maleic Anhydride Copolymer Pellets)</v>
       </c>
       <c r="J110" s="1" t="str">
@@ -16484,19 +16488,19 @@
         <v>12</v>
       </c>
       <c r="F111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="G111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="H111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="I111" s="1" t="str">
-        <f>IF($N111, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N111, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J111&amp;IF($N111, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Ultra-High-Molecular-Weight PolyEthylene Pellets)</v>
       </c>
       <c r="J111" s="1" t="str">
@@ -16533,19 +16537,19 @@
         <v>8</v>
       </c>
       <c r="F112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="G112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="H112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="I112" s="1" t="str">
-        <f>IF($N112, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N112, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J112&amp;IF($N112, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Urea-Formaldehyde Polymers Pellets)</v>
       </c>
       <c r="J112" s="1" t="str">
@@ -16585,19 +16589,19 @@
         <v>4</v>
       </c>
       <c r="F113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="G113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="H113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="I113" s="1" t="str">
-        <f>IF($N113, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N113, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J113&amp;IF($N113, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Very-Low-Density PolyEthylene Pellets)</v>
       </c>
       <c r="J113" s="1" t="str">
@@ -16637,19 +16641,19 @@
         <v>0</v>
       </c>
       <c r="F114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="G114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="H114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="I114" s="1" t="str">
-        <f>IF($N114, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N114, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J114&amp;IF($N114, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Vinyl Acetate-Acrylic Acid Pellets)</v>
       </c>
       <c r="J114" s="1" t="str">
@@ -16689,19 +16693,19 @@
         <v>1853</v>
       </c>
       <c r="F115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Bag (Polycaprolactam Pellets)</v>
       </c>
       <c r="G115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Sack (Polycaprolactam Pellets)</v>
       </c>
       <c r="H115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Powder Keg (Polycaprolactam Pellets)</v>
       </c>
       <c r="I115" s="1" t="str">
-        <f>IF($N115, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N115, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J115&amp;IF($N115, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Silo (Polycaprolactam Pellets)</v>
       </c>
       <c r="J115" s="1" t="str">
@@ -16741,19 +16745,19 @@
         <v>2412</v>
       </c>
       <c r="F116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="G116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="H116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="I116" s="1" t="str">
-        <f>IF($N116, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N116, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J116&amp;IF($N116, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Epoxy-Carbon Fiber Resin)</v>
       </c>
       <c r="J116" s="1" t="str">
@@ -16793,19 +16797,19 @@
         <v>2416</v>
       </c>
       <c r="F117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="G117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="H117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="I117" s="1" t="str">
-        <f>IF($N117, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N117, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J117&amp;IF($N117, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Phenolic-Carbon Fiber Resin)</v>
       </c>
       <c r="J117" s="1" t="str">
@@ -16845,19 +16849,19 @@
         <v>2420</v>
       </c>
       <c r="F118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Negative Photoresist)</v>
       </c>
       <c r="G118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Negative Photoresist)</v>
       </c>
       <c r="H118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Negative Photoresist)</v>
       </c>
       <c r="I118" s="1" t="str">
-        <f>IF($N118, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N118, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J118&amp;IF($N118, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Negative Photoresist)</v>
       </c>
       <c r="J118" s="1" t="str">
@@ -16897,19 +16901,19 @@
         <v>2424</v>
       </c>
       <c r="F119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$35, [1]Enums!$A$36)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$36, [1]Enums!$A$37)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Vial (Positive Photoresist)</v>
       </c>
       <c r="G119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$38, [1]Enums!$A$39)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$39, [1]Enums!$A$40)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Beaker (Positive Photoresist)</v>
       </c>
       <c r="H119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$41, [1]Enums!$A$42)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$42, [1]Enums!$A$43)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Drum (Positive Photoresist)</v>
       </c>
       <c r="I119" s="1" t="str">
-        <f>IF($N119, [1]Enums!$A$44, [1]Enums!$A$45)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
+        <f>IF($N119, [1]Enums!$A$45, [1]Enums!$A$46)&amp;" ("&amp;$J119&amp;IF($N119, " "&amp;$J$1, "")&amp;")"</f>
         <v>Chemical Vat (Positive Photoresist)</v>
       </c>
       <c r="J119" s="1" t="str">
@@ -17824,11 +17828,11 @@
         <v>2651</v>
       </c>
       <c r="C1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="D1" s="7" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$84</f>
+        <f xml:space="preserve"> [1]Enums!$B$85</f>
         <v>Mold Type</v>
       </c>
       <c r="E1" s="19" t="str">
@@ -17864,7 +17868,7 @@
         <v>Mask (Solar Cell)(PR Backplane)</v>
       </c>
       <c r="D2" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E2" s="15" t="str">
@@ -17888,7 +17892,7 @@
         <v>Mask (Solar Cell)(PR Semiconductor)</v>
       </c>
       <c r="D3" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E3" s="15" t="str">
@@ -17912,7 +17916,7 @@
         <v>Mask (Solar Cell)(PR Dielectric)</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E4" s="15" t="str">
@@ -17936,7 +17940,7 @@
         <v>Mask (Solar Cell)(PR Traces)</v>
       </c>
       <c r="D5" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E5" s="15" t="str">
@@ -17960,7 +17964,7 @@
         <v>Mask (Solar Cell)(PR Encapsulation)</v>
       </c>
       <c r="D6" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E6" s="15" t="str">
@@ -17984,7 +17988,7 @@
         <v>Mask (Processor)(PR Backplane)</v>
       </c>
       <c r="D7" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E7" s="15" t="str">
@@ -18008,7 +18012,7 @@
         <v>Mask (Processor)(PR n-Type Semiconductor)</v>
       </c>
       <c r="D8" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E8" s="15" t="str">
@@ -18032,7 +18036,7 @@
         <v>Mask (Processor)(PR p-Type Semiconductor)</v>
       </c>
       <c r="D9" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E9" s="15" t="str">
@@ -18056,7 +18060,7 @@
         <v>Mask (Processor)(PR Dielectric)</v>
       </c>
       <c r="D10" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E10" s="15" t="str">
@@ -18080,7 +18084,7 @@
         <v>Mask (Processor)(PR Inner Traces)</v>
       </c>
       <c r="D11" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E11" s="15" t="str">
@@ -18104,7 +18108,7 @@
         <v>Mask (Processor)(PR Through Vias)</v>
       </c>
       <c r="D12" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E12" s="15" t="str">
@@ -18128,7 +18132,7 @@
         <v>Mask (Processor)(PR Outer Traces)</v>
       </c>
       <c r="D13" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E13" s="15" t="str">
@@ -18152,7 +18156,7 @@
         <v>Mask (Processor)(PR Encapsulation)</v>
       </c>
       <c r="D14" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E14" s="15" t="str">
@@ -18176,7 +18180,7 @@
         <v>Mask (Temperature Sensor)(PR Backplane)</v>
       </c>
       <c r="D15" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E15" s="15" t="str">
@@ -18200,7 +18204,7 @@
         <v>Mask (Temperature Sensor)(PR Semiconductor)</v>
       </c>
       <c r="D16" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E16" s="15" t="str">
@@ -18224,7 +18228,7 @@
         <v>Mask (Temperature Sensor)(PR Dielectric)</v>
       </c>
       <c r="D17" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E17" s="15" t="str">
@@ -18248,7 +18252,7 @@
         <v>Mask (Temperature Sensor)(PR Traces)</v>
       </c>
       <c r="D18" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E18" s="15" t="str">
@@ -18272,7 +18276,7 @@
         <v>Mask (Temperature Sensor)(PR Encapsulation)</v>
       </c>
       <c r="D19" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E19" s="15" t="str">
@@ -18296,7 +18300,7 @@
         <v>Mask (Pressure Sensor)(PR Backplane)</v>
       </c>
       <c r="D20" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E20" s="15" t="str">
@@ -18320,7 +18324,7 @@
         <v>Mask (Pressure Sensor)(PR Semiconductor)</v>
       </c>
       <c r="D21" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E21" s="15" t="str">
@@ -18344,7 +18348,7 @@
         <v>Mask (Pressure Sensor)(PR Dielectric)</v>
       </c>
       <c r="D22" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E22" s="15" t="str">
@@ -18368,7 +18372,7 @@
         <v>Mask (Pressure Sensor)(PR Traces)</v>
       </c>
       <c r="D23" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E23" s="15" t="str">
@@ -18392,7 +18396,7 @@
         <v>Mask (Pressure Sensor)(PR Encapsulation)</v>
       </c>
       <c r="D24" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E24" s="15" t="str">
@@ -18416,7 +18420,7 @@
         <v>Mask (Low Power Radio)(PR Backplane)</v>
       </c>
       <c r="D25" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E25" s="15" t="str">
@@ -18440,7 +18444,7 @@
         <v>Mask (Low Power Radio)(PR n-Type Semiconductor)</v>
       </c>
       <c r="D26" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E26" s="15" t="str">
@@ -18464,7 +18468,7 @@
         <v>Mask (Low Power Radio)(PR p-Type Semiconductor)</v>
       </c>
       <c r="D27" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E27" s="15" t="str">
@@ -18488,7 +18492,7 @@
         <v>Mask (Low Power Radio)(PR Dielectric)</v>
       </c>
       <c r="D28" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E28" s="15" t="str">
@@ -18512,7 +18516,7 @@
         <v>Mask (Low Power Radio)(PR Inner Traces)</v>
       </c>
       <c r="D29" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E29" s="15" t="str">
@@ -18536,7 +18540,7 @@
         <v>Mask (Low Power Radio)(PR Through Vias)</v>
       </c>
       <c r="D30" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E30" s="15" t="str">
@@ -18560,7 +18564,7 @@
         <v>Mask (Low Power Radio)(PR Outer Traces)</v>
       </c>
       <c r="D31" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E31" s="15" t="str">
@@ -18584,7 +18588,7 @@
         <v>Mask (Low Power Radio)(PR Encapsulation)</v>
       </c>
       <c r="D32" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E32" s="15" t="str">
@@ -18608,7 +18612,7 @@
         <v>Mask (DSP)(PR Backplane)</v>
       </c>
       <c r="D33" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E33" s="15" t="str">
@@ -18632,7 +18636,7 @@
         <v>Mask (DSP)(PR n-Type Semiconductor)</v>
       </c>
       <c r="D34" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E34" s="15" t="str">
@@ -18656,7 +18660,7 @@
         <v>Mask (DSP)(PR p-Type Semiconductor)</v>
       </c>
       <c r="D35" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E35" s="15" t="str">
@@ -18680,7 +18684,7 @@
         <v>Mask (DSP)(PR Dielectric)</v>
       </c>
       <c r="D36" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E36" s="15" t="str">
@@ -18704,7 +18708,7 @@
         <v>Mask (DSP)(PR Inner Traces)</v>
       </c>
       <c r="D37" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E37" s="15" t="str">
@@ -18728,7 +18732,7 @@
         <v>Mask (DSP)(PR Through Vias)</v>
       </c>
       <c r="D38" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E38" s="15" t="str">
@@ -18752,7 +18756,7 @@
         <v>Mask (DSP)(PR Outer Traces)</v>
       </c>
       <c r="D39" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E39" s="15" t="str">
@@ -18776,7 +18780,7 @@
         <v>Mask (DSP)(PR Encapsulation)</v>
       </c>
       <c r="D40" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E40" s="15" t="str">
@@ -18800,7 +18804,7 @@
         <v>Mask (Digital Analog Convertor)(PR Backplane)</v>
       </c>
       <c r="D41" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E41" s="15" t="str">
@@ -18824,7 +18828,7 @@
         <v>Mask (Digital Analog Convertor)(PR Semiconductor)</v>
       </c>
       <c r="D42" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E42" s="15" t="str">
@@ -18848,7 +18852,7 @@
         <v>Mask (Digital Analog Convertor)(PR Dielectric)</v>
       </c>
       <c r="D43" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E43" s="15" t="str">
@@ -18872,7 +18876,7 @@
         <v>Mask (Digital Analog Convertor)(PR Traces)</v>
       </c>
       <c r="D44" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E44" s="15" t="str">
@@ -18896,7 +18900,7 @@
         <v>Mask (Digital Analog Convertor)(PR Encapsulation)</v>
       </c>
       <c r="D45" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E45" s="15" t="str">
@@ -18920,7 +18924,7 @@
         <v>Mask (Amplifier)(PR Backplane)</v>
       </c>
       <c r="D46" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E46" s="15" t="str">
@@ -18944,7 +18948,7 @@
         <v>Mask (Amplifier)(PR Semiconductor)</v>
       </c>
       <c r="D47" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E47" s="15" t="str">
@@ -18968,7 +18972,7 @@
         <v>Mask (Amplifier)(PR Dielectric)</v>
       </c>
       <c r="D48" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E48" s="15" t="str">
@@ -18992,7 +18996,7 @@
         <v>Mask (Amplifier)(PR Traces)</v>
       </c>
       <c r="D49" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E49" s="15" t="str">
@@ -19016,7 +19020,7 @@
         <v>Mask (Amplifier)(PR Encapsulation)</v>
       </c>
       <c r="D50" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E50" s="15" t="str">
@@ -19040,7 +19044,7 @@
         <v>Mask (OLED Array)(PR Backplane)</v>
       </c>
       <c r="D51" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E51" s="15" t="str">
@@ -19064,7 +19068,7 @@
         <v>Mask (OLED Array)(PR Semiconductor)</v>
       </c>
       <c r="D52" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E52" s="15" t="str">
@@ -19088,7 +19092,7 @@
         <v>Mask (OLED Array)(PR Dielectric)</v>
       </c>
       <c r="D53" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E53" s="15" t="str">
@@ -19112,7 +19116,7 @@
         <v>Mask (OLED Array)(PR Traces)</v>
       </c>
       <c r="D54" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E54" s="15" t="str">
@@ -19136,7 +19140,7 @@
         <v>Mask (OLED Array)(PR Encapsulation)</v>
       </c>
       <c r="D55" s="10" t="str">
-        <f xml:space="preserve"> [1]Enums!$B$97</f>
+        <f xml:space="preserve"> [1]Enums!$B$98</f>
         <v>Mask</v>
       </c>
       <c r="E55" s="15" t="str">
@@ -25386,7 +25390,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I2" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H2, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Steel</v>
       </c>
       <c r="J2" s="45">
@@ -25434,7 +25438,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I3" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H3, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Stainless Steel</v>
       </c>
       <c r="J3" s="45">
@@ -25482,7 +25486,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I4" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H4, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Brass</v>
       </c>
       <c r="J4" s="45">
@@ -25530,7 +25534,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I5" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H5, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Bronze</v>
       </c>
       <c r="J5" s="45">
@@ -25578,7 +25582,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I6" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H6, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Tungsten Carbide</v>
       </c>
       <c r="J6" s="45">
@@ -25626,7 +25630,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I7" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H7, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Nichrome</v>
       </c>
       <c r="J7" s="45">
@@ -25674,7 +25678,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I8" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H8, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Composite Antimony-Lead</v>
       </c>
       <c r="J8" s="45">
@@ -25722,7 +25726,7 @@
         <v>Steel Ingot</v>
       </c>
       <c r="I9" s="45" t="str">
-        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$152&amp;" "&amp;VLOOKUP(H9, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Steel</v>
       </c>
       <c r="J9" s="45">
@@ -25770,7 +25774,7 @@
         <v>Stainless Steel Ingot</v>
       </c>
       <c r="I10" s="45" t="str">
-        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$152&amp;" "&amp;VLOOKUP(H10, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Stainless Steel</v>
       </c>
       <c r="J10" s="45">
@@ -25818,7 +25822,7 @@
         <v>Brass Ingot</v>
       </c>
       <c r="I11" s="45" t="str">
-        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$152&amp;" "&amp;VLOOKUP(H11, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Brass</v>
       </c>
       <c r="J11" s="45">
@@ -25866,7 +25870,7 @@
         <v>Bronze Ingot</v>
       </c>
       <c r="I12" s="45" t="str">
-        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$152&amp;" "&amp;VLOOKUP(H12, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Bronze</v>
       </c>
       <c r="J12" s="45">
@@ -25914,7 +25918,7 @@
         <v>Tungsten Carbide Ingot</v>
       </c>
       <c r="I13" s="45" t="str">
-        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$152&amp;" "&amp;VLOOKUP(H13, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Tungsten Carbide</v>
       </c>
       <c r="J13" s="45">
@@ -25962,7 +25966,7 @@
         <v>Nichrome Ingot</v>
       </c>
       <c r="I14" s="45" t="str">
-        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$152&amp;" "&amp;VLOOKUP(H14, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Nichrome</v>
       </c>
       <c r="J14" s="45">
@@ -26010,7 +26014,7 @@
         <v>Antimony-Lead Ingot</v>
       </c>
       <c r="I15" s="45" t="str">
-        <f>[1]Enums!$A$151&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
+        <f>[1]Enums!$A$152&amp;" "&amp;VLOOKUP(H15, [2]Ingots!$C$2:$E$39, 3,FALSE)</f>
         <v>Engineered Antimony-Lead</v>
       </c>
       <c r="J15" s="45">
@@ -26058,7 +26062,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I16" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" Iron"</f>
+        <f>[1]Enums!$A$151&amp;" Iron"</f>
         <v>Composite Iron</v>
       </c>
       <c r="J16" s="45">
@@ -26106,7 +26110,7 @@
         <v>Iron Ingot</v>
       </c>
       <c r="I17" s="45" t="str">
-        <f>[1]Enums!$A$151&amp;" Iron"</f>
+        <f>[1]Enums!$A$152&amp;" Iron"</f>
         <v>Engineered Iron</v>
       </c>
       <c r="J17" s="45">
@@ -26154,7 +26158,7 @@
         <v>Diamond</v>
       </c>
       <c r="I18" s="45" t="str">
-        <f>[1]Enums!$A$150&amp;" Diamond"</f>
+        <f>[1]Enums!$A$151&amp;" Diamond"</f>
         <v>Composite Diamond</v>
       </c>
       <c r="J18" s="45">
@@ -26202,7 +26206,7 @@
         <v>Diamond</v>
       </c>
       <c r="I19" s="45" t="str">
-        <f>[1]Enums!$A$151&amp;" Diamond"</f>
+        <f>[1]Enums!$A$152&amp;" Diamond"</f>
         <v>Engineered Diamond</v>
       </c>
       <c r="J19" s="45">
@@ -26503,7 +26507,7 @@
         <v>Molded Item</v>
       </c>
       <c r="F1" s="36" t="str">
-        <f xml:space="preserve"> [1]Enums!$A$115</f>
+        <f xml:space="preserve"> [1]Enums!$A$116</f>
         <v>Base Material</v>
       </c>
       <c r="G1" s="30" t="s">
@@ -26531,7 +26535,7 @@
         <v>1812</v>
       </c>
       <c r="C2" s="22" t="str">
-        <f>[1]Enums!$A$112&amp;" "&amp;D2</f>
+        <f>[1]Enums!$A$113&amp;" "&amp;D2</f>
         <v>Gripped Iron Shovel</v>
       </c>
       <c r="D2" s="24" t="str">
@@ -26543,7 +26547,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F2" s="34" t="str">
-        <f>[1]Enums!$A$118</f>
+        <f>[1]Enums!$A$119</f>
         <v>Iron</v>
       </c>
       <c r="G2" s="24">
@@ -26568,7 +26572,7 @@
         <v>1811</v>
       </c>
       <c r="C3" s="22" t="str">
-        <f>[1]Enums!$A$112&amp;" "&amp;D3</f>
+        <f>[1]Enums!$A$113&amp;" "&amp;D3</f>
         <v>Gripped Iron Pickaxe</v>
       </c>
       <c r="D3" s="21" t="str">
@@ -26580,7 +26584,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F3" s="34" t="str">
-        <f>[1]Enums!$A$118</f>
+        <f>[1]Enums!$A$119</f>
         <v>Iron</v>
       </c>
       <c r="G3" s="24">
@@ -26605,7 +26609,7 @@
         <v>1810</v>
       </c>
       <c r="C4" s="22" t="str">
-        <f>[1]Enums!$A$112&amp;" "&amp;D4</f>
+        <f>[1]Enums!$A$113&amp;" "&amp;D4</f>
         <v>Gripped Iron Axe</v>
       </c>
       <c r="D4" s="21" t="str">
@@ -26617,7 +26621,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F4" s="34" t="str">
-        <f>[1]Enums!$A$118</f>
+        <f>[1]Enums!$A$119</f>
         <v>Iron</v>
       </c>
       <c r="G4" s="24">
@@ -26642,7 +26646,7 @@
         <v>1809</v>
       </c>
       <c r="C5" s="22" t="str">
-        <f>[1]Enums!$A$112&amp;" "&amp;D5</f>
+        <f>[1]Enums!$A$113&amp;" "&amp;D5</f>
         <v>Gripped Iron Sword</v>
       </c>
       <c r="D5" s="21" t="str">
@@ -26654,7 +26658,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F5" s="34" t="str">
-        <f>[1]Enums!$A$118</f>
+        <f>[1]Enums!$A$119</f>
         <v>Iron</v>
       </c>
       <c r="G5" s="24">
@@ -26679,7 +26683,7 @@
         <v>1808</v>
       </c>
       <c r="C6" s="22" t="str">
-        <f>[1]Enums!$A$112&amp;" "&amp;D6</f>
+        <f>[1]Enums!$A$113&amp;" "&amp;D6</f>
         <v>Gripped Wooden Sword</v>
       </c>
       <c r="D6" s="21" t="str">
@@ -26691,7 +26695,7 @@
         <v>Grip (Natural Rubber)</v>
       </c>
       <c r="F6" s="34" t="str">
-        <f>[1]Enums!$A$116</f>
+        <f>[1]Enums!$A$117</f>
         <v>Wooden</v>
       </c>
       <c r="G6" s="24">
@@ -26716,7 +26720,7 @@
         <v>1807</v>
       </c>
       <c r="C7" s="22" t="str">
-        <f>[1]Enums!$A$112&amp;" "&amp;D7</f>
+        <f>[1]Enums!$A$113&amp;" "&amp;D7</f>
         <v>Gripped Wooden Shovel</v>
       </c>
       <c r="D7" s="21" t="str">
@@ -26728,7 +26732,7 @@
         <v>Gri